<commit_message>
Att até o jogo 6
Corrigido o nome do Atlético Madrid. Corrigida largura das colunas de gols marcados, sofridos e saldo.
+ Minor changes.
</commit_message>
<xml_diff>
--- a/Mundial de Clubes FIFA 2025.xlsx
+++ b/Mundial de Clubes FIFA 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjunior\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CFD63883-BBEB-4B6C-AA07-4BB8366F3CB2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{890005AA-DE05-4B21-98EB-AFF6787F7368}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="1185" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{076F3B28-812E-4458-A424-96085A053123}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="565" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="112">
   <si>
     <t>Times</t>
   </si>
@@ -330,9 +330,6 @@
     <t>Inter Miami</t>
   </si>
   <si>
-    <t>Atlétido de Madrid</t>
-  </si>
-  <si>
     <t>II</t>
   </si>
   <si>
@@ -364,6 +361,9 @@
   </si>
   <si>
     <t>Los Angeles FC</t>
+  </si>
+  <si>
+    <t>2025 Mundial de Clubes FIFA</t>
   </si>
 </sst>
 </file>
@@ -1106,7 +1106,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="183">
+  <cellXfs count="185">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1609,6 +1609,12 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2083,13 +2089,6 @@
       </border>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="4" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="6" tint="0.79998168889431442"/>
@@ -2111,6 +2110,13 @@
         <vertical/>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="4" tint="-0.24994659260841701"/>
+      </font>
     </dxf>
     <dxf>
       <fill>
@@ -2949,10 +2955,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC3FB449-6DA7-4D03-B64B-1C2132537955}">
-  <dimension ref="B1:D34"/>
+  <dimension ref="B1:F35"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -2964,167 +2970,165 @@
     <col min="5" max="16384" width="9.140625" style="119"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="101" t="s">
+    <row r="1" spans="2:6" ht="22.5" x14ac:dyDescent="0.3">
+      <c r="B1" s="183" t="s">
+        <v>111</v>
+      </c>
+      <c r="C1" s="184"/>
+      <c r="D1" s="184"/>
+      <c r="E1" s="184"/>
+      <c r="F1" s="184"/>
+    </row>
+    <row r="2" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B3" s="101" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="102" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" s="103" t="s">
+      <c r="C3" s="102" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="103" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="104">
+    <row r="4" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="104">
         <v>1</v>
       </c>
-      <c r="C3" s="170" t="s">
+      <c r="C4" s="170" t="s">
         <v>69</v>
-      </c>
-      <c r="D3" s="106" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="104">
-        <v>2</v>
-      </c>
-      <c r="C4" s="171" t="s">
-        <v>70</v>
       </c>
       <c r="D4" s="106" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="104">
-        <v>3</v>
-      </c>
-      <c r="C5" s="170" t="s">
-        <v>71</v>
+        <v>2</v>
+      </c>
+      <c r="C5" s="171" t="s">
+        <v>70</v>
       </c>
       <c r="D5" s="106" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="6" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="104">
-        <v>4</v>
-      </c>
-      <c r="C6" s="171" t="s">
-        <v>72</v>
+        <v>3</v>
+      </c>
+      <c r="C6" s="170" t="s">
+        <v>71</v>
       </c>
       <c r="D6" s="106" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="104">
-        <v>5</v>
-      </c>
-      <c r="C7" s="170" t="s">
-        <v>73</v>
+        <v>4</v>
+      </c>
+      <c r="C7" s="171" t="s">
+        <v>72</v>
       </c>
       <c r="D7" s="106" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="104">
-        <v>6</v>
-      </c>
-      <c r="C8" s="171" t="s">
-        <v>74</v>
+        <v>5</v>
+      </c>
+      <c r="C8" s="170" t="s">
+        <v>73</v>
       </c>
       <c r="D8" s="106" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="104">
-        <v>7</v>
-      </c>
-      <c r="C9" s="170" t="s">
-        <v>75</v>
+        <v>6</v>
+      </c>
+      <c r="C9" s="171" t="s">
+        <v>74</v>
       </c>
       <c r="D9" s="106" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="104">
-        <v>8</v>
-      </c>
-      <c r="C10" s="171" t="s">
-        <v>76</v>
+        <v>7</v>
+      </c>
+      <c r="C10" s="170" t="s">
+        <v>75</v>
       </c>
       <c r="D10" s="106" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="104">
-        <v>9</v>
-      </c>
-      <c r="C11" s="170" t="s">
-        <v>77</v>
+        <v>8</v>
+      </c>
+      <c r="C11" s="171" t="s">
+        <v>76</v>
       </c>
       <c r="D11" s="106" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="104">
-        <v>10</v>
-      </c>
-      <c r="C12" s="171" t="s">
-        <v>78</v>
+        <v>9</v>
+      </c>
+      <c r="C12" s="170" t="s">
+        <v>77</v>
       </c>
       <c r="D12" s="106" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="104">
-        <v>11</v>
-      </c>
-      <c r="C13" s="170" t="s">
-        <v>79</v>
+        <v>10</v>
+      </c>
+      <c r="C13" s="171" t="s">
+        <v>78</v>
       </c>
       <c r="D13" s="106" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="14" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="104">
-        <v>12</v>
-      </c>
-      <c r="C14" s="171" t="s">
-        <v>80</v>
+        <v>11</v>
+      </c>
+      <c r="C14" s="170" t="s">
+        <v>79</v>
       </c>
       <c r="D14" s="106" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="104">
+        <v>12</v>
+      </c>
+      <c r="C15" s="171" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="106" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="104">
         <v>13</v>
       </c>
-      <c r="C15" s="170" t="s">
+      <c r="C16" s="170" t="s">
         <v>81</v>
-      </c>
-      <c r="D15" s="106" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="16" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="104">
-        <v>14</v>
-      </c>
-      <c r="C16" s="171" t="s">
-        <v>82</v>
       </c>
       <c r="D16" s="106" t="s">
         <v>6</v>
@@ -3132,10 +3136,10 @@
     </row>
     <row r="17" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="104">
-        <v>15</v>
-      </c>
-      <c r="C17" s="170" t="s">
-        <v>83</v>
+        <v>14</v>
+      </c>
+      <c r="C17" s="171" t="s">
+        <v>82</v>
       </c>
       <c r="D17" s="106" t="s">
         <v>6</v>
@@ -3143,10 +3147,10 @@
     </row>
     <row r="18" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="104">
-        <v>16</v>
-      </c>
-      <c r="C18" s="171" t="s">
-        <v>84</v>
+        <v>15</v>
+      </c>
+      <c r="C18" s="170" t="s">
+        <v>83</v>
       </c>
       <c r="D18" s="106" t="s">
         <v>6</v>
@@ -3154,10 +3158,10 @@
     </row>
     <row r="19" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="104">
-        <v>17</v>
-      </c>
-      <c r="C19" s="170" t="s">
-        <v>85</v>
+        <v>16</v>
+      </c>
+      <c r="C19" s="171" t="s">
+        <v>84</v>
       </c>
       <c r="D19" s="106" t="s">
         <v>6</v>
@@ -3165,10 +3169,10 @@
     </row>
     <row r="20" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="104">
-        <v>18</v>
-      </c>
-      <c r="C20" s="171" t="s">
-        <v>86</v>
+        <v>17</v>
+      </c>
+      <c r="C20" s="170" t="s">
+        <v>85</v>
       </c>
       <c r="D20" s="106" t="s">
         <v>6</v>
@@ -3176,21 +3180,21 @@
     </row>
     <row r="21" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="104">
-        <v>19</v>
-      </c>
-      <c r="C21" s="170" t="s">
-        <v>87</v>
+        <v>18</v>
+      </c>
+      <c r="C21" s="171" t="s">
+        <v>86</v>
       </c>
       <c r="D21" s="106" t="s">
-        <v>3</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="104">
-        <v>20</v>
-      </c>
-      <c r="C22" s="171" t="s">
-        <v>88</v>
+        <v>19</v>
+      </c>
+      <c r="C22" s="170" t="s">
+        <v>87</v>
       </c>
       <c r="D22" s="106" t="s">
         <v>3</v>
@@ -3198,10 +3202,10 @@
     </row>
     <row r="23" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="104">
-        <v>21</v>
-      </c>
-      <c r="C23" s="170" t="s">
-        <v>89</v>
+        <v>20</v>
+      </c>
+      <c r="C23" s="171" t="s">
+        <v>88</v>
       </c>
       <c r="D23" s="106" t="s">
         <v>3</v>
@@ -3209,10 +3213,10 @@
     </row>
     <row r="24" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="104">
-        <v>22</v>
-      </c>
-      <c r="C24" s="171" t="s">
-        <v>90</v>
+        <v>21</v>
+      </c>
+      <c r="C24" s="170" t="s">
+        <v>89</v>
       </c>
       <c r="D24" s="106" t="s">
         <v>3</v>
@@ -3220,21 +3224,21 @@
     </row>
     <row r="25" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="104">
-        <v>23</v>
-      </c>
-      <c r="C25" s="170" t="s">
-        <v>91</v>
+        <v>22</v>
+      </c>
+      <c r="C25" s="171" t="s">
+        <v>90</v>
       </c>
       <c r="D25" s="106" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="104">
-        <v>24</v>
-      </c>
-      <c r="C26" s="171" t="s">
-        <v>92</v>
+        <v>23</v>
+      </c>
+      <c r="C26" s="170" t="s">
+        <v>91</v>
       </c>
       <c r="D26" s="106" t="s">
         <v>4</v>
@@ -3242,10 +3246,10 @@
     </row>
     <row r="27" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="104">
-        <v>25</v>
-      </c>
-      <c r="C27" s="170" t="s">
-        <v>93</v>
+        <v>24</v>
+      </c>
+      <c r="C27" s="171" t="s">
+        <v>92</v>
       </c>
       <c r="D27" s="106" t="s">
         <v>4</v>
@@ -3253,10 +3257,10 @@
     </row>
     <row r="28" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="104">
-        <v>26</v>
-      </c>
-      <c r="C28" s="171" t="s">
-        <v>94</v>
+        <v>25</v>
+      </c>
+      <c r="C28" s="170" t="s">
+        <v>93</v>
       </c>
       <c r="D28" s="106" t="s">
         <v>4</v>
@@ -3264,21 +3268,21 @@
     </row>
     <row r="29" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="104">
-        <v>27</v>
-      </c>
-      <c r="C29" s="170" t="s">
-        <v>95</v>
+        <v>26</v>
+      </c>
+      <c r="C29" s="171" t="s">
+        <v>94</v>
       </c>
       <c r="D29" s="106" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="30" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="104">
-        <v>28</v>
-      </c>
-      <c r="C30" s="171" t="s">
-        <v>96</v>
+        <v>27</v>
+      </c>
+      <c r="C30" s="170" t="s">
+        <v>95</v>
       </c>
       <c r="D30" s="106" t="s">
         <v>5</v>
@@ -3286,10 +3290,10 @@
     </row>
     <row r="31" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="104">
-        <v>29</v>
-      </c>
-      <c r="C31" s="170" t="s">
-        <v>97</v>
+        <v>28</v>
+      </c>
+      <c r="C31" s="171" t="s">
+        <v>96</v>
       </c>
       <c r="D31" s="106" t="s">
         <v>5</v>
@@ -3297,10 +3301,10 @@
     </row>
     <row r="32" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="104">
-        <v>30</v>
-      </c>
-      <c r="C32" s="171" t="s">
-        <v>111</v>
+        <v>29</v>
+      </c>
+      <c r="C32" s="170" t="s">
+        <v>97</v>
       </c>
       <c r="D32" s="106" t="s">
         <v>5</v>
@@ -3308,23 +3312,34 @@
     </row>
     <row r="33" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B33" s="104">
+        <v>30</v>
+      </c>
+      <c r="C33" s="171" t="s">
+        <v>110</v>
+      </c>
+      <c r="D33" s="106" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="34" spans="2:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="104">
         <v>31</v>
       </c>
-      <c r="C33" s="170" t="s">
+      <c r="C34" s="170" t="s">
         <v>98</v>
       </c>
-      <c r="D33" s="106" t="s">
+      <c r="D34" s="106" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="34" spans="2:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="105">
+    <row r="35" spans="2:4" ht="14.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="105">
         <v>32</v>
       </c>
-      <c r="C34" s="172" t="s">
+      <c r="C35" s="172" t="s">
         <v>99</v>
       </c>
-      <c r="D34" s="107" t="s">
+      <c r="D35" s="107" t="s">
         <v>67</v>
       </c>
     </row>
@@ -3361,7 +3376,7 @@
   <sheetData>
     <row r="1" spans="2:12" ht="22.5" x14ac:dyDescent="0.3">
       <c r="B1" s="120" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C1" s="120"/>
       <c r="D1" s="120"/>
@@ -3456,7 +3471,7 @@
         <v>2</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>100</v>
+        <v>79</v>
       </c>
       <c r="H7" s="6">
         <v>2</v>
@@ -3520,7 +3535,7 @@
         <v>4</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="2:12" ht="15" thickBot="1" x14ac:dyDescent="0.25"/>
@@ -4004,7 +4019,7 @@
   <dimension ref="A1:AN50"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4036,7 +4051,8 @@
     <col min="30" max="30" width="3" style="29" hidden="1" customWidth="1"/>
     <col min="31" max="31" width="2.7109375" style="29" customWidth="1"/>
     <col min="32" max="32" width="22.7109375" style="29" customWidth="1"/>
-    <col min="33" max="40" width="3.7109375" style="29" customWidth="1"/>
+    <col min="33" max="37" width="3.7109375" style="29" customWidth="1"/>
+    <col min="38" max="40" width="4.7109375" style="29" customWidth="1"/>
     <col min="41" max="41" width="9.140625" style="29"/>
     <col min="42" max="42" width="3.7109375" style="29" customWidth="1"/>
     <col min="43" max="43" width="20.7109375" style="29" customWidth="1"/>
@@ -4046,7 +4062,7 @@
     <row r="1" spans="1:40" s="95" customFormat="1" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="94"/>
       <c r="B1" s="96" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C1" s="96"/>
       <c r="D1" s="96"/>
@@ -4160,11 +4176,15 @@
         <f>P5</f>
         <v>Palmeiras</v>
       </c>
-      <c r="F3" s="21"/>
+      <c r="F3" s="21">
+        <v>0</v>
+      </c>
       <c r="G3" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="21"/>
+      <c r="H3" s="21">
+        <v>0</v>
+      </c>
       <c r="I3" s="13" t="str">
         <f>P6</f>
         <v>Porto</v>
@@ -4175,11 +4195,11 @@
       </c>
       <c r="K3" s="43" t="str">
         <f t="shared" ref="K3:K34" si="1">IF(F3="","",IF(H3="","",IF(J3="empate",E3,"")))</f>
-        <v/>
+        <v>Palmeiras</v>
       </c>
       <c r="L3" s="43" t="str">
         <f t="shared" ref="L3:L34" si="2">IF(E3="","",IF(F3="","",IF(M3="empate",I3,"")))</f>
-        <v/>
+        <v>Porto</v>
       </c>
       <c r="M3" s="44" t="str">
         <f t="shared" ref="M3:M34" si="3">IF(F3=H3,"empate",IF(F3&lt;H3,E3,I3))</f>
@@ -4232,11 +4252,15 @@
         <f>P7</f>
         <v>Al-Ahly</v>
       </c>
-      <c r="F4" s="21"/>
+      <c r="F4" s="21">
+        <v>0</v>
+      </c>
       <c r="G4" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H4" s="21"/>
+      <c r="H4" s="21">
+        <v>0</v>
+      </c>
       <c r="I4" s="13" t="str">
         <f>P8</f>
         <v>Inter Miami</v>
@@ -4247,11 +4271,11 @@
       </c>
       <c r="K4" s="43" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Al-Ahly</v>
       </c>
       <c r="L4" s="43" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>Inter Miami</v>
       </c>
       <c r="M4" s="44" t="str">
         <f t="shared" si="3"/>
@@ -4386,11 +4410,11 @@
       </c>
       <c r="Q5" s="43">
         <f>(S5*3)+(T5*1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R5" s="43">
         <f>SUM(S5:U5)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S5" s="43">
         <f>COUNTIF(J:J,P5)</f>
@@ -4398,7 +4422,7 @@
       </c>
       <c r="T5" s="43">
         <f>COUNTIF(K:K,P5)+COUNTIF(L:L,P5)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U5" s="43">
         <f>COUNTIF(M:M,P5)</f>
@@ -4445,11 +4469,11 @@
       </c>
       <c r="AG5" s="90">
         <f>VLOOKUP($AE5,$O$5:$X$8,3,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH5" s="90">
         <f>VLOOKUP($AE5,$O$5:$X$8,4,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI5" s="90">
         <f>VLOOKUP($AE5,$O$5:$X$8,5,FALSE)</f>
@@ -4457,7 +4481,7 @@
       </c>
       <c r="AJ5" s="90">
         <f>VLOOKUP($AE5,$O$5:$X$8,6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK5" s="90">
         <f>VLOOKUP($AE5,$O$5:$X$8,7,FALSE)</f>
@@ -4527,11 +4551,11 @@
       </c>
       <c r="Q6" s="43">
         <f t="shared" ref="Q6:Q8" si="5">(S6*3)+(T6*1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R6" s="43">
         <f t="shared" ref="R6:R8" si="6">SUM(S6:U6)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S6" s="43">
         <f>COUNTIF(J:J,P6)</f>
@@ -4539,7 +4563,7 @@
       </c>
       <c r="T6" s="43">
         <f>COUNTIF(K:K,P6)+COUNTIF(L:L,P6)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U6" s="43">
         <f>COUNTIF(M:M,P6)</f>
@@ -4586,11 +4610,11 @@
       </c>
       <c r="AG6" s="90">
         <f t="shared" ref="AG6:AG8" si="13">VLOOKUP($AE6,$O$5:$X$8,3,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH6" s="90">
         <f t="shared" ref="AH6:AH8" si="14">VLOOKUP($AE6,$O$5:$X$8,4,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI6" s="90">
         <f t="shared" ref="AI6:AI8" si="15">VLOOKUP($AE6,$O$5:$X$8,5,FALSE)</f>
@@ -4598,7 +4622,7 @@
       </c>
       <c r="AJ6" s="90">
         <f t="shared" ref="AJ6:AJ8" si="16">VLOOKUP($AE6,$O$5:$X$8,6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK6" s="90">
         <f t="shared" ref="AK6:AK8" si="17">VLOOKUP($AE6,$O$5:$X$8,7,FALSE)</f>
@@ -4668,11 +4692,11 @@
       </c>
       <c r="Q7" s="43">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R7" s="43">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S7" s="43">
         <f>COUNTIF(J:J,P7)</f>
@@ -4680,7 +4704,7 @@
       </c>
       <c r="T7" s="43">
         <f>COUNTIF(K:K,P7)+COUNTIF(L:L,P7)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U7" s="43">
         <f>COUNTIF(M:M,P7)</f>
@@ -4727,11 +4751,11 @@
       </c>
       <c r="AG7" s="90">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH7" s="90">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI7" s="90">
         <f t="shared" si="15"/>
@@ -4739,7 +4763,7 @@
       </c>
       <c r="AJ7" s="90">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK7" s="90">
         <f t="shared" si="17"/>
@@ -4809,11 +4833,11 @@
       </c>
       <c r="Q8" s="43">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R8" s="43">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S8" s="43">
         <f>COUNTIF(J:J,P8)</f>
@@ -4821,7 +4845,7 @@
       </c>
       <c r="T8" s="43">
         <f>COUNTIF(K:K,P8)+COUNTIF(L:L,P8)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U8" s="43">
         <f>COUNTIF(M:M,P8)</f>
@@ -4868,11 +4892,11 @@
       </c>
       <c r="AG8" s="92">
         <f t="shared" si="13"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH8" s="92">
         <f t="shared" si="14"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI8" s="92">
         <f t="shared" si="15"/>
@@ -4880,7 +4904,7 @@
       </c>
       <c r="AJ8" s="92">
         <f t="shared" si="16"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK8" s="92">
         <f t="shared" si="17"/>
@@ -4914,18 +4938,22 @@
         <f>P11</f>
         <v>Paris Saint-Germain</v>
       </c>
-      <c r="F9" s="21"/>
+      <c r="F9" s="21">
+        <v>4</v>
+      </c>
       <c r="G9" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="H9" s="21"/>
+      <c r="H9" s="21">
+        <v>0</v>
+      </c>
       <c r="I9" s="85" t="str">
         <f>P12</f>
-        <v>Atlétido de Madrid</v>
+        <v>Atlético de Madrid</v>
       </c>
       <c r="J9" s="63" t="str">
         <f t="shared" si="0"/>
-        <v>empate</v>
+        <v>Paris Saint-Germain</v>
       </c>
       <c r="K9" s="64" t="str">
         <f t="shared" si="1"/>
@@ -4937,7 +4965,7 @@
       </c>
       <c r="M9" s="65" t="str">
         <f t="shared" si="3"/>
-        <v>empate</v>
+        <v>Atlético de Madrid</v>
       </c>
       <c r="N9" s="66"/>
       <c r="O9" s="67"/>
@@ -4986,18 +5014,22 @@
         <f>P13</f>
         <v>Botafogo</v>
       </c>
-      <c r="F10" s="21"/>
+      <c r="F10" s="21">
+        <v>2</v>
+      </c>
       <c r="G10" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="21"/>
+      <c r="H10" s="21">
+        <v>1</v>
+      </c>
       <c r="I10" s="26" t="str">
         <f>P14</f>
         <v>Seattle Sounders</v>
       </c>
       <c r="J10" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>empate</v>
+        <v>Botafogo</v>
       </c>
       <c r="K10" s="43" t="str">
         <f t="shared" si="1"/>
@@ -5009,7 +5041,7 @@
       </c>
       <c r="M10" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>empate</v>
+        <v>Seattle Sounders</v>
       </c>
       <c r="N10" s="51"/>
       <c r="O10" s="52" t="s">
@@ -5140,15 +5172,15 @@
       </c>
       <c r="Q11" s="43">
         <f>(S11*3)+(T11*1)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R11" s="43">
         <f>SUM(S11:U11)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S11" s="43">
         <f>COUNTIF(J:J,P11)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T11" s="43">
         <f>COUNTIF(K:K,P11)+COUNTIF(L:L,P11)</f>
@@ -5160,7 +5192,7 @@
       </c>
       <c r="V11" s="43">
         <f>SUMIF(E:E,P11,F:F)+SUMIF(I:I,P11,H:H)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W11" s="43">
         <f>SUMIF(E:E,P11,H:H)+SUMIF(I:I,P11,F:F)</f>
@@ -5168,7 +5200,7 @@
       </c>
       <c r="X11" s="43">
         <f>V11-W11</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Y11" s="43">
         <f>SUMPRODUCT(($Q$11:$Q$14=Q11)*($X$11:$X$14&gt;X11))</f>
@@ -5199,15 +5231,15 @@
       </c>
       <c r="AG11" s="90">
         <f>VLOOKUP($AE11,$O$11:$X$14,3,FALSE)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH11" s="90">
         <f>VLOOKUP($AE11,$O$11:$X$14,4,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI11" s="90">
         <f>VLOOKUP($AE11,$O$11:$X$14,5,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ11" s="90">
         <f>VLOOKUP($AE11,$O$11:$X$14,6,FALSE)</f>
@@ -5219,7 +5251,7 @@
       </c>
       <c r="AL11" s="90">
         <f>VLOOKUP($AE11,$O$11:$X$14,8,FALSE)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AM11" s="90">
         <f>VLOOKUP($AE11,$O$11:$X$14,9,FALSE)</f>
@@ -5227,7 +5259,7 @@
       </c>
       <c r="AN11" s="91">
         <f>VLOOKUP($AE11,$O$11:$X$14,10,FALSE)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.25">
@@ -5252,7 +5284,7 @@
       <c r="H12" s="21"/>
       <c r="I12" s="26" t="str">
         <f>P12</f>
-        <v>Atlétido de Madrid</v>
+        <v>Atlético de Madrid</v>
       </c>
       <c r="J12" s="42" t="str">
         <f t="shared" si="0"/>
@@ -5273,11 +5305,11 @@
       <c r="N12" s="51"/>
       <c r="O12" s="52">
         <f t="shared" ref="O12:O14" si="21">RANK(Q12,$Q$11:$Q$14)+SUM(Y12:AB12)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P12" s="53" t="str">
         <f>Sorteios!F7</f>
-        <v>Atlétido de Madrid</v>
+        <v>Atlético de Madrid</v>
       </c>
       <c r="Q12" s="43">
         <f t="shared" ref="Q12:Q14" si="22">(S12*3)+(T12*1)</f>
@@ -5285,7 +5317,7 @@
       </c>
       <c r="R12" s="43">
         <f t="shared" ref="R12:R14" si="23">SUM(S12:U12)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S12" s="43">
         <f>COUNTIF(J:J,P12)</f>
@@ -5297,7 +5329,7 @@
       </c>
       <c r="U12" s="43">
         <f>COUNTIF(M:M,P12)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V12" s="43">
         <f>SUMIF(E:E,P12,F:F)+SUMIF(I:I,P12,H:H)</f>
@@ -5305,15 +5337,15 @@
       </c>
       <c r="W12" s="43">
         <f>SUMIF(E:E,P12,H:H)+SUMIF(I:I,P12,F:F)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X12" s="43">
         <f t="shared" ref="X12:X14" si="24">V12-W12</f>
-        <v>0</v>
+        <v>-4</v>
       </c>
       <c r="Y12" s="43">
         <f t="shared" ref="Y12:Y14" si="25">SUMPRODUCT(($Q$11:$Q$14=Q12)*($X$11:$X$14&gt;X12))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z12" s="43">
         <f t="shared" ref="Z12:Z14" si="26">SUMPRODUCT(($Q$11:$Q$14=Q12)*($X$11:$X$14=X12)*($V$11:$V$14&gt;V12))</f>
@@ -5325,7 +5357,7 @@
       </c>
       <c r="AB12" s="43">
         <f t="shared" ref="AB12:AB14" si="28">SUMPRODUCT(($Q$11:$Q$14=Q12)*($X$11:$X$14=X12)*($V$11:$V$14=V12)*($W$11:$W$14=W12)*($AC$11:$AC$14&lt;AC12))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC12" s="44">
         <v>2</v>
@@ -5336,19 +5368,19 @@
       </c>
       <c r="AF12" s="83" t="str">
         <f t="shared" ref="AF12:AF14" si="29">VLOOKUP($AE12,$O$11:$X$14,2,FALSE)</f>
-        <v>Atlétido de Madrid</v>
+        <v>Botafogo</v>
       </c>
       <c r="AG12" s="90">
         <f t="shared" ref="AG12:AG14" si="30">VLOOKUP($AE12,$O$11:$X$14,3,FALSE)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH12" s="90">
         <f t="shared" ref="AH12:AH14" si="31">VLOOKUP($AE12,$O$11:$X$14,4,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI12" s="90">
         <f t="shared" ref="AI12:AI14" si="32">VLOOKUP($AE12,$O$11:$X$14,5,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ12" s="90">
         <f t="shared" ref="AJ12:AJ14" si="33">VLOOKUP($AE12,$O$11:$X$14,6,FALSE)</f>
@@ -5360,15 +5392,15 @@
       </c>
       <c r="AL12" s="90">
         <f t="shared" ref="AL12:AL14" si="35">VLOOKUP($AE12,$O$11:$X$14,8,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM12" s="90">
         <f t="shared" ref="AM12:AM14" si="36">VLOOKUP($AE12,$O$11:$X$14,9,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN12" s="91">
         <f t="shared" ref="AN12:AN14" si="37">VLOOKUP($AE12,$O$11:$X$14,10,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.25">
@@ -5414,7 +5446,7 @@
       <c r="N13" s="51"/>
       <c r="O13" s="52">
         <f t="shared" si="21"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P13" s="53" t="str">
         <f>Sorteios!F8</f>
@@ -5422,15 +5454,15 @@
       </c>
       <c r="Q13" s="43">
         <f t="shared" si="22"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R13" s="43">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S13" s="43">
         <f>COUNTIF(J:J,P13)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T13" s="43">
         <f>COUNTIF(K:K,P13)+COUNTIF(L:L,P13)</f>
@@ -5442,19 +5474,19 @@
       </c>
       <c r="V13" s="43">
         <f>SUMIF(E:E,P13,F:F)+SUMIF(I:I,P13,H:H)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W13" s="43">
         <f>SUMIF(E:E,P13,H:H)+SUMIF(I:I,P13,F:F)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X13" s="43">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y13" s="43">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z13" s="43">
         <f t="shared" si="26"/>
@@ -5466,7 +5498,7 @@
       </c>
       <c r="AB13" s="43">
         <f t="shared" si="28"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC13" s="44">
         <v>3</v>
@@ -5477,7 +5509,7 @@
       </c>
       <c r="AF13" s="83" t="str">
         <f t="shared" si="29"/>
-        <v>Botafogo</v>
+        <v>Seattle Sounders</v>
       </c>
       <c r="AG13" s="90">
         <f t="shared" si="30"/>
@@ -5485,7 +5517,7 @@
       </c>
       <c r="AH13" s="90">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI13" s="90">
         <f t="shared" si="32"/>
@@ -5497,19 +5529,19 @@
       </c>
       <c r="AK13" s="90">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL13" s="90">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM13" s="90">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN13" s="91">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="14" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5525,7 +5557,7 @@
       </c>
       <c r="E14" s="84" t="str">
         <f>P12</f>
-        <v>Atlétido de Madrid</v>
+        <v>Atlético de Madrid</v>
       </c>
       <c r="F14" s="22"/>
       <c r="G14" s="92" t="s">
@@ -5555,7 +5587,7 @@
       <c r="N14" s="59"/>
       <c r="O14" s="60">
         <f t="shared" si="21"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P14" s="53" t="str">
         <f>Sorteios!F9</f>
@@ -5567,7 +5599,7 @@
       </c>
       <c r="R14" s="57">
         <f t="shared" si="23"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S14" s="43">
         <f>COUNTIF(J:J,P14)</f>
@@ -5579,19 +5611,19 @@
       </c>
       <c r="U14" s="43">
         <f>COUNTIF(M:M,P14)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V14" s="57">
         <f>SUMIF(E:E,P14,F:F)+SUMIF(I:I,P14,H:H)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W14" s="57">
         <f>SUMIF(E:E,P14,H:H)+SUMIF(I:I,P14,F:F)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X14" s="57">
         <f t="shared" si="24"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y14" s="57">
         <f t="shared" si="25"/>
@@ -5607,7 +5639,7 @@
       </c>
       <c r="AB14" s="57">
         <f t="shared" si="28"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AC14" s="58">
         <v>4</v>
@@ -5618,7 +5650,7 @@
       </c>
       <c r="AF14" s="84" t="str">
         <f t="shared" si="29"/>
-        <v>Seattle Sounders</v>
+        <v>Atlético de Madrid</v>
       </c>
       <c r="AG14" s="92">
         <f t="shared" si="30"/>
@@ -5626,7 +5658,7 @@
       </c>
       <c r="AH14" s="92">
         <f t="shared" si="31"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI14" s="92">
         <f t="shared" si="32"/>
@@ -5638,7 +5670,7 @@
       </c>
       <c r="AK14" s="92">
         <f t="shared" si="34"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL14" s="92">
         <f t="shared" si="35"/>
@@ -5646,11 +5678,11 @@
       </c>
       <c r="AM14" s="92">
         <f t="shared" si="36"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AN14" s="93">
         <f t="shared" si="37"/>
-        <v>0</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.25">
@@ -5668,18 +5700,22 @@
         <f>P17</f>
         <v>Bayern de Munique</v>
       </c>
-      <c r="F15" s="21"/>
+      <c r="F15" s="21">
+        <v>10</v>
+      </c>
       <c r="G15" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H15" s="21"/>
+      <c r="H15" s="21">
+        <v>0</v>
+      </c>
       <c r="I15" s="13" t="str">
         <f>P18</f>
         <v>Auckland City</v>
       </c>
       <c r="J15" s="63" t="str">
         <f t="shared" si="0"/>
-        <v>empate</v>
+        <v>Bayern de Munique</v>
       </c>
       <c r="K15" s="64" t="str">
         <f t="shared" si="1"/>
@@ -5691,7 +5727,7 @@
       </c>
       <c r="M15" s="65" t="str">
         <f t="shared" si="3"/>
-        <v>empate</v>
+        <v>Auckland City</v>
       </c>
       <c r="N15" s="66"/>
       <c r="O15" s="67"/>
@@ -5894,15 +5930,15 @@
       </c>
       <c r="Q17" s="43">
         <f>(S17*3)+(T17*1)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R17" s="43">
         <f>SUM(S17:U17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S17" s="43">
         <f>COUNTIF(J:J,P17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T17" s="43">
         <f>COUNTIF(K:K,P17)+COUNTIF(L:L,P17)</f>
@@ -5914,7 +5950,7 @@
       </c>
       <c r="V17" s="43">
         <f>SUMIF(E:E,P17,F:F)+SUMIF(I:I,P17,H:H)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="W17" s="43">
         <f>SUMIF(E:E,P17,H:H)+SUMIF(I:I,P17,F:F)</f>
@@ -5922,7 +5958,7 @@
       </c>
       <c r="X17" s="43">
         <f>V17-W17</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="Y17" s="43">
         <f>SUMPRODUCT(($Q$17:$Q$20=Q17)*($X$17:$X$20&gt;X17))</f>
@@ -5953,15 +5989,15 @@
       </c>
       <c r="AG17" s="90">
         <f>VLOOKUP($AE17,$O$17:$X$20,3,FALSE)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH17" s="90">
         <f>VLOOKUP($AE17,$O$17:$X$20,4,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI17" s="90">
         <f>VLOOKUP($AE17,$O$17:$X$20,5,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ17" s="90">
         <f>VLOOKUP($AE17,$O$17:$X$20,6,FALSE)</f>
@@ -5973,7 +6009,7 @@
       </c>
       <c r="AL17" s="90">
         <f>VLOOKUP($AE17,$O$17:$X$20,8,FALSE)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AM17" s="90">
         <f>VLOOKUP($AE17,$O$17:$X$20,9,FALSE)</f>
@@ -5981,7 +6017,7 @@
       </c>
       <c r="AN17" s="91">
         <f>VLOOKUP($AE17,$O$17:$X$20,10,FALSE)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.25">
@@ -6027,7 +6063,7 @@
       <c r="N18" s="51"/>
       <c r="O18" s="52">
         <f t="shared" ref="O18:O20" si="38">RANK(Q18,$Q$17:$Q$20)+SUM(Y18:AB18)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P18" s="53" t="str">
         <f>Sorteios!I7</f>
@@ -6039,7 +6075,7 @@
       </c>
       <c r="R18" s="43">
         <f t="shared" ref="R18:R20" si="40">SUM(S18:U18)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S18" s="43">
         <f>COUNTIF(J:J,P18)</f>
@@ -6051,7 +6087,7 @@
       </c>
       <c r="U18" s="43">
         <f>COUNTIF(M:M,P18)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V18" s="43">
         <f>SUMIF(E:E,P18,F:F)+SUMIF(I:I,P18,H:H)</f>
@@ -6059,15 +6095,15 @@
       </c>
       <c r="W18" s="43">
         <f>SUMIF(E:E,P18,H:H)+SUMIF(I:I,P18,F:F)</f>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="X18" s="43">
         <f t="shared" ref="X18:X20" si="41">V18-W18</f>
-        <v>0</v>
+        <v>-10</v>
       </c>
       <c r="Y18" s="43">
         <f t="shared" ref="Y18:Y20" si="42">SUMPRODUCT(($Q$17:$Q$20=Q18)*($X$17:$X$20&gt;X18))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z18" s="43">
         <f t="shared" ref="Z18:Z20" si="43">SUMPRODUCT(($Q$17:$Q$20=Q18)*($X$17:$X$20=X18)*($V$17:$V$20&gt;V18))</f>
@@ -6079,7 +6115,7 @@
       </c>
       <c r="AB18" s="43">
         <f t="shared" ref="AB18:AB20" si="45">SUMPRODUCT(($Q$17:$Q$20=Q18)*($X$17:$X$20=X18)*($V$17:$V$20=V18)*($W$17:$W$20=W18)*($AC$17:$AC$20&lt;AC18))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC18" s="44">
         <v>2</v>
@@ -6090,7 +6126,7 @@
       </c>
       <c r="AF18" s="83" t="str">
         <f t="shared" ref="AF18:AF20" si="46">VLOOKUP($AE18,$O$17:$X$20,2,FALSE)</f>
-        <v>Auckland City</v>
+        <v>Boca Juniors</v>
       </c>
       <c r="AG18" s="90">
         <f t="shared" ref="AG18:AG20" si="47">VLOOKUP($AE18,$O$17:$X$20,3,FALSE)</f>
@@ -6168,7 +6204,7 @@
       <c r="N19" s="51"/>
       <c r="O19" s="52">
         <f t="shared" si="38"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P19" s="53" t="str">
         <f>Sorteios!I8</f>
@@ -6220,7 +6256,7 @@
       </c>
       <c r="AB19" s="43">
         <f t="shared" si="45"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC19" s="44">
         <v>3</v>
@@ -6231,7 +6267,7 @@
       </c>
       <c r="AF19" s="83" t="str">
         <f t="shared" si="46"/>
-        <v>Boca Juniors</v>
+        <v>Benfica</v>
       </c>
       <c r="AG19" s="90">
         <f t="shared" si="47"/>
@@ -6309,7 +6345,7 @@
       <c r="N20" s="59"/>
       <c r="O20" s="60">
         <f t="shared" si="38"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P20" s="53" t="str">
         <f>Sorteios!I9</f>
@@ -6361,7 +6397,7 @@
       </c>
       <c r="AB20" s="57">
         <f t="shared" si="45"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AC20" s="58">
         <v>4</v>
@@ -6372,7 +6408,7 @@
       </c>
       <c r="AF20" s="84" t="str">
         <f t="shared" si="46"/>
-        <v>Benfica</v>
+        <v>Auckland City</v>
       </c>
       <c r="AG20" s="92">
         <f t="shared" si="47"/>
@@ -6380,7 +6416,7 @@
       </c>
       <c r="AH20" s="92">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI20" s="92">
         <f t="shared" si="49"/>
@@ -6392,7 +6428,7 @@
       </c>
       <c r="AK20" s="92">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL20" s="92">
         <f t="shared" si="52"/>
@@ -6400,11 +6436,11 @@
       </c>
       <c r="AM20" s="92">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="AN20" s="93">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.25">
@@ -10322,7 +10358,7 @@
     <row r="1" spans="1:17" ht="22.5" x14ac:dyDescent="0.3">
       <c r="A1" s="108"/>
       <c r="B1" s="28" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C1" s="28"/>
       <c r="D1" s="28"/>
@@ -10427,7 +10463,7 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" s="127" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C7" s="123">
         <v>45836</v>
@@ -10461,7 +10497,7 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B8" s="127" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C8" s="123">
         <v>45837</v>
@@ -10495,7 +10531,7 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B9" s="127" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C9" s="123">
         <v>45837</v>
@@ -10563,7 +10599,7 @@
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" s="127" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C11" s="123">
         <v>45838</v>
@@ -10597,7 +10633,7 @@
     </row>
     <row r="12" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B12" s="127" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C12" s="123">
         <v>45839</v>
@@ -10631,7 +10667,7 @@
     </row>
     <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="128" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C13" s="139">
         <v>45839</v>
@@ -11093,7 +11129,7 @@
     <row r="37" spans="1:17" s="137" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="135"/>
       <c r="B37" s="182" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C37" s="182"/>
       <c r="D37" s="182"/>
@@ -11254,11 +11290,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:K13">
-    <cfRule type="expression" dxfId="29" priority="126">
+    <cfRule type="expression" dxfId="29" priority="12">
+      <formula>$K6=$M6</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="126">
       <formula>Q6="emp"</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="12">
-      <formula>$K6=$M6</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K6:K13">
@@ -11408,6 +11444,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
@@ -11415,7 +11460,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DBF2846C41E31A469E3CED25F2422E48" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0c08e4af4d80db6585ac36ba965bb3a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2c8c20e6-817c-474f-b9c2-eb2b1ac24837" xmlns:ns4="dc8c2798-6aba-4af7-93a4-b89253b03650" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4e7db2db65f9cb533b4933096bc9b657" ns3:_="" ns4:_="">
     <xsd:import namespace="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
@@ -11648,33 +11693,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83E7837-68AD-48B2-A1AB-AAB452317AF5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A45D7D45-1E18-48AE-827B-096C3C02C976}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83E7837-68AD-48B2-A1AB-AAB452317AF5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFBCCD5-5BDE-495C-BFE9-46A98A6BC529}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11691,12 +11735,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A45D7D45-1E18-48AE-827B-096C3C02C976}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Att até o jogo 8
</commit_message>
<xml_diff>
--- a/Mundial de Clubes FIFA 2025.xlsx
+++ b/Mundial de Clubes FIFA 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjunior\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{890005AA-DE05-4B21-98EB-AFF6787F7368}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{852E9631-EB85-4A1C-A6DD-17B81FBF2398}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="1185" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{076F3B28-812E-4458-A424-96085A053123}"/>
   </bookViews>
@@ -1589,9 +1589,18 @@
     <xf numFmtId="0" fontId="20" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="centerContinuous" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1606,15 +1615,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -2971,13 +2971,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="22.5" x14ac:dyDescent="0.3">
-      <c r="B1" s="183" t="s">
+      <c r="B1" s="176" t="s">
         <v>111</v>
       </c>
-      <c r="C1" s="184"/>
-      <c r="D1" s="184"/>
-      <c r="E1" s="184"/>
-      <c r="F1" s="184"/>
+      <c r="C1" s="177"/>
+      <c r="D1" s="177"/>
+      <c r="E1" s="177"/>
+      <c r="F1" s="177"/>
     </row>
     <row r="2" spans="2:6" ht="13.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="2:6" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -4019,7 +4019,7 @@
   <dimension ref="A1:AN50"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4117,11 +4117,11 @@
       <c r="E2" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="176" t="s">
+      <c r="F2" s="178" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="176"/>
-      <c r="H2" s="176"/>
+      <c r="G2" s="178"/>
+      <c r="H2" s="178"/>
       <c r="I2" s="77" t="s">
         <v>68</v>
       </c>
@@ -5776,11 +5776,15 @@
         <f>P19</f>
         <v>Boca Juniors</v>
       </c>
-      <c r="F16" s="21"/>
+      <c r="F16" s="21">
+        <v>2</v>
+      </c>
       <c r="G16" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H16" s="21"/>
+      <c r="H16" s="21">
+        <v>2</v>
+      </c>
       <c r="I16" s="13" t="str">
         <f>P20</f>
         <v>Benfica</v>
@@ -5791,11 +5795,11 @@
       </c>
       <c r="K16" s="43" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Boca Juniors</v>
       </c>
       <c r="L16" s="43" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>Benfica</v>
       </c>
       <c r="M16" s="44" t="str">
         <f t="shared" si="3"/>
@@ -6103,7 +6107,7 @@
       </c>
       <c r="Y18" s="43">
         <f t="shared" ref="Y18:Y20" si="42">SUMPRODUCT(($Q$17:$Q$20=Q18)*($X$17:$X$20&gt;X18))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z18" s="43">
         <f t="shared" ref="Z18:Z20" si="43">SUMPRODUCT(($Q$17:$Q$20=Q18)*($X$17:$X$20=X18)*($V$17:$V$20&gt;V18))</f>
@@ -6130,11 +6134,11 @@
       </c>
       <c r="AG18" s="90">
         <f t="shared" ref="AG18:AG20" si="47">VLOOKUP($AE18,$O$17:$X$20,3,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH18" s="90">
         <f t="shared" ref="AH18:AH20" si="48">VLOOKUP($AE18,$O$17:$X$20,4,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI18" s="90">
         <f t="shared" ref="AI18:AI20" si="49">VLOOKUP($AE18,$O$17:$X$20,5,FALSE)</f>
@@ -6142,7 +6146,7 @@
       </c>
       <c r="AJ18" s="90">
         <f t="shared" ref="AJ18:AJ20" si="50">VLOOKUP($AE18,$O$17:$X$20,6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK18" s="90">
         <f t="shared" ref="AK18:AK20" si="51">VLOOKUP($AE18,$O$17:$X$20,7,FALSE)</f>
@@ -6150,11 +6154,11 @@
       </c>
       <c r="AL18" s="90">
         <f t="shared" ref="AL18:AL20" si="52">VLOOKUP($AE18,$O$17:$X$20,8,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM18" s="90">
         <f t="shared" ref="AM18:AM20" si="53">VLOOKUP($AE18,$O$17:$X$20,9,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN18" s="91">
         <f t="shared" ref="AN18:AN20" si="54">VLOOKUP($AE18,$O$17:$X$20,10,FALSE)</f>
@@ -6212,11 +6216,11 @@
       </c>
       <c r="Q19" s="43">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R19" s="43">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S19" s="43">
         <f>COUNTIF(J:J,P19)</f>
@@ -6224,7 +6228,7 @@
       </c>
       <c r="T19" s="43">
         <f>COUNTIF(K:K,P19)+COUNTIF(L:L,P19)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U19" s="43">
         <f>COUNTIF(M:M,P19)</f>
@@ -6232,11 +6236,11 @@
       </c>
       <c r="V19" s="43">
         <f>SUMIF(E:E,P19,F:F)+SUMIF(I:I,P19,H:H)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W19" s="43">
         <f>SUMIF(E:E,P19,H:H)+SUMIF(I:I,P19,F:F)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X19" s="43">
         <f t="shared" si="41"/>
@@ -6271,11 +6275,11 @@
       </c>
       <c r="AG19" s="90">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH19" s="90">
         <f t="shared" si="48"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI19" s="90">
         <f t="shared" si="49"/>
@@ -6283,7 +6287,7 @@
       </c>
       <c r="AJ19" s="90">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK19" s="90">
         <f t="shared" si="51"/>
@@ -6291,11 +6295,11 @@
       </c>
       <c r="AL19" s="90">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM19" s="90">
         <f t="shared" si="53"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN19" s="91">
         <f t="shared" si="54"/>
@@ -6353,11 +6357,11 @@
       </c>
       <c r="Q20" s="57">
         <f t="shared" si="39"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R20" s="57">
         <f t="shared" si="40"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S20" s="43">
         <f>COUNTIF(J:J,P20)</f>
@@ -6365,7 +6369,7 @@
       </c>
       <c r="T20" s="43">
         <f>COUNTIF(K:K,P20)+COUNTIF(L:L,P20)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U20" s="43">
         <f>COUNTIF(M:M,P20)</f>
@@ -6373,11 +6377,11 @@
       </c>
       <c r="V20" s="57">
         <f>SUMIF(E:E,P20,F:F)+SUMIF(I:I,P20,H:H)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W20" s="57">
         <f>SUMIF(E:E,P20,H:H)+SUMIF(I:I,P20,F:F)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X20" s="57">
         <f t="shared" si="41"/>
@@ -6530,18 +6534,22 @@
         <f>P25</f>
         <v>Chelsea</v>
       </c>
-      <c r="F22" s="21"/>
+      <c r="F22" s="21">
+        <v>2</v>
+      </c>
       <c r="G22" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="H22" s="21"/>
+      <c r="H22" s="21">
+        <v>0</v>
+      </c>
       <c r="I22" s="26" t="str">
         <f>P26</f>
         <v>Los Angeles FC</v>
       </c>
       <c r="J22" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>empate</v>
+        <v>Chelsea</v>
       </c>
       <c r="K22" s="43" t="str">
         <f t="shared" si="1"/>
@@ -6553,7 +6561,7 @@
       </c>
       <c r="M22" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>empate</v>
+        <v>Los Angeles FC</v>
       </c>
       <c r="N22" s="50"/>
       <c r="O22" s="52" t="s">
@@ -6676,7 +6684,7 @@
       <c r="N23" s="50"/>
       <c r="O23" s="52">
         <f>RANK(Q23,$Q$23:$Q$26)+SUM(Y23:AB23)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P23" s="53" t="str">
         <f>Sorteios!L6</f>
@@ -6739,19 +6747,19 @@
       </c>
       <c r="AF23" s="83" t="str">
         <f>VLOOKUP($AE23,$O$23:$X$26,2,FALSE)</f>
-        <v>Flamengo</v>
+        <v>Chelsea</v>
       </c>
       <c r="AG23" s="90">
         <f>VLOOKUP($AE23,$O$23:$X$26,3,FALSE)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH23" s="90">
         <f>VLOOKUP($AE23,$O$23:$X$26,4,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI23" s="90">
         <f>VLOOKUP($AE23,$O$23:$X$26,5,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ23" s="90">
         <f>VLOOKUP($AE23,$O$23:$X$26,6,FALSE)</f>
@@ -6763,7 +6771,7 @@
       </c>
       <c r="AL23" s="90">
         <f>VLOOKUP($AE23,$O$23:$X$26,8,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM23" s="90">
         <f>VLOOKUP($AE23,$O$23:$X$26,9,FALSE)</f>
@@ -6771,7 +6779,7 @@
       </c>
       <c r="AN23" s="91">
         <f>VLOOKUP($AE23,$O$23:$X$26,10,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.25">
@@ -6817,7 +6825,7 @@
       <c r="N24" s="50"/>
       <c r="O24" s="52">
         <f t="shared" ref="O24:O26" si="55">RANK(Q24,$Q$23:$Q$26)+SUM(Y24:AB24)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P24" s="53" t="str">
         <f>Sorteios!L7</f>
@@ -6880,7 +6888,7 @@
       </c>
       <c r="AF24" s="83" t="str">
         <f t="shared" ref="AF24:AF26" si="63">VLOOKUP($AE24,$O$23:$X$26,2,FALSE)</f>
-        <v>Espérance de Tunis</v>
+        <v>Flamengo</v>
       </c>
       <c r="AG24" s="90">
         <f t="shared" ref="AG24:AG26" si="64">VLOOKUP($AE24,$O$23:$X$26,3,FALSE)</f>
@@ -6958,7 +6966,7 @@
       <c r="N25" s="50"/>
       <c r="O25" s="52">
         <f t="shared" si="55"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P25" s="53" t="str">
         <f>Sorteios!L8</f>
@@ -6966,15 +6974,15 @@
       </c>
       <c r="Q25" s="43">
         <f t="shared" si="56"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R25" s="43">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S25" s="43">
         <f>COUNTIF(J:J,P25)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T25" s="43">
         <f>COUNTIF(K:K,P25)+COUNTIF(L:L,P25)</f>
@@ -6986,7 +6994,7 @@
       </c>
       <c r="V25" s="43">
         <f>SUMIF(E:E,P25,F:F)+SUMIF(I:I,P25,H:H)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W25" s="43">
         <f>SUMIF(E:E,P25,H:H)+SUMIF(I:I,P25,F:F)</f>
@@ -6994,7 +7002,7 @@
       </c>
       <c r="X25" s="43">
         <f t="shared" si="58"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y25" s="43">
         <f t="shared" si="59"/>
@@ -7010,7 +7018,7 @@
       </c>
       <c r="AB25" s="43">
         <f t="shared" si="62"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC25" s="44">
         <v>3</v>
@@ -7021,7 +7029,7 @@
       </c>
       <c r="AF25" s="83" t="str">
         <f t="shared" si="63"/>
-        <v>Chelsea</v>
+        <v>Espérance de Tunis</v>
       </c>
       <c r="AG25" s="90">
         <f t="shared" si="64"/>
@@ -7111,7 +7119,7 @@
       </c>
       <c r="R26" s="57">
         <f t="shared" si="57"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S26" s="43">
         <f>COUNTIF(J:J,P26)</f>
@@ -7123,7 +7131,7 @@
       </c>
       <c r="U26" s="43">
         <f>COUNTIF(M:M,P26)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V26" s="57">
         <f>SUMIF(E:E,P26,F:F)+SUMIF(I:I,P26,H:H)</f>
@@ -7131,15 +7139,15 @@
       </c>
       <c r="W26" s="57">
         <f>SUMIF(E:E,P26,H:H)+SUMIF(I:I,P26,F:F)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X26" s="57">
         <f t="shared" si="58"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="Y26" s="57">
         <f t="shared" si="59"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z26" s="57">
         <f t="shared" si="60"/>
@@ -7151,7 +7159,7 @@
       </c>
       <c r="AB26" s="57">
         <f t="shared" si="62"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AC26" s="58">
         <v>4</v>
@@ -7170,7 +7178,7 @@
       </c>
       <c r="AH26" s="92">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI26" s="92">
         <f t="shared" si="66"/>
@@ -7182,7 +7190,7 @@
       </c>
       <c r="AK26" s="92">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL26" s="92">
         <f t="shared" si="69"/>
@@ -7190,11 +7198,11 @@
       </c>
       <c r="AM26" s="92">
         <f t="shared" si="70"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN26" s="93">
         <f t="shared" si="71"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.25">
@@ -10379,18 +10387,18 @@
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="109"/>
-      <c r="B4" s="177" t="s">
+      <c r="B4" s="180" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="178"/>
-      <c r="D4" s="178"/>
-      <c r="E4" s="178"/>
-      <c r="F4" s="178"/>
-      <c r="G4" s="178"/>
-      <c r="H4" s="178"/>
-      <c r="I4" s="178"/>
-      <c r="J4" s="178"/>
-      <c r="K4" s="179"/>
+      <c r="C4" s="181"/>
+      <c r="D4" s="181"/>
+      <c r="E4" s="181"/>
+      <c r="F4" s="181"/>
+      <c r="G4" s="181"/>
+      <c r="H4" s="181"/>
+      <c r="I4" s="181"/>
+      <c r="J4" s="181"/>
+      <c r="K4" s="182"/>
       <c r="L4" s="110"/>
       <c r="M4" s="111"/>
       <c r="N4" s="111"/>
@@ -10407,19 +10415,19 @@
       <c r="D5" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="180" t="s">
+      <c r="E5" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="180"/>
-      <c r="G5" s="180" t="s">
+      <c r="F5" s="183"/>
+      <c r="G5" s="183" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="180"/>
-      <c r="I5" s="180"/>
-      <c r="J5" s="180" t="s">
+      <c r="H5" s="183"/>
+      <c r="I5" s="183"/>
+      <c r="J5" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="181"/>
+      <c r="K5" s="184"/>
       <c r="L5" s="113"/>
       <c r="M5" s="113"/>
       <c r="N5" s="113"/>
@@ -10707,18 +10715,18 @@
     </row>
     <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="109"/>
-      <c r="B16" s="177" t="s">
+      <c r="B16" s="180" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="178"/>
-      <c r="D16" s="178"/>
-      <c r="E16" s="178"/>
-      <c r="F16" s="178"/>
-      <c r="G16" s="178"/>
-      <c r="H16" s="178"/>
-      <c r="I16" s="178"/>
-      <c r="J16" s="178"/>
-      <c r="K16" s="179"/>
+      <c r="C16" s="181"/>
+      <c r="D16" s="181"/>
+      <c r="E16" s="181"/>
+      <c r="F16" s="181"/>
+      <c r="G16" s="181"/>
+      <c r="H16" s="181"/>
+      <c r="I16" s="181"/>
+      <c r="J16" s="181"/>
+      <c r="K16" s="182"/>
       <c r="L16" s="110"/>
       <c r="M16" s="111"/>
       <c r="N16" s="111"/>
@@ -10731,19 +10739,19 @@
       <c r="D17" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="180" t="s">
+      <c r="E17" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="180"/>
-      <c r="G17" s="180" t="s">
+      <c r="F17" s="183"/>
+      <c r="G17" s="183" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="180"/>
-      <c r="I17" s="180"/>
-      <c r="J17" s="180" t="s">
+      <c r="H17" s="183"/>
+      <c r="I17" s="183"/>
+      <c r="J17" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="K17" s="181"/>
+      <c r="K17" s="184"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B18" s="129" t="s">
@@ -10889,18 +10897,18 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="109"/>
-      <c r="B24" s="177" t="s">
+      <c r="B24" s="180" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="178"/>
-      <c r="D24" s="178"/>
-      <c r="E24" s="178"/>
-      <c r="F24" s="178"/>
-      <c r="G24" s="178"/>
-      <c r="H24" s="178"/>
-      <c r="I24" s="178"/>
-      <c r="J24" s="178"/>
-      <c r="K24" s="179"/>
+      <c r="C24" s="181"/>
+      <c r="D24" s="181"/>
+      <c r="E24" s="181"/>
+      <c r="F24" s="181"/>
+      <c r="G24" s="181"/>
+      <c r="H24" s="181"/>
+      <c r="I24" s="181"/>
+      <c r="J24" s="181"/>
+      <c r="K24" s="182"/>
       <c r="L24" s="110"/>
       <c r="M24" s="111"/>
       <c r="N24" s="111"/>
@@ -10916,19 +10924,19 @@
       <c r="D25" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="180" t="s">
+      <c r="E25" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="180"/>
-      <c r="G25" s="180" t="s">
+      <c r="F25" s="183"/>
+      <c r="G25" s="183" t="s">
         <v>13</v>
       </c>
-      <c r="H25" s="180"/>
-      <c r="I25" s="180"/>
-      <c r="J25" s="180" t="s">
+      <c r="H25" s="183"/>
+      <c r="I25" s="183"/>
+      <c r="J25" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="K25" s="181"/>
+      <c r="K25" s="184"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="151" t="s">
@@ -11017,18 +11025,18 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="109"/>
-      <c r="B31" s="177" t="s">
+      <c r="B31" s="180" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="178"/>
-      <c r="D31" s="178"/>
-      <c r="E31" s="178"/>
-      <c r="F31" s="178"/>
-      <c r="G31" s="178"/>
-      <c r="H31" s="178"/>
-      <c r="I31" s="178"/>
-      <c r="J31" s="178"/>
-      <c r="K31" s="179"/>
+      <c r="C31" s="181"/>
+      <c r="D31" s="181"/>
+      <c r="E31" s="181"/>
+      <c r="F31" s="181"/>
+      <c r="G31" s="181"/>
+      <c r="H31" s="181"/>
+      <c r="I31" s="181"/>
+      <c r="J31" s="181"/>
+      <c r="K31" s="182"/>
       <c r="L31" s="110"/>
       <c r="M31" s="111"/>
       <c r="N31" s="111"/>
@@ -11044,19 +11052,19 @@
       <c r="D32" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="180" t="s">
+      <c r="E32" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="180"/>
-      <c r="G32" s="180" t="s">
+      <c r="F32" s="183"/>
+      <c r="G32" s="183" t="s">
         <v>13</v>
       </c>
-      <c r="H32" s="180"/>
-      <c r="I32" s="180"/>
-      <c r="J32" s="180" t="s">
+      <c r="H32" s="183"/>
+      <c r="I32" s="183"/>
+      <c r="J32" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="K32" s="181"/>
+      <c r="K32" s="184"/>
     </row>
     <row r="33" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="161" t="s">
@@ -11104,11 +11112,11 @@
     </row>
     <row r="36" spans="1:17" s="137" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="135"/>
-      <c r="B36" s="182" t="s">
+      <c r="B36" s="179" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="182"/>
-      <c r="D36" s="182"/>
+      <c r="C36" s="179"/>
+      <c r="D36" s="179"/>
       <c r="E36" s="173" t="str">
         <f>IF(M33="1º Lugar","",M33)</f>
         <v/>
@@ -11128,11 +11136,11 @@
     </row>
     <row r="37" spans="1:17" s="137" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="135"/>
-      <c r="B37" s="182" t="s">
+      <c r="B37" s="179" t="s">
         <v>106</v>
       </c>
-      <c r="C37" s="182"/>
-      <c r="D37" s="182"/>
+      <c r="C37" s="179"/>
+      <c r="D37" s="179"/>
       <c r="E37" s="175" t="str">
         <f>IF(M34="2º Lugar","",M34)</f>
         <v/>
@@ -11260,12 +11268,11 @@
   </sheetData>
   <sheetProtection password="CC01" sheet="1" selectLockedCells="1"/>
   <mergeCells count="18">
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B31:K31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="B16:K16"/>
     <mergeCell ref="B24:K24"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="G25:I25"/>
@@ -11273,11 +11280,12 @@
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="B16:K16"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B31:K31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="B36:D36"/>
   </mergeCells>
   <conditionalFormatting sqref="F6">
     <cfRule type="expression" dxfId="31" priority="128">
@@ -11444,23 +11452,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DBF2846C41E31A469E3CED25F2422E48" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0c08e4af4d80db6585ac36ba965bb3a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2c8c20e6-817c-474f-b9c2-eb2b1ac24837" xmlns:ns4="dc8c2798-6aba-4af7-93a4-b89253b03650" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4e7db2db65f9cb533b4933096bc9b657" ns3:_="" ns4:_="">
     <xsd:import namespace="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
@@ -11693,32 +11684,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A45D7D45-1E18-48AE-827B-096C3C02C976}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83E7837-68AD-48B2-A1AB-AAB452317AF5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFBCCD5-5BDE-495C-BFE9-46A98A6BC529}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11735,4 +11718,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83E7837-68AD-48B2-A1AB-AAB452317AF5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
+    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A45D7D45-1E18-48AE-827B-096C3C02C976}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Att até jogo 11
</commit_message>
<xml_diff>
--- a/Mundial de Clubes FIFA 2025.xlsx
+++ b/Mundial de Clubes FIFA 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjunior\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{852E9631-EB85-4A1C-A6DD-17B81FBF2398}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB6C4004-51DA-49C7-AE04-05AABE333700}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="1185" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{076F3B28-812E-4458-A424-96085A053123}"/>
   </bookViews>
@@ -1598,23 +1598,23 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4018,8 +4018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45896CCF-F333-49AF-850B-159476231F1C}">
   <dimension ref="A1:AN50"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6462,18 +6462,22 @@
         <f>P23</f>
         <v>Flamengo</v>
       </c>
-      <c r="F21" s="21"/>
+      <c r="F21" s="21">
+        <v>2</v>
+      </c>
       <c r="G21" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="H21" s="21"/>
+      <c r="H21" s="21">
+        <v>0</v>
+      </c>
       <c r="I21" s="85" t="str">
         <f>P24</f>
         <v>Espérance de Tunis</v>
       </c>
       <c r="J21" s="63" t="str">
         <f t="shared" si="0"/>
-        <v>empate</v>
+        <v>Flamengo</v>
       </c>
       <c r="K21" s="64" t="str">
         <f t="shared" si="1"/>
@@ -6485,7 +6489,7 @@
       </c>
       <c r="M21" s="65" t="str">
         <f t="shared" si="3"/>
-        <v>empate</v>
+        <v>Espérance de Tunis</v>
       </c>
       <c r="N21" s="69"/>
       <c r="O21" s="67"/>
@@ -6684,7 +6688,7 @@
       <c r="N23" s="50"/>
       <c r="O23" s="52">
         <f>RANK(Q23,$Q$23:$Q$26)+SUM(Y23:AB23)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P23" s="53" t="str">
         <f>Sorteios!L6</f>
@@ -6692,15 +6696,15 @@
       </c>
       <c r="Q23" s="43">
         <f>(S23*3)+(T23*1)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R23" s="43">
         <f>SUM(S23:U23)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S23" s="43">
         <f>COUNTIF(J:J,P23)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T23" s="43">
         <f>COUNTIF(K:K,P23)+COUNTIF(L:L,P23)</f>
@@ -6712,7 +6716,7 @@
       </c>
       <c r="V23" s="43">
         <f>SUMIF(E:E,P23,F:F)+SUMIF(I:I,P23,H:H)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W23" s="43">
         <f>SUMIF(E:E,P23,H:H)+SUMIF(I:I,P23,F:F)</f>
@@ -6720,7 +6724,7 @@
       </c>
       <c r="X23" s="43">
         <f>V23-W23</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y23" s="43">
         <f>SUMPRODUCT(($Q$23:$Q$26=Q23)*($X$23:$X$26&gt;X23))</f>
@@ -6747,7 +6751,7 @@
       </c>
       <c r="AF23" s="83" t="str">
         <f>VLOOKUP($AE23,$O$23:$X$26,2,FALSE)</f>
-        <v>Chelsea</v>
+        <v>Flamengo</v>
       </c>
       <c r="AG23" s="90">
         <f>VLOOKUP($AE23,$O$23:$X$26,3,FALSE)</f>
@@ -6837,7 +6841,7 @@
       </c>
       <c r="R24" s="43">
         <f t="shared" ref="R24:R26" si="57">SUM(S24:U24)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S24" s="43">
         <f>COUNTIF(J:J,P24)</f>
@@ -6849,7 +6853,7 @@
       </c>
       <c r="U24" s="43">
         <f>COUNTIF(M:M,P24)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V24" s="43">
         <f>SUMIF(E:E,P24,F:F)+SUMIF(I:I,P24,H:H)</f>
@@ -6857,11 +6861,11 @@
       </c>
       <c r="W24" s="43">
         <f>SUMIF(E:E,P24,H:H)+SUMIF(I:I,P24,F:F)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X24" s="43">
         <f t="shared" ref="X24:X26" si="58">V24-W24</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="Y24" s="43">
         <f t="shared" ref="Y24:Y26" si="59">SUMPRODUCT(($Q$23:$Q$26=Q24)*($X$23:$X$26&gt;X24))</f>
@@ -6877,7 +6881,7 @@
       </c>
       <c r="AB24" s="43">
         <f t="shared" ref="AB24:AB26" si="62">SUMPRODUCT(($Q$23:$Q$26=Q24)*($X$23:$X$26=X24)*($V$23:$V$26=V24)*($W$23:$W$26=W24)*($AC$23:$AC$26&lt;AC24))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC24" s="44">
         <v>2</v>
@@ -6888,19 +6892,19 @@
       </c>
       <c r="AF24" s="83" t="str">
         <f t="shared" ref="AF24:AF26" si="63">VLOOKUP($AE24,$O$23:$X$26,2,FALSE)</f>
-        <v>Flamengo</v>
+        <v>Chelsea</v>
       </c>
       <c r="AG24" s="90">
         <f t="shared" ref="AG24:AG26" si="64">VLOOKUP($AE24,$O$23:$X$26,3,FALSE)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH24" s="90">
         <f t="shared" ref="AH24:AH26" si="65">VLOOKUP($AE24,$O$23:$X$26,4,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI24" s="90">
         <f t="shared" ref="AI24:AI26" si="66">VLOOKUP($AE24,$O$23:$X$26,5,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ24" s="90">
         <f t="shared" ref="AJ24:AJ26" si="67">VLOOKUP($AE24,$O$23:$X$26,6,FALSE)</f>
@@ -6912,7 +6916,7 @@
       </c>
       <c r="AL24" s="90">
         <f t="shared" ref="AL24:AL26" si="69">VLOOKUP($AE24,$O$23:$X$26,8,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM24" s="90">
         <f t="shared" ref="AM24:AM26" si="70">VLOOKUP($AE24,$O$23:$X$26,9,FALSE)</f>
@@ -6920,7 +6924,7 @@
       </c>
       <c r="AN24" s="91">
         <f t="shared" ref="AN24:AN26" si="71">VLOOKUP($AE24,$O$23:$X$26,10,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.25">
@@ -6966,7 +6970,7 @@
       <c r="N25" s="50"/>
       <c r="O25" s="52">
         <f t="shared" si="55"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P25" s="53" t="str">
         <f>Sorteios!L8</f>
@@ -7018,7 +7022,7 @@
       </c>
       <c r="AB25" s="43">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC25" s="44">
         <v>3</v>
@@ -7037,7 +7041,7 @@
       </c>
       <c r="AH25" s="90">
         <f t="shared" si="65"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI25" s="90">
         <f t="shared" si="66"/>
@@ -7049,7 +7053,7 @@
       </c>
       <c r="AK25" s="90">
         <f t="shared" si="68"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL25" s="90">
         <f t="shared" si="69"/>
@@ -7057,11 +7061,11 @@
       </c>
       <c r="AM25" s="90">
         <f t="shared" si="70"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN25" s="91">
         <f t="shared" si="71"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="26" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7147,7 +7151,7 @@
       </c>
       <c r="Y26" s="57">
         <f t="shared" si="59"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z26" s="57">
         <f t="shared" si="60"/>
@@ -7159,7 +7163,7 @@
       </c>
       <c r="AB26" s="57">
         <f t="shared" si="62"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AC26" s="58">
         <v>4</v>
@@ -7220,18 +7224,22 @@
         <f>P29</f>
         <v>River Plate</v>
       </c>
-      <c r="F27" s="21"/>
+      <c r="F27" s="21">
+        <v>3</v>
+      </c>
       <c r="G27" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H27" s="21"/>
+      <c r="H27" s="21">
+        <v>1</v>
+      </c>
       <c r="I27" s="13" t="str">
         <f>P30</f>
         <v>Urawa Red Diamonds</v>
       </c>
       <c r="J27" s="63" t="str">
         <f t="shared" si="0"/>
-        <v>empate</v>
+        <v>River Plate</v>
       </c>
       <c r="K27" s="64" t="str">
         <f t="shared" si="1"/>
@@ -7243,7 +7251,7 @@
       </c>
       <c r="M27" s="65" t="str">
         <f t="shared" si="3"/>
-        <v>empate</v>
+        <v>Urawa Red Diamonds</v>
       </c>
       <c r="N27" s="66"/>
       <c r="O27" s="67"/>
@@ -7446,15 +7454,15 @@
       </c>
       <c r="Q29" s="43">
         <f>(S29*3)+(T29*1)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R29" s="43">
         <f>SUM(S29:U29)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S29" s="43">
         <f>COUNTIF(J:J,P29)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T29" s="43">
         <f>COUNTIF(K:K,P29)+COUNTIF(L:L,P29)</f>
@@ -7466,15 +7474,15 @@
       </c>
       <c r="V29" s="43">
         <f>SUMIF(E:E,P29,F:F)+SUMIF(I:I,P29,H:H)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W29" s="43">
         <f>SUMIF(E:E,P29,H:H)+SUMIF(I:I,P29,F:F)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X29" s="43">
         <f>V29-W29</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y29" s="43">
         <f>SUMPRODUCT(($Q$29:$Q$32=Q29)*($X$29:$X$32&gt;X29))</f>
@@ -7505,15 +7513,15 @@
       </c>
       <c r="AG29" s="90">
         <f>VLOOKUP($AE29,$O$29:$X$32,3,FALSE)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH29" s="90">
         <f>VLOOKUP($AE29,$O$29:$X$32,4,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI29" s="90">
         <f>VLOOKUP($AE29,$O$29:$X$32,5,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ29" s="90">
         <f>VLOOKUP($AE29,$O$29:$X$32,6,FALSE)</f>
@@ -7525,15 +7533,15 @@
       </c>
       <c r="AL29" s="90">
         <f>VLOOKUP($AE29,$O$29:$X$32,8,FALSE)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AM29" s="90">
         <f>VLOOKUP($AE29,$O$29:$X$32,9,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN29" s="91">
         <f>VLOOKUP($AE29,$O$29:$X$32,10,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="30" spans="1:40" x14ac:dyDescent="0.25">
@@ -7579,7 +7587,7 @@
       <c r="N30" s="51"/>
       <c r="O30" s="52">
         <f t="shared" ref="O30:O32" si="72">RANK(Q30,$Q$29:$Q$32)+SUM(Y30:AB30)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P30" s="53" t="str">
         <f>Sorteios!C15</f>
@@ -7591,7 +7599,7 @@
       </c>
       <c r="R30" s="43">
         <f t="shared" ref="R30:R32" si="74">SUM(S30:U30)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S30" s="43">
         <f>COUNTIF(J:J,P30)</f>
@@ -7603,23 +7611,23 @@
       </c>
       <c r="U30" s="43">
         <f>COUNTIF(M:M,P30)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V30" s="43">
         <f>SUMIF(E:E,P30,F:F)+SUMIF(I:I,P30,H:H)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W30" s="43">
         <f>SUMIF(E:E,P30,H:H)+SUMIF(I:I,P30,F:F)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X30" s="43">
         <f t="shared" ref="X30:X32" si="75">V30-W30</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="Y30" s="43">
         <f t="shared" ref="Y30:Y32" si="76">SUMPRODUCT(($Q$29:$Q$32=Q30)*($X$29:$X$32&gt;X30))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z30" s="43">
         <f t="shared" ref="Z30:Z32" si="77">SUMPRODUCT(($Q$29:$Q$32=Q30)*($X$29:$X$32=X30)*($V$29:$V$32&gt;V30))</f>
@@ -7631,7 +7639,7 @@
       </c>
       <c r="AB30" s="43">
         <f t="shared" ref="AB30:AB32" si="79">SUMPRODUCT(($Q$29:$Q$32=Q30)*($X$29:$X$32=X30)*($V$29:$V$32=V30)*($W$29:$W$32=W30)*($AC$29:$AC$32&lt;AC30))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC30" s="44">
         <v>2</v>
@@ -7642,7 +7650,7 @@
       </c>
       <c r="AF30" s="83" t="str">
         <f t="shared" ref="AF30:AF32" si="80">VLOOKUP($AE30,$O$29:$X$32,2,FALSE)</f>
-        <v>Urawa Red Diamonds</v>
+        <v>Monterrey</v>
       </c>
       <c r="AG30" s="90">
         <f t="shared" ref="AG30:AG32" si="81">VLOOKUP($AE30,$O$29:$X$32,3,FALSE)</f>
@@ -7720,7 +7728,7 @@
       <c r="N31" s="51"/>
       <c r="O31" s="52">
         <f t="shared" si="72"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P31" s="53" t="str">
         <f>Sorteios!C16</f>
@@ -7772,7 +7780,7 @@
       </c>
       <c r="AB31" s="43">
         <f t="shared" si="79"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC31" s="44">
         <v>3</v>
@@ -7783,7 +7791,7 @@
       </c>
       <c r="AF31" s="83" t="str">
         <f t="shared" si="80"/>
-        <v>Monterrey</v>
+        <v>Internazionale</v>
       </c>
       <c r="AG31" s="90">
         <f t="shared" si="81"/>
@@ -7861,7 +7869,7 @@
       <c r="N32" s="59"/>
       <c r="O32" s="60">
         <f t="shared" si="72"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P32" s="53" t="str">
         <f>Sorteios!C17</f>
@@ -7913,7 +7921,7 @@
       </c>
       <c r="AB32" s="57">
         <f t="shared" si="79"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AC32" s="58">
         <v>4</v>
@@ -7924,7 +7932,7 @@
       </c>
       <c r="AF32" s="84" t="str">
         <f t="shared" si="80"/>
-        <v>Internazionale</v>
+        <v>Urawa Red Diamonds</v>
       </c>
       <c r="AG32" s="92">
         <f t="shared" si="81"/>
@@ -7932,7 +7940,7 @@
       </c>
       <c r="AH32" s="92">
         <f t="shared" si="82"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI32" s="92">
         <f t="shared" si="83"/>
@@ -7944,19 +7952,19 @@
       </c>
       <c r="AK32" s="92">
         <f t="shared" si="85"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL32" s="92">
         <f t="shared" si="86"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM32" s="92">
         <f t="shared" si="87"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AN32" s="93">
         <f t="shared" si="88"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.25">
@@ -7974,11 +7982,15 @@
         <f>P35</f>
         <v>Fluminense</v>
       </c>
-      <c r="F33" s="21"/>
+      <c r="F33" s="21">
+        <v>0</v>
+      </c>
       <c r="G33" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="H33" s="21"/>
+      <c r="H33" s="21">
+        <v>0</v>
+      </c>
       <c r="I33" s="85" t="str">
         <f>P36</f>
         <v>Borussia Dortmund</v>
@@ -7989,11 +8001,11 @@
       </c>
       <c r="K33" s="64" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Fluminense</v>
       </c>
       <c r="L33" s="64" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>Borussia Dortmund</v>
       </c>
       <c r="M33" s="65" t="str">
         <f t="shared" si="3"/>
@@ -8046,18 +8058,22 @@
         <f>P37</f>
         <v>Ulsan</v>
       </c>
-      <c r="F34" s="21"/>
+      <c r="F34" s="21">
+        <v>0</v>
+      </c>
       <c r="G34" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="H34" s="21"/>
+      <c r="H34" s="21">
+        <v>1</v>
+      </c>
       <c r="I34" s="26" t="str">
         <f>P38</f>
         <v>Mamelodi Sundowns</v>
       </c>
       <c r="J34" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>empate</v>
+        <v>Mamelodi Sundowns</v>
       </c>
       <c r="K34" s="43" t="str">
         <f t="shared" si="1"/>
@@ -8069,7 +8085,7 @@
       </c>
       <c r="M34" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>empate</v>
+        <v>Ulsan</v>
       </c>
       <c r="N34" s="50"/>
       <c r="O34" s="52" t="s">
@@ -8192,7 +8208,7 @@
       <c r="N35" s="50"/>
       <c r="O35" s="52">
         <f>RANK(Q35,$Q$35:$Q$38)+SUM(Y35:AB35)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P35" s="53" t="str">
         <f>Sorteios!F14</f>
@@ -8200,11 +8216,11 @@
       </c>
       <c r="Q35" s="43">
         <f>(S35*3)+(T35*1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R35" s="43">
         <f>SUM(S35:U35)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S35" s="43">
         <f>COUNTIF(J:J,P35)</f>
@@ -8212,7 +8228,7 @@
       </c>
       <c r="T35" s="43">
         <f>COUNTIF(K:K,P35)+COUNTIF(L:L,P35)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U35" s="43">
         <f>COUNTIF(M:M,P35)</f>
@@ -8255,19 +8271,19 @@
       </c>
       <c r="AF35" s="83" t="str">
         <f>VLOOKUP($AE35,$O$35:$X$38,2,FALSE)</f>
-        <v>Fluminense</v>
+        <v>Mamelodi Sundowns</v>
       </c>
       <c r="AG35" s="90">
         <f>VLOOKUP($AE35,$O$35:$X$38,3,FALSE)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH35" s="90">
         <f>VLOOKUP($AE35,$O$35:$X$38,4,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI35" s="90">
         <f>VLOOKUP($AE35,$O$35:$X$38,5,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ35" s="90">
         <f>VLOOKUP($AE35,$O$35:$X$38,6,FALSE)</f>
@@ -8279,7 +8295,7 @@
       </c>
       <c r="AL35" s="90">
         <f>VLOOKUP($AE35,$O$35:$X$38,8,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM35" s="90">
         <f>VLOOKUP($AE35,$O$35:$X$38,9,FALSE)</f>
@@ -8287,7 +8303,7 @@
       </c>
       <c r="AN35" s="91">
         <f>VLOOKUP($AE35,$O$35:$X$38,10,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.25">
@@ -8333,7 +8349,7 @@
       <c r="N36" s="50"/>
       <c r="O36" s="52">
         <f t="shared" ref="O36:O38" si="93">RANK(Q36,$Q$35:$Q$38)+SUM(Y36:AB36)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P36" s="53" t="str">
         <f>Sorteios!F15</f>
@@ -8341,11 +8357,11 @@
       </c>
       <c r="Q36" s="43">
         <f t="shared" ref="Q36:Q38" si="94">(S36*3)+(T36*1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R36" s="43">
         <f t="shared" ref="R36:R38" si="95">SUM(S36:U36)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S36" s="43">
         <f>COUNTIF(J:J,P36)</f>
@@ -8353,7 +8369,7 @@
       </c>
       <c r="T36" s="43">
         <f>COUNTIF(K:K,P36)+COUNTIF(L:L,P36)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U36" s="43">
         <f>COUNTIF(M:M,P36)</f>
@@ -8396,15 +8412,15 @@
       </c>
       <c r="AF36" s="83" t="str">
         <f t="shared" ref="AF36:AF38" si="101">VLOOKUP($AE36,$O$35:$X$38,2,FALSE)</f>
-        <v>Borussia Dortmund</v>
+        <v>Fluminense</v>
       </c>
       <c r="AG36" s="90">
         <f t="shared" ref="AG36:AG38" si="102">VLOOKUP($AE36,$O$35:$X$38,3,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH36" s="90">
         <f t="shared" ref="AH36:AH38" si="103">VLOOKUP($AE36,$O$35:$X$38,4,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI36" s="90">
         <f t="shared" ref="AI36:AI38" si="104">VLOOKUP($AE36,$O$35:$X$38,5,FALSE)</f>
@@ -8412,7 +8428,7 @@
       </c>
       <c r="AJ36" s="90">
         <f t="shared" ref="AJ36:AJ38" si="105">VLOOKUP($AE36,$O$35:$X$38,6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK36" s="90">
         <f t="shared" ref="AK36:AK38" si="106">VLOOKUP($AE36,$O$35:$X$38,7,FALSE)</f>
@@ -8474,7 +8490,7 @@
       <c r="N37" s="50"/>
       <c r="O37" s="52">
         <f t="shared" si="93"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P37" s="53" t="str">
         <f>Sorteios!F16</f>
@@ -8486,7 +8502,7 @@
       </c>
       <c r="R37" s="43">
         <f t="shared" si="95"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S37" s="43">
         <f>COUNTIF(J:J,P37)</f>
@@ -8498,7 +8514,7 @@
       </c>
       <c r="U37" s="43">
         <f>COUNTIF(M:M,P37)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V37" s="43">
         <f>SUMIF(E:E,P37,F:F)+SUMIF(I:I,P37,H:H)</f>
@@ -8506,11 +8522,11 @@
       </c>
       <c r="W37" s="43">
         <f>SUMIF(E:E,P37,H:H)+SUMIF(I:I,P37,F:F)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X37" s="43">
         <f t="shared" si="96"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y37" s="43">
         <f t="shared" si="97"/>
@@ -8526,7 +8542,7 @@
       </c>
       <c r="AB37" s="43">
         <f t="shared" si="100"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC37" s="44">
         <v>3</v>
@@ -8537,15 +8553,15 @@
       </c>
       <c r="AF37" s="83" t="str">
         <f t="shared" si="101"/>
-        <v>Ulsan</v>
+        <v>Borussia Dortmund</v>
       </c>
       <c r="AG37" s="90">
         <f t="shared" si="102"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH37" s="90">
         <f t="shared" si="103"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI37" s="90">
         <f t="shared" si="104"/>
@@ -8553,7 +8569,7 @@
       </c>
       <c r="AJ37" s="90">
         <f t="shared" si="105"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK37" s="90">
         <f t="shared" si="106"/>
@@ -8615,7 +8631,7 @@
       <c r="N38" s="61"/>
       <c r="O38" s="60">
         <f t="shared" si="93"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P38" s="53" t="str">
         <f>Sorteios!F17</f>
@@ -8623,15 +8639,15 @@
       </c>
       <c r="Q38" s="57">
         <f t="shared" si="94"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R38" s="57">
         <f t="shared" si="95"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S38" s="43">
         <f>COUNTIF(J:J,P38)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T38" s="43">
         <f>COUNTIF(K:K,P38)+COUNTIF(L:L,P38)</f>
@@ -8643,7 +8659,7 @@
       </c>
       <c r="V38" s="57">
         <f>SUMIF(E:E,P38,F:F)+SUMIF(I:I,P38,H:H)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W38" s="57">
         <f>SUMIF(E:E,P38,H:H)+SUMIF(I:I,P38,F:F)</f>
@@ -8651,7 +8667,7 @@
       </c>
       <c r="X38" s="57">
         <f t="shared" si="96"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y38" s="57">
         <f t="shared" si="97"/>
@@ -8667,7 +8683,7 @@
       </c>
       <c r="AB38" s="57">
         <f t="shared" si="100"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AC38" s="58">
         <v>4</v>
@@ -8678,7 +8694,7 @@
       </c>
       <c r="AF38" s="84" t="str">
         <f t="shared" si="101"/>
-        <v>Mamelodi Sundowns</v>
+        <v>Ulsan</v>
       </c>
       <c r="AG38" s="92">
         <f t="shared" si="102"/>
@@ -8686,7 +8702,7 @@
       </c>
       <c r="AH38" s="92">
         <f t="shared" si="103"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI38" s="92">
         <f t="shared" si="104"/>
@@ -8698,7 +8714,7 @@
       </c>
       <c r="AK38" s="92">
         <f t="shared" si="106"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL38" s="92">
         <f t="shared" si="107"/>
@@ -8706,11 +8722,11 @@
       </c>
       <c r="AM38" s="92">
         <f t="shared" si="108"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN38" s="93">
         <f t="shared" si="109"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.25">
@@ -10387,18 +10403,18 @@
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="109"/>
-      <c r="B4" s="180" t="s">
+      <c r="B4" s="179" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="181"/>
-      <c r="D4" s="181"/>
-      <c r="E4" s="181"/>
-      <c r="F4" s="181"/>
-      <c r="G4" s="181"/>
-      <c r="H4" s="181"/>
-      <c r="I4" s="181"/>
-      <c r="J4" s="181"/>
-      <c r="K4" s="182"/>
+      <c r="C4" s="180"/>
+      <c r="D4" s="180"/>
+      <c r="E4" s="180"/>
+      <c r="F4" s="180"/>
+      <c r="G4" s="180"/>
+      <c r="H4" s="180"/>
+      <c r="I4" s="180"/>
+      <c r="J4" s="180"/>
+      <c r="K4" s="181"/>
       <c r="L4" s="110"/>
       <c r="M4" s="111"/>
       <c r="N4" s="111"/>
@@ -10415,19 +10431,19 @@
       <c r="D5" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="183" t="s">
+      <c r="E5" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="183"/>
-      <c r="G5" s="183" t="s">
+      <c r="F5" s="182"/>
+      <c r="G5" s="182" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="183"/>
-      <c r="I5" s="183"/>
-      <c r="J5" s="183" t="s">
+      <c r="H5" s="182"/>
+      <c r="I5" s="182"/>
+      <c r="J5" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="184"/>
+      <c r="K5" s="183"/>
       <c r="L5" s="113"/>
       <c r="M5" s="113"/>
       <c r="N5" s="113"/>
@@ -10715,18 +10731,18 @@
     </row>
     <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="109"/>
-      <c r="B16" s="180" t="s">
+      <c r="B16" s="179" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="181"/>
-      <c r="D16" s="181"/>
-      <c r="E16" s="181"/>
-      <c r="F16" s="181"/>
-      <c r="G16" s="181"/>
-      <c r="H16" s="181"/>
-      <c r="I16" s="181"/>
-      <c r="J16" s="181"/>
-      <c r="K16" s="182"/>
+      <c r="C16" s="180"/>
+      <c r="D16" s="180"/>
+      <c r="E16" s="180"/>
+      <c r="F16" s="180"/>
+      <c r="G16" s="180"/>
+      <c r="H16" s="180"/>
+      <c r="I16" s="180"/>
+      <c r="J16" s="180"/>
+      <c r="K16" s="181"/>
       <c r="L16" s="110"/>
       <c r="M16" s="111"/>
       <c r="N16" s="111"/>
@@ -10739,19 +10755,19 @@
       <c r="D17" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="183" t="s">
+      <c r="E17" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="183"/>
-      <c r="G17" s="183" t="s">
+      <c r="F17" s="182"/>
+      <c r="G17" s="182" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="183"/>
-      <c r="I17" s="183"/>
-      <c r="J17" s="183" t="s">
+      <c r="H17" s="182"/>
+      <c r="I17" s="182"/>
+      <c r="J17" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="K17" s="184"/>
+      <c r="K17" s="183"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B18" s="129" t="s">
@@ -10897,18 +10913,18 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="109"/>
-      <c r="B24" s="180" t="s">
+      <c r="B24" s="179" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="181"/>
-      <c r="D24" s="181"/>
-      <c r="E24" s="181"/>
-      <c r="F24" s="181"/>
-      <c r="G24" s="181"/>
-      <c r="H24" s="181"/>
-      <c r="I24" s="181"/>
-      <c r="J24" s="181"/>
-      <c r="K24" s="182"/>
+      <c r="C24" s="180"/>
+      <c r="D24" s="180"/>
+      <c r="E24" s="180"/>
+      <c r="F24" s="180"/>
+      <c r="G24" s="180"/>
+      <c r="H24" s="180"/>
+      <c r="I24" s="180"/>
+      <c r="J24" s="180"/>
+      <c r="K24" s="181"/>
       <c r="L24" s="110"/>
       <c r="M24" s="111"/>
       <c r="N24" s="111"/>
@@ -10924,19 +10940,19 @@
       <c r="D25" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="183" t="s">
+      <c r="E25" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="183"/>
-      <c r="G25" s="183" t="s">
+      <c r="F25" s="182"/>
+      <c r="G25" s="182" t="s">
         <v>13</v>
       </c>
-      <c r="H25" s="183"/>
-      <c r="I25" s="183"/>
-      <c r="J25" s="183" t="s">
+      <c r="H25" s="182"/>
+      <c r="I25" s="182"/>
+      <c r="J25" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="K25" s="184"/>
+      <c r="K25" s="183"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="151" t="s">
@@ -11025,18 +11041,18 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="109"/>
-      <c r="B31" s="180" t="s">
+      <c r="B31" s="179" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="181"/>
-      <c r="D31" s="181"/>
-      <c r="E31" s="181"/>
-      <c r="F31" s="181"/>
-      <c r="G31" s="181"/>
-      <c r="H31" s="181"/>
-      <c r="I31" s="181"/>
-      <c r="J31" s="181"/>
-      <c r="K31" s="182"/>
+      <c r="C31" s="180"/>
+      <c r="D31" s="180"/>
+      <c r="E31" s="180"/>
+      <c r="F31" s="180"/>
+      <c r="G31" s="180"/>
+      <c r="H31" s="180"/>
+      <c r="I31" s="180"/>
+      <c r="J31" s="180"/>
+      <c r="K31" s="181"/>
       <c r="L31" s="110"/>
       <c r="M31" s="111"/>
       <c r="N31" s="111"/>
@@ -11052,19 +11068,19 @@
       <c r="D32" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="183" t="s">
+      <c r="E32" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="183"/>
-      <c r="G32" s="183" t="s">
+      <c r="F32" s="182"/>
+      <c r="G32" s="182" t="s">
         <v>13</v>
       </c>
-      <c r="H32" s="183"/>
-      <c r="I32" s="183"/>
-      <c r="J32" s="183" t="s">
+      <c r="H32" s="182"/>
+      <c r="I32" s="182"/>
+      <c r="J32" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="K32" s="184"/>
+      <c r="K32" s="183"/>
     </row>
     <row r="33" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="161" t="s">
@@ -11112,11 +11128,11 @@
     </row>
     <row r="36" spans="1:17" s="137" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="135"/>
-      <c r="B36" s="179" t="s">
+      <c r="B36" s="184" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="179"/>
-      <c r="D36" s="179"/>
+      <c r="C36" s="184"/>
+      <c r="D36" s="184"/>
       <c r="E36" s="173" t="str">
         <f>IF(M33="1º Lugar","",M33)</f>
         <v/>
@@ -11136,11 +11152,11 @@
     </row>
     <row r="37" spans="1:17" s="137" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="135"/>
-      <c r="B37" s="179" t="s">
+      <c r="B37" s="184" t="s">
         <v>106</v>
       </c>
-      <c r="C37" s="179"/>
-      <c r="D37" s="179"/>
+      <c r="C37" s="184"/>
+      <c r="D37" s="184"/>
       <c r="E37" s="175" t="str">
         <f>IF(M34="2º Lugar","",M34)</f>
         <v/>
@@ -11268,11 +11284,12 @@
   </sheetData>
   <sheetProtection password="CC01" sheet="1" selectLockedCells="1"/>
   <mergeCells count="18">
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="B16:K16"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B31:K31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="B36:D36"/>
     <mergeCell ref="B24:K24"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="G25:I25"/>
@@ -11280,12 +11297,11 @@
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B31:K31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="B16:K16"/>
   </mergeCells>
   <conditionalFormatting sqref="F6">
     <cfRule type="expression" dxfId="31" priority="128">
@@ -11452,6 +11468,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DBF2846C41E31A469E3CED25F2422E48" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0c08e4af4d80db6585ac36ba965bb3a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2c8c20e6-817c-474f-b9c2-eb2b1ac24837" xmlns:ns4="dc8c2798-6aba-4af7-93a4-b89253b03650" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4e7db2db65f9cb533b4933096bc9b657" ns3:_="" ns4:_="">
     <xsd:import namespace="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
@@ -11684,14 +11708,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -11702,6 +11718,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83E7837-68AD-48B2-A1AB-AAB452317AF5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
+    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFBCCD5-5BDE-495C-BFE9-46A98A6BC529}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11720,23 +11753,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83E7837-68AD-48B2-A1AB-AAB452317AF5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
-    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A45D7D45-1E18-48AE-827B-096C3C02C976}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Att até Jogo 15
</commit_message>
<xml_diff>
--- a/Mundial de Clubes FIFA 2025.xlsx
+++ b/Mundial de Clubes FIFA 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjunior\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FB6C4004-51DA-49C7-AE04-05AABE333700}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F7E8A6C-B9E9-41A4-8728-BB29611283FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="1185" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{076F3B28-812E-4458-A424-96085A053123}"/>
   </bookViews>
@@ -4019,7 +4019,7 @@
   <dimension ref="A1:AN50"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+      <selection activeCell="F40" sqref="F40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7300,11 +7300,15 @@
         <f>P31</f>
         <v>Monterrey</v>
       </c>
-      <c r="F28" s="21"/>
+      <c r="F28" s="21">
+        <v>1</v>
+      </c>
       <c r="G28" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H28" s="21"/>
+      <c r="H28" s="21">
+        <v>1</v>
+      </c>
       <c r="I28" s="13" t="str">
         <f>P32</f>
         <v>Internazionale</v>
@@ -7315,11 +7319,11 @@
       </c>
       <c r="K28" s="43" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Monterrey</v>
       </c>
       <c r="L28" s="43" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>Internazionale</v>
       </c>
       <c r="M28" s="44" t="str">
         <f t="shared" si="3"/>
@@ -7627,7 +7631,7 @@
       </c>
       <c r="Y30" s="43">
         <f t="shared" ref="Y30:Y32" si="76">SUMPRODUCT(($Q$29:$Q$32=Q30)*($X$29:$X$32&gt;X30))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z30" s="43">
         <f t="shared" ref="Z30:Z32" si="77">SUMPRODUCT(($Q$29:$Q$32=Q30)*($X$29:$X$32=X30)*($V$29:$V$32&gt;V30))</f>
@@ -7654,11 +7658,11 @@
       </c>
       <c r="AG30" s="90">
         <f t="shared" ref="AG30:AG32" si="81">VLOOKUP($AE30,$O$29:$X$32,3,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH30" s="90">
         <f t="shared" ref="AH30:AH32" si="82">VLOOKUP($AE30,$O$29:$X$32,4,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI30" s="90">
         <f t="shared" ref="AI30:AI32" si="83">VLOOKUP($AE30,$O$29:$X$32,5,FALSE)</f>
@@ -7666,7 +7670,7 @@
       </c>
       <c r="AJ30" s="90">
         <f t="shared" ref="AJ30:AJ32" si="84">VLOOKUP($AE30,$O$29:$X$32,6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK30" s="90">
         <f t="shared" ref="AK30:AK32" si="85">VLOOKUP($AE30,$O$29:$X$32,7,FALSE)</f>
@@ -7674,11 +7678,11 @@
       </c>
       <c r="AL30" s="90">
         <f t="shared" ref="AL30:AL32" si="86">VLOOKUP($AE30,$O$29:$X$32,8,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM30" s="90">
         <f t="shared" ref="AM30:AM32" si="87">VLOOKUP($AE30,$O$29:$X$32,9,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN30" s="91">
         <f t="shared" ref="AN30:AN32" si="88">VLOOKUP($AE30,$O$29:$X$32,10,FALSE)</f>
@@ -7736,11 +7740,11 @@
       </c>
       <c r="Q31" s="43">
         <f t="shared" si="73"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R31" s="43">
         <f t="shared" si="74"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S31" s="43">
         <f>COUNTIF(J:J,P31)</f>
@@ -7748,7 +7752,7 @@
       </c>
       <c r="T31" s="43">
         <f>COUNTIF(K:K,P31)+COUNTIF(L:L,P31)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U31" s="43">
         <f>COUNTIF(M:M,P31)</f>
@@ -7756,11 +7760,11 @@
       </c>
       <c r="V31" s="43">
         <f>SUMIF(E:E,P31,F:F)+SUMIF(I:I,P31,H:H)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W31" s="43">
         <f>SUMIF(E:E,P31,H:H)+SUMIF(I:I,P31,F:F)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X31" s="43">
         <f t="shared" si="75"/>
@@ -7795,11 +7799,11 @@
       </c>
       <c r="AG31" s="90">
         <f t="shared" si="81"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH31" s="90">
         <f t="shared" si="82"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI31" s="90">
         <f t="shared" si="83"/>
@@ -7807,7 +7811,7 @@
       </c>
       <c r="AJ31" s="90">
         <f t="shared" si="84"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK31" s="90">
         <f t="shared" si="85"/>
@@ -7815,11 +7819,11 @@
       </c>
       <c r="AL31" s="90">
         <f t="shared" si="86"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM31" s="90">
         <f t="shared" si="87"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN31" s="91">
         <f t="shared" si="88"/>
@@ -7877,11 +7881,11 @@
       </c>
       <c r="Q32" s="57">
         <f t="shared" si="73"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R32" s="57">
         <f t="shared" si="74"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S32" s="43">
         <f>COUNTIF(J:J,P32)</f>
@@ -7889,7 +7893,7 @@
       </c>
       <c r="T32" s="43">
         <f>COUNTIF(K:K,P32)+COUNTIF(L:L,P32)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U32" s="43">
         <f>COUNTIF(M:M,P32)</f>
@@ -7897,11 +7901,11 @@
       </c>
       <c r="V32" s="57">
         <f>SUMIF(E:E,P32,F:F)+SUMIF(I:I,P32,H:H)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W32" s="57">
         <f>SUMIF(E:E,P32,H:H)+SUMIF(I:I,P32,F:F)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X32" s="57">
         <f t="shared" si="75"/>
@@ -8744,18 +8748,22 @@
         <f>P41</f>
         <v>Manchester City</v>
       </c>
-      <c r="F39" s="21"/>
+      <c r="F39" s="21">
+        <v>2</v>
+      </c>
       <c r="G39" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H39" s="21"/>
+      <c r="H39" s="21">
+        <v>0</v>
+      </c>
       <c r="I39" s="13" t="str">
         <f>P42</f>
         <v>Wydad Casablanca</v>
       </c>
       <c r="J39" s="63" t="str">
         <f t="shared" si="89"/>
-        <v>empate</v>
+        <v>Manchester City</v>
       </c>
       <c r="K39" s="64" t="str">
         <f t="shared" si="90"/>
@@ -8767,7 +8775,7 @@
       </c>
       <c r="M39" s="65" t="str">
         <f t="shared" si="92"/>
-        <v>empate</v>
+        <v>Wydad Casablanca</v>
       </c>
       <c r="N39" s="66"/>
       <c r="O39" s="67"/>
@@ -8970,15 +8978,15 @@
       </c>
       <c r="Q41" s="43">
         <f>(S41*3)+(T41*1)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R41" s="43">
         <f>SUM(S41:U41)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S41" s="43">
         <f>COUNTIF(J:J,P41)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T41" s="43">
         <f>COUNTIF(K:K,P41)+COUNTIF(L:L,P41)</f>
@@ -8990,7 +8998,7 @@
       </c>
       <c r="V41" s="43">
         <f>SUMIF(E:E,P41,F:F)+SUMIF(I:I,P41,H:H)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W41" s="43">
         <f>SUMIF(E:E,P41,H:H)+SUMIF(I:I,P41,F:F)</f>
@@ -8998,7 +9006,7 @@
       </c>
       <c r="X41" s="43">
         <f>V41-W41</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y41" s="43">
         <f>SUMPRODUCT(($Q$41:$Q$44=Q41)*($X$41:$X$44&gt;X41))</f>
@@ -9029,15 +9037,15 @@
       </c>
       <c r="AG41" s="90">
         <f>VLOOKUP($AE41,$O$41:$X$44,3,FALSE)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH41" s="90">
         <f>VLOOKUP($AE41,$O$41:$X$44,4,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI41" s="90">
         <f>VLOOKUP($AE41,$O$41:$X$44,5,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ41" s="90">
         <f>VLOOKUP($AE41,$O$41:$X$44,6,FALSE)</f>
@@ -9049,7 +9057,7 @@
       </c>
       <c r="AL41" s="90">
         <f>VLOOKUP($AE41,$O$41:$X$44,8,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM41" s="90">
         <f>VLOOKUP($AE41,$O$41:$X$44,9,FALSE)</f>
@@ -9057,7 +9065,7 @@
       </c>
       <c r="AN41" s="91">
         <f>VLOOKUP($AE41,$O$41:$X$44,10,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="42" spans="1:40" x14ac:dyDescent="0.25">
@@ -9103,7 +9111,7 @@
       <c r="N42" s="51"/>
       <c r="O42" s="52">
         <f t="shared" ref="O42:O44" si="110">RANK(Q42,$Q$41:$Q$44)+SUM(Y42:AB42)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P42" s="53" t="str">
         <f>Sorteios!I15</f>
@@ -9115,7 +9123,7 @@
       </c>
       <c r="R42" s="43">
         <f t="shared" ref="R42:R44" si="112">SUM(S42:U42)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S42" s="43">
         <f>COUNTIF(J:J,P42)</f>
@@ -9127,7 +9135,7 @@
       </c>
       <c r="U42" s="43">
         <f>COUNTIF(M:M,P42)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V42" s="43">
         <f>SUMIF(E:E,P42,F:F)+SUMIF(I:I,P42,H:H)</f>
@@ -9135,15 +9143,15 @@
       </c>
       <c r="W42" s="43">
         <f>SUMIF(E:E,P42,H:H)+SUMIF(I:I,P42,F:F)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X42" s="43">
         <f t="shared" ref="X42:X44" si="113">V42-W42</f>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="Y42" s="43">
         <f t="shared" ref="Y42:Y44" si="114">SUMPRODUCT(($Q$41:$Q$44=Q42)*($X$41:$X$44&gt;X42))</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Z42" s="43">
         <f t="shared" ref="Z42:Z44" si="115">SUMPRODUCT(($Q$41:$Q$44=Q42)*($X$41:$X$44=X42)*($V$41:$V$44&gt;V42))</f>
@@ -9155,7 +9163,7 @@
       </c>
       <c r="AB42" s="43">
         <f t="shared" ref="AB42:AB44" si="117">SUMPRODUCT(($Q$41:$Q$44=Q42)*($X$41:$X$44=X42)*($V$41:$V$44=V42)*($W$41:$W$44=W42)*($AC$41:$AC$44&lt;AC42))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC42" s="44">
         <v>2</v>
@@ -9166,7 +9174,7 @@
       </c>
       <c r="AF42" s="83" t="str">
         <f t="shared" ref="AF42:AF44" si="118">VLOOKUP($AE42,$O$41:$X$44,2,FALSE)</f>
-        <v>Wydad Casablanca</v>
+        <v>Al Ain</v>
       </c>
       <c r="AG42" s="90">
         <f t="shared" ref="AG42:AG44" si="119">VLOOKUP($AE42,$O$41:$X$44,3,FALSE)</f>
@@ -9244,7 +9252,7 @@
       <c r="N43" s="51"/>
       <c r="O43" s="52">
         <f t="shared" si="110"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P43" s="53" t="str">
         <f>Sorteios!I16</f>
@@ -9296,7 +9304,7 @@
       </c>
       <c r="AB43" s="43">
         <f t="shared" si="117"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC43" s="44">
         <v>3</v>
@@ -9307,7 +9315,7 @@
       </c>
       <c r="AF43" s="83" t="str">
         <f t="shared" si="118"/>
-        <v>Al Ain</v>
+        <v>Juventus</v>
       </c>
       <c r="AG43" s="90">
         <f t="shared" si="119"/>
@@ -9385,7 +9393,7 @@
       <c r="N44" s="59"/>
       <c r="O44" s="60">
         <f t="shared" si="110"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P44" s="53" t="str">
         <f>Sorteios!I17</f>
@@ -9437,7 +9445,7 @@
       </c>
       <c r="AB44" s="57">
         <f t="shared" si="117"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="AC44" s="58">
         <v>4</v>
@@ -9448,7 +9456,7 @@
       </c>
       <c r="AF44" s="84" t="str">
         <f t="shared" si="118"/>
-        <v>Juventus</v>
+        <v>Wydad Casablanca</v>
       </c>
       <c r="AG44" s="92">
         <f t="shared" si="119"/>
@@ -9456,7 +9464,7 @@
       </c>
       <c r="AH44" s="92">
         <f t="shared" si="120"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI44" s="92">
         <f t="shared" si="121"/>
@@ -9468,7 +9476,7 @@
       </c>
       <c r="AK44" s="92">
         <f t="shared" si="123"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL44" s="92">
         <f t="shared" si="124"/>
@@ -9476,11 +9484,11 @@
       </c>
       <c r="AM44" s="92">
         <f t="shared" si="125"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN44" s="93">
         <f t="shared" si="126"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="45" spans="1:40" x14ac:dyDescent="0.25">
@@ -9498,11 +9506,15 @@
         <f>P47</f>
         <v>Real Madrid</v>
       </c>
-      <c r="F45" s="21"/>
+      <c r="F45" s="21">
+        <v>1</v>
+      </c>
       <c r="G45" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="H45" s="21"/>
+      <c r="H45" s="21">
+        <v>1</v>
+      </c>
       <c r="I45" s="85" t="str">
         <f>P48</f>
         <v>Al-Hilal</v>
@@ -9513,11 +9525,11 @@
       </c>
       <c r="K45" s="64" t="str">
         <f t="shared" si="90"/>
-        <v/>
+        <v>Real Madrid</v>
       </c>
       <c r="L45" s="64" t="str">
         <f t="shared" si="91"/>
-        <v/>
+        <v>Al-Hilal</v>
       </c>
       <c r="M45" s="65" t="str">
         <f t="shared" si="92"/>
@@ -9570,18 +9582,22 @@
         <f>P49</f>
         <v>Pachuca</v>
       </c>
-      <c r="F46" s="21"/>
+      <c r="F46" s="21">
+        <v>1</v>
+      </c>
       <c r="G46" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="H46" s="21"/>
+      <c r="H46" s="21">
+        <v>2</v>
+      </c>
       <c r="I46" s="26" t="str">
         <f>P50</f>
         <v>Red Bull Salzburg</v>
       </c>
       <c r="J46" s="42" t="str">
         <f t="shared" si="89"/>
-        <v>empate</v>
+        <v>Red Bull Salzburg</v>
       </c>
       <c r="K46" s="43" t="str">
         <f t="shared" si="90"/>
@@ -9593,7 +9609,7 @@
       </c>
       <c r="M46" s="44" t="str">
         <f t="shared" si="92"/>
-        <v>empate</v>
+        <v>Pachuca</v>
       </c>
       <c r="N46" s="50"/>
       <c r="O46" s="52" t="s">
@@ -9716,7 +9732,7 @@
       <c r="N47" s="50"/>
       <c r="O47" s="52">
         <f>RANK(Q47,$Q$47:$Q$50)+SUM(Y47:AB47)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P47" s="53" t="str">
         <f>Sorteios!L14</f>
@@ -9724,11 +9740,11 @@
       </c>
       <c r="Q47" s="43">
         <f>(S47*3)+(T47*1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R47" s="43">
         <f>SUM(S47:U47)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S47" s="43">
         <f>COUNTIF(J:J,P47)</f>
@@ -9736,7 +9752,7 @@
       </c>
       <c r="T47" s="43">
         <f>COUNTIF(K:K,P47)+COUNTIF(L:L,P47)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U47" s="43">
         <f>COUNTIF(M:M,P47)</f>
@@ -9744,11 +9760,11 @@
       </c>
       <c r="V47" s="43">
         <f>SUMIF(E:E,P47,F:F)+SUMIF(I:I,P47,H:H)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W47" s="43">
         <f>SUMIF(E:E,P47,H:H)+SUMIF(I:I,P47,F:F)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X47" s="43">
         <f>V47-W47</f>
@@ -9779,19 +9795,19 @@
       </c>
       <c r="AF47" s="83" t="str">
         <f>VLOOKUP($AE47,$O$47:$X$50,2,FALSE)</f>
-        <v>Real Madrid</v>
+        <v>Red Bull Salzburg</v>
       </c>
       <c r="AG47" s="90">
         <f>VLOOKUP($AE47,$O$47:$X$50,3,FALSE)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH47" s="90">
         <f>VLOOKUP($AE47,$O$47:$X$50,4,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI47" s="90">
         <f>VLOOKUP($AE47,$O$47:$X$50,5,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ47" s="90">
         <f>VLOOKUP($AE47,$O$47:$X$50,6,FALSE)</f>
@@ -9803,15 +9819,15 @@
       </c>
       <c r="AL47" s="90">
         <f>VLOOKUP($AE47,$O$47:$X$50,8,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM47" s="90">
         <f>VLOOKUP($AE47,$O$47:$X$50,9,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN47" s="91">
         <f>VLOOKUP($AE47,$O$47:$X$50,10,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="48" spans="1:40" x14ac:dyDescent="0.25">
@@ -9857,7 +9873,7 @@
       <c r="N48" s="50"/>
       <c r="O48" s="52">
         <f>RANK(Q48,$Q$47:$Q$50)+SUM(Y48:AB48)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P48" s="53" t="str">
         <f>Sorteios!L15</f>
@@ -9865,11 +9881,11 @@
       </c>
       <c r="Q48" s="43">
         <f t="shared" ref="Q48:Q50" si="127">(S48*3)+(T48*1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R48" s="43">
         <f t="shared" ref="R48:R50" si="128">SUM(S48:U48)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S48" s="43">
         <f>COUNTIF(J:J,P48)</f>
@@ -9877,7 +9893,7 @@
       </c>
       <c r="T48" s="43">
         <f>COUNTIF(K:K,P48)+COUNTIF(L:L,P48)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U48" s="43">
         <f>COUNTIF(M:M,P48)</f>
@@ -9885,11 +9901,11 @@
       </c>
       <c r="V48" s="43">
         <f>SUMIF(E:E,P48,F:F)+SUMIF(I:I,P48,H:H)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W48" s="43">
         <f>SUMIF(E:E,P48,H:H)+SUMIF(I:I,P48,F:F)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X48" s="43">
         <f t="shared" ref="X48:X50" si="129">V48-W48</f>
@@ -9920,15 +9936,15 @@
       </c>
       <c r="AF48" s="83" t="str">
         <f t="shared" ref="AF48:AF50" si="134">VLOOKUP($AE48,$O$47:$X$50,2,FALSE)</f>
-        <v>Al-Hilal</v>
+        <v>Real Madrid</v>
       </c>
       <c r="AG48" s="90">
         <f t="shared" ref="AG48:AG50" si="135">VLOOKUP($AE48,$O$47:$X$50,3,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH48" s="90">
         <f t="shared" ref="AH48:AH50" si="136">VLOOKUP($AE48,$O$47:$X$50,4,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI48" s="90">
         <f t="shared" ref="AI48:AI50" si="137">VLOOKUP($AE48,$O$47:$X$50,5,FALSE)</f>
@@ -9936,7 +9952,7 @@
       </c>
       <c r="AJ48" s="90">
         <f t="shared" ref="AJ48:AJ50" si="138">VLOOKUP($AE48,$O$47:$X$50,6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK48" s="90">
         <f t="shared" ref="AK48:AK50" si="139">VLOOKUP($AE48,$O$47:$X$50,7,FALSE)</f>
@@ -9944,11 +9960,11 @@
       </c>
       <c r="AL48" s="90">
         <f t="shared" ref="AL48:AL50" si="140">VLOOKUP($AE48,$O$47:$X$50,8,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM48" s="90">
         <f t="shared" ref="AM48:AM50" si="141">VLOOKUP($AE48,$O$47:$X$50,9,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN48" s="91">
         <f t="shared" ref="AN48:AN50" si="142">VLOOKUP($AE48,$O$47:$X$50,10,FALSE)</f>
@@ -9998,7 +10014,7 @@
       <c r="N49" s="50"/>
       <c r="O49" s="52">
         <f t="shared" ref="O49:O50" si="143">RANK(Q49,$Q$47:$Q$50)+SUM(Y49:AB49)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P49" s="53" t="str">
         <f>Sorteios!L16</f>
@@ -10010,7 +10026,7 @@
       </c>
       <c r="R49" s="43">
         <f t="shared" si="128"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S49" s="43">
         <f>COUNTIF(J:J,P49)</f>
@@ -10022,19 +10038,19 @@
       </c>
       <c r="U49" s="43">
         <f>COUNTIF(M:M,P49)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V49" s="43">
         <f>SUMIF(E:E,P49,F:F)+SUMIF(I:I,P49,H:H)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W49" s="43">
         <f>SUMIF(E:E,P49,H:H)+SUMIF(I:I,P49,F:F)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X49" s="43">
         <f t="shared" si="129"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y49" s="43">
         <f t="shared" si="130"/>
@@ -10050,7 +10066,7 @@
       </c>
       <c r="AB49" s="43">
         <f t="shared" si="133"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC49" s="44">
         <v>3</v>
@@ -10061,15 +10077,15 @@
       </c>
       <c r="AF49" s="83" t="str">
         <f t="shared" si="134"/>
-        <v>Pachuca</v>
+        <v>Al-Hilal</v>
       </c>
       <c r="AG49" s="90">
         <f t="shared" si="135"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH49" s="90">
         <f t="shared" si="136"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI49" s="90">
         <f t="shared" si="137"/>
@@ -10077,7 +10093,7 @@
       </c>
       <c r="AJ49" s="90">
         <f t="shared" si="138"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK49" s="90">
         <f t="shared" si="139"/>
@@ -10085,11 +10101,11 @@
       </c>
       <c r="AL49" s="90">
         <f t="shared" si="140"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM49" s="90">
         <f t="shared" si="141"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN49" s="91">
         <f t="shared" si="142"/>
@@ -10139,7 +10155,7 @@
       <c r="N50" s="50"/>
       <c r="O50" s="73">
         <f t="shared" si="143"/>
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P50" s="53" t="str">
         <f>Sorteios!L17</f>
@@ -10147,15 +10163,15 @@
       </c>
       <c r="Q50" s="57">
         <f t="shared" si="127"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R50" s="57">
         <f t="shared" si="128"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="S50" s="43">
         <f>COUNTIF(J:J,P50)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T50" s="43">
         <f>COUNTIF(K:K,P50)+COUNTIF(L:L,P50)</f>
@@ -10167,15 +10183,15 @@
       </c>
       <c r="V50" s="57">
         <f>SUMIF(E:E,P50,F:F)+SUMIF(I:I,P50,H:H)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W50" s="57">
         <f>SUMIF(E:E,P50,H:H)+SUMIF(I:I,P50,F:F)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X50" s="57">
         <f t="shared" si="129"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y50" s="57">
         <f t="shared" si="130"/>
@@ -10191,7 +10207,7 @@
       </c>
       <c r="AB50" s="57">
         <f t="shared" si="133"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AC50" s="58">
         <v>4</v>
@@ -10202,7 +10218,7 @@
       </c>
       <c r="AF50" s="84" t="str">
         <f t="shared" si="134"/>
-        <v>Red Bull Salzburg</v>
+        <v>Pachuca</v>
       </c>
       <c r="AG50" s="92">
         <f t="shared" si="135"/>
@@ -10210,7 +10226,7 @@
       </c>
       <c r="AH50" s="92">
         <f t="shared" si="136"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AI50" s="92">
         <f t="shared" si="137"/>
@@ -10222,19 +10238,19 @@
       </c>
       <c r="AK50" s="92">
         <f t="shared" si="139"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL50" s="92">
         <f t="shared" si="140"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM50" s="92">
         <f t="shared" si="141"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN50" s="93">
         <f t="shared" si="142"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
   </sheetData>
@@ -11460,7 +11476,7 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
   <ignoredErrors>
     <ignoredError sqref="E19:E20 K19:K20" formula="1"/>
   </ignoredErrors>
@@ -11468,6 +11484,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
@@ -11475,7 +11500,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DBF2846C41E31A469E3CED25F2422E48" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0c08e4af4d80db6585ac36ba965bb3a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2c8c20e6-817c-474f-b9c2-eb2b1ac24837" xmlns:ns4="dc8c2798-6aba-4af7-93a4-b89253b03650" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4e7db2db65f9cb533b4933096bc9b657" ns3:_="" ns4:_="">
     <xsd:import namespace="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
@@ -11708,33 +11733,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A45D7D45-1E18-48AE-827B-096C3C02C976}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83E7837-68AD-48B2-A1AB-AAB452317AF5}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
     <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
     <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFBCCD5-5BDE-495C-BFE9-46A98A6BC529}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11751,12 +11775,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A45D7D45-1E18-48AE-827B-096C3C02C976}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Att até jogo 32
Minor changes. Correção de uma data errada da 1ª fase.
</commit_message>
<xml_diff>
--- a/Mundial de Clubes FIFA 2025.xlsx
+++ b/Mundial de Clubes FIFA 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjunior\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2F7E8A6C-B9E9-41A4-8728-BB29611283FB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{07D0F67C-3835-4B35-9AC7-CC16D9173FC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="1185" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{076F3B28-812E-4458-A424-96085A053123}"/>
   </bookViews>
@@ -1598,6 +1598,9 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1612,9 +1615,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4018,8 +4018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45896CCF-F333-49AF-850B-159476231F1C}">
   <dimension ref="A1:AN50"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4374,18 +4374,22 @@
         <f>P5</f>
         <v>Palmeiras</v>
       </c>
-      <c r="F5" s="21"/>
+      <c r="F5" s="21">
+        <v>2</v>
+      </c>
       <c r="G5" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H5" s="21"/>
+      <c r="H5" s="21">
+        <v>0</v>
+      </c>
       <c r="I5" s="13" t="str">
         <f>P7</f>
         <v>Al-Ahly</v>
       </c>
       <c r="J5" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>empate</v>
+        <v>Palmeiras</v>
       </c>
       <c r="K5" s="43" t="str">
         <f t="shared" si="1"/>
@@ -4397,7 +4401,7 @@
       </c>
       <c r="M5" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>empate</v>
+        <v>Al-Ahly</v>
       </c>
       <c r="N5" s="51"/>
       <c r="O5" s="52">
@@ -4410,15 +4414,15 @@
       </c>
       <c r="Q5" s="43">
         <f>(S5*3)+(T5*1)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R5" s="43">
         <f>SUM(S5:U5)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S5" s="43">
         <f>COUNTIF(J:J,P5)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T5" s="43">
         <f>COUNTIF(K:K,P5)+COUNTIF(L:L,P5)</f>
@@ -4430,7 +4434,7 @@
       </c>
       <c r="V5" s="43">
         <f>SUMIF(E:E,P5,F:F)+SUMIF(I:I,P5,H:H)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W5" s="43">
         <f>SUMIF(E:E,P5,H:H)+SUMIF(I:I,P5,F:F)</f>
@@ -4438,7 +4442,7 @@
       </c>
       <c r="X5" s="43">
         <f>V5-W5</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y5" s="43">
         <f>SUMPRODUCT(($Q$5:$Q$8=Q5)*($X$5:$X$8&gt;X5))</f>
@@ -4469,15 +4473,15 @@
       </c>
       <c r="AG5" s="90">
         <f>VLOOKUP($AE5,$O$5:$X$8,3,FALSE)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AH5" s="90">
         <f>VLOOKUP($AE5,$O$5:$X$8,4,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI5" s="90">
         <f>VLOOKUP($AE5,$O$5:$X$8,5,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ5" s="90">
         <f>VLOOKUP($AE5,$O$5:$X$8,6,FALSE)</f>
@@ -4489,7 +4493,7 @@
       </c>
       <c r="AL5" s="90">
         <f>VLOOKUP($AE5,$O$5:$X$8,8,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM5" s="90">
         <f>VLOOKUP($AE5,$O$5:$X$8,9,FALSE)</f>
@@ -4497,7 +4501,7 @@
       </c>
       <c r="AN5" s="91">
         <f>VLOOKUP($AE5,$O$5:$X$8,10,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.25">
@@ -4515,18 +4519,22 @@
         <f>P8</f>
         <v>Inter Miami</v>
       </c>
-      <c r="F6" s="21"/>
+      <c r="F6" s="21">
+        <v>2</v>
+      </c>
       <c r="G6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H6" s="21"/>
+      <c r="H6" s="21">
+        <v>1</v>
+      </c>
       <c r="I6" s="13" t="str">
         <f>P6</f>
         <v>Porto</v>
       </c>
       <c r="J6" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>empate</v>
+        <v>Inter Miami</v>
       </c>
       <c r="K6" s="43" t="str">
         <f t="shared" si="1"/>
@@ -4538,12 +4546,12 @@
       </c>
       <c r="M6" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>empate</v>
+        <v>Porto</v>
       </c>
       <c r="N6" s="51"/>
       <c r="O6" s="52">
         <f t="shared" ref="O6:O8" si="4">RANK(Q6,$Q$5:$Q$8)+SUM(Y6:AB6)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P6" s="53" t="str">
         <f>Sorteios!C7</f>
@@ -4555,7 +4563,7 @@
       </c>
       <c r="R6" s="43">
         <f t="shared" ref="R6:R8" si="6">SUM(S6:U6)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S6" s="43">
         <f>COUNTIF(J:J,P6)</f>
@@ -4567,19 +4575,19 @@
       </c>
       <c r="U6" s="43">
         <f>COUNTIF(M:M,P6)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V6" s="43">
         <f>SUMIF(E:E,P6,F:F)+SUMIF(I:I,P6,H:H)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W6" s="43">
         <f>SUMIF(E:E,P6,H:H)+SUMIF(I:I,P6,F:F)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X6" s="43">
         <f t="shared" ref="X6:X8" si="7">V6-W6</f>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y6" s="43">
         <f t="shared" ref="Y6:Y8" si="8">SUMPRODUCT(($Q$5:$Q$8=Q6)*($X$5:$X$8&gt;X6))</f>
@@ -4595,7 +4603,7 @@
       </c>
       <c r="AB6" s="43">
         <f t="shared" ref="AB6:AB8" si="11">SUMPRODUCT(($Q$5:$Q$8=Q6)*($X$5:$X$8=X6)*($V$5:$V$8=V6)*($W$5:$W$8=W6)*($AC$5:$AC$8&lt;AC6))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC6" s="44">
         <v>2</v>
@@ -4606,19 +4614,19 @@
       </c>
       <c r="AF6" s="83" t="str">
         <f t="shared" ref="AF6:AF8" si="12">VLOOKUP($AE6,$O$5:$X$8,2,FALSE)</f>
-        <v>Porto</v>
+        <v>Inter Miami</v>
       </c>
       <c r="AG6" s="90">
         <f t="shared" ref="AG6:AG8" si="13">VLOOKUP($AE6,$O$5:$X$8,3,FALSE)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AH6" s="90">
         <f t="shared" ref="AH6:AH8" si="14">VLOOKUP($AE6,$O$5:$X$8,4,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI6" s="90">
         <f t="shared" ref="AI6:AI8" si="15">VLOOKUP($AE6,$O$5:$X$8,5,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ6" s="90">
         <f t="shared" ref="AJ6:AJ8" si="16">VLOOKUP($AE6,$O$5:$X$8,6,FALSE)</f>
@@ -4630,15 +4638,15 @@
       </c>
       <c r="AL6" s="90">
         <f t="shared" ref="AL6:AL8" si="18">VLOOKUP($AE6,$O$5:$X$8,8,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM6" s="90">
         <f t="shared" ref="AM6:AM8" si="19">VLOOKUP($AE6,$O$5:$X$8,9,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN6" s="91">
         <f t="shared" ref="AN6:AN8" si="20">VLOOKUP($AE6,$O$5:$X$8,10,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.25">
@@ -4647,7 +4655,7 @@
         <v>15</v>
       </c>
       <c r="C7" s="80">
-        <v>45861</v>
+        <v>45831</v>
       </c>
       <c r="D7" s="40" t="s">
         <v>42</v>
@@ -4684,7 +4692,7 @@
       <c r="N7" s="51"/>
       <c r="O7" s="52">
         <f t="shared" si="4"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P7" s="53" t="str">
         <f>Sorteios!C8</f>
@@ -4696,7 +4704,7 @@
       </c>
       <c r="R7" s="43">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S7" s="43">
         <f>COUNTIF(J:J,P7)</f>
@@ -4708,7 +4716,7 @@
       </c>
       <c r="U7" s="43">
         <f>COUNTIF(M:M,P7)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V7" s="43">
         <f>SUMIF(E:E,P7,F:F)+SUMIF(I:I,P7,H:H)</f>
@@ -4716,15 +4724,15 @@
       </c>
       <c r="W7" s="43">
         <f>SUMIF(E:E,P7,H:H)+SUMIF(I:I,P7,F:F)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X7" s="43">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="Y7" s="43">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z7" s="43">
         <f t="shared" si="9"/>
@@ -4736,7 +4744,7 @@
       </c>
       <c r="AB7" s="43">
         <f t="shared" si="11"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="AC7" s="44">
         <v>3</v>
@@ -4747,7 +4755,7 @@
       </c>
       <c r="AF7" s="83" t="str">
         <f t="shared" si="12"/>
-        <v>Al-Ahly</v>
+        <v>Porto</v>
       </c>
       <c r="AG7" s="90">
         <f t="shared" si="13"/>
@@ -4755,7 +4763,7 @@
       </c>
       <c r="AH7" s="90">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI7" s="90">
         <f t="shared" si="15"/>
@@ -4767,19 +4775,19 @@
       </c>
       <c r="AK7" s="90">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL7" s="90">
         <f t="shared" si="18"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM7" s="90">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN7" s="91">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="8" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -4825,7 +4833,7 @@
       <c r="N8" s="59"/>
       <c r="O8" s="60">
         <f t="shared" si="4"/>
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="P8" s="53" t="str">
         <f>Sorteios!C9</f>
@@ -4833,15 +4841,15 @@
       </c>
       <c r="Q8" s="43">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R8" s="43">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S8" s="43">
         <f>COUNTIF(J:J,P8)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T8" s="43">
         <f>COUNTIF(K:K,P8)+COUNTIF(L:L,P8)</f>
@@ -4853,19 +4861,19 @@
       </c>
       <c r="V8" s="43">
         <f>SUMIF(E:E,P8,F:F)+SUMIF(I:I,P8,H:H)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W8" s="43">
         <f>SUMIF(E:E,P8,H:H)+SUMIF(I:I,P8,F:F)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X8" s="43">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y8" s="43">
         <f t="shared" si="8"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z8" s="43">
         <f t="shared" si="9"/>
@@ -4877,7 +4885,7 @@
       </c>
       <c r="AB8" s="43">
         <f t="shared" si="11"/>
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="AC8" s="58">
         <v>4</v>
@@ -4888,7 +4896,7 @@
       </c>
       <c r="AF8" s="84" t="str">
         <f t="shared" si="12"/>
-        <v>Inter Miami</v>
+        <v>Al-Ahly</v>
       </c>
       <c r="AG8" s="92">
         <f t="shared" si="13"/>
@@ -4896,7 +4904,7 @@
       </c>
       <c r="AH8" s="92">
         <f t="shared" si="14"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI8" s="92">
         <f t="shared" si="15"/>
@@ -4908,7 +4916,7 @@
       </c>
       <c r="AK8" s="92">
         <f t="shared" si="17"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL8" s="92">
         <f t="shared" si="18"/>
@@ -4916,11 +4924,11 @@
       </c>
       <c r="AM8" s="92">
         <f t="shared" si="19"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN8" s="93">
         <f t="shared" si="20"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.25">
@@ -5136,18 +5144,22 @@
         <f>P11</f>
         <v>Paris Saint-Germain</v>
       </c>
-      <c r="F11" s="21"/>
+      <c r="F11" s="21">
+        <v>0</v>
+      </c>
       <c r="G11" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="H11" s="21"/>
+      <c r="H11" s="21">
+        <v>1</v>
+      </c>
       <c r="I11" s="26" t="str">
         <f>P13</f>
         <v>Botafogo</v>
       </c>
       <c r="J11" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>empate</v>
+        <v>Botafogo</v>
       </c>
       <c r="K11" s="43" t="str">
         <f t="shared" si="1"/>
@@ -5159,12 +5171,12 @@
       </c>
       <c r="M11" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>empate</v>
+        <v>Paris Saint-Germain</v>
       </c>
       <c r="N11" s="51"/>
       <c r="O11" s="52">
         <f>RANK(Q11,$Q$11:$Q$14)+SUM(Y11:AB11)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P11" s="53" t="str">
         <f>Sorteios!F6</f>
@@ -5176,7 +5188,7 @@
       </c>
       <c r="R11" s="43">
         <f>SUM(S11:U11)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S11" s="43">
         <f>COUNTIF(J:J,P11)</f>
@@ -5188,7 +5200,7 @@
       </c>
       <c r="U11" s="43">
         <f>COUNTIF(M:M,P11)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V11" s="43">
         <f>SUMIF(E:E,P11,F:F)+SUMIF(I:I,P11,H:H)</f>
@@ -5196,11 +5208,11 @@
       </c>
       <c r="W11" s="43">
         <f>SUMIF(E:E,P11,H:H)+SUMIF(I:I,P11,F:F)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X11" s="43">
         <f>V11-W11</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="Y11" s="43">
         <f>SUMPRODUCT(($Q$11:$Q$14=Q11)*($X$11:$X$14&gt;X11))</f>
@@ -5227,19 +5239,19 @@
       </c>
       <c r="AF11" s="83" t="str">
         <f>VLOOKUP($AE11,$O$11:$X$14,2,FALSE)</f>
-        <v>Paris Saint-Germain</v>
+        <v>Botafogo</v>
       </c>
       <c r="AG11" s="90">
         <f>VLOOKUP($AE11,$O$11:$X$14,3,FALSE)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AH11" s="90">
         <f>VLOOKUP($AE11,$O$11:$X$14,4,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI11" s="90">
         <f>VLOOKUP($AE11,$O$11:$X$14,5,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ11" s="90">
         <f>VLOOKUP($AE11,$O$11:$X$14,6,FALSE)</f>
@@ -5251,15 +5263,15 @@
       </c>
       <c r="AL11" s="90">
         <f>VLOOKUP($AE11,$O$11:$X$14,8,FALSE)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AM11" s="90">
         <f>VLOOKUP($AE11,$O$11:$X$14,9,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN11" s="91">
         <f>VLOOKUP($AE11,$O$11:$X$14,10,FALSE)</f>
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.25">
@@ -5277,18 +5289,22 @@
         <f>P14</f>
         <v>Seattle Sounders</v>
       </c>
-      <c r="F12" s="21"/>
+      <c r="F12" s="21">
+        <v>1</v>
+      </c>
       <c r="G12" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="H12" s="21"/>
+      <c r="H12" s="21">
+        <v>3</v>
+      </c>
       <c r="I12" s="26" t="str">
         <f>P12</f>
         <v>Atlético de Madrid</v>
       </c>
       <c r="J12" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>empate</v>
+        <v>Atlético de Madrid</v>
       </c>
       <c r="K12" s="43" t="str">
         <f t="shared" si="1"/>
@@ -5300,12 +5316,12 @@
       </c>
       <c r="M12" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>empate</v>
+        <v>Seattle Sounders</v>
       </c>
       <c r="N12" s="51"/>
       <c r="O12" s="52">
         <f t="shared" ref="O12:O14" si="21">RANK(Q12,$Q$11:$Q$14)+SUM(Y12:AB12)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P12" s="53" t="str">
         <f>Sorteios!F7</f>
@@ -5313,15 +5329,15 @@
       </c>
       <c r="Q12" s="43">
         <f t="shared" ref="Q12:Q14" si="22">(S12*3)+(T12*1)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R12" s="43">
         <f t="shared" ref="R12:R14" si="23">SUM(S12:U12)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S12" s="43">
         <f>COUNTIF(J:J,P12)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T12" s="43">
         <f>COUNTIF(K:K,P12)+COUNTIF(L:L,P12)</f>
@@ -5333,15 +5349,15 @@
       </c>
       <c r="V12" s="43">
         <f>SUMIF(E:E,P12,F:F)+SUMIF(I:I,P12,H:H)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="W12" s="43">
         <f>SUMIF(E:E,P12,H:H)+SUMIF(I:I,P12,F:F)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="X12" s="43">
         <f t="shared" ref="X12:X14" si="24">V12-W12</f>
-        <v>-4</v>
+        <v>-2</v>
       </c>
       <c r="Y12" s="43">
         <f t="shared" ref="Y12:Y14" si="25">SUMPRODUCT(($Q$11:$Q$14=Q12)*($X$11:$X$14&gt;X12))</f>
@@ -5368,7 +5384,7 @@
       </c>
       <c r="AF12" s="83" t="str">
         <f t="shared" ref="AF12:AF14" si="29">VLOOKUP($AE12,$O$11:$X$14,2,FALSE)</f>
-        <v>Botafogo</v>
+        <v>Paris Saint-Germain</v>
       </c>
       <c r="AG12" s="90">
         <f t="shared" ref="AG12:AG14" si="30">VLOOKUP($AE12,$O$11:$X$14,3,FALSE)</f>
@@ -5376,7 +5392,7 @@
       </c>
       <c r="AH12" s="90">
         <f t="shared" ref="AH12:AH14" si="31">VLOOKUP($AE12,$O$11:$X$14,4,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI12" s="90">
         <f t="shared" ref="AI12:AI14" si="32">VLOOKUP($AE12,$O$11:$X$14,5,FALSE)</f>
@@ -5388,11 +5404,11 @@
       </c>
       <c r="AK12" s="90">
         <f t="shared" ref="AK12:AK14" si="34">VLOOKUP($AE12,$O$11:$X$14,7,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL12" s="90">
         <f t="shared" ref="AL12:AL14" si="35">VLOOKUP($AE12,$O$11:$X$14,8,FALSE)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AM12" s="90">
         <f t="shared" ref="AM12:AM14" si="36">VLOOKUP($AE12,$O$11:$X$14,9,FALSE)</f>
@@ -5400,7 +5416,7 @@
       </c>
       <c r="AN12" s="91">
         <f t="shared" ref="AN12:AN14" si="37">VLOOKUP($AE12,$O$11:$X$14,10,FALSE)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.25">
@@ -5446,7 +5462,7 @@
       <c r="N13" s="51"/>
       <c r="O13" s="52">
         <f t="shared" si="21"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P13" s="53" t="str">
         <f>Sorteios!F8</f>
@@ -5454,15 +5470,15 @@
       </c>
       <c r="Q13" s="43">
         <f t="shared" si="22"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R13" s="43">
         <f t="shared" si="23"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S13" s="43">
         <f>COUNTIF(J:J,P13)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T13" s="43">
         <f>COUNTIF(K:K,P13)+COUNTIF(L:L,P13)</f>
@@ -5474,7 +5490,7 @@
       </c>
       <c r="V13" s="43">
         <f>SUMIF(E:E,P13,F:F)+SUMIF(I:I,P13,H:H)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W13" s="43">
         <f>SUMIF(E:E,P13,H:H)+SUMIF(I:I,P13,F:F)</f>
@@ -5482,11 +5498,11 @@
       </c>
       <c r="X13" s="43">
         <f t="shared" si="24"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y13" s="43">
         <f t="shared" si="25"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z13" s="43">
         <f t="shared" si="26"/>
@@ -5509,19 +5525,19 @@
       </c>
       <c r="AF13" s="83" t="str">
         <f t="shared" si="29"/>
-        <v>Seattle Sounders</v>
+        <v>Atlético de Madrid</v>
       </c>
       <c r="AG13" s="90">
         <f t="shared" si="30"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH13" s="90">
         <f t="shared" si="31"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI13" s="90">
         <f t="shared" si="32"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ13" s="90">
         <f t="shared" si="33"/>
@@ -5533,15 +5549,15 @@
       </c>
       <c r="AL13" s="90">
         <f t="shared" si="35"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AM13" s="90">
         <f t="shared" si="36"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AN13" s="91">
         <f t="shared" si="37"/>
-        <v>-1</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="14" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5587,7 +5603,7 @@
       <c r="N14" s="59"/>
       <c r="O14" s="60">
         <f t="shared" si="21"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P14" s="53" t="str">
         <f>Sorteios!F9</f>
@@ -5599,7 +5615,7 @@
       </c>
       <c r="R14" s="57">
         <f t="shared" si="23"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S14" s="43">
         <f>COUNTIF(J:J,P14)</f>
@@ -5611,19 +5627,19 @@
       </c>
       <c r="U14" s="43">
         <f>COUNTIF(M:M,P14)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V14" s="57">
         <f>SUMIF(E:E,P14,F:F)+SUMIF(I:I,P14,H:H)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W14" s="57">
         <f>SUMIF(E:E,P14,H:H)+SUMIF(I:I,P14,F:F)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="X14" s="57">
         <f t="shared" si="24"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="Y14" s="57">
         <f t="shared" si="25"/>
@@ -5650,7 +5666,7 @@
       </c>
       <c r="AF14" s="84" t="str">
         <f t="shared" si="29"/>
-        <v>Atlético de Madrid</v>
+        <v>Seattle Sounders</v>
       </c>
       <c r="AG14" s="92">
         <f t="shared" si="30"/>
@@ -5658,7 +5674,7 @@
       </c>
       <c r="AH14" s="92">
         <f t="shared" si="31"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI14" s="92">
         <f t="shared" si="32"/>
@@ -5670,19 +5686,19 @@
       </c>
       <c r="AK14" s="92">
         <f t="shared" si="34"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL14" s="92">
         <f t="shared" si="35"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM14" s="92">
         <f t="shared" si="36"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AN14" s="93">
         <f t="shared" si="37"/>
-        <v>-4</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.25">
@@ -5898,18 +5914,22 @@
         <f>P17</f>
         <v>Bayern de Munique</v>
       </c>
-      <c r="F17" s="21"/>
+      <c r="F17" s="21">
+        <v>2</v>
+      </c>
       <c r="G17" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H17" s="21"/>
+      <c r="H17" s="21">
+        <v>1</v>
+      </c>
       <c r="I17" s="13" t="str">
         <f>P19</f>
         <v>Boca Juniors</v>
       </c>
       <c r="J17" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>empate</v>
+        <v>Bayern de Munique</v>
       </c>
       <c r="K17" s="43" t="str">
         <f t="shared" si="1"/>
@@ -5921,7 +5941,7 @@
       </c>
       <c r="M17" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>empate</v>
+        <v>Boca Juniors</v>
       </c>
       <c r="N17" s="51"/>
       <c r="O17" s="52">
@@ -5934,15 +5954,15 @@
       </c>
       <c r="Q17" s="43">
         <f>(S17*3)+(T17*1)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R17" s="43">
         <f>SUM(S17:U17)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S17" s="43">
         <f>COUNTIF(J:J,P17)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T17" s="43">
         <f>COUNTIF(K:K,P17)+COUNTIF(L:L,P17)</f>
@@ -5954,15 +5974,15 @@
       </c>
       <c r="V17" s="43">
         <f>SUMIF(E:E,P17,F:F)+SUMIF(I:I,P17,H:H)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="W17" s="43">
         <f>SUMIF(E:E,P17,H:H)+SUMIF(I:I,P17,F:F)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X17" s="43">
         <f>V17-W17</f>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="Y17" s="43">
         <f>SUMPRODUCT(($Q$17:$Q$20=Q17)*($X$17:$X$20&gt;X17))</f>
@@ -5993,15 +6013,15 @@
       </c>
       <c r="AG17" s="90">
         <f>VLOOKUP($AE17,$O$17:$X$20,3,FALSE)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AH17" s="90">
         <f>VLOOKUP($AE17,$O$17:$X$20,4,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI17" s="90">
         <f>VLOOKUP($AE17,$O$17:$X$20,5,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ17" s="90">
         <f>VLOOKUP($AE17,$O$17:$X$20,6,FALSE)</f>
@@ -6013,15 +6033,15 @@
       </c>
       <c r="AL17" s="90">
         <f>VLOOKUP($AE17,$O$17:$X$20,8,FALSE)</f>
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="AM17" s="90">
         <f>VLOOKUP($AE17,$O$17:$X$20,9,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN17" s="91">
         <f>VLOOKUP($AE17,$O$17:$X$20,10,FALSE)</f>
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.25">
@@ -6039,18 +6059,22 @@
         <f>P20</f>
         <v>Benfica</v>
       </c>
-      <c r="F18" s="21"/>
+      <c r="F18" s="21">
+        <v>6</v>
+      </c>
       <c r="G18" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H18" s="21"/>
+      <c r="H18" s="21">
+        <v>0</v>
+      </c>
       <c r="I18" s="13" t="str">
         <f>P18</f>
         <v>Auckland City</v>
       </c>
       <c r="J18" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>empate</v>
+        <v>Benfica</v>
       </c>
       <c r="K18" s="43" t="str">
         <f t="shared" si="1"/>
@@ -6062,7 +6086,7 @@
       </c>
       <c r="M18" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>empate</v>
+        <v>Auckland City</v>
       </c>
       <c r="N18" s="51"/>
       <c r="O18" s="52">
@@ -6079,7 +6103,7 @@
       </c>
       <c r="R18" s="43">
         <f t="shared" ref="R18:R20" si="40">SUM(S18:U18)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S18" s="43">
         <f>COUNTIF(J:J,P18)</f>
@@ -6091,7 +6115,7 @@
       </c>
       <c r="U18" s="43">
         <f>COUNTIF(M:M,P18)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V18" s="43">
         <f>SUMIF(E:E,P18,F:F)+SUMIF(I:I,P18,H:H)</f>
@@ -6099,11 +6123,11 @@
       </c>
       <c r="W18" s="43">
         <f>SUMIF(E:E,P18,H:H)+SUMIF(I:I,P18,F:F)</f>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="X18" s="43">
         <f t="shared" ref="X18:X20" si="41">V18-W18</f>
-        <v>-10</v>
+        <v>-16</v>
       </c>
       <c r="Y18" s="43">
         <f t="shared" ref="Y18:Y20" si="42">SUMPRODUCT(($Q$17:$Q$20=Q18)*($X$17:$X$20&gt;X18))</f>
@@ -6130,19 +6154,19 @@
       </c>
       <c r="AF18" s="83" t="str">
         <f t="shared" ref="AF18:AF20" si="46">VLOOKUP($AE18,$O$17:$X$20,2,FALSE)</f>
-        <v>Boca Juniors</v>
+        <v>Benfica</v>
       </c>
       <c r="AG18" s="90">
         <f t="shared" ref="AG18:AG20" si="47">VLOOKUP($AE18,$O$17:$X$20,3,FALSE)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AH18" s="90">
         <f t="shared" ref="AH18:AH20" si="48">VLOOKUP($AE18,$O$17:$X$20,4,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI18" s="90">
         <f t="shared" ref="AI18:AI20" si="49">VLOOKUP($AE18,$O$17:$X$20,5,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ18" s="90">
         <f t="shared" ref="AJ18:AJ20" si="50">VLOOKUP($AE18,$O$17:$X$20,6,FALSE)</f>
@@ -6154,7 +6178,7 @@
       </c>
       <c r="AL18" s="90">
         <f t="shared" ref="AL18:AL20" si="52">VLOOKUP($AE18,$O$17:$X$20,8,FALSE)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="AM18" s="90">
         <f t="shared" ref="AM18:AM20" si="53">VLOOKUP($AE18,$O$17:$X$20,9,FALSE)</f>
@@ -6162,7 +6186,7 @@
       </c>
       <c r="AN18" s="91">
         <f t="shared" ref="AN18:AN20" si="54">VLOOKUP($AE18,$O$17:$X$20,10,FALSE)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.25">
@@ -6208,7 +6232,7 @@
       <c r="N19" s="51"/>
       <c r="O19" s="52">
         <f t="shared" si="38"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P19" s="53" t="str">
         <f>Sorteios!I8</f>
@@ -6220,7 +6244,7 @@
       </c>
       <c r="R19" s="43">
         <f t="shared" si="40"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S19" s="43">
         <f>COUNTIF(J:J,P19)</f>
@@ -6232,19 +6256,19 @@
       </c>
       <c r="U19" s="43">
         <f>COUNTIF(M:M,P19)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V19" s="43">
         <f>SUMIF(E:E,P19,F:F)+SUMIF(I:I,P19,H:H)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W19" s="43">
         <f>SUMIF(E:E,P19,H:H)+SUMIF(I:I,P19,F:F)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="X19" s="43">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="Y19" s="43">
         <f t="shared" si="42"/>
@@ -6271,7 +6295,7 @@
       </c>
       <c r="AF19" s="83" t="str">
         <f t="shared" si="46"/>
-        <v>Benfica</v>
+        <v>Boca Juniors</v>
       </c>
       <c r="AG19" s="90">
         <f t="shared" si="47"/>
@@ -6279,7 +6303,7 @@
       </c>
       <c r="AH19" s="90">
         <f t="shared" si="48"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI19" s="90">
         <f t="shared" si="49"/>
@@ -6291,19 +6315,19 @@
       </c>
       <c r="AK19" s="90">
         <f t="shared" si="51"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL19" s="90">
         <f t="shared" si="52"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AM19" s="90">
         <f t="shared" si="53"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AN19" s="91">
         <f t="shared" si="54"/>
-        <v>0</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="20" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -6349,7 +6373,7 @@
       <c r="N20" s="59"/>
       <c r="O20" s="60">
         <f t="shared" si="38"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P20" s="53" t="str">
         <f>Sorteios!I9</f>
@@ -6357,15 +6381,15 @@
       </c>
       <c r="Q20" s="57">
         <f t="shared" si="39"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R20" s="57">
         <f t="shared" si="40"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S20" s="43">
         <f>COUNTIF(J:J,P20)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T20" s="43">
         <f>COUNTIF(K:K,P20)+COUNTIF(L:L,P20)</f>
@@ -6377,7 +6401,7 @@
       </c>
       <c r="V20" s="57">
         <f>SUMIF(E:E,P20,F:F)+SUMIF(I:I,P20,H:H)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="W20" s="57">
         <f>SUMIF(E:E,P20,H:H)+SUMIF(I:I,P20,F:F)</f>
@@ -6385,7 +6409,7 @@
       </c>
       <c r="X20" s="57">
         <f t="shared" si="41"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="Y20" s="57">
         <f t="shared" si="42"/>
@@ -6401,7 +6425,7 @@
       </c>
       <c r="AB20" s="57">
         <f t="shared" si="45"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC20" s="58">
         <v>4</v>
@@ -6420,7 +6444,7 @@
       </c>
       <c r="AH20" s="92">
         <f t="shared" si="48"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI20" s="92">
         <f t="shared" si="49"/>
@@ -6432,7 +6456,7 @@
       </c>
       <c r="AK20" s="92">
         <f t="shared" si="51"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL20" s="92">
         <f t="shared" si="52"/>
@@ -6440,11 +6464,11 @@
       </c>
       <c r="AM20" s="92">
         <f t="shared" si="53"/>
-        <v>10</v>
+        <v>16</v>
       </c>
       <c r="AN20" s="93">
         <f t="shared" si="54"/>
-        <v>-10</v>
+        <v>-16</v>
       </c>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.25">
@@ -6660,18 +6684,22 @@
         <f>P23</f>
         <v>Flamengo</v>
       </c>
-      <c r="F23" s="21"/>
+      <c r="F23" s="21">
+        <v>3</v>
+      </c>
       <c r="G23" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="H23" s="21"/>
+      <c r="H23" s="21">
+        <v>1</v>
+      </c>
       <c r="I23" s="26" t="str">
         <f>P25</f>
         <v>Chelsea</v>
       </c>
       <c r="J23" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>empate</v>
+        <v>Flamengo</v>
       </c>
       <c r="K23" s="43" t="str">
         <f t="shared" si="1"/>
@@ -6683,7 +6711,7 @@
       </c>
       <c r="M23" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>empate</v>
+        <v>Chelsea</v>
       </c>
       <c r="N23" s="50"/>
       <c r="O23" s="52">
@@ -6696,15 +6724,15 @@
       </c>
       <c r="Q23" s="43">
         <f>(S23*3)+(T23*1)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R23" s="43">
         <f>SUM(S23:U23)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S23" s="43">
         <f>COUNTIF(J:J,P23)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T23" s="43">
         <f>COUNTIF(K:K,P23)+COUNTIF(L:L,P23)</f>
@@ -6716,15 +6744,15 @@
       </c>
       <c r="V23" s="43">
         <f>SUMIF(E:E,P23,F:F)+SUMIF(I:I,P23,H:H)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="W23" s="43">
         <f>SUMIF(E:E,P23,H:H)+SUMIF(I:I,P23,F:F)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X23" s="43">
         <f>V23-W23</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="Y23" s="43">
         <f>SUMPRODUCT(($Q$23:$Q$26=Q23)*($X$23:$X$26&gt;X23))</f>
@@ -6755,15 +6783,15 @@
       </c>
       <c r="AG23" s="90">
         <f>VLOOKUP($AE23,$O$23:$X$26,3,FALSE)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AH23" s="90">
         <f>VLOOKUP($AE23,$O$23:$X$26,4,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI23" s="90">
         <f>VLOOKUP($AE23,$O$23:$X$26,5,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ23" s="90">
         <f>VLOOKUP($AE23,$O$23:$X$26,6,FALSE)</f>
@@ -6775,15 +6803,15 @@
       </c>
       <c r="AL23" s="90">
         <f>VLOOKUP($AE23,$O$23:$X$26,8,FALSE)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AM23" s="90">
         <f>VLOOKUP($AE23,$O$23:$X$26,9,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN23" s="91">
         <f>VLOOKUP($AE23,$O$23:$X$26,10,FALSE)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.25">
@@ -6801,18 +6829,22 @@
         <f>P26</f>
         <v>Los Angeles FC</v>
       </c>
-      <c r="F24" s="21"/>
+      <c r="F24" s="21">
+        <v>0</v>
+      </c>
       <c r="G24" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="H24" s="21"/>
+      <c r="H24" s="21">
+        <v>1</v>
+      </c>
       <c r="I24" s="26" t="str">
         <f>P24</f>
         <v>Espérance de Tunis</v>
       </c>
       <c r="J24" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>empate</v>
+        <v>Espérance de Tunis</v>
       </c>
       <c r="K24" s="43" t="str">
         <f t="shared" si="1"/>
@@ -6824,7 +6856,7 @@
       </c>
       <c r="M24" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>empate</v>
+        <v>Los Angeles FC</v>
       </c>
       <c r="N24" s="50"/>
       <c r="O24" s="52">
@@ -6837,15 +6869,15 @@
       </c>
       <c r="Q24" s="43">
         <f t="shared" ref="Q24:Q26" si="56">(S24*3)+(T24*1)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R24" s="43">
         <f t="shared" ref="R24:R26" si="57">SUM(S24:U24)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S24" s="43">
         <f>COUNTIF(J:J,P24)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T24" s="43">
         <f>COUNTIF(K:K,P24)+COUNTIF(L:L,P24)</f>
@@ -6857,7 +6889,7 @@
       </c>
       <c r="V24" s="43">
         <f>SUMIF(E:E,P24,F:F)+SUMIF(I:I,P24,H:H)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W24" s="43">
         <f>SUMIF(E:E,P24,H:H)+SUMIF(I:I,P24,F:F)</f>
@@ -6865,11 +6897,11 @@
       </c>
       <c r="X24" s="43">
         <f t="shared" ref="X24:X26" si="58">V24-W24</f>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="Y24" s="43">
         <f t="shared" ref="Y24:Y26" si="59">SUMPRODUCT(($Q$23:$Q$26=Q24)*($X$23:$X$26&gt;X24))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z24" s="43">
         <f t="shared" ref="Z24:Z26" si="60">SUMPRODUCT(($Q$23:$Q$26=Q24)*($X$23:$X$26=X24)*($V$23:$V$26&gt;V24))</f>
@@ -6900,7 +6932,7 @@
       </c>
       <c r="AH24" s="90">
         <f t="shared" ref="AH24:AH26" si="65">VLOOKUP($AE24,$O$23:$X$26,4,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI24" s="90">
         <f t="shared" ref="AI24:AI26" si="66">VLOOKUP($AE24,$O$23:$X$26,5,FALSE)</f>
@@ -6912,19 +6944,19 @@
       </c>
       <c r="AK24" s="90">
         <f t="shared" ref="AK24:AK26" si="68">VLOOKUP($AE24,$O$23:$X$26,7,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL24" s="90">
         <f t="shared" ref="AL24:AL26" si="69">VLOOKUP($AE24,$O$23:$X$26,8,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AM24" s="90">
         <f t="shared" ref="AM24:AM26" si="70">VLOOKUP($AE24,$O$23:$X$26,9,FALSE)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AN24" s="91">
         <f t="shared" ref="AN24:AN26" si="71">VLOOKUP($AE24,$O$23:$X$26,10,FALSE)</f>
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.25">
@@ -6982,7 +7014,7 @@
       </c>
       <c r="R25" s="43">
         <f t="shared" si="57"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S25" s="43">
         <f>COUNTIF(J:J,P25)</f>
@@ -6994,19 +7026,19 @@
       </c>
       <c r="U25" s="43">
         <f>COUNTIF(M:M,P25)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V25" s="43">
         <f>SUMIF(E:E,P25,F:F)+SUMIF(I:I,P25,H:H)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="W25" s="43">
         <f>SUMIF(E:E,P25,H:H)+SUMIF(I:I,P25,F:F)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X25" s="43">
         <f t="shared" si="58"/>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y25" s="43">
         <f t="shared" si="59"/>
@@ -7022,7 +7054,7 @@
       </c>
       <c r="AB25" s="43">
         <f t="shared" si="62"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC25" s="44">
         <v>3</v>
@@ -7037,15 +7069,15 @@
       </c>
       <c r="AG25" s="90">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH25" s="90">
         <f t="shared" si="65"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI25" s="90">
         <f t="shared" si="66"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ25" s="90">
         <f t="shared" si="67"/>
@@ -7057,7 +7089,7 @@
       </c>
       <c r="AL25" s="90">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM25" s="90">
         <f t="shared" si="70"/>
@@ -7065,7 +7097,7 @@
       </c>
       <c r="AN25" s="91">
         <f t="shared" si="71"/>
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="26" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7123,7 +7155,7 @@
       </c>
       <c r="R26" s="57">
         <f t="shared" si="57"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S26" s="43">
         <f>COUNTIF(J:J,P26)</f>
@@ -7135,7 +7167,7 @@
       </c>
       <c r="U26" s="43">
         <f>COUNTIF(M:M,P26)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V26" s="57">
         <f>SUMIF(E:E,P26,F:F)+SUMIF(I:I,P26,H:H)</f>
@@ -7143,11 +7175,11 @@
       </c>
       <c r="W26" s="57">
         <f>SUMIF(E:E,P26,H:H)+SUMIF(I:I,P26,F:F)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X26" s="57">
         <f t="shared" si="58"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="Y26" s="57">
         <f t="shared" si="59"/>
@@ -7163,7 +7195,7 @@
       </c>
       <c r="AB26" s="57">
         <f t="shared" si="62"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC26" s="58">
         <v>4</v>
@@ -7182,7 +7214,7 @@
       </c>
       <c r="AH26" s="92">
         <f t="shared" si="65"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI26" s="92">
         <f t="shared" si="66"/>
@@ -7194,7 +7226,7 @@
       </c>
       <c r="AK26" s="92">
         <f t="shared" si="68"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL26" s="92">
         <f t="shared" si="69"/>
@@ -7202,11 +7234,11 @@
       </c>
       <c r="AM26" s="92">
         <f t="shared" si="70"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AN26" s="93">
         <f t="shared" si="71"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.25">
@@ -7422,11 +7454,15 @@
         <f>P29</f>
         <v>River Plate</v>
       </c>
-      <c r="F29" s="21"/>
+      <c r="F29" s="21">
+        <v>0</v>
+      </c>
       <c r="G29" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H29" s="21"/>
+      <c r="H29" s="21">
+        <v>0</v>
+      </c>
       <c r="I29" s="13" t="str">
         <f>P31</f>
         <v>Monterrey</v>
@@ -7437,11 +7473,11 @@
       </c>
       <c r="K29" s="43" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>River Plate</v>
       </c>
       <c r="L29" s="43" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>Monterrey</v>
       </c>
       <c r="M29" s="44" t="str">
         <f t="shared" si="3"/>
@@ -7458,11 +7494,11 @@
       </c>
       <c r="Q29" s="43">
         <f>(S29*3)+(T29*1)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R29" s="43">
         <f>SUM(S29:U29)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S29" s="43">
         <f>COUNTIF(J:J,P29)</f>
@@ -7470,7 +7506,7 @@
       </c>
       <c r="T29" s="43">
         <f>COUNTIF(K:K,P29)+COUNTIF(L:L,P29)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U29" s="43">
         <f>COUNTIF(M:M,P29)</f>
@@ -7517,11 +7553,11 @@
       </c>
       <c r="AG29" s="90">
         <f>VLOOKUP($AE29,$O$29:$X$32,3,FALSE)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH29" s="90">
         <f>VLOOKUP($AE29,$O$29:$X$32,4,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI29" s="90">
         <f>VLOOKUP($AE29,$O$29:$X$32,5,FALSE)</f>
@@ -7529,7 +7565,7 @@
       </c>
       <c r="AJ29" s="90">
         <f>VLOOKUP($AE29,$O$29:$X$32,6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK29" s="90">
         <f>VLOOKUP($AE29,$O$29:$X$32,7,FALSE)</f>
@@ -7563,18 +7599,22 @@
         <f>P32</f>
         <v>Internazionale</v>
       </c>
-      <c r="F30" s="21"/>
+      <c r="F30" s="21">
+        <v>2</v>
+      </c>
       <c r="G30" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H30" s="21"/>
+      <c r="H30" s="21">
+        <v>1</v>
+      </c>
       <c r="I30" s="13" t="str">
         <f>P30</f>
         <v>Urawa Red Diamonds</v>
       </c>
       <c r="J30" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>empate</v>
+        <v>Internazionale</v>
       </c>
       <c r="K30" s="43" t="str">
         <f t="shared" si="1"/>
@@ -7586,7 +7626,7 @@
       </c>
       <c r="M30" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>empate</v>
+        <v>Urawa Red Diamonds</v>
       </c>
       <c r="N30" s="51"/>
       <c r="O30" s="52">
@@ -7603,7 +7643,7 @@
       </c>
       <c r="R30" s="43">
         <f t="shared" ref="R30:R32" si="74">SUM(S30:U30)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S30" s="43">
         <f>COUNTIF(J:J,P30)</f>
@@ -7615,19 +7655,19 @@
       </c>
       <c r="U30" s="43">
         <f>COUNTIF(M:M,P30)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V30" s="43">
         <f>SUMIF(E:E,P30,F:F)+SUMIF(I:I,P30,H:H)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W30" s="43">
         <f>SUMIF(E:E,P30,H:H)+SUMIF(I:I,P30,F:F)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="X30" s="43">
         <f t="shared" ref="X30:X32" si="75">V30-W30</f>
-        <v>-2</v>
+        <v>-3</v>
       </c>
       <c r="Y30" s="43">
         <f t="shared" ref="Y30:Y32" si="76">SUMPRODUCT(($Q$29:$Q$32=Q30)*($X$29:$X$32&gt;X30))</f>
@@ -7654,19 +7694,19 @@
       </c>
       <c r="AF30" s="83" t="str">
         <f t="shared" ref="AF30:AF32" si="80">VLOOKUP($AE30,$O$29:$X$32,2,FALSE)</f>
-        <v>Monterrey</v>
+        <v>Internazionale</v>
       </c>
       <c r="AG30" s="90">
         <f t="shared" ref="AG30:AG32" si="81">VLOOKUP($AE30,$O$29:$X$32,3,FALSE)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AH30" s="90">
         <f t="shared" ref="AH30:AH32" si="82">VLOOKUP($AE30,$O$29:$X$32,4,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI30" s="90">
         <f t="shared" ref="AI30:AI32" si="83">VLOOKUP($AE30,$O$29:$X$32,5,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ30" s="90">
         <f t="shared" ref="AJ30:AJ32" si="84">VLOOKUP($AE30,$O$29:$X$32,6,FALSE)</f>
@@ -7678,15 +7718,15 @@
       </c>
       <c r="AL30" s="90">
         <f t="shared" ref="AL30:AL32" si="86">VLOOKUP($AE30,$O$29:$X$32,8,FALSE)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AM30" s="90">
         <f t="shared" ref="AM30:AM32" si="87">VLOOKUP($AE30,$O$29:$X$32,9,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AN30" s="91">
         <f t="shared" ref="AN30:AN32" si="88">VLOOKUP($AE30,$O$29:$X$32,10,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="31" spans="1:40" x14ac:dyDescent="0.25">
@@ -7732,7 +7772,7 @@
       <c r="N31" s="51"/>
       <c r="O31" s="52">
         <f t="shared" si="72"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P31" s="53" t="str">
         <f>Sorteios!C16</f>
@@ -7740,11 +7780,11 @@
       </c>
       <c r="Q31" s="43">
         <f t="shared" si="73"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R31" s="43">
         <f t="shared" si="74"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S31" s="43">
         <f>COUNTIF(J:J,P31)</f>
@@ -7752,7 +7792,7 @@
       </c>
       <c r="T31" s="43">
         <f>COUNTIF(K:K,P31)+COUNTIF(L:L,P31)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U31" s="43">
         <f>COUNTIF(M:M,P31)</f>
@@ -7795,15 +7835,15 @@
       </c>
       <c r="AF31" s="83" t="str">
         <f t="shared" si="80"/>
-        <v>Internazionale</v>
+        <v>Monterrey</v>
       </c>
       <c r="AG31" s="90">
         <f t="shared" si="81"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH31" s="90">
         <f t="shared" si="82"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI31" s="90">
         <f t="shared" si="83"/>
@@ -7811,7 +7851,7 @@
       </c>
       <c r="AJ31" s="90">
         <f t="shared" si="84"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK31" s="90">
         <f t="shared" si="85"/>
@@ -7873,7 +7913,7 @@
       <c r="N32" s="59"/>
       <c r="O32" s="60">
         <f t="shared" si="72"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P32" s="53" t="str">
         <f>Sorteios!C17</f>
@@ -7881,15 +7921,15 @@
       </c>
       <c r="Q32" s="57">
         <f t="shared" si="73"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R32" s="57">
         <f t="shared" si="74"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S32" s="43">
         <f>COUNTIF(J:J,P32)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T32" s="43">
         <f>COUNTIF(K:K,P32)+COUNTIF(L:L,P32)</f>
@@ -7901,19 +7941,19 @@
       </c>
       <c r="V32" s="57">
         <f>SUMIF(E:E,P32,F:F)+SUMIF(I:I,P32,H:H)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W32" s="57">
         <f>SUMIF(E:E,P32,H:H)+SUMIF(I:I,P32,F:F)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X32" s="57">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y32" s="57">
         <f t="shared" si="76"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z32" s="57">
         <f t="shared" si="77"/>
@@ -7925,7 +7965,7 @@
       </c>
       <c r="AB32" s="57">
         <f t="shared" si="79"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC32" s="58">
         <v>4</v>
@@ -7944,7 +7984,7 @@
       </c>
       <c r="AH32" s="92">
         <f t="shared" si="82"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI32" s="92">
         <f t="shared" si="83"/>
@@ -7956,19 +7996,19 @@
       </c>
       <c r="AK32" s="92">
         <f t="shared" si="85"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL32" s="92">
         <f t="shared" si="86"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AM32" s="92">
         <f t="shared" si="87"/>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AN32" s="93">
         <f t="shared" si="88"/>
-        <v>-2</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.25">
@@ -8184,18 +8224,22 @@
         <f>P35</f>
         <v>Fluminense</v>
       </c>
-      <c r="F35" s="21"/>
+      <c r="F35" s="21">
+        <v>4</v>
+      </c>
       <c r="G35" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="H35" s="21"/>
+      <c r="H35" s="21">
+        <v>2</v>
+      </c>
       <c r="I35" s="26" t="str">
         <f>P37</f>
         <v>Ulsan</v>
       </c>
       <c r="J35" s="42" t="str">
         <f t="shared" ref="J35:J50" si="89">IF(F35=H35,"empate",IF(F35&gt;H35,E35,I35))</f>
-        <v>empate</v>
+        <v>Fluminense</v>
       </c>
       <c r="K35" s="43" t="str">
         <f t="shared" ref="K35:K50" si="90">IF(F35="","",IF(H35="","",IF(J35="empate",E35,"")))</f>
@@ -8207,12 +8251,12 @@
       </c>
       <c r="M35" s="44" t="str">
         <f t="shared" ref="M35:M50" si="92">IF(F35=H35,"empate",IF(F35&lt;H35,E35,I35))</f>
-        <v>empate</v>
+        <v>Ulsan</v>
       </c>
       <c r="N35" s="50"/>
       <c r="O35" s="52">
         <f>RANK(Q35,$Q$35:$Q$38)+SUM(Y35:AB35)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P35" s="53" t="str">
         <f>Sorteios!F14</f>
@@ -8220,15 +8264,15 @@
       </c>
       <c r="Q35" s="43">
         <f>(S35*3)+(T35*1)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R35" s="43">
         <f>SUM(S35:U35)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S35" s="43">
         <f>COUNTIF(J:J,P35)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T35" s="43">
         <f>COUNTIF(K:K,P35)+COUNTIF(L:L,P35)</f>
@@ -8240,15 +8284,15 @@
       </c>
       <c r="V35" s="43">
         <f>SUMIF(E:E,P35,F:F)+SUMIF(I:I,P35,H:H)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W35" s="43">
         <f>SUMIF(E:E,P35,H:H)+SUMIF(I:I,P35,F:F)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X35" s="43">
         <f>V35-W35</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y35" s="43">
         <f>SUMPRODUCT(($Q$35:$Q$38=Q35)*($X$35:$X$38&gt;X35))</f>
@@ -8275,15 +8319,15 @@
       </c>
       <c r="AF35" s="83" t="str">
         <f>VLOOKUP($AE35,$O$35:$X$38,2,FALSE)</f>
-        <v>Mamelodi Sundowns</v>
+        <v>Fluminense</v>
       </c>
       <c r="AG35" s="90">
         <f>VLOOKUP($AE35,$O$35:$X$38,3,FALSE)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH35" s="90">
         <f>VLOOKUP($AE35,$O$35:$X$38,4,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI35" s="90">
         <f>VLOOKUP($AE35,$O$35:$X$38,5,FALSE)</f>
@@ -8291,7 +8335,7 @@
       </c>
       <c r="AJ35" s="90">
         <f>VLOOKUP($AE35,$O$35:$X$38,6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK35" s="90">
         <f>VLOOKUP($AE35,$O$35:$X$38,7,FALSE)</f>
@@ -8299,15 +8343,15 @@
       </c>
       <c r="AL35" s="90">
         <f>VLOOKUP($AE35,$O$35:$X$38,8,FALSE)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AM35" s="90">
         <f>VLOOKUP($AE35,$O$35:$X$38,9,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AN35" s="91">
         <f>VLOOKUP($AE35,$O$35:$X$38,10,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.25">
@@ -8325,18 +8369,22 @@
         <f>P38</f>
         <v>Mamelodi Sundowns</v>
       </c>
-      <c r="F36" s="21"/>
+      <c r="F36" s="21">
+        <v>3</v>
+      </c>
       <c r="G36" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="H36" s="21"/>
+      <c r="H36" s="21">
+        <v>4</v>
+      </c>
       <c r="I36" s="26" t="str">
         <f>P36</f>
         <v>Borussia Dortmund</v>
       </c>
       <c r="J36" s="42" t="str">
         <f t="shared" si="89"/>
-        <v>empate</v>
+        <v>Borussia Dortmund</v>
       </c>
       <c r="K36" s="43" t="str">
         <f t="shared" si="90"/>
@@ -8348,12 +8396,12 @@
       </c>
       <c r="M36" s="44" t="str">
         <f t="shared" si="92"/>
-        <v>empate</v>
+        <v>Mamelodi Sundowns</v>
       </c>
       <c r="N36" s="50"/>
       <c r="O36" s="52">
         <f t="shared" ref="O36:O38" si="93">RANK(Q36,$Q$35:$Q$38)+SUM(Y36:AB36)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P36" s="53" t="str">
         <f>Sorteios!F15</f>
@@ -8361,15 +8409,15 @@
       </c>
       <c r="Q36" s="43">
         <f t="shared" ref="Q36:Q38" si="94">(S36*3)+(T36*1)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R36" s="43">
         <f t="shared" ref="R36:R38" si="95">SUM(S36:U36)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S36" s="43">
         <f>COUNTIF(J:J,P36)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T36" s="43">
         <f>COUNTIF(K:K,P36)+COUNTIF(L:L,P36)</f>
@@ -8381,19 +8429,19 @@
       </c>
       <c r="V36" s="43">
         <f>SUMIF(E:E,P36,F:F)+SUMIF(I:I,P36,H:H)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="W36" s="43">
         <f>SUMIF(E:E,P36,H:H)+SUMIF(I:I,P36,F:F)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="X36" s="43">
         <f t="shared" ref="X36:X38" si="96">V36-W36</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Y36" s="43">
         <f t="shared" ref="Y36:Y38" si="97">SUMPRODUCT(($Q$35:$Q$38=Q36)*($X$35:$X$38&gt;X36))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z36" s="43">
         <f t="shared" ref="Z36:Z38" si="98">SUMPRODUCT(($Q$35:$Q$38=Q36)*($X$35:$X$38=X36)*($V$35:$V$38&gt;V36))</f>
@@ -8405,7 +8453,7 @@
       </c>
       <c r="AB36" s="43">
         <f t="shared" ref="AB36:AB38" si="100">SUMPRODUCT(($Q$35:$Q$38=Q36)*($X$35:$X$38=X36)*($V$35:$V$38=V36)*($W$35:$W$38=W36)*($AC$35:$AC$38&lt;AC36))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC36" s="44">
         <v>2</v>
@@ -8416,19 +8464,19 @@
       </c>
       <c r="AF36" s="83" t="str">
         <f t="shared" ref="AF36:AF38" si="101">VLOOKUP($AE36,$O$35:$X$38,2,FALSE)</f>
-        <v>Fluminense</v>
+        <v>Borussia Dortmund</v>
       </c>
       <c r="AG36" s="90">
         <f t="shared" ref="AG36:AG38" si="102">VLOOKUP($AE36,$O$35:$X$38,3,FALSE)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AH36" s="90">
         <f t="shared" ref="AH36:AH38" si="103">VLOOKUP($AE36,$O$35:$X$38,4,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI36" s="90">
         <f t="shared" ref="AI36:AI38" si="104">VLOOKUP($AE36,$O$35:$X$38,5,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ36" s="90">
         <f t="shared" ref="AJ36:AJ38" si="105">VLOOKUP($AE36,$O$35:$X$38,6,FALSE)</f>
@@ -8440,15 +8488,15 @@
       </c>
       <c r="AL36" s="90">
         <f t="shared" ref="AL36:AL38" si="107">VLOOKUP($AE36,$O$35:$X$38,8,FALSE)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AM36" s="90">
         <f t="shared" ref="AM36:AM38" si="108">VLOOKUP($AE36,$O$35:$X$38,9,FALSE)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AN36" s="91">
         <f t="shared" ref="AN36:AN38" si="109">VLOOKUP($AE36,$O$35:$X$38,10,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:40" x14ac:dyDescent="0.25">
@@ -8506,7 +8554,7 @@
       </c>
       <c r="R37" s="43">
         <f t="shared" si="95"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S37" s="43">
         <f>COUNTIF(J:J,P37)</f>
@@ -8518,19 +8566,19 @@
       </c>
       <c r="U37" s="43">
         <f>COUNTIF(M:M,P37)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V37" s="43">
         <f>SUMIF(E:E,P37,F:F)+SUMIF(I:I,P37,H:H)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W37" s="43">
         <f>SUMIF(E:E,P37,H:H)+SUMIF(I:I,P37,F:F)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="X37" s="43">
         <f t="shared" si="96"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="Y37" s="43">
         <f t="shared" si="97"/>
@@ -8557,35 +8605,35 @@
       </c>
       <c r="AF37" s="83" t="str">
         <f t="shared" si="101"/>
-        <v>Borussia Dortmund</v>
+        <v>Mamelodi Sundowns</v>
       </c>
       <c r="AG37" s="90">
         <f t="shared" si="102"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AH37" s="90">
         <f t="shared" si="103"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI37" s="90">
         <f t="shared" si="104"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ37" s="90">
         <f t="shared" si="105"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK37" s="90">
         <f t="shared" si="106"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL37" s="90">
         <f t="shared" si="107"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AM37" s="90">
         <f t="shared" si="108"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="AN37" s="91">
         <f t="shared" si="109"/>
@@ -8635,7 +8683,7 @@
       <c r="N38" s="61"/>
       <c r="O38" s="60">
         <f t="shared" si="93"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P38" s="53" t="str">
         <f>Sorteios!F17</f>
@@ -8647,7 +8695,7 @@
       </c>
       <c r="R38" s="57">
         <f t="shared" si="95"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S38" s="43">
         <f>COUNTIF(J:J,P38)</f>
@@ -8659,19 +8707,19 @@
       </c>
       <c r="U38" s="43">
         <f>COUNTIF(M:M,P38)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V38" s="57">
         <f>SUMIF(E:E,P38,F:F)+SUMIF(I:I,P38,H:H)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="W38" s="57">
         <f>SUMIF(E:E,P38,H:H)+SUMIF(I:I,P38,F:F)</f>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="X38" s="57">
         <f t="shared" si="96"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Y38" s="57">
         <f t="shared" si="97"/>
@@ -8706,7 +8754,7 @@
       </c>
       <c r="AH38" s="92">
         <f t="shared" si="103"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI38" s="92">
         <f t="shared" si="104"/>
@@ -8718,19 +8766,19 @@
       </c>
       <c r="AK38" s="92">
         <f t="shared" si="106"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL38" s="92">
         <f t="shared" si="107"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM38" s="92">
         <f t="shared" si="108"/>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="AN38" s="93">
         <f t="shared" si="109"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.25">
@@ -8824,18 +8872,22 @@
         <f>P43</f>
         <v>Al Ain</v>
       </c>
-      <c r="F40" s="21"/>
+      <c r="F40" s="21">
+        <v>0</v>
+      </c>
       <c r="G40" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H40" s="21"/>
+      <c r="H40" s="21">
+        <v>5</v>
+      </c>
       <c r="I40" s="13" t="str">
         <f>P44</f>
         <v>Juventus</v>
       </c>
       <c r="J40" s="42" t="str">
         <f t="shared" si="89"/>
-        <v>empate</v>
+        <v>Juventus</v>
       </c>
       <c r="K40" s="43" t="str">
         <f t="shared" si="90"/>
@@ -8847,7 +8899,7 @@
       </c>
       <c r="M40" s="44" t="str">
         <f t="shared" si="92"/>
-        <v>empate</v>
+        <v>Al Ain</v>
       </c>
       <c r="N40" s="51"/>
       <c r="O40" s="52" t="s">
@@ -8942,18 +8994,22 @@
         <f>P41</f>
         <v>Manchester City</v>
       </c>
-      <c r="F41" s="21"/>
+      <c r="F41" s="21">
+        <v>6</v>
+      </c>
       <c r="G41" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H41" s="21"/>
+      <c r="H41" s="21">
+        <v>0</v>
+      </c>
       <c r="I41" s="13" t="str">
         <f>P43</f>
         <v>Al Ain</v>
       </c>
       <c r="J41" s="42" t="str">
         <f t="shared" si="89"/>
-        <v>empate</v>
+        <v>Manchester City</v>
       </c>
       <c r="K41" s="43" t="str">
         <f t="shared" si="90"/>
@@ -8965,12 +9021,12 @@
       </c>
       <c r="M41" s="44" t="str">
         <f t="shared" si="92"/>
-        <v>empate</v>
+        <v>Al Ain</v>
       </c>
       <c r="N41" s="51"/>
       <c r="O41" s="52">
         <f>RANK(Q41,$Q$41:$Q$44)+SUM(Y41:AB41)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P41" s="53" t="str">
         <f>Sorteios!I14</f>
@@ -8978,15 +9034,15 @@
       </c>
       <c r="Q41" s="43">
         <f>(S41*3)+(T41*1)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R41" s="43">
         <f>SUM(S41:U41)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S41" s="43">
         <f>COUNTIF(J:J,P41)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T41" s="43">
         <f>COUNTIF(K:K,P41)+COUNTIF(L:L,P41)</f>
@@ -8998,7 +9054,7 @@
       </c>
       <c r="V41" s="43">
         <f>SUMIF(E:E,P41,F:F)+SUMIF(I:I,P41,H:H)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="W41" s="43">
         <f>SUMIF(E:E,P41,H:H)+SUMIF(I:I,P41,F:F)</f>
@@ -9006,7 +9062,7 @@
       </c>
       <c r="X41" s="43">
         <f>V41-W41</f>
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="Y41" s="43">
         <f>SUMPRODUCT(($Q$41:$Q$44=Q41)*($X$41:$X$44&gt;X41))</f>
@@ -9014,7 +9070,7 @@
       </c>
       <c r="Z41" s="43">
         <f>SUMPRODUCT(($Q$41:$Q$44=Q41)*($X$41:$X$44=X41)*($V$41:$V$44&gt;V41))</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AA41" s="43">
         <f>SUMPRODUCT(($Q$41:$Q$44=Q41)*($X$41:$X$44=X41)*($V$41:$V$44=V41)*($W$41:$W$44&gt;W41))</f>
@@ -9033,19 +9089,19 @@
       </c>
       <c r="AF41" s="83" t="str">
         <f>VLOOKUP($AE41,$O$41:$X$44,2,FALSE)</f>
-        <v>Manchester City</v>
+        <v>Juventus</v>
       </c>
       <c r="AG41" s="90">
         <f>VLOOKUP($AE41,$O$41:$X$44,3,FALSE)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AH41" s="90">
         <f>VLOOKUP($AE41,$O$41:$X$44,4,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI41" s="90">
         <f>VLOOKUP($AE41,$O$41:$X$44,5,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ41" s="90">
         <f>VLOOKUP($AE41,$O$41:$X$44,6,FALSE)</f>
@@ -9057,15 +9113,15 @@
       </c>
       <c r="AL41" s="90">
         <f>VLOOKUP($AE41,$O$41:$X$44,8,FALSE)</f>
-        <v>2</v>
+        <v>9</v>
       </c>
       <c r="AM41" s="90">
         <f>VLOOKUP($AE41,$O$41:$X$44,9,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AN41" s="91">
         <f>VLOOKUP($AE41,$O$41:$X$44,10,FALSE)</f>
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="42" spans="1:40" x14ac:dyDescent="0.25">
@@ -9083,18 +9139,22 @@
         <f>P44</f>
         <v>Juventus</v>
       </c>
-      <c r="F42" s="21"/>
+      <c r="F42" s="21">
+        <v>4</v>
+      </c>
       <c r="G42" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H42" s="21"/>
+      <c r="H42" s="21">
+        <v>1</v>
+      </c>
       <c r="I42" s="13" t="str">
         <f>P42</f>
         <v>Wydad Casablanca</v>
       </c>
       <c r="J42" s="42" t="str">
         <f t="shared" si="89"/>
-        <v>empate</v>
+        <v>Juventus</v>
       </c>
       <c r="K42" s="43" t="str">
         <f t="shared" si="90"/>
@@ -9106,12 +9166,12 @@
       </c>
       <c r="M42" s="44" t="str">
         <f t="shared" si="92"/>
-        <v>empate</v>
+        <v>Wydad Casablanca</v>
       </c>
       <c r="N42" s="51"/>
       <c r="O42" s="52">
         <f t="shared" ref="O42:O44" si="110">RANK(Q42,$Q$41:$Q$44)+SUM(Y42:AB42)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P42" s="53" t="str">
         <f>Sorteios!I15</f>
@@ -9123,7 +9183,7 @@
       </c>
       <c r="R42" s="43">
         <f t="shared" ref="R42:R44" si="112">SUM(S42:U42)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S42" s="43">
         <f>COUNTIF(J:J,P42)</f>
@@ -9135,23 +9195,23 @@
       </c>
       <c r="U42" s="43">
         <f>COUNTIF(M:M,P42)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V42" s="43">
         <f>SUMIF(E:E,P42,F:F)+SUMIF(I:I,P42,H:H)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W42" s="43">
         <f>SUMIF(E:E,P42,H:H)+SUMIF(I:I,P42,F:F)</f>
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="X42" s="43">
         <f t="shared" ref="X42:X44" si="113">V42-W42</f>
-        <v>-2</v>
+        <v>-5</v>
       </c>
       <c r="Y42" s="43">
         <f t="shared" ref="Y42:Y44" si="114">SUMPRODUCT(($Q$41:$Q$44=Q42)*($X$41:$X$44&gt;X42))</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Z42" s="43">
         <f t="shared" ref="Z42:Z44" si="115">SUMPRODUCT(($Q$41:$Q$44=Q42)*($X$41:$X$44=X42)*($V$41:$V$44&gt;V42))</f>
@@ -9174,19 +9234,19 @@
       </c>
       <c r="AF42" s="83" t="str">
         <f t="shared" ref="AF42:AF44" si="118">VLOOKUP($AE42,$O$41:$X$44,2,FALSE)</f>
-        <v>Al Ain</v>
+        <v>Manchester City</v>
       </c>
       <c r="AG42" s="90">
         <f t="shared" ref="AG42:AG44" si="119">VLOOKUP($AE42,$O$41:$X$44,3,FALSE)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AH42" s="90">
         <f t="shared" ref="AH42:AH44" si="120">VLOOKUP($AE42,$O$41:$X$44,4,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI42" s="90">
         <f t="shared" ref="AI42:AI44" si="121">VLOOKUP($AE42,$O$41:$X$44,5,FALSE)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AJ42" s="90">
         <f t="shared" ref="AJ42:AJ44" si="122">VLOOKUP($AE42,$O$41:$X$44,6,FALSE)</f>
@@ -9198,7 +9258,7 @@
       </c>
       <c r="AL42" s="90">
         <f t="shared" ref="AL42:AL44" si="124">VLOOKUP($AE42,$O$41:$X$44,8,FALSE)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="AM42" s="90">
         <f t="shared" ref="AM42:AM44" si="125">VLOOKUP($AE42,$O$41:$X$44,9,FALSE)</f>
@@ -9206,7 +9266,7 @@
       </c>
       <c r="AN42" s="91">
         <f t="shared" ref="AN42:AN44" si="126">VLOOKUP($AE42,$O$41:$X$44,10,FALSE)</f>
-        <v>0</v>
+        <v>8</v>
       </c>
     </row>
     <row r="43" spans="1:40" x14ac:dyDescent="0.25">
@@ -9252,7 +9312,7 @@
       <c r="N43" s="51"/>
       <c r="O43" s="52">
         <f t="shared" si="110"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="P43" s="53" t="str">
         <f>Sorteios!I16</f>
@@ -9264,7 +9324,7 @@
       </c>
       <c r="R43" s="43">
         <f t="shared" si="112"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S43" s="43">
         <f>COUNTIF(J:J,P43)</f>
@@ -9276,7 +9336,7 @@
       </c>
       <c r="U43" s="43">
         <f>COUNTIF(M:M,P43)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="V43" s="43">
         <f>SUMIF(E:E,P43,F:F)+SUMIF(I:I,P43,H:H)</f>
@@ -9284,15 +9344,15 @@
       </c>
       <c r="W43" s="43">
         <f>SUMIF(E:E,P43,H:H)+SUMIF(I:I,P43,F:F)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
       <c r="X43" s="43">
         <f t="shared" si="113"/>
-        <v>0</v>
+        <v>-11</v>
       </c>
       <c r="Y43" s="43">
         <f t="shared" si="114"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z43" s="43">
         <f t="shared" si="115"/>
@@ -9315,7 +9375,7 @@
       </c>
       <c r="AF43" s="83" t="str">
         <f t="shared" si="118"/>
-        <v>Juventus</v>
+        <v>Wydad Casablanca</v>
       </c>
       <c r="AG43" s="90">
         <f t="shared" si="119"/>
@@ -9323,7 +9383,7 @@
       </c>
       <c r="AH43" s="90">
         <f t="shared" si="120"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AI43" s="90">
         <f t="shared" si="121"/>
@@ -9335,19 +9395,19 @@
       </c>
       <c r="AK43" s="90">
         <f t="shared" si="123"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AL43" s="90">
         <f t="shared" si="124"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM43" s="90">
         <f t="shared" si="125"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AN43" s="91">
         <f t="shared" si="126"/>
-        <v>0</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="44" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9393,7 +9453,7 @@
       <c r="N44" s="59"/>
       <c r="O44" s="60">
         <f t="shared" si="110"/>
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="P44" s="53" t="str">
         <f>Sorteios!I17</f>
@@ -9401,15 +9461,15 @@
       </c>
       <c r="Q44" s="57">
         <f t="shared" si="111"/>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="R44" s="57">
         <f t="shared" si="112"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="S44" s="43">
         <f>COUNTIF(J:J,P44)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="T44" s="43">
         <f>COUNTIF(K:K,P44)+COUNTIF(L:L,P44)</f>
@@ -9421,15 +9481,15 @@
       </c>
       <c r="V44" s="57">
         <f>SUMIF(E:E,P44,F:F)+SUMIF(I:I,P44,H:H)</f>
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="W44" s="57">
         <f>SUMIF(E:E,P44,H:H)+SUMIF(I:I,P44,F:F)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="X44" s="57">
         <f t="shared" si="113"/>
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="Y44" s="57">
         <f t="shared" si="114"/>
@@ -9445,7 +9505,7 @@
       </c>
       <c r="AB44" s="57">
         <f t="shared" si="117"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC44" s="58">
         <v>4</v>
@@ -9456,7 +9516,7 @@
       </c>
       <c r="AF44" s="84" t="str">
         <f t="shared" si="118"/>
-        <v>Wydad Casablanca</v>
+        <v>Al Ain</v>
       </c>
       <c r="AG44" s="92">
         <f t="shared" si="119"/>
@@ -9464,7 +9524,7 @@
       </c>
       <c r="AH44" s="92">
         <f t="shared" si="120"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI44" s="92">
         <f t="shared" si="121"/>
@@ -9476,7 +9536,7 @@
       </c>
       <c r="AK44" s="92">
         <f t="shared" si="123"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL44" s="92">
         <f t="shared" si="124"/>
@@ -9484,11 +9544,11 @@
       </c>
       <c r="AM44" s="92">
         <f t="shared" si="125"/>
-        <v>2</v>
+        <v>11</v>
       </c>
       <c r="AN44" s="93">
         <f t="shared" si="126"/>
-        <v>-2</v>
+        <v>-11</v>
       </c>
     </row>
     <row r="45" spans="1:40" x14ac:dyDescent="0.25">
@@ -9704,18 +9764,22 @@
         <f>P47</f>
         <v>Real Madrid</v>
       </c>
-      <c r="F47" s="21"/>
+      <c r="F47" s="21">
+        <v>3</v>
+      </c>
       <c r="G47" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="H47" s="21"/>
+      <c r="H47" s="21">
+        <v>1</v>
+      </c>
       <c r="I47" s="26" t="str">
         <f>P49</f>
         <v>Pachuca</v>
       </c>
       <c r="J47" s="42" t="str">
         <f t="shared" si="89"/>
-        <v>empate</v>
+        <v>Real Madrid</v>
       </c>
       <c r="K47" s="43" t="str">
         <f t="shared" si="90"/>
@@ -9727,12 +9791,12 @@
       </c>
       <c r="M47" s="44" t="str">
         <f t="shared" si="92"/>
-        <v>empate</v>
+        <v>Pachuca</v>
       </c>
       <c r="N47" s="50"/>
       <c r="O47" s="52">
         <f>RANK(Q47,$Q$47:$Q$50)+SUM(Y47:AB47)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P47" s="53" t="str">
         <f>Sorteios!L14</f>
@@ -9740,15 +9804,15 @@
       </c>
       <c r="Q47" s="43">
         <f>(S47*3)+(T47*1)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="R47" s="43">
         <f>SUM(S47:U47)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S47" s="43">
         <f>COUNTIF(J:J,P47)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T47" s="43">
         <f>COUNTIF(K:K,P47)+COUNTIF(L:L,P47)</f>
@@ -9760,15 +9824,15 @@
       </c>
       <c r="V47" s="43">
         <f>SUMIF(E:E,P47,F:F)+SUMIF(I:I,P47,H:H)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="W47" s="43">
         <f>SUMIF(E:E,P47,H:H)+SUMIF(I:I,P47,F:F)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X47" s="43">
         <f>V47-W47</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y47" s="43">
         <f>SUMPRODUCT(($Q$47:$Q$50=Q47)*($X$47:$X$50&gt;X47))</f>
@@ -9795,15 +9859,15 @@
       </c>
       <c r="AF47" s="83" t="str">
         <f>VLOOKUP($AE47,$O$47:$X$50,2,FALSE)</f>
-        <v>Red Bull Salzburg</v>
+        <v>Real Madrid</v>
       </c>
       <c r="AG47" s="90">
         <f>VLOOKUP($AE47,$O$47:$X$50,3,FALSE)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH47" s="90">
         <f>VLOOKUP($AE47,$O$47:$X$50,4,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI47" s="90">
         <f>VLOOKUP($AE47,$O$47:$X$50,5,FALSE)</f>
@@ -9811,7 +9875,7 @@
       </c>
       <c r="AJ47" s="90">
         <f>VLOOKUP($AE47,$O$47:$X$50,6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK47" s="90">
         <f>VLOOKUP($AE47,$O$47:$X$50,7,FALSE)</f>
@@ -9819,15 +9883,15 @@
       </c>
       <c r="AL47" s="90">
         <f>VLOOKUP($AE47,$O$47:$X$50,8,FALSE)</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AM47" s="90">
         <f>VLOOKUP($AE47,$O$47:$X$50,9,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AN47" s="91">
         <f>VLOOKUP($AE47,$O$47:$X$50,10,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="48" spans="1:40" x14ac:dyDescent="0.25">
@@ -9845,11 +9909,15 @@
         <f>P50</f>
         <v>Red Bull Salzburg</v>
       </c>
-      <c r="F48" s="21"/>
+      <c r="F48" s="21">
+        <v>0</v>
+      </c>
       <c r="G48" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="H48" s="21"/>
+      <c r="H48" s="21">
+        <v>0</v>
+      </c>
       <c r="I48" s="26" t="str">
         <f>P48</f>
         <v>Al-Hilal</v>
@@ -9860,11 +9928,11 @@
       </c>
       <c r="K48" s="43" t="str">
         <f t="shared" si="90"/>
-        <v/>
+        <v>Red Bull Salzburg</v>
       </c>
       <c r="L48" s="43" t="str">
         <f t="shared" si="91"/>
-        <v/>
+        <v>Al-Hilal</v>
       </c>
       <c r="M48" s="44" t="str">
         <f t="shared" si="92"/>
@@ -9881,11 +9949,11 @@
       </c>
       <c r="Q48" s="43">
         <f t="shared" ref="Q48:Q50" si="127">(S48*3)+(T48*1)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R48" s="43">
         <f t="shared" ref="R48:R50" si="128">SUM(S48:U48)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S48" s="43">
         <f>COUNTIF(J:J,P48)</f>
@@ -9893,7 +9961,7 @@
       </c>
       <c r="T48" s="43">
         <f>COUNTIF(K:K,P48)+COUNTIF(L:L,P48)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U48" s="43">
         <f>COUNTIF(M:M,P48)</f>
@@ -9925,7 +9993,7 @@
       </c>
       <c r="AB48" s="43">
         <f t="shared" ref="AB48:AB50" si="133">SUMPRODUCT(($Q$47:$Q$50=Q48)*($X$47:$X$50=X48)*($V$47:$V$50=V48)*($W$47:$W$50=W48)*($AC$47:$AC$50&lt;AC48))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AC48" s="44">
         <v>2</v>
@@ -9936,19 +10004,19 @@
       </c>
       <c r="AF48" s="83" t="str">
         <f t="shared" ref="AF48:AF50" si="134">VLOOKUP($AE48,$O$47:$X$50,2,FALSE)</f>
-        <v>Real Madrid</v>
+        <v>Red Bull Salzburg</v>
       </c>
       <c r="AG48" s="90">
         <f t="shared" ref="AG48:AG50" si="135">VLOOKUP($AE48,$O$47:$X$50,3,FALSE)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AH48" s="90">
         <f t="shared" ref="AH48:AH50" si="136">VLOOKUP($AE48,$O$47:$X$50,4,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI48" s="90">
         <f t="shared" ref="AI48:AI50" si="137">VLOOKUP($AE48,$O$47:$X$50,5,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ48" s="90">
         <f t="shared" ref="AJ48:AJ50" si="138">VLOOKUP($AE48,$O$47:$X$50,6,FALSE)</f>
@@ -9960,7 +10028,7 @@
       </c>
       <c r="AL48" s="90">
         <f t="shared" ref="AL48:AL50" si="140">VLOOKUP($AE48,$O$47:$X$50,8,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AM48" s="90">
         <f t="shared" ref="AM48:AM50" si="141">VLOOKUP($AE48,$O$47:$X$50,9,FALSE)</f>
@@ -9968,7 +10036,7 @@
       </c>
       <c r="AN48" s="91">
         <f t="shared" ref="AN48:AN50" si="142">VLOOKUP($AE48,$O$47:$X$50,10,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:40" x14ac:dyDescent="0.25">
@@ -10026,7 +10094,7 @@
       </c>
       <c r="R49" s="43">
         <f t="shared" si="128"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S49" s="43">
         <f>COUNTIF(J:J,P49)</f>
@@ -10038,19 +10106,19 @@
       </c>
       <c r="U49" s="43">
         <f>COUNTIF(M:M,P49)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V49" s="43">
         <f>SUMIF(E:E,P49,F:F)+SUMIF(I:I,P49,H:H)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W49" s="43">
         <f>SUMIF(E:E,P49,H:H)+SUMIF(I:I,P49,F:F)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="X49" s="43">
         <f t="shared" si="129"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
       <c r="Y49" s="43">
         <f t="shared" si="130"/>
@@ -10081,11 +10149,11 @@
       </c>
       <c r="AG49" s="90">
         <f t="shared" si="135"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH49" s="90">
         <f t="shared" si="136"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI49" s="90">
         <f t="shared" si="137"/>
@@ -10093,7 +10161,7 @@
       </c>
       <c r="AJ49" s="90">
         <f t="shared" si="138"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK49" s="90">
         <f t="shared" si="139"/>
@@ -10155,7 +10223,7 @@
       <c r="N50" s="50"/>
       <c r="O50" s="73">
         <f t="shared" si="143"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P50" s="53" t="str">
         <f>Sorteios!L17</f>
@@ -10163,11 +10231,11 @@
       </c>
       <c r="Q50" s="57">
         <f t="shared" si="127"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R50" s="57">
         <f t="shared" si="128"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="S50" s="43">
         <f>COUNTIF(J:J,P50)</f>
@@ -10175,7 +10243,7 @@
       </c>
       <c r="T50" s="43">
         <f>COUNTIF(K:K,P50)+COUNTIF(L:L,P50)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U50" s="43">
         <f>COUNTIF(M:M,P50)</f>
@@ -10195,7 +10263,7 @@
       </c>
       <c r="Y50" s="57">
         <f t="shared" si="130"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z50" s="57">
         <f t="shared" si="131"/>
@@ -10226,7 +10294,7 @@
       </c>
       <c r="AH50" s="92">
         <f t="shared" si="136"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AI50" s="92">
         <f t="shared" si="137"/>
@@ -10238,19 +10306,19 @@
       </c>
       <c r="AK50" s="92">
         <f t="shared" si="139"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL50" s="92">
         <f t="shared" si="140"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AM50" s="92">
         <f t="shared" si="141"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AN50" s="93">
         <f t="shared" si="142"/>
-        <v>-1</v>
+        <v>-3</v>
       </c>
     </row>
   </sheetData>
@@ -10419,18 +10487,18 @@
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="109"/>
-      <c r="B4" s="179" t="s">
+      <c r="B4" s="180" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="180"/>
-      <c r="D4" s="180"/>
-      <c r="E4" s="180"/>
-      <c r="F4" s="180"/>
-      <c r="G4" s="180"/>
-      <c r="H4" s="180"/>
-      <c r="I4" s="180"/>
-      <c r="J4" s="180"/>
-      <c r="K4" s="181"/>
+      <c r="C4" s="181"/>
+      <c r="D4" s="181"/>
+      <c r="E4" s="181"/>
+      <c r="F4" s="181"/>
+      <c r="G4" s="181"/>
+      <c r="H4" s="181"/>
+      <c r="I4" s="181"/>
+      <c r="J4" s="181"/>
+      <c r="K4" s="182"/>
       <c r="L4" s="110"/>
       <c r="M4" s="111"/>
       <c r="N4" s="111"/>
@@ -10447,19 +10515,19 @@
       <c r="D5" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="182" t="s">
+      <c r="E5" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="182"/>
-      <c r="G5" s="182" t="s">
+      <c r="F5" s="183"/>
+      <c r="G5" s="183" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="182"/>
-      <c r="I5" s="182"/>
-      <c r="J5" s="182" t="s">
+      <c r="H5" s="183"/>
+      <c r="I5" s="183"/>
+      <c r="J5" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="183"/>
+      <c r="K5" s="184"/>
       <c r="L5" s="113"/>
       <c r="M5" s="113"/>
       <c r="N5" s="113"/>
@@ -10747,18 +10815,18 @@
     </row>
     <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="109"/>
-      <c r="B16" s="179" t="s">
+      <c r="B16" s="180" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="180"/>
-      <c r="D16" s="180"/>
-      <c r="E16" s="180"/>
-      <c r="F16" s="180"/>
-      <c r="G16" s="180"/>
-      <c r="H16" s="180"/>
-      <c r="I16" s="180"/>
-      <c r="J16" s="180"/>
-      <c r="K16" s="181"/>
+      <c r="C16" s="181"/>
+      <c r="D16" s="181"/>
+      <c r="E16" s="181"/>
+      <c r="F16" s="181"/>
+      <c r="G16" s="181"/>
+      <c r="H16" s="181"/>
+      <c r="I16" s="181"/>
+      <c r="J16" s="181"/>
+      <c r="K16" s="182"/>
       <c r="L16" s="110"/>
       <c r="M16" s="111"/>
       <c r="N16" s="111"/>
@@ -10771,19 +10839,19 @@
       <c r="D17" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="182" t="s">
+      <c r="E17" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="182"/>
-      <c r="G17" s="182" t="s">
+      <c r="F17" s="183"/>
+      <c r="G17" s="183" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="182"/>
-      <c r="I17" s="182"/>
-      <c r="J17" s="182" t="s">
+      <c r="H17" s="183"/>
+      <c r="I17" s="183"/>
+      <c r="J17" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="K17" s="183"/>
+      <c r="K17" s="184"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B18" s="129" t="s">
@@ -10929,18 +10997,18 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="109"/>
-      <c r="B24" s="179" t="s">
+      <c r="B24" s="180" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="180"/>
-      <c r="D24" s="180"/>
-      <c r="E24" s="180"/>
-      <c r="F24" s="180"/>
-      <c r="G24" s="180"/>
-      <c r="H24" s="180"/>
-      <c r="I24" s="180"/>
-      <c r="J24" s="180"/>
-      <c r="K24" s="181"/>
+      <c r="C24" s="181"/>
+      <c r="D24" s="181"/>
+      <c r="E24" s="181"/>
+      <c r="F24" s="181"/>
+      <c r="G24" s="181"/>
+      <c r="H24" s="181"/>
+      <c r="I24" s="181"/>
+      <c r="J24" s="181"/>
+      <c r="K24" s="182"/>
       <c r="L24" s="110"/>
       <c r="M24" s="111"/>
       <c r="N24" s="111"/>
@@ -10956,19 +11024,19 @@
       <c r="D25" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="182" t="s">
+      <c r="E25" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="182"/>
-      <c r="G25" s="182" t="s">
+      <c r="F25" s="183"/>
+      <c r="G25" s="183" t="s">
         <v>13</v>
       </c>
-      <c r="H25" s="182"/>
-      <c r="I25" s="182"/>
-      <c r="J25" s="182" t="s">
+      <c r="H25" s="183"/>
+      <c r="I25" s="183"/>
+      <c r="J25" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="K25" s="183"/>
+      <c r="K25" s="184"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="151" t="s">
@@ -11057,18 +11125,18 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="109"/>
-      <c r="B31" s="179" t="s">
+      <c r="B31" s="180" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="180"/>
-      <c r="D31" s="180"/>
-      <c r="E31" s="180"/>
-      <c r="F31" s="180"/>
-      <c r="G31" s="180"/>
-      <c r="H31" s="180"/>
-      <c r="I31" s="180"/>
-      <c r="J31" s="180"/>
-      <c r="K31" s="181"/>
+      <c r="C31" s="181"/>
+      <c r="D31" s="181"/>
+      <c r="E31" s="181"/>
+      <c r="F31" s="181"/>
+      <c r="G31" s="181"/>
+      <c r="H31" s="181"/>
+      <c r="I31" s="181"/>
+      <c r="J31" s="181"/>
+      <c r="K31" s="182"/>
       <c r="L31" s="110"/>
       <c r="M31" s="111"/>
       <c r="N31" s="111"/>
@@ -11084,19 +11152,19 @@
       <c r="D32" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="182" t="s">
+      <c r="E32" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="182"/>
-      <c r="G32" s="182" t="s">
+      <c r="F32" s="183"/>
+      <c r="G32" s="183" t="s">
         <v>13</v>
       </c>
-      <c r="H32" s="182"/>
-      <c r="I32" s="182"/>
-      <c r="J32" s="182" t="s">
+      <c r="H32" s="183"/>
+      <c r="I32" s="183"/>
+      <c r="J32" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="K32" s="183"/>
+      <c r="K32" s="184"/>
     </row>
     <row r="33" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="161" t="s">
@@ -11144,11 +11212,11 @@
     </row>
     <row r="36" spans="1:17" s="137" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="135"/>
-      <c r="B36" s="184" t="s">
+      <c r="B36" s="179" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="184"/>
-      <c r="D36" s="184"/>
+      <c r="C36" s="179"/>
+      <c r="D36" s="179"/>
       <c r="E36" s="173" t="str">
         <f>IF(M33="1º Lugar","",M33)</f>
         <v/>
@@ -11168,11 +11236,11 @@
     </row>
     <row r="37" spans="1:17" s="137" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="135"/>
-      <c r="B37" s="184" t="s">
+      <c r="B37" s="179" t="s">
         <v>106</v>
       </c>
-      <c r="C37" s="184"/>
-      <c r="D37" s="184"/>
+      <c r="C37" s="179"/>
+      <c r="D37" s="179"/>
       <c r="E37" s="175" t="str">
         <f>IF(M34="2º Lugar","",M34)</f>
         <v/>
@@ -11300,12 +11368,11 @@
   </sheetData>
   <sheetProtection password="CC01" sheet="1" selectLockedCells="1"/>
   <mergeCells count="18">
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B31:K31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="B16:K16"/>
     <mergeCell ref="B24:K24"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="G25:I25"/>
@@ -11313,11 +11380,12 @@
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="B16:K16"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B31:K31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="B36:D36"/>
   </mergeCells>
   <conditionalFormatting sqref="F6">
     <cfRule type="expression" dxfId="31" priority="128">
@@ -11484,23 +11552,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DBF2846C41E31A469E3CED25F2422E48" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0c08e4af4d80db6585ac36ba965bb3a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2c8c20e6-817c-474f-b9c2-eb2b1ac24837" xmlns:ns4="dc8c2798-6aba-4af7-93a4-b89253b03650" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4e7db2db65f9cb533b4933096bc9b657" ns3:_="" ns4:_="">
     <xsd:import namespace="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
@@ -11733,32 +11784,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A45D7D45-1E18-48AE-827B-096C3C02C976}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83E7837-68AD-48B2-A1AB-AAB452317AF5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
-    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFBCCD5-5BDE-495C-BFE9-46A98A6BC529}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11775,4 +11818,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83E7837-68AD-48B2-A1AB-AAB452317AF5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A45D7D45-1E18-48AE-827B-096C3C02C976}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Att até jogo 34
+ Correção de erro no chaveamento das oitavas.
</commit_message>
<xml_diff>
--- a/Mundial de Clubes FIFA 2025.xlsx
+++ b/Mundial de Clubes FIFA 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjunior\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{07D0F67C-3835-4B35-9AC7-CC16D9173FC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E6A35FF-B645-4CAF-BF54-0B6D87B6ACA2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="1185" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{076F3B28-812E-4458-A424-96085A053123}"/>
   </bookViews>
@@ -1598,23 +1598,23 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -5176,7 +5176,7 @@
       <c r="N11" s="51"/>
       <c r="O11" s="52">
         <f>RANK(Q11,$Q$11:$Q$14)+SUM(Y11:AB11)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P11" s="53" t="str">
         <f>Sorteios!F6</f>
@@ -5184,15 +5184,15 @@
       </c>
       <c r="Q11" s="43">
         <f>(S11*3)+(T11*1)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R11" s="43">
         <f>SUM(S11:U11)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S11" s="43">
         <f>COUNTIF(J:J,P11)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T11" s="43">
         <f>COUNTIF(K:K,P11)+COUNTIF(L:L,P11)</f>
@@ -5204,7 +5204,7 @@
       </c>
       <c r="V11" s="43">
         <f>SUMIF(E:E,P11,F:F)+SUMIF(I:I,P11,H:H)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="W11" s="43">
         <f>SUMIF(E:E,P11,H:H)+SUMIF(I:I,P11,F:F)</f>
@@ -5212,7 +5212,7 @@
       </c>
       <c r="X11" s="43">
         <f>V11-W11</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Y11" s="43">
         <f>SUMPRODUCT(($Q$11:$Q$14=Q11)*($X$11:$X$14&gt;X11))</f>
@@ -5239,7 +5239,7 @@
       </c>
       <c r="AF11" s="83" t="str">
         <f>VLOOKUP($AE11,$O$11:$X$14,2,FALSE)</f>
-        <v>Botafogo</v>
+        <v>Paris Saint-Germain</v>
       </c>
       <c r="AG11" s="90">
         <f>VLOOKUP($AE11,$O$11:$X$14,3,FALSE)</f>
@@ -5247,7 +5247,7 @@
       </c>
       <c r="AH11" s="90">
         <f>VLOOKUP($AE11,$O$11:$X$14,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI11" s="90">
         <f>VLOOKUP($AE11,$O$11:$X$14,5,FALSE)</f>
@@ -5259,11 +5259,11 @@
       </c>
       <c r="AK11" s="90">
         <f>VLOOKUP($AE11,$O$11:$X$14,7,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL11" s="90">
         <f>VLOOKUP($AE11,$O$11:$X$14,8,FALSE)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AM11" s="90">
         <f>VLOOKUP($AE11,$O$11:$X$14,9,FALSE)</f>
@@ -5271,7 +5271,7 @@
       </c>
       <c r="AN11" s="91">
         <f>VLOOKUP($AE11,$O$11:$X$14,10,FALSE)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.25">
@@ -5329,15 +5329,15 @@
       </c>
       <c r="Q12" s="43">
         <f t="shared" ref="Q12:Q14" si="22">(S12*3)+(T12*1)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R12" s="43">
         <f t="shared" ref="R12:R14" si="23">SUM(S12:U12)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S12" s="43">
         <f>COUNTIF(J:J,P12)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T12" s="43">
         <f>COUNTIF(K:K,P12)+COUNTIF(L:L,P12)</f>
@@ -5349,7 +5349,7 @@
       </c>
       <c r="V12" s="43">
         <f>SUMIF(E:E,P12,F:F)+SUMIF(I:I,P12,H:H)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W12" s="43">
         <f>SUMIF(E:E,P12,H:H)+SUMIF(I:I,P12,F:F)</f>
@@ -5357,11 +5357,11 @@
       </c>
       <c r="X12" s="43">
         <f t="shared" ref="X12:X14" si="24">V12-W12</f>
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="Y12" s="43">
         <f t="shared" ref="Y12:Y14" si="25">SUMPRODUCT(($Q$11:$Q$14=Q12)*($X$11:$X$14&gt;X12))</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Z12" s="43">
         <f t="shared" ref="Z12:Z14" si="26">SUMPRODUCT(($Q$11:$Q$14=Q12)*($X$11:$X$14=X12)*($V$11:$V$14&gt;V12))</f>
@@ -5384,19 +5384,19 @@
       </c>
       <c r="AF12" s="83" t="str">
         <f t="shared" ref="AF12:AF14" si="29">VLOOKUP($AE12,$O$11:$X$14,2,FALSE)</f>
-        <v>Paris Saint-Germain</v>
+        <v>Botafogo</v>
       </c>
       <c r="AG12" s="90">
         <f t="shared" ref="AG12:AG14" si="30">VLOOKUP($AE12,$O$11:$X$14,3,FALSE)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AH12" s="90">
         <f t="shared" ref="AH12:AH14" si="31">VLOOKUP($AE12,$O$11:$X$14,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI12" s="90">
         <f t="shared" ref="AI12:AI14" si="32">VLOOKUP($AE12,$O$11:$X$14,5,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ12" s="90">
         <f t="shared" ref="AJ12:AJ14" si="33">VLOOKUP($AE12,$O$11:$X$14,6,FALSE)</f>
@@ -5408,15 +5408,15 @@
       </c>
       <c r="AL12" s="90">
         <f t="shared" ref="AL12:AL14" si="35">VLOOKUP($AE12,$O$11:$X$14,8,FALSE)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="AM12" s="90">
         <f t="shared" ref="AM12:AM14" si="36">VLOOKUP($AE12,$O$11:$X$14,9,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AN12" s="91">
         <f t="shared" ref="AN12:AN14" si="37">VLOOKUP($AE12,$O$11:$X$14,10,FALSE)</f>
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.25">
@@ -5434,18 +5434,22 @@
         <f>P14</f>
         <v>Seattle Sounders</v>
       </c>
-      <c r="F13" s="21"/>
+      <c r="F13" s="21">
+        <v>0</v>
+      </c>
       <c r="G13" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="H13" s="21"/>
+      <c r="H13" s="21">
+        <v>2</v>
+      </c>
       <c r="I13" s="26" t="str">
         <f>P11</f>
         <v>Paris Saint-Germain</v>
       </c>
       <c r="J13" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>empate</v>
+        <v>Paris Saint-Germain</v>
       </c>
       <c r="K13" s="43" t="str">
         <f t="shared" si="1"/>
@@ -5457,12 +5461,12 @@
       </c>
       <c r="M13" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>empate</v>
+        <v>Seattle Sounders</v>
       </c>
       <c r="N13" s="51"/>
       <c r="O13" s="52">
         <f t="shared" si="21"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P13" s="53" t="str">
         <f>Sorteios!F8</f>
@@ -5474,7 +5478,7 @@
       </c>
       <c r="R13" s="43">
         <f t="shared" si="23"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S13" s="43">
         <f>COUNTIF(J:J,P13)</f>
@@ -5486,7 +5490,7 @@
       </c>
       <c r="U13" s="43">
         <f>COUNTIF(M:M,P13)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V13" s="43">
         <f>SUMIF(E:E,P13,F:F)+SUMIF(I:I,P13,H:H)</f>
@@ -5494,15 +5498,15 @@
       </c>
       <c r="W13" s="43">
         <f>SUMIF(E:E,P13,H:H)+SUMIF(I:I,P13,F:F)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X13" s="43">
         <f t="shared" si="24"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="Y13" s="43">
         <f t="shared" si="25"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Z13" s="43">
         <f t="shared" si="26"/>
@@ -5529,15 +5533,15 @@
       </c>
       <c r="AG13" s="90">
         <f t="shared" si="30"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AH13" s="90">
         <f t="shared" si="31"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI13" s="90">
         <f t="shared" si="32"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ13" s="90">
         <f t="shared" si="33"/>
@@ -5549,7 +5553,7 @@
       </c>
       <c r="AL13" s="90">
         <f t="shared" si="35"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AM13" s="90">
         <f t="shared" si="36"/>
@@ -5557,7 +5561,7 @@
       </c>
       <c r="AN13" s="91">
         <f t="shared" si="37"/>
-        <v>-2</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="14" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -5575,18 +5579,22 @@
         <f>P12</f>
         <v>Atlético de Madrid</v>
       </c>
-      <c r="F14" s="22"/>
+      <c r="F14" s="22">
+        <v>1</v>
+      </c>
       <c r="G14" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="H14" s="22"/>
+      <c r="H14" s="22">
+        <v>0</v>
+      </c>
       <c r="I14" s="27" t="str">
         <f>P13</f>
         <v>Botafogo</v>
       </c>
       <c r="J14" s="56" t="str">
         <f t="shared" si="0"/>
-        <v>empate</v>
+        <v>Atlético de Madrid</v>
       </c>
       <c r="K14" s="57" t="str">
         <f t="shared" si="1"/>
@@ -5598,7 +5606,7 @@
       </c>
       <c r="M14" s="58" t="str">
         <f t="shared" si="3"/>
-        <v>empate</v>
+        <v>Botafogo</v>
       </c>
       <c r="N14" s="59"/>
       <c r="O14" s="60">
@@ -5615,7 +5623,7 @@
       </c>
       <c r="R14" s="57">
         <f t="shared" si="23"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S14" s="43">
         <f>COUNTIF(J:J,P14)</f>
@@ -5627,7 +5635,7 @@
       </c>
       <c r="U14" s="43">
         <f>COUNTIF(M:M,P14)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V14" s="57">
         <f>SUMIF(E:E,P14,F:F)+SUMIF(I:I,P14,H:H)</f>
@@ -5635,11 +5643,11 @@
       </c>
       <c r="W14" s="57">
         <f>SUMIF(E:E,P14,H:H)+SUMIF(I:I,P14,F:F)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="X14" s="57">
         <f t="shared" si="24"/>
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="Y14" s="57">
         <f t="shared" si="25"/>
@@ -5674,7 +5682,7 @@
       </c>
       <c r="AH14" s="92">
         <f t="shared" si="31"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI14" s="92">
         <f t="shared" si="32"/>
@@ -5686,7 +5694,7 @@
       </c>
       <c r="AK14" s="92">
         <f t="shared" si="34"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL14" s="92">
         <f t="shared" si="35"/>
@@ -5694,11 +5702,11 @@
       </c>
       <c r="AM14" s="92">
         <f t="shared" si="36"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AN14" s="93">
         <f t="shared" si="37"/>
-        <v>-3</v>
+        <v>-5</v>
       </c>
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.25">
@@ -10487,18 +10495,18 @@
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="109"/>
-      <c r="B4" s="180" t="s">
+      <c r="B4" s="179" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="181"/>
-      <c r="D4" s="181"/>
-      <c r="E4" s="181"/>
-      <c r="F4" s="181"/>
-      <c r="G4" s="181"/>
-      <c r="H4" s="181"/>
-      <c r="I4" s="181"/>
-      <c r="J4" s="181"/>
-      <c r="K4" s="182"/>
+      <c r="C4" s="180"/>
+      <c r="D4" s="180"/>
+      <c r="E4" s="180"/>
+      <c r="F4" s="180"/>
+      <c r="G4" s="180"/>
+      <c r="H4" s="180"/>
+      <c r="I4" s="180"/>
+      <c r="J4" s="180"/>
+      <c r="K4" s="181"/>
       <c r="L4" s="110"/>
       <c r="M4" s="111"/>
       <c r="N4" s="111"/>
@@ -10515,19 +10523,19 @@
       <c r="D5" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="183" t="s">
+      <c r="E5" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="183"/>
-      <c r="G5" s="183" t="s">
+      <c r="F5" s="182"/>
+      <c r="G5" s="182" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="183"/>
-      <c r="I5" s="183"/>
-      <c r="J5" s="183" t="s">
+      <c r="H5" s="182"/>
+      <c r="I5" s="182"/>
+      <c r="J5" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="184"/>
+      <c r="K5" s="183"/>
       <c r="L5" s="113"/>
       <c r="M5" s="113"/>
       <c r="N5" s="113"/>
@@ -10557,8 +10565,8 @@
       <c r="I6" s="23"/>
       <c r="J6" s="154"/>
       <c r="K6" s="155" t="str">
-        <f>IF('Fase de Grupos'!AH12=3,'Fase de Grupos'!AF23,"2º do Grupo B")</f>
-        <v>2º do Grupo B</v>
+        <f>IF('Fase de Grupos'!AH12=3,'Fase de Grupos'!AF12,"2º do Grupo B")</f>
+        <v>Botafogo</v>
       </c>
       <c r="L6" s="114" t="str">
         <f>IF(OR(G6="",I6=""),"",IF(G6=I6,"emp",""))</f>
@@ -10615,7 +10623,7 @@
       </c>
       <c r="E8" s="11" t="str">
         <f>IF('Fase de Grupos'!AH11=3,'Fase de Grupos'!AF11,"1º do Grupo B")</f>
-        <v>1º do Grupo B</v>
+        <v>Paris Saint-Germain</v>
       </c>
       <c r="F8" s="121"/>
       <c r="G8" s="21"/>
@@ -10815,18 +10823,18 @@
     </row>
     <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="109"/>
-      <c r="B16" s="180" t="s">
+      <c r="B16" s="179" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="181"/>
-      <c r="D16" s="181"/>
-      <c r="E16" s="181"/>
-      <c r="F16" s="181"/>
-      <c r="G16" s="181"/>
-      <c r="H16" s="181"/>
-      <c r="I16" s="181"/>
-      <c r="J16" s="181"/>
-      <c r="K16" s="182"/>
+      <c r="C16" s="180"/>
+      <c r="D16" s="180"/>
+      <c r="E16" s="180"/>
+      <c r="F16" s="180"/>
+      <c r="G16" s="180"/>
+      <c r="H16" s="180"/>
+      <c r="I16" s="180"/>
+      <c r="J16" s="180"/>
+      <c r="K16" s="181"/>
       <c r="L16" s="110"/>
       <c r="M16" s="111"/>
       <c r="N16" s="111"/>
@@ -10839,19 +10847,19 @@
       <c r="D17" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="183" t="s">
+      <c r="E17" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="183"/>
-      <c r="G17" s="183" t="s">
+      <c r="F17" s="182"/>
+      <c r="G17" s="182" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="183"/>
-      <c r="I17" s="183"/>
-      <c r="J17" s="183" t="s">
+      <c r="H17" s="182"/>
+      <c r="I17" s="182"/>
+      <c r="J17" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="K17" s="184"/>
+      <c r="K17" s="183"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B18" s="129" t="s">
@@ -10997,18 +11005,18 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="109"/>
-      <c r="B24" s="180" t="s">
+      <c r="B24" s="179" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="181"/>
-      <c r="D24" s="181"/>
-      <c r="E24" s="181"/>
-      <c r="F24" s="181"/>
-      <c r="G24" s="181"/>
-      <c r="H24" s="181"/>
-      <c r="I24" s="181"/>
-      <c r="J24" s="181"/>
-      <c r="K24" s="182"/>
+      <c r="C24" s="180"/>
+      <c r="D24" s="180"/>
+      <c r="E24" s="180"/>
+      <c r="F24" s="180"/>
+      <c r="G24" s="180"/>
+      <c r="H24" s="180"/>
+      <c r="I24" s="180"/>
+      <c r="J24" s="180"/>
+      <c r="K24" s="181"/>
       <c r="L24" s="110"/>
       <c r="M24" s="111"/>
       <c r="N24" s="111"/>
@@ -11024,19 +11032,19 @@
       <c r="D25" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="183" t="s">
+      <c r="E25" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="183"/>
-      <c r="G25" s="183" t="s">
+      <c r="F25" s="182"/>
+      <c r="G25" s="182" t="s">
         <v>13</v>
       </c>
-      <c r="H25" s="183"/>
-      <c r="I25" s="183"/>
-      <c r="J25" s="183" t="s">
+      <c r="H25" s="182"/>
+      <c r="I25" s="182"/>
+      <c r="J25" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="K25" s="184"/>
+      <c r="K25" s="183"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="151" t="s">
@@ -11125,18 +11133,18 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="109"/>
-      <c r="B31" s="180" t="s">
+      <c r="B31" s="179" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="181"/>
-      <c r="D31" s="181"/>
-      <c r="E31" s="181"/>
-      <c r="F31" s="181"/>
-      <c r="G31" s="181"/>
-      <c r="H31" s="181"/>
-      <c r="I31" s="181"/>
-      <c r="J31" s="181"/>
-      <c r="K31" s="182"/>
+      <c r="C31" s="180"/>
+      <c r="D31" s="180"/>
+      <c r="E31" s="180"/>
+      <c r="F31" s="180"/>
+      <c r="G31" s="180"/>
+      <c r="H31" s="180"/>
+      <c r="I31" s="180"/>
+      <c r="J31" s="180"/>
+      <c r="K31" s="181"/>
       <c r="L31" s="110"/>
       <c r="M31" s="111"/>
       <c r="N31" s="111"/>
@@ -11152,19 +11160,19 @@
       <c r="D32" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="183" t="s">
+      <c r="E32" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="183"/>
-      <c r="G32" s="183" t="s">
+      <c r="F32" s="182"/>
+      <c r="G32" s="182" t="s">
         <v>13</v>
       </c>
-      <c r="H32" s="183"/>
-      <c r="I32" s="183"/>
-      <c r="J32" s="183" t="s">
+      <c r="H32" s="182"/>
+      <c r="I32" s="182"/>
+      <c r="J32" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="K32" s="184"/>
+      <c r="K32" s="183"/>
     </row>
     <row r="33" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="161" t="s">
@@ -11212,11 +11220,11 @@
     </row>
     <row r="36" spans="1:17" s="137" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="135"/>
-      <c r="B36" s="179" t="s">
+      <c r="B36" s="184" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="179"/>
-      <c r="D36" s="179"/>
+      <c r="C36" s="184"/>
+      <c r="D36" s="184"/>
       <c r="E36" s="173" t="str">
         <f>IF(M33="1º Lugar","",M33)</f>
         <v/>
@@ -11236,11 +11244,11 @@
     </row>
     <row r="37" spans="1:17" s="137" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="135"/>
-      <c r="B37" s="179" t="s">
+      <c r="B37" s="184" t="s">
         <v>106</v>
       </c>
-      <c r="C37" s="179"/>
-      <c r="D37" s="179"/>
+      <c r="C37" s="184"/>
+      <c r="D37" s="184"/>
       <c r="E37" s="175" t="str">
         <f>IF(M34="2º Lugar","",M34)</f>
         <v/>
@@ -11368,11 +11376,12 @@
   </sheetData>
   <sheetProtection password="CC01" sheet="1" selectLockedCells="1"/>
   <mergeCells count="18">
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="B16:K16"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B31:K31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="B36:D36"/>
     <mergeCell ref="B24:K24"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="G25:I25"/>
@@ -11380,12 +11389,11 @@
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B31:K31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="B16:K16"/>
   </mergeCells>
   <conditionalFormatting sqref="F6">
     <cfRule type="expression" dxfId="31" priority="128">
@@ -11552,6 +11560,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DBF2846C41E31A469E3CED25F2422E48" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0c08e4af4d80db6585ac36ba965bb3a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2c8c20e6-817c-474f-b9c2-eb2b1ac24837" xmlns:ns4="dc8c2798-6aba-4af7-93a4-b89253b03650" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4e7db2db65f9cb533b4933096bc9b657" ns3:_="" ns4:_="">
     <xsd:import namespace="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
@@ -11784,24 +11809,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A45D7D45-1E18-48AE-827B-096C3C02C976}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83E7837-68AD-48B2-A1AB-AAB452317AF5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFBCCD5-5BDE-495C-BFE9-46A98A6BC529}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11818,29 +11851,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83E7837-68AD-48B2-A1AB-AAB452317AF5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A45D7D45-1E18-48AE-827B-096C3C02C976}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Att até Jogo 38
</commit_message>
<xml_diff>
--- a/Mundial de Clubes FIFA 2025.xlsx
+++ b/Mundial de Clubes FIFA 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjunior\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5F359DCE-2C49-4B1A-8E3C-CA6B5B68B0B2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F8C17AC-39E8-407F-B1BC-0C405CA1B6A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="1185" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{076F3B28-812E-4458-A424-96085A053123}"/>
   </bookViews>
@@ -1598,23 +1598,23 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4019,7 +4019,7 @@
   <dimension ref="A1:AN50"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5962,7 +5962,7 @@
       <c r="N17" s="51"/>
       <c r="O17" s="52">
         <f>RANK(Q17,$Q$17:$Q$20)+SUM(Y17:AB17)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P17" s="53" t="str">
         <f>Sorteios!I6</f>
@@ -5974,7 +5974,7 @@
       </c>
       <c r="R17" s="43">
         <f>SUM(S17:U17)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S17" s="43">
         <f>COUNTIF(J:J,P17)</f>
@@ -5986,7 +5986,7 @@
       </c>
       <c r="U17" s="43">
         <f>COUNTIF(M:M,P17)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V17" s="43">
         <f>SUMIF(E:E,P17,F:F)+SUMIF(I:I,P17,H:H)</f>
@@ -5994,11 +5994,11 @@
       </c>
       <c r="W17" s="43">
         <f>SUMIF(E:E,P17,H:H)+SUMIF(I:I,P17,F:F)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X17" s="43">
         <f>V17-W17</f>
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="Y17" s="43">
         <f>SUMPRODUCT(($Q$17:$Q$20=Q17)*($X$17:$X$20&gt;X17))</f>
@@ -6025,15 +6025,15 @@
       </c>
       <c r="AF17" s="83" t="str">
         <f>VLOOKUP($AE17,$O$17:$X$20,2,FALSE)</f>
-        <v>Bayern de Munique</v>
+        <v>Benfica</v>
       </c>
       <c r="AG17" s="90">
         <f>VLOOKUP($AE17,$O$17:$X$20,3,FALSE)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AH17" s="90">
         <f>VLOOKUP($AE17,$O$17:$X$20,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI17" s="90">
         <f>VLOOKUP($AE17,$O$17:$X$20,5,FALSE)</f>
@@ -6041,7 +6041,7 @@
       </c>
       <c r="AJ17" s="90">
         <f>VLOOKUP($AE17,$O$17:$X$20,6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK17" s="90">
         <f>VLOOKUP($AE17,$O$17:$X$20,7,FALSE)</f>
@@ -6049,15 +6049,15 @@
       </c>
       <c r="AL17" s="90">
         <f>VLOOKUP($AE17,$O$17:$X$20,8,FALSE)</f>
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="AM17" s="90">
         <f>VLOOKUP($AE17,$O$17:$X$20,9,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AN17" s="91">
         <f>VLOOKUP($AE17,$O$17:$X$20,10,FALSE)</f>
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.25">
@@ -6115,11 +6115,11 @@
       </c>
       <c r="Q18" s="43">
         <f t="shared" ref="Q18:Q20" si="39">(S18*3)+(T18*1)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R18" s="43">
         <f t="shared" ref="R18:R20" si="40">SUM(S18:U18)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S18" s="43">
         <f>COUNTIF(J:J,P18)</f>
@@ -6127,7 +6127,7 @@
       </c>
       <c r="T18" s="43">
         <f>COUNTIF(K:K,P18)+COUNTIF(L:L,P18)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U18" s="43">
         <f>COUNTIF(M:M,P18)</f>
@@ -6135,11 +6135,11 @@
       </c>
       <c r="V18" s="43">
         <f>SUMIF(E:E,P18,F:F)+SUMIF(I:I,P18,H:H)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W18" s="43">
         <f>SUMIF(E:E,P18,H:H)+SUMIF(I:I,P18,F:F)</f>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="X18" s="43">
         <f t="shared" ref="X18:X20" si="41">V18-W18</f>
@@ -6170,31 +6170,31 @@
       </c>
       <c r="AF18" s="83" t="str">
         <f t="shared" ref="AF18:AF20" si="46">VLOOKUP($AE18,$O$17:$X$20,2,FALSE)</f>
-        <v>Benfica</v>
+        <v>Bayern de Munique</v>
       </c>
       <c r="AG18" s="90">
         <f t="shared" ref="AG18:AG20" si="47">VLOOKUP($AE18,$O$17:$X$20,3,FALSE)</f>
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="AH18" s="90">
         <f t="shared" ref="AH18:AH20" si="48">VLOOKUP($AE18,$O$17:$X$20,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI18" s="90">
         <f t="shared" ref="AI18:AI20" si="49">VLOOKUP($AE18,$O$17:$X$20,5,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ18" s="90">
         <f t="shared" ref="AJ18:AJ20" si="50">VLOOKUP($AE18,$O$17:$X$20,6,FALSE)</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AK18" s="90">
         <f t="shared" ref="AK18:AK20" si="51">VLOOKUP($AE18,$O$17:$X$20,7,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL18" s="90">
         <f t="shared" ref="AL18:AL20" si="52">VLOOKUP($AE18,$O$17:$X$20,8,FALSE)</f>
-        <v>8</v>
+        <v>12</v>
       </c>
       <c r="AM18" s="90">
         <f t="shared" ref="AM18:AM20" si="53">VLOOKUP($AE18,$O$17:$X$20,9,FALSE)</f>
@@ -6202,7 +6202,7 @@
       </c>
       <c r="AN18" s="91">
         <f t="shared" ref="AN18:AN20" si="54">VLOOKUP($AE18,$O$17:$X$20,10,FALSE)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.25">
@@ -6220,18 +6220,22 @@
         <f>P20</f>
         <v>Benfica</v>
       </c>
-      <c r="F19" s="21"/>
+      <c r="F19" s="21">
+        <v>1</v>
+      </c>
       <c r="G19" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H19" s="21"/>
+      <c r="H19" s="21">
+        <v>0</v>
+      </c>
       <c r="I19" s="13" t="str">
         <f>P17</f>
         <v>Bayern de Munique</v>
       </c>
       <c r="J19" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>empate</v>
+        <v>Benfica</v>
       </c>
       <c r="K19" s="43" t="str">
         <f t="shared" si="1"/>
@@ -6243,7 +6247,7 @@
       </c>
       <c r="M19" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>empate</v>
+        <v>Bayern de Munique</v>
       </c>
       <c r="N19" s="51"/>
       <c r="O19" s="52">
@@ -6256,11 +6260,11 @@
       </c>
       <c r="Q19" s="43">
         <f t="shared" si="39"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="R19" s="43">
         <f t="shared" si="40"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S19" s="43">
         <f>COUNTIF(J:J,P19)</f>
@@ -6268,7 +6272,7 @@
       </c>
       <c r="T19" s="43">
         <f>COUNTIF(K:K,P19)+COUNTIF(L:L,P19)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U19" s="43">
         <f>COUNTIF(M:M,P19)</f>
@@ -6276,11 +6280,11 @@
       </c>
       <c r="V19" s="43">
         <f>SUMIF(E:E,P19,F:F)+SUMIF(I:I,P19,H:H)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="W19" s="43">
         <f>SUMIF(E:E,P19,H:H)+SUMIF(I:I,P19,F:F)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="X19" s="43">
         <f t="shared" si="41"/>
@@ -6315,11 +6319,11 @@
       </c>
       <c r="AG19" s="90">
         <f t="shared" si="47"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AH19" s="90">
         <f t="shared" si="48"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI19" s="90">
         <f t="shared" si="49"/>
@@ -6327,7 +6331,7 @@
       </c>
       <c r="AJ19" s="90">
         <f t="shared" si="50"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK19" s="90">
         <f t="shared" si="51"/>
@@ -6335,11 +6339,11 @@
       </c>
       <c r="AL19" s="90">
         <f t="shared" si="52"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AM19" s="90">
         <f t="shared" si="53"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AN19" s="91">
         <f t="shared" si="54"/>
@@ -6361,11 +6365,15 @@
         <f>P18</f>
         <v>Auckland City</v>
       </c>
-      <c r="F20" s="22"/>
+      <c r="F20" s="22">
+        <v>1</v>
+      </c>
       <c r="G20" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="H20" s="22"/>
+      <c r="H20" s="22">
+        <v>1</v>
+      </c>
       <c r="I20" s="17" t="str">
         <f>P19</f>
         <v>Boca Juniors</v>
@@ -6376,11 +6384,11 @@
       </c>
       <c r="K20" s="57" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Auckland City</v>
       </c>
       <c r="L20" s="57" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>Boca Juniors</v>
       </c>
       <c r="M20" s="58" t="str">
         <f t="shared" si="3"/>
@@ -6389,7 +6397,7 @@
       <c r="N20" s="59"/>
       <c r="O20" s="60">
         <f t="shared" si="38"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P20" s="53" t="str">
         <f>Sorteios!I9</f>
@@ -6397,15 +6405,15 @@
       </c>
       <c r="Q20" s="57">
         <f t="shared" si="39"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="R20" s="57">
         <f t="shared" si="40"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S20" s="43">
         <f>COUNTIF(J:J,P20)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T20" s="43">
         <f>COUNTIF(K:K,P20)+COUNTIF(L:L,P20)</f>
@@ -6417,7 +6425,7 @@
       </c>
       <c r="V20" s="57">
         <f>SUMIF(E:E,P20,F:F)+SUMIF(I:I,P20,H:H)</f>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="W20" s="57">
         <f>SUMIF(E:E,P20,H:H)+SUMIF(I:I,P20,F:F)</f>
@@ -6425,7 +6433,7 @@
       </c>
       <c r="X20" s="57">
         <f t="shared" si="41"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="Y20" s="57">
         <f t="shared" si="42"/>
@@ -6456,11 +6464,11 @@
       </c>
       <c r="AG20" s="92">
         <f t="shared" si="47"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH20" s="92">
         <f t="shared" si="48"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI20" s="92">
         <f t="shared" si="49"/>
@@ -6468,7 +6476,7 @@
       </c>
       <c r="AJ20" s="92">
         <f t="shared" si="50"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK20" s="92">
         <f t="shared" si="51"/>
@@ -6476,11 +6484,11 @@
       </c>
       <c r="AL20" s="92">
         <f t="shared" si="52"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM20" s="92">
         <f t="shared" si="53"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AN20" s="93">
         <f t="shared" si="54"/>
@@ -10503,18 +10511,18 @@
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="109"/>
-      <c r="B4" s="180" t="s">
+      <c r="B4" s="179" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="181"/>
-      <c r="D4" s="181"/>
-      <c r="E4" s="181"/>
-      <c r="F4" s="181"/>
-      <c r="G4" s="181"/>
-      <c r="H4" s="181"/>
-      <c r="I4" s="181"/>
-      <c r="J4" s="181"/>
-      <c r="K4" s="182"/>
+      <c r="C4" s="180"/>
+      <c r="D4" s="180"/>
+      <c r="E4" s="180"/>
+      <c r="F4" s="180"/>
+      <c r="G4" s="180"/>
+      <c r="H4" s="180"/>
+      <c r="I4" s="180"/>
+      <c r="J4" s="180"/>
+      <c r="K4" s="181"/>
       <c r="L4" s="110"/>
       <c r="M4" s="111"/>
       <c r="N4" s="111"/>
@@ -10531,19 +10539,19 @@
       <c r="D5" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="183" t="s">
+      <c r="E5" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="183"/>
-      <c r="G5" s="183" t="s">
+      <c r="F5" s="182"/>
+      <c r="G5" s="182" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="183"/>
-      <c r="I5" s="183"/>
-      <c r="J5" s="183" t="s">
+      <c r="H5" s="182"/>
+      <c r="I5" s="182"/>
+      <c r="J5" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="184"/>
+      <c r="K5" s="183"/>
       <c r="L5" s="113"/>
       <c r="M5" s="113"/>
       <c r="N5" s="113"/>
@@ -10597,7 +10605,7 @@
       </c>
       <c r="E7" s="11" t="str">
         <f>IF('Fase de Grupos'!AH17=3,'Fase de Grupos'!AF17,"1º do Grupo C")</f>
-        <v>1º do Grupo C</v>
+        <v>Benfica</v>
       </c>
       <c r="F7" s="121"/>
       <c r="G7" s="21"/>
@@ -10676,7 +10684,7 @@
       <c r="J9" s="122"/>
       <c r="K9" s="138" t="str">
         <f>IF('Fase de Grupos'!AH18=3,'Fase de Grupos'!AF18,"2º do Grupo C")</f>
-        <v>2º do Grupo C</v>
+        <v>Bayern de Munique</v>
       </c>
       <c r="L9" s="114" t="str">
         <f t="shared" si="0"/>
@@ -10831,18 +10839,18 @@
     </row>
     <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="109"/>
-      <c r="B16" s="180" t="s">
+      <c r="B16" s="179" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="181"/>
-      <c r="D16" s="181"/>
-      <c r="E16" s="181"/>
-      <c r="F16" s="181"/>
-      <c r="G16" s="181"/>
-      <c r="H16" s="181"/>
-      <c r="I16" s="181"/>
-      <c r="J16" s="181"/>
-      <c r="K16" s="182"/>
+      <c r="C16" s="180"/>
+      <c r="D16" s="180"/>
+      <c r="E16" s="180"/>
+      <c r="F16" s="180"/>
+      <c r="G16" s="180"/>
+      <c r="H16" s="180"/>
+      <c r="I16" s="180"/>
+      <c r="J16" s="180"/>
+      <c r="K16" s="181"/>
       <c r="L16" s="110"/>
       <c r="M16" s="111"/>
       <c r="N16" s="111"/>
@@ -10855,19 +10863,19 @@
       <c r="D17" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="183" t="s">
+      <c r="E17" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="183"/>
-      <c r="G17" s="183" t="s">
+      <c r="F17" s="182"/>
+      <c r="G17" s="182" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="183"/>
-      <c r="I17" s="183"/>
-      <c r="J17" s="183" t="s">
+      <c r="H17" s="182"/>
+      <c r="I17" s="182"/>
+      <c r="J17" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="K17" s="184"/>
+      <c r="K17" s="183"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B18" s="129" t="s">
@@ -11013,18 +11021,18 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="109"/>
-      <c r="B24" s="180" t="s">
+      <c r="B24" s="179" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="181"/>
-      <c r="D24" s="181"/>
-      <c r="E24" s="181"/>
-      <c r="F24" s="181"/>
-      <c r="G24" s="181"/>
-      <c r="H24" s="181"/>
-      <c r="I24" s="181"/>
-      <c r="J24" s="181"/>
-      <c r="K24" s="182"/>
+      <c r="C24" s="180"/>
+      <c r="D24" s="180"/>
+      <c r="E24" s="180"/>
+      <c r="F24" s="180"/>
+      <c r="G24" s="180"/>
+      <c r="H24" s="180"/>
+      <c r="I24" s="180"/>
+      <c r="J24" s="180"/>
+      <c r="K24" s="181"/>
       <c r="L24" s="110"/>
       <c r="M24" s="111"/>
       <c r="N24" s="111"/>
@@ -11040,19 +11048,19 @@
       <c r="D25" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="183" t="s">
+      <c r="E25" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="183"/>
-      <c r="G25" s="183" t="s">
+      <c r="F25" s="182"/>
+      <c r="G25" s="182" t="s">
         <v>13</v>
       </c>
-      <c r="H25" s="183"/>
-      <c r="I25" s="183"/>
-      <c r="J25" s="183" t="s">
+      <c r="H25" s="182"/>
+      <c r="I25" s="182"/>
+      <c r="J25" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="K25" s="184"/>
+      <c r="K25" s="183"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="151" t="s">
@@ -11141,18 +11149,18 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="109"/>
-      <c r="B31" s="180" t="s">
+      <c r="B31" s="179" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="181"/>
-      <c r="D31" s="181"/>
-      <c r="E31" s="181"/>
-      <c r="F31" s="181"/>
-      <c r="G31" s="181"/>
-      <c r="H31" s="181"/>
-      <c r="I31" s="181"/>
-      <c r="J31" s="181"/>
-      <c r="K31" s="182"/>
+      <c r="C31" s="180"/>
+      <c r="D31" s="180"/>
+      <c r="E31" s="180"/>
+      <c r="F31" s="180"/>
+      <c r="G31" s="180"/>
+      <c r="H31" s="180"/>
+      <c r="I31" s="180"/>
+      <c r="J31" s="180"/>
+      <c r="K31" s="181"/>
       <c r="L31" s="110"/>
       <c r="M31" s="111"/>
       <c r="N31" s="111"/>
@@ -11168,19 +11176,19 @@
       <c r="D32" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="183" t="s">
+      <c r="E32" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="183"/>
-      <c r="G32" s="183" t="s">
+      <c r="F32" s="182"/>
+      <c r="G32" s="182" t="s">
         <v>13</v>
       </c>
-      <c r="H32" s="183"/>
-      <c r="I32" s="183"/>
-      <c r="J32" s="183" t="s">
+      <c r="H32" s="182"/>
+      <c r="I32" s="182"/>
+      <c r="J32" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="K32" s="184"/>
+      <c r="K32" s="183"/>
     </row>
     <row r="33" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="161" t="s">
@@ -11228,11 +11236,11 @@
     </row>
     <row r="36" spans="1:17" s="137" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="135"/>
-      <c r="B36" s="179" t="s">
+      <c r="B36" s="184" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="179"/>
-      <c r="D36" s="179"/>
+      <c r="C36" s="184"/>
+      <c r="D36" s="184"/>
       <c r="E36" s="173" t="str">
         <f>IF(M33="1º Lugar","",M33)</f>
         <v/>
@@ -11252,11 +11260,11 @@
     </row>
     <row r="37" spans="1:17" s="137" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="135"/>
-      <c r="B37" s="179" t="s">
+      <c r="B37" s="184" t="s">
         <v>106</v>
       </c>
-      <c r="C37" s="179"/>
-      <c r="D37" s="179"/>
+      <c r="C37" s="184"/>
+      <c r="D37" s="184"/>
       <c r="E37" s="175" t="str">
         <f>IF(M34="2º Lugar","",M34)</f>
         <v/>
@@ -11384,11 +11392,12 @@
   </sheetData>
   <sheetProtection password="CC01" sheet="1" selectLockedCells="1"/>
   <mergeCells count="18">
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="B16:K16"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B31:K31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="B36:D36"/>
     <mergeCell ref="B24:K24"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="G25:I25"/>
@@ -11396,12 +11405,11 @@
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B31:K31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="B16:K16"/>
   </mergeCells>
   <conditionalFormatting sqref="F6">
     <cfRule type="expression" dxfId="31" priority="128">
@@ -11568,6 +11576,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DBF2846C41E31A469E3CED25F2422E48" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0c08e4af4d80db6585ac36ba965bb3a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2c8c20e6-817c-474f-b9c2-eb2b1ac24837" xmlns:ns4="dc8c2798-6aba-4af7-93a4-b89253b03650" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4e7db2db65f9cb533b4933096bc9b657" ns3:_="" ns4:_="">
     <xsd:import namespace="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
@@ -11800,14 +11816,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -11818,6 +11826,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83E7837-68AD-48B2-A1AB-AAB452317AF5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
+    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFBCCD5-5BDE-495C-BFE9-46A98A6BC529}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11836,23 +11861,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83E7837-68AD-48B2-A1AB-AAB452317AF5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A45D7D45-1E18-48AE-827B-096C3C02C976}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Att até Jogo 42
</commit_message>
<xml_diff>
--- a/Mundial de Clubes FIFA 2025.xlsx
+++ b/Mundial de Clubes FIFA 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjunior\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9F8C17AC-39E8-407F-B1BC-0C405CA1B6A0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1743B171-F3DD-4BED-A60D-DF4AB53588B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="1185" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{076F3B28-812E-4458-A424-96085A053123}"/>
   </bookViews>
@@ -4018,8 +4018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45896CCF-F333-49AF-850B-159476231F1C}">
   <dimension ref="A1:AN50"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6748,11 +6748,11 @@
       </c>
       <c r="Q23" s="43">
         <f>(S23*3)+(T23*1)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="R23" s="43">
         <f>SUM(S23:U23)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S23" s="43">
         <f>COUNTIF(J:J,P23)</f>
@@ -6760,7 +6760,7 @@
       </c>
       <c r="T23" s="43">
         <f>COUNTIF(K:K,P23)+COUNTIF(L:L,P23)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U23" s="43">
         <f>COUNTIF(M:M,P23)</f>
@@ -6768,11 +6768,11 @@
       </c>
       <c r="V23" s="43">
         <f>SUMIF(E:E,P23,F:F)+SUMIF(I:I,P23,H:H)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="W23" s="43">
         <f>SUMIF(E:E,P23,H:H)+SUMIF(I:I,P23,F:F)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="X23" s="43">
         <f>V23-W23</f>
@@ -6807,11 +6807,11 @@
       </c>
       <c r="AG23" s="90">
         <f>VLOOKUP($AE23,$O$23:$X$26,3,FALSE)</f>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="AH23" s="90">
         <f>VLOOKUP($AE23,$O$23:$X$26,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI23" s="90">
         <f>VLOOKUP($AE23,$O$23:$X$26,5,FALSE)</f>
@@ -6819,7 +6819,7 @@
       </c>
       <c r="AJ23" s="90">
         <f>VLOOKUP($AE23,$O$23:$X$26,6,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK23" s="90">
         <f>VLOOKUP($AE23,$O$23:$X$26,7,FALSE)</f>
@@ -6827,11 +6827,11 @@
       </c>
       <c r="AL23" s="90">
         <f>VLOOKUP($AE23,$O$23:$X$26,8,FALSE)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AM23" s="90">
         <f>VLOOKUP($AE23,$O$23:$X$26,9,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AN23" s="91">
         <f>VLOOKUP($AE23,$O$23:$X$26,10,FALSE)</f>
@@ -6897,7 +6897,7 @@
       </c>
       <c r="R24" s="43">
         <f t="shared" ref="R24:R26" si="57">SUM(S24:U24)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S24" s="43">
         <f>COUNTIF(J:J,P24)</f>
@@ -6909,7 +6909,7 @@
       </c>
       <c r="U24" s="43">
         <f>COUNTIF(M:M,P24)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="V24" s="43">
         <f>SUMIF(E:E,P24,F:F)+SUMIF(I:I,P24,H:H)</f>
@@ -6917,15 +6917,15 @@
       </c>
       <c r="W24" s="43">
         <f>SUMIF(E:E,P24,H:H)+SUMIF(I:I,P24,F:F)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="X24" s="43">
         <f t="shared" ref="X24:X26" si="58">V24-W24</f>
-        <v>-1</v>
+        <v>-4</v>
       </c>
       <c r="Y24" s="43">
         <f t="shared" ref="Y24:Y26" si="59">SUMPRODUCT(($Q$23:$Q$26=Q24)*($X$23:$X$26&gt;X24))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z24" s="43">
         <f t="shared" ref="Z24:Z26" si="60">SUMPRODUCT(($Q$23:$Q$26=Q24)*($X$23:$X$26=X24)*($V$23:$V$26&gt;V24))</f>
@@ -6952,15 +6952,15 @@
       </c>
       <c r="AG24" s="90">
         <f t="shared" ref="AG24:AG26" si="64">VLOOKUP($AE24,$O$23:$X$26,3,FALSE)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AH24" s="90">
         <f t="shared" ref="AH24:AH26" si="65">VLOOKUP($AE24,$O$23:$X$26,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI24" s="90">
         <f t="shared" ref="AI24:AI26" si="66">VLOOKUP($AE24,$O$23:$X$26,5,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ24" s="90">
         <f t="shared" ref="AJ24:AJ26" si="67">VLOOKUP($AE24,$O$23:$X$26,6,FALSE)</f>
@@ -6972,7 +6972,7 @@
       </c>
       <c r="AL24" s="90">
         <f t="shared" ref="AL24:AL26" si="69">VLOOKUP($AE24,$O$23:$X$26,8,FALSE)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="AM24" s="90">
         <f t="shared" ref="AM24:AM26" si="70">VLOOKUP($AE24,$O$23:$X$26,9,FALSE)</f>
@@ -6980,7 +6980,7 @@
       </c>
       <c r="AN24" s="91">
         <f t="shared" ref="AN24:AN26" si="71">VLOOKUP($AE24,$O$23:$X$26,10,FALSE)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.25">
@@ -6998,11 +6998,15 @@
         <f>P26</f>
         <v>Los Angeles FC</v>
       </c>
-      <c r="F25" s="21"/>
+      <c r="F25" s="21">
+        <v>1</v>
+      </c>
       <c r="G25" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="H25" s="21"/>
+      <c r="H25" s="21">
+        <v>1</v>
+      </c>
       <c r="I25" s="26" t="str">
         <f>P23</f>
         <v>Flamengo</v>
@@ -7013,11 +7017,11 @@
       </c>
       <c r="K25" s="43" t="str">
         <f t="shared" si="1"/>
-        <v/>
+        <v>Los Angeles FC</v>
       </c>
       <c r="L25" s="43" t="str">
         <f t="shared" si="2"/>
-        <v/>
+        <v>Flamengo</v>
       </c>
       <c r="M25" s="44" t="str">
         <f t="shared" si="3"/>
@@ -7034,15 +7038,15 @@
       </c>
       <c r="Q25" s="43">
         <f t="shared" si="56"/>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="R25" s="43">
         <f t="shared" si="57"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S25" s="43">
         <f>COUNTIF(J:J,P25)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T25" s="43">
         <f>COUNTIF(K:K,P25)+COUNTIF(L:L,P25)</f>
@@ -7054,7 +7058,7 @@
       </c>
       <c r="V25" s="43">
         <f>SUMIF(E:E,P25,F:F)+SUMIF(I:I,P25,H:H)</f>
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="W25" s="43">
         <f>SUMIF(E:E,P25,H:H)+SUMIF(I:I,P25,F:F)</f>
@@ -7062,7 +7066,7 @@
       </c>
       <c r="X25" s="43">
         <f t="shared" si="58"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="Y25" s="43">
         <f t="shared" si="59"/>
@@ -7097,7 +7101,7 @@
       </c>
       <c r="AH25" s="90">
         <f t="shared" si="65"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI25" s="90">
         <f t="shared" si="66"/>
@@ -7109,7 +7113,7 @@
       </c>
       <c r="AK25" s="90">
         <f t="shared" si="68"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AL25" s="90">
         <f t="shared" si="69"/>
@@ -7117,11 +7121,11 @@
       </c>
       <c r="AM25" s="90">
         <f t="shared" si="70"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="AN25" s="91">
         <f t="shared" si="71"/>
-        <v>-1</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="26" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -7139,18 +7143,22 @@
         <f>P24</f>
         <v>Espérance de Tunis</v>
       </c>
-      <c r="F26" s="22"/>
+      <c r="F26" s="22">
+        <v>0</v>
+      </c>
       <c r="G26" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="H26" s="22"/>
+      <c r="H26" s="22">
+        <v>3</v>
+      </c>
       <c r="I26" s="27" t="str">
         <f>P25</f>
         <v>Chelsea</v>
       </c>
       <c r="J26" s="56" t="str">
         <f t="shared" si="0"/>
-        <v>empate</v>
+        <v>Chelsea</v>
       </c>
       <c r="K26" s="57" t="str">
         <f t="shared" si="1"/>
@@ -7162,7 +7170,7 @@
       </c>
       <c r="M26" s="58" t="str">
         <f t="shared" si="3"/>
-        <v>empate</v>
+        <v>Espérance de Tunis</v>
       </c>
       <c r="N26" s="61"/>
       <c r="O26" s="60">
@@ -7175,11 +7183,11 @@
       </c>
       <c r="Q26" s="57">
         <f t="shared" si="56"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="R26" s="57">
         <f t="shared" si="57"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S26" s="43">
         <f>COUNTIF(J:J,P26)</f>
@@ -7187,7 +7195,7 @@
       </c>
       <c r="T26" s="43">
         <f>COUNTIF(K:K,P26)+COUNTIF(L:L,P26)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U26" s="43">
         <f>COUNTIF(M:M,P26)</f>
@@ -7195,11 +7203,11 @@
       </c>
       <c r="V26" s="57">
         <f>SUMIF(E:E,P26,F:F)+SUMIF(I:I,P26,H:H)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="W26" s="57">
         <f>SUMIF(E:E,P26,H:H)+SUMIF(I:I,P26,F:F)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="X26" s="57">
         <f t="shared" si="58"/>
@@ -7234,11 +7242,11 @@
       </c>
       <c r="AG26" s="92">
         <f t="shared" si="64"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AH26" s="92">
         <f t="shared" si="65"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI26" s="92">
         <f t="shared" si="66"/>
@@ -7246,7 +7254,7 @@
       </c>
       <c r="AJ26" s="92">
         <f t="shared" si="67"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK26" s="92">
         <f t="shared" si="68"/>
@@ -7254,11 +7262,11 @@
       </c>
       <c r="AL26" s="92">
         <f t="shared" si="69"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AM26" s="92">
         <f t="shared" si="70"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AN26" s="93">
         <f t="shared" si="71"/>
@@ -8280,7 +8288,7 @@
       <c r="N35" s="50"/>
       <c r="O35" s="52">
         <f>RANK(Q35,$Q$35:$Q$38)+SUM(Y35:AB35)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P35" s="53" t="str">
         <f>Sorteios!F14</f>
@@ -8288,11 +8296,11 @@
       </c>
       <c r="Q35" s="43">
         <f>(S35*3)+(T35*1)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="R35" s="43">
         <f>SUM(S35:U35)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S35" s="43">
         <f>COUNTIF(J:J,P35)</f>
@@ -8300,7 +8308,7 @@
       </c>
       <c r="T35" s="43">
         <f>COUNTIF(K:K,P35)+COUNTIF(L:L,P35)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="U35" s="43">
         <f>COUNTIF(M:M,P35)</f>
@@ -8343,19 +8351,19 @@
       </c>
       <c r="AF35" s="83" t="str">
         <f>VLOOKUP($AE35,$O$35:$X$38,2,FALSE)</f>
-        <v>Fluminense</v>
+        <v>Borussia Dortmund</v>
       </c>
       <c r="AG35" s="90">
         <f>VLOOKUP($AE35,$O$35:$X$38,3,FALSE)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AH35" s="90">
         <f>VLOOKUP($AE35,$O$35:$X$38,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI35" s="90">
         <f>VLOOKUP($AE35,$O$35:$X$38,5,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ35" s="90">
         <f>VLOOKUP($AE35,$O$35:$X$38,6,FALSE)</f>
@@ -8367,11 +8375,11 @@
       </c>
       <c r="AL35" s="90">
         <f>VLOOKUP($AE35,$O$35:$X$38,8,FALSE)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AM35" s="90">
         <f>VLOOKUP($AE35,$O$35:$X$38,9,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AN35" s="91">
         <f>VLOOKUP($AE35,$O$35:$X$38,10,FALSE)</f>
@@ -8425,7 +8433,7 @@
       <c r="N36" s="50"/>
       <c r="O36" s="52">
         <f t="shared" ref="O36:O38" si="93">RANK(Q36,$Q$35:$Q$38)+SUM(Y36:AB36)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P36" s="53" t="str">
         <f>Sorteios!F15</f>
@@ -8433,15 +8441,15 @@
       </c>
       <c r="Q36" s="43">
         <f t="shared" ref="Q36:Q38" si="94">(S36*3)+(T36*1)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="R36" s="43">
         <f t="shared" ref="R36:R38" si="95">SUM(S36:U36)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S36" s="43">
         <f>COUNTIF(J:J,P36)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T36" s="43">
         <f>COUNTIF(K:K,P36)+COUNTIF(L:L,P36)</f>
@@ -8453,7 +8461,7 @@
       </c>
       <c r="V36" s="43">
         <f>SUMIF(E:E,P36,F:F)+SUMIF(I:I,P36,H:H)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="W36" s="43">
         <f>SUMIF(E:E,P36,H:H)+SUMIF(I:I,P36,F:F)</f>
@@ -8461,11 +8469,11 @@
       </c>
       <c r="X36" s="43">
         <f t="shared" ref="X36:X38" si="96">V36-W36</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="Y36" s="43">
         <f t="shared" ref="Y36:Y38" si="97">SUMPRODUCT(($Q$35:$Q$38=Q36)*($X$35:$X$38&gt;X36))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z36" s="43">
         <f t="shared" ref="Z36:Z38" si="98">SUMPRODUCT(($Q$35:$Q$38=Q36)*($X$35:$X$38=X36)*($V$35:$V$38&gt;V36))</f>
@@ -8488,15 +8496,15 @@
       </c>
       <c r="AF36" s="83" t="str">
         <f t="shared" ref="AF36:AF38" si="101">VLOOKUP($AE36,$O$35:$X$38,2,FALSE)</f>
-        <v>Borussia Dortmund</v>
+        <v>Fluminense</v>
       </c>
       <c r="AG36" s="90">
         <f t="shared" ref="AG36:AG38" si="102">VLOOKUP($AE36,$O$35:$X$38,3,FALSE)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH36" s="90">
         <f t="shared" ref="AH36:AH38" si="103">VLOOKUP($AE36,$O$35:$X$38,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI36" s="90">
         <f t="shared" ref="AI36:AI38" si="104">VLOOKUP($AE36,$O$35:$X$38,5,FALSE)</f>
@@ -8504,7 +8512,7 @@
       </c>
       <c r="AJ36" s="90">
         <f t="shared" ref="AJ36:AJ38" si="105">VLOOKUP($AE36,$O$35:$X$38,6,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK36" s="90">
         <f t="shared" ref="AK36:AK38" si="106">VLOOKUP($AE36,$O$35:$X$38,7,FALSE)</f>
@@ -8516,11 +8524,11 @@
       </c>
       <c r="AM36" s="90">
         <f t="shared" ref="AM36:AM38" si="108">VLOOKUP($AE36,$O$35:$X$38,9,FALSE)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="AN36" s="91">
         <f t="shared" ref="AN36:AN38" si="109">VLOOKUP($AE36,$O$35:$X$38,10,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="37" spans="1:40" x14ac:dyDescent="0.25">
@@ -8538,11 +8546,15 @@
         <f>P38</f>
         <v>Mamelodi Sundowns</v>
       </c>
-      <c r="F37" s="21"/>
+      <c r="F37" s="21">
+        <v>0</v>
+      </c>
       <c r="G37" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="H37" s="21"/>
+      <c r="H37" s="21">
+        <v>0</v>
+      </c>
       <c r="I37" s="26" t="str">
         <f>P35</f>
         <v>Fluminense</v>
@@ -8553,11 +8565,11 @@
       </c>
       <c r="K37" s="43" t="str">
         <f t="shared" si="90"/>
-        <v/>
+        <v>Mamelodi Sundowns</v>
       </c>
       <c r="L37" s="43" t="str">
         <f t="shared" si="91"/>
-        <v/>
+        <v>Fluminense</v>
       </c>
       <c r="M37" s="44" t="str">
         <f t="shared" si="92"/>
@@ -8578,7 +8590,7 @@
       </c>
       <c r="R37" s="43">
         <f t="shared" si="95"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S37" s="43">
         <f>COUNTIF(J:J,P37)</f>
@@ -8590,7 +8602,7 @@
       </c>
       <c r="U37" s="43">
         <f>COUNTIF(M:M,P37)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V37" s="43">
         <f>SUMIF(E:E,P37,F:F)+SUMIF(I:I,P37,H:H)</f>
@@ -8598,11 +8610,11 @@
       </c>
       <c r="W37" s="43">
         <f>SUMIF(E:E,P37,H:H)+SUMIF(I:I,P37,F:F)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="X37" s="43">
         <f t="shared" si="96"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
       <c r="Y37" s="43">
         <f t="shared" si="97"/>
@@ -8633,11 +8645,11 @@
       </c>
       <c r="AG37" s="90">
         <f t="shared" si="102"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="AH37" s="90">
         <f t="shared" si="103"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI37" s="90">
         <f t="shared" si="104"/>
@@ -8645,7 +8657,7 @@
       </c>
       <c r="AJ37" s="90">
         <f t="shared" si="105"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AK37" s="90">
         <f t="shared" si="106"/>
@@ -8679,18 +8691,22 @@
         <f>P36</f>
         <v>Borussia Dortmund</v>
       </c>
-      <c r="F38" s="22"/>
+      <c r="F38" s="22">
+        <v>1</v>
+      </c>
       <c r="G38" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="H38" s="22"/>
+      <c r="H38" s="22">
+        <v>0</v>
+      </c>
       <c r="I38" s="27" t="str">
         <f>P37</f>
         <v>Ulsan</v>
       </c>
       <c r="J38" s="56" t="str">
         <f t="shared" si="89"/>
-        <v>empate</v>
+        <v>Borussia Dortmund</v>
       </c>
       <c r="K38" s="57" t="str">
         <f t="shared" si="90"/>
@@ -8702,7 +8718,7 @@
       </c>
       <c r="M38" s="58" t="str">
         <f t="shared" si="92"/>
-        <v>empate</v>
+        <v>Ulsan</v>
       </c>
       <c r="N38" s="61"/>
       <c r="O38" s="60">
@@ -8715,11 +8731,11 @@
       </c>
       <c r="Q38" s="57">
         <f t="shared" si="94"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="R38" s="57">
         <f t="shared" si="95"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S38" s="43">
         <f>COUNTIF(J:J,P38)</f>
@@ -8727,7 +8743,7 @@
       </c>
       <c r="T38" s="43">
         <f>COUNTIF(K:K,P38)+COUNTIF(L:L,P38)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="U38" s="43">
         <f>COUNTIF(M:M,P38)</f>
@@ -8778,7 +8794,7 @@
       </c>
       <c r="AH38" s="92">
         <f t="shared" si="103"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI38" s="92">
         <f t="shared" si="104"/>
@@ -8790,7 +8806,7 @@
       </c>
       <c r="AK38" s="92">
         <f t="shared" si="106"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL38" s="92">
         <f t="shared" si="107"/>
@@ -8798,11 +8814,11 @@
       </c>
       <c r="AM38" s="92">
         <f t="shared" si="108"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AN38" s="93">
         <f t="shared" si="109"/>
-        <v>-3</v>
+        <v>-4</v>
       </c>
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.25">
@@ -9299,7 +9315,7 @@
         <v>55</v>
       </c>
       <c r="C43" s="80">
-        <v>45836</v>
+        <v>45834</v>
       </c>
       <c r="D43" s="40" t="s">
         <v>41</v>
@@ -9440,7 +9456,7 @@
         <v>55</v>
       </c>
       <c r="C44" s="81">
-        <v>45836</v>
+        <v>45834</v>
       </c>
       <c r="D44" s="54" t="s">
         <v>41</v>
@@ -10069,7 +10085,7 @@
         <v>57</v>
       </c>
       <c r="C49" s="10">
-        <v>45833</v>
+        <v>45834</v>
       </c>
       <c r="D49" s="41" t="s">
         <v>42</v>
@@ -10210,7 +10226,7 @@
         <v>57</v>
       </c>
       <c r="C50" s="14">
-        <v>45833</v>
+        <v>45834</v>
       </c>
       <c r="D50" s="55" t="s">
         <v>42</v>
@@ -10616,7 +10632,7 @@
       <c r="J7" s="122"/>
       <c r="K7" s="138" t="str">
         <f>IF('Fase de Grupos'!AH24=3,'Fase de Grupos'!AF24,"2º do Grupo D")</f>
-        <v>2º do Grupo D</v>
+        <v>Chelsea</v>
       </c>
       <c r="L7" s="114" t="str">
         <f t="shared" ref="L7:L13" si="0">IF(OR(G7="",I7=""),"",IF(G7=I7,"emp",""))</f>
@@ -10673,7 +10689,7 @@
       </c>
       <c r="E9" s="11" t="str">
         <f>IF('Fase de Grupos'!AH23=3,'Fase de Grupos'!AF23,"1º do Grupo D")</f>
-        <v>1º do Grupo D</v>
+        <v>Flamengo</v>
       </c>
       <c r="F9" s="121"/>
       <c r="G9" s="21"/>
@@ -10718,7 +10734,7 @@
       <c r="J10" s="122"/>
       <c r="K10" s="138" t="str">
         <f>IF('Fase de Grupos'!AH36=3,'Fase de Grupos'!AF36,"2º do Grupo F")</f>
-        <v>2º do Grupo F</v>
+        <v>Fluminense</v>
       </c>
       <c r="L10" s="114" t="str">
         <f t="shared" si="0"/>
@@ -10775,7 +10791,7 @@
       </c>
       <c r="E12" s="11" t="str">
         <f>IF('Fase de Grupos'!AH35=3,'Fase de Grupos'!AF35,"1º do Grupo F")</f>
-        <v>1º do Grupo F</v>
+        <v>Borussia Dortmund</v>
       </c>
       <c r="F12" s="121"/>
       <c r="G12" s="21"/>
@@ -11576,14 +11592,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DBF2846C41E31A469E3CED25F2422E48" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0c08e4af4d80db6585ac36ba965bb3a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2c8c20e6-817c-474f-b9c2-eb2b1ac24837" xmlns:ns4="dc8c2798-6aba-4af7-93a4-b89253b03650" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4e7db2db65f9cb533b4933096bc9b657" ns3:_="" ns4:_="">
     <xsd:import namespace="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
@@ -11816,7 +11824,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -11825,24 +11833,15 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83E7837-68AD-48B2-A1AB-AAB452317AF5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
-    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFBCCD5-5BDE-495C-BFE9-46A98A6BC529}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11861,10 +11860,27 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A45D7D45-1E18-48AE-827B-096C3C02C976}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83E7837-68AD-48B2-A1AB-AAB452317AF5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
+    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Att até Jogo 44
</commit_message>
<xml_diff>
--- a/Mundial de Clubes FIFA 2025.xlsx
+++ b/Mundial de Clubes FIFA 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjunior\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1743B171-F3DD-4BED-A60D-DF4AB53588B7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFEF0FA7-3635-4A44-86F7-8028F6F9421E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="1185" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{076F3B28-812E-4458-A424-96085A053123}"/>
   </bookViews>
@@ -1598,6 +1598,9 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1612,9 +1615,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4019,7 +4019,7 @@
   <dimension ref="A1:AN50"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31"/>
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -7518,7 +7518,7 @@
       <c r="N29" s="51"/>
       <c r="O29" s="52">
         <f>RANK(Q29,$Q$29:$Q$32)+SUM(Y29:AB29)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="P29" s="53" t="str">
         <f>Sorteios!C14</f>
@@ -7530,7 +7530,7 @@
       </c>
       <c r="R29" s="43">
         <f>SUM(S29:U29)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S29" s="43">
         <f>COUNTIF(J:J,P29)</f>
@@ -7542,7 +7542,7 @@
       </c>
       <c r="U29" s="43">
         <f>COUNTIF(M:M,P29)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V29" s="43">
         <f>SUMIF(E:E,P29,F:F)+SUMIF(I:I,P29,H:H)</f>
@@ -7550,11 +7550,11 @@
       </c>
       <c r="W29" s="43">
         <f>SUMIF(E:E,P29,H:H)+SUMIF(I:I,P29,F:F)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="X29" s="43">
         <f>V29-W29</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="Y29" s="43">
         <f>SUMPRODUCT(($Q$29:$Q$32=Q29)*($X$29:$X$32&gt;X29))</f>
@@ -7581,19 +7581,19 @@
       </c>
       <c r="AF29" s="83" t="str">
         <f>VLOOKUP($AE29,$O$29:$X$32,2,FALSE)</f>
-        <v>River Plate</v>
+        <v>Internazionale</v>
       </c>
       <c r="AG29" s="90">
         <f>VLOOKUP($AE29,$O$29:$X$32,3,FALSE)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AH29" s="90">
         <f>VLOOKUP($AE29,$O$29:$X$32,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI29" s="90">
         <f>VLOOKUP($AE29,$O$29:$X$32,5,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ29" s="90">
         <f>VLOOKUP($AE29,$O$29:$X$32,6,FALSE)</f>
@@ -7605,15 +7605,15 @@
       </c>
       <c r="AL29" s="90">
         <f>VLOOKUP($AE29,$O$29:$X$32,8,FALSE)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AM29" s="90">
         <f>VLOOKUP($AE29,$O$29:$X$32,9,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AN29" s="91">
         <f>VLOOKUP($AE29,$O$29:$X$32,10,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="30" spans="1:40" x14ac:dyDescent="0.25">
@@ -7675,7 +7675,7 @@
       </c>
       <c r="R30" s="43">
         <f t="shared" ref="R30:R32" si="74">SUM(S30:U30)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S30" s="43">
         <f>COUNTIF(J:J,P30)</f>
@@ -7687,7 +7687,7 @@
       </c>
       <c r="U30" s="43">
         <f>COUNTIF(M:M,P30)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V30" s="43">
         <f>SUMIF(E:E,P30,F:F)+SUMIF(I:I,P30,H:H)</f>
@@ -7695,11 +7695,11 @@
       </c>
       <c r="W30" s="43">
         <f>SUMIF(E:E,P30,H:H)+SUMIF(I:I,P30,F:F)</f>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="X30" s="43">
         <f t="shared" ref="X30:X32" si="75">V30-W30</f>
-        <v>-3</v>
+        <v>-7</v>
       </c>
       <c r="Y30" s="43">
         <f t="shared" ref="Y30:Y32" si="76">SUMPRODUCT(($Q$29:$Q$32=Q30)*($X$29:$X$32&gt;X30))</f>
@@ -7726,15 +7726,15 @@
       </c>
       <c r="AF30" s="83" t="str">
         <f t="shared" ref="AF30:AF32" si="80">VLOOKUP($AE30,$O$29:$X$32,2,FALSE)</f>
-        <v>Internazionale</v>
+        <v>Monterrey</v>
       </c>
       <c r="AG30" s="90">
         <f t="shared" ref="AG30:AG32" si="81">VLOOKUP($AE30,$O$29:$X$32,3,FALSE)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH30" s="90">
         <f t="shared" ref="AH30:AH32" si="82">VLOOKUP($AE30,$O$29:$X$32,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI30" s="90">
         <f t="shared" ref="AI30:AI32" si="83">VLOOKUP($AE30,$O$29:$X$32,5,FALSE)</f>
@@ -7742,7 +7742,7 @@
       </c>
       <c r="AJ30" s="90">
         <f t="shared" ref="AJ30:AJ32" si="84">VLOOKUP($AE30,$O$29:$X$32,6,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK30" s="90">
         <f t="shared" ref="AK30:AK32" si="85">VLOOKUP($AE30,$O$29:$X$32,7,FALSE)</f>
@@ -7750,15 +7750,15 @@
       </c>
       <c r="AL30" s="90">
         <f t="shared" ref="AL30:AL32" si="86">VLOOKUP($AE30,$O$29:$X$32,8,FALSE)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="AM30" s="90">
         <f t="shared" ref="AM30:AM32" si="87">VLOOKUP($AE30,$O$29:$X$32,9,FALSE)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AN30" s="91">
         <f t="shared" ref="AN30:AN32" si="88">VLOOKUP($AE30,$O$29:$X$32,10,FALSE)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="31" spans="1:40" x14ac:dyDescent="0.25">
@@ -7776,18 +7776,22 @@
         <f>P32</f>
         <v>Internazionale</v>
       </c>
-      <c r="F31" s="21"/>
+      <c r="F31" s="21">
+        <v>2</v>
+      </c>
       <c r="G31" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H31" s="21"/>
+      <c r="H31" s="21">
+        <v>0</v>
+      </c>
       <c r="I31" s="13" t="str">
         <f>P29</f>
         <v>River Plate</v>
       </c>
       <c r="J31" s="42" t="str">
         <f t="shared" si="0"/>
-        <v>empate</v>
+        <v>Internazionale</v>
       </c>
       <c r="K31" s="43" t="str">
         <f t="shared" si="1"/>
@@ -7799,12 +7803,12 @@
       </c>
       <c r="M31" s="44" t="str">
         <f t="shared" si="3"/>
-        <v>empate</v>
+        <v>River Plate</v>
       </c>
       <c r="N31" s="51"/>
       <c r="O31" s="52">
         <f t="shared" si="72"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P31" s="53" t="str">
         <f>Sorteios!C16</f>
@@ -7812,15 +7816,15 @@
       </c>
       <c r="Q31" s="43">
         <f t="shared" si="73"/>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R31" s="43">
         <f t="shared" si="74"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S31" s="43">
         <f>COUNTIF(J:J,P31)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T31" s="43">
         <f>COUNTIF(K:K,P31)+COUNTIF(L:L,P31)</f>
@@ -7832,7 +7836,7 @@
       </c>
       <c r="V31" s="43">
         <f>SUMIF(E:E,P31,F:F)+SUMIF(I:I,P31,H:H)</f>
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="W31" s="43">
         <f>SUMIF(E:E,P31,H:H)+SUMIF(I:I,P31,F:F)</f>
@@ -7840,7 +7844,7 @@
       </c>
       <c r="X31" s="43">
         <f t="shared" si="75"/>
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="Y31" s="43">
         <f t="shared" si="76"/>
@@ -7867,35 +7871,35 @@
       </c>
       <c r="AF31" s="83" t="str">
         <f t="shared" si="80"/>
-        <v>Monterrey</v>
+        <v>River Plate</v>
       </c>
       <c r="AG31" s="90">
         <f t="shared" si="81"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AH31" s="90">
         <f t="shared" si="82"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI31" s="90">
         <f t="shared" si="83"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ31" s="90">
         <f t="shared" si="84"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK31" s="90">
         <f t="shared" si="85"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL31" s="90">
         <f t="shared" si="86"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AM31" s="90">
         <f t="shared" si="87"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="AN31" s="91">
         <f t="shared" si="88"/>
@@ -7917,18 +7921,22 @@
         <f>P30</f>
         <v>Urawa Red Diamonds</v>
       </c>
-      <c r="F32" s="22"/>
+      <c r="F32" s="22">
+        <v>0</v>
+      </c>
       <c r="G32" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="H32" s="22"/>
+      <c r="H32" s="22">
+        <v>4</v>
+      </c>
       <c r="I32" s="17" t="str">
         <f>P31</f>
         <v>Monterrey</v>
       </c>
       <c r="J32" s="56" t="str">
         <f t="shared" si="0"/>
-        <v>empate</v>
+        <v>Monterrey</v>
       </c>
       <c r="K32" s="57" t="str">
         <f t="shared" si="1"/>
@@ -7940,12 +7948,12 @@
       </c>
       <c r="M32" s="58" t="str">
         <f t="shared" si="3"/>
-        <v>empate</v>
+        <v>Urawa Red Diamonds</v>
       </c>
       <c r="N32" s="59"/>
       <c r="O32" s="60">
         <f t="shared" si="72"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P32" s="53" t="str">
         <f>Sorteios!C17</f>
@@ -7953,15 +7961,15 @@
       </c>
       <c r="Q32" s="57">
         <f t="shared" si="73"/>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="R32" s="57">
         <f t="shared" si="74"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S32" s="43">
         <f>COUNTIF(J:J,P32)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T32" s="43">
         <f>COUNTIF(K:K,P32)+COUNTIF(L:L,P32)</f>
@@ -7973,7 +7981,7 @@
       </c>
       <c r="V32" s="57">
         <f>SUMIF(E:E,P32,F:F)+SUMIF(I:I,P32,H:H)</f>
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="W32" s="57">
         <f>SUMIF(E:E,P32,H:H)+SUMIF(I:I,P32,F:F)</f>
@@ -7981,11 +7989,11 @@
       </c>
       <c r="X32" s="57">
         <f t="shared" si="75"/>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="Y32" s="57">
         <f t="shared" si="76"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z32" s="57">
         <f t="shared" si="77"/>
@@ -8016,7 +8024,7 @@
       </c>
       <c r="AH32" s="92">
         <f t="shared" si="82"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI32" s="92">
         <f t="shared" si="83"/>
@@ -8028,7 +8036,7 @@
       </c>
       <c r="AK32" s="92">
         <f t="shared" si="85"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL32" s="92">
         <f t="shared" si="86"/>
@@ -8036,11 +8044,11 @@
       </c>
       <c r="AM32" s="92">
         <f t="shared" si="87"/>
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="AN32" s="93">
         <f t="shared" si="88"/>
-        <v>-3</v>
+        <v>-7</v>
       </c>
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.25">
@@ -10527,18 +10535,18 @@
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="109"/>
-      <c r="B4" s="179" t="s">
+      <c r="B4" s="180" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="180"/>
-      <c r="D4" s="180"/>
-      <c r="E4" s="180"/>
-      <c r="F4" s="180"/>
-      <c r="G4" s="180"/>
-      <c r="H4" s="180"/>
-      <c r="I4" s="180"/>
-      <c r="J4" s="180"/>
-      <c r="K4" s="181"/>
+      <c r="C4" s="181"/>
+      <c r="D4" s="181"/>
+      <c r="E4" s="181"/>
+      <c r="F4" s="181"/>
+      <c r="G4" s="181"/>
+      <c r="H4" s="181"/>
+      <c r="I4" s="181"/>
+      <c r="J4" s="181"/>
+      <c r="K4" s="182"/>
       <c r="L4" s="110"/>
       <c r="M4" s="111"/>
       <c r="N4" s="111"/>
@@ -10555,19 +10563,19 @@
       <c r="D5" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="182" t="s">
+      <c r="E5" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="182"/>
-      <c r="G5" s="182" t="s">
+      <c r="F5" s="183"/>
+      <c r="G5" s="183" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="182"/>
-      <c r="I5" s="182"/>
-      <c r="J5" s="182" t="s">
+      <c r="H5" s="183"/>
+      <c r="I5" s="183"/>
+      <c r="J5" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="183"/>
+      <c r="K5" s="184"/>
       <c r="L5" s="113"/>
       <c r="M5" s="113"/>
       <c r="N5" s="113"/>
@@ -10723,7 +10731,7 @@
       </c>
       <c r="E10" s="11" t="str">
         <f>IF('Fase de Grupos'!AH29=3,'Fase de Grupos'!AF29,"1º do Grupo E")</f>
-        <v>1º do Grupo E</v>
+        <v>Internazionale</v>
       </c>
       <c r="F10" s="121"/>
       <c r="G10" s="21"/>
@@ -10802,7 +10810,7 @@
       <c r="J12" s="122"/>
       <c r="K12" s="138" t="str">
         <f>IF('Fase de Grupos'!AH30=3,'Fase de Grupos'!AF30,"2º do Grupo E")</f>
-        <v>2º do Grupo E</v>
+        <v>Monterrey</v>
       </c>
       <c r="L12" s="114" t="str">
         <f t="shared" si="0"/>
@@ -10855,18 +10863,18 @@
     </row>
     <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="109"/>
-      <c r="B16" s="179" t="s">
+      <c r="B16" s="180" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="180"/>
-      <c r="D16" s="180"/>
-      <c r="E16" s="180"/>
-      <c r="F16" s="180"/>
-      <c r="G16" s="180"/>
-      <c r="H16" s="180"/>
-      <c r="I16" s="180"/>
-      <c r="J16" s="180"/>
-      <c r="K16" s="181"/>
+      <c r="C16" s="181"/>
+      <c r="D16" s="181"/>
+      <c r="E16" s="181"/>
+      <c r="F16" s="181"/>
+      <c r="G16" s="181"/>
+      <c r="H16" s="181"/>
+      <c r="I16" s="181"/>
+      <c r="J16" s="181"/>
+      <c r="K16" s="182"/>
       <c r="L16" s="110"/>
       <c r="M16" s="111"/>
       <c r="N16" s="111"/>
@@ -10879,19 +10887,19 @@
       <c r="D17" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="182" t="s">
+      <c r="E17" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="182"/>
-      <c r="G17" s="182" t="s">
+      <c r="F17" s="183"/>
+      <c r="G17" s="183" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="182"/>
-      <c r="I17" s="182"/>
-      <c r="J17" s="182" t="s">
+      <c r="H17" s="183"/>
+      <c r="I17" s="183"/>
+      <c r="J17" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="K17" s="183"/>
+      <c r="K17" s="184"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B18" s="129" t="s">
@@ -11037,18 +11045,18 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="109"/>
-      <c r="B24" s="179" t="s">
+      <c r="B24" s="180" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="180"/>
-      <c r="D24" s="180"/>
-      <c r="E24" s="180"/>
-      <c r="F24" s="180"/>
-      <c r="G24" s="180"/>
-      <c r="H24" s="180"/>
-      <c r="I24" s="180"/>
-      <c r="J24" s="180"/>
-      <c r="K24" s="181"/>
+      <c r="C24" s="181"/>
+      <c r="D24" s="181"/>
+      <c r="E24" s="181"/>
+      <c r="F24" s="181"/>
+      <c r="G24" s="181"/>
+      <c r="H24" s="181"/>
+      <c r="I24" s="181"/>
+      <c r="J24" s="181"/>
+      <c r="K24" s="182"/>
       <c r="L24" s="110"/>
       <c r="M24" s="111"/>
       <c r="N24" s="111"/>
@@ -11064,19 +11072,19 @@
       <c r="D25" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="182" t="s">
+      <c r="E25" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="182"/>
-      <c r="G25" s="182" t="s">
+      <c r="F25" s="183"/>
+      <c r="G25" s="183" t="s">
         <v>13</v>
       </c>
-      <c r="H25" s="182"/>
-      <c r="I25" s="182"/>
-      <c r="J25" s="182" t="s">
+      <c r="H25" s="183"/>
+      <c r="I25" s="183"/>
+      <c r="J25" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="K25" s="183"/>
+      <c r="K25" s="184"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="151" t="s">
@@ -11165,18 +11173,18 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="109"/>
-      <c r="B31" s="179" t="s">
+      <c r="B31" s="180" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="180"/>
-      <c r="D31" s="180"/>
-      <c r="E31" s="180"/>
-      <c r="F31" s="180"/>
-      <c r="G31" s="180"/>
-      <c r="H31" s="180"/>
-      <c r="I31" s="180"/>
-      <c r="J31" s="180"/>
-      <c r="K31" s="181"/>
+      <c r="C31" s="181"/>
+      <c r="D31" s="181"/>
+      <c r="E31" s="181"/>
+      <c r="F31" s="181"/>
+      <c r="G31" s="181"/>
+      <c r="H31" s="181"/>
+      <c r="I31" s="181"/>
+      <c r="J31" s="181"/>
+      <c r="K31" s="182"/>
       <c r="L31" s="110"/>
       <c r="M31" s="111"/>
       <c r="N31" s="111"/>
@@ -11192,19 +11200,19 @@
       <c r="D32" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="182" t="s">
+      <c r="E32" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="182"/>
-      <c r="G32" s="182" t="s">
+      <c r="F32" s="183"/>
+      <c r="G32" s="183" t="s">
         <v>13</v>
       </c>
-      <c r="H32" s="182"/>
-      <c r="I32" s="182"/>
-      <c r="J32" s="182" t="s">
+      <c r="H32" s="183"/>
+      <c r="I32" s="183"/>
+      <c r="J32" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="K32" s="183"/>
+      <c r="K32" s="184"/>
     </row>
     <row r="33" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="161" t="s">
@@ -11252,11 +11260,11 @@
     </row>
     <row r="36" spans="1:17" s="137" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="135"/>
-      <c r="B36" s="184" t="s">
+      <c r="B36" s="179" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="184"/>
-      <c r="D36" s="184"/>
+      <c r="C36" s="179"/>
+      <c r="D36" s="179"/>
       <c r="E36" s="173" t="str">
         <f>IF(M33="1º Lugar","",M33)</f>
         <v/>
@@ -11276,11 +11284,11 @@
     </row>
     <row r="37" spans="1:17" s="137" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="135"/>
-      <c r="B37" s="184" t="s">
+      <c r="B37" s="179" t="s">
         <v>106</v>
       </c>
-      <c r="C37" s="184"/>
-      <c r="D37" s="184"/>
+      <c r="C37" s="179"/>
+      <c r="D37" s="179"/>
       <c r="E37" s="175" t="str">
         <f>IF(M34="2º Lugar","",M34)</f>
         <v/>
@@ -11408,12 +11416,11 @@
   </sheetData>
   <sheetProtection password="CC01" sheet="1" selectLockedCells="1"/>
   <mergeCells count="18">
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B31:K31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="B16:K16"/>
     <mergeCell ref="B24:K24"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="G25:I25"/>
@@ -11421,11 +11428,12 @@
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="B16:K16"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B31:K31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="B36:D36"/>
   </mergeCells>
   <conditionalFormatting sqref="F6">
     <cfRule type="expression" dxfId="31" priority="128">
@@ -11825,20 +11833,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11861,26 +11869,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83E7837-68AD-48B2-A1AB-AAB452317AF5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A45D7D45-1E18-48AE-827B-096C3C02C976}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83E7837-68AD-48B2-A1AB-AAB452317AF5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
-    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Att até Jogo 46
</commit_message>
<xml_diff>
--- a/Mundial de Clubes FIFA 2025.xlsx
+++ b/Mundial de Clubes FIFA 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjunior\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FFEF0FA7-3635-4A44-86F7-8028F6F9421E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF1DF614-1E29-4DC4-8FBC-057CA8F53B7E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="1185" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{076F3B28-812E-4458-A424-96085A053123}"/>
   </bookViews>
@@ -1598,23 +1598,23 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4019,7 +4019,7 @@
   <dimension ref="A1:AN50"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F43" sqref="F43"/>
+      <selection activeCell="F49" sqref="F49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9074,7 +9074,7 @@
       <c r="N41" s="51"/>
       <c r="O41" s="52">
         <f>RANK(Q41,$Q$41:$Q$44)+SUM(Y41:AB41)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="P41" s="53" t="str">
         <f>Sorteios!I14</f>
@@ -9082,15 +9082,15 @@
       </c>
       <c r="Q41" s="43">
         <f>(S41*3)+(T41*1)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="R41" s="43">
         <f>SUM(S41:U41)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S41" s="43">
         <f>COUNTIF(J:J,P41)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="T41" s="43">
         <f>COUNTIF(K:K,P41)+COUNTIF(L:L,P41)</f>
@@ -9102,15 +9102,15 @@
       </c>
       <c r="V41" s="43">
         <f>SUMIF(E:E,P41,F:F)+SUMIF(I:I,P41,H:H)</f>
-        <v>8</v>
+        <v>13</v>
       </c>
       <c r="W41" s="43">
         <f>SUMIF(E:E,P41,H:H)+SUMIF(I:I,P41,F:F)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="X41" s="43">
         <f>V41-W41</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="Y41" s="43">
         <f>SUMPRODUCT(($Q$41:$Q$44=Q41)*($X$41:$X$44&gt;X41))</f>
@@ -9118,7 +9118,7 @@
       </c>
       <c r="Z41" s="43">
         <f>SUMPRODUCT(($Q$41:$Q$44=Q41)*($X$41:$X$44=X41)*($V$41:$V$44&gt;V41))</f>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA41" s="43">
         <f>SUMPRODUCT(($Q$41:$Q$44=Q41)*($X$41:$X$44=X41)*($V$41:$V$44=V41)*($W$41:$W$44&gt;W41))</f>
@@ -9137,19 +9137,19 @@
       </c>
       <c r="AF41" s="83" t="str">
         <f>VLOOKUP($AE41,$O$41:$X$44,2,FALSE)</f>
-        <v>Juventus</v>
+        <v>Manchester City</v>
       </c>
       <c r="AG41" s="90">
         <f>VLOOKUP($AE41,$O$41:$X$44,3,FALSE)</f>
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="AH41" s="90">
         <f>VLOOKUP($AE41,$O$41:$X$44,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI41" s="90">
         <f>VLOOKUP($AE41,$O$41:$X$44,5,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AJ41" s="90">
         <f>VLOOKUP($AE41,$O$41:$X$44,6,FALSE)</f>
@@ -9161,15 +9161,15 @@
       </c>
       <c r="AL41" s="90">
         <f>VLOOKUP($AE41,$O$41:$X$44,8,FALSE)</f>
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="AM41" s="90">
         <f>VLOOKUP($AE41,$O$41:$X$44,9,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AN41" s="91">
         <f>VLOOKUP($AE41,$O$41:$X$44,10,FALSE)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="42" spans="1:40" x14ac:dyDescent="0.25">
@@ -9219,7 +9219,7 @@
       <c r="N42" s="51"/>
       <c r="O42" s="52">
         <f t="shared" ref="O42:O44" si="110">RANK(Q42,$Q$41:$Q$44)+SUM(Y42:AB42)</f>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P42" s="53" t="str">
         <f>Sorteios!I15</f>
@@ -9231,7 +9231,7 @@
       </c>
       <c r="R42" s="43">
         <f t="shared" ref="R42:R44" si="112">SUM(S42:U42)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S42" s="43">
         <f>COUNTIF(J:J,P42)</f>
@@ -9243,19 +9243,19 @@
       </c>
       <c r="U42" s="43">
         <f>COUNTIF(M:M,P42)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V42" s="43">
         <f>SUMIF(E:E,P42,F:F)+SUMIF(I:I,P42,H:H)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W42" s="43">
         <f>SUMIF(E:E,P42,H:H)+SUMIF(I:I,P42,F:F)</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="X42" s="43">
         <f t="shared" ref="X42:X44" si="113">V42-W42</f>
-        <v>-5</v>
+        <v>-6</v>
       </c>
       <c r="Y42" s="43">
         <f t="shared" ref="Y42:Y44" si="114">SUMPRODUCT(($Q$41:$Q$44=Q42)*($X$41:$X$44&gt;X42))</f>
@@ -9282,7 +9282,7 @@
       </c>
       <c r="AF42" s="83" t="str">
         <f t="shared" ref="AF42:AF44" si="118">VLOOKUP($AE42,$O$41:$X$44,2,FALSE)</f>
-        <v>Manchester City</v>
+        <v>Juventus</v>
       </c>
       <c r="AG42" s="90">
         <f t="shared" ref="AG42:AG44" si="119">VLOOKUP($AE42,$O$41:$X$44,3,FALSE)</f>
@@ -9290,7 +9290,7 @@
       </c>
       <c r="AH42" s="90">
         <f t="shared" ref="AH42:AH44" si="120">VLOOKUP($AE42,$O$41:$X$44,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI42" s="90">
         <f t="shared" ref="AI42:AI44" si="121">VLOOKUP($AE42,$O$41:$X$44,5,FALSE)</f>
@@ -9302,19 +9302,19 @@
       </c>
       <c r="AK42" s="90">
         <f t="shared" ref="AK42:AK44" si="123">VLOOKUP($AE42,$O$41:$X$44,7,FALSE)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL42" s="90">
         <f t="shared" ref="AL42:AL44" si="124">VLOOKUP($AE42,$O$41:$X$44,8,FALSE)</f>
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="AM42" s="90">
         <f t="shared" ref="AM42:AM44" si="125">VLOOKUP($AE42,$O$41:$X$44,9,FALSE)</f>
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="AN42" s="91">
         <f t="shared" ref="AN42:AN44" si="126">VLOOKUP($AE42,$O$41:$X$44,10,FALSE)</f>
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="43" spans="1:40" x14ac:dyDescent="0.25">
@@ -9332,18 +9332,22 @@
         <f>P44</f>
         <v>Juventus</v>
       </c>
-      <c r="F43" s="21"/>
+      <c r="F43" s="21">
+        <v>2</v>
+      </c>
       <c r="G43" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H43" s="21"/>
+      <c r="H43" s="21">
+        <v>5</v>
+      </c>
       <c r="I43" s="13" t="str">
         <f>P41</f>
         <v>Manchester City</v>
       </c>
       <c r="J43" s="42" t="str">
         <f t="shared" si="89"/>
-        <v>empate</v>
+        <v>Manchester City</v>
       </c>
       <c r="K43" s="43" t="str">
         <f t="shared" si="90"/>
@@ -9355,12 +9359,12 @@
       </c>
       <c r="M43" s="44" t="str">
         <f t="shared" si="92"/>
-        <v>empate</v>
+        <v>Juventus</v>
       </c>
       <c r="N43" s="51"/>
       <c r="O43" s="52">
         <f t="shared" si="110"/>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="P43" s="53" t="str">
         <f>Sorteios!I16</f>
@@ -9368,15 +9372,15 @@
       </c>
       <c r="Q43" s="43">
         <f t="shared" si="111"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="R43" s="43">
         <f t="shared" si="112"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S43" s="43">
         <f>COUNTIF(J:J,P43)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T43" s="43">
         <f>COUNTIF(K:K,P43)+COUNTIF(L:L,P43)</f>
@@ -9388,19 +9392,19 @@
       </c>
       <c r="V43" s="43">
         <f>SUMIF(E:E,P43,F:F)+SUMIF(I:I,P43,H:H)</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="W43" s="43">
         <f>SUMIF(E:E,P43,H:H)+SUMIF(I:I,P43,F:F)</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="X43" s="43">
         <f t="shared" si="113"/>
-        <v>-11</v>
+        <v>-10</v>
       </c>
       <c r="Y43" s="43">
         <f t="shared" si="114"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z43" s="43">
         <f t="shared" si="115"/>
@@ -9423,19 +9427,19 @@
       </c>
       <c r="AF43" s="83" t="str">
         <f t="shared" si="118"/>
-        <v>Wydad Casablanca</v>
+        <v>Al Ain</v>
       </c>
       <c r="AG43" s="90">
         <f t="shared" si="119"/>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="AH43" s="90">
         <f t="shared" si="120"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI43" s="90">
         <f t="shared" si="121"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ43" s="90">
         <f t="shared" si="122"/>
@@ -9447,15 +9451,15 @@
       </c>
       <c r="AL43" s="90">
         <f t="shared" si="124"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AM43" s="90">
         <f t="shared" si="125"/>
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="AN43" s="91">
         <f t="shared" si="126"/>
-        <v>-5</v>
+        <v>-10</v>
       </c>
     </row>
     <row r="44" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -9473,18 +9477,22 @@
         <f>P42</f>
         <v>Wydad Casablanca</v>
       </c>
-      <c r="F44" s="22"/>
+      <c r="F44" s="22">
+        <v>1</v>
+      </c>
       <c r="G44" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="H44" s="22"/>
+      <c r="H44" s="22">
+        <v>2</v>
+      </c>
       <c r="I44" s="17" t="str">
         <f>P43</f>
         <v>Al Ain</v>
       </c>
       <c r="J44" s="56" t="str">
         <f t="shared" si="89"/>
-        <v>empate</v>
+        <v>Al Ain</v>
       </c>
       <c r="K44" s="57" t="str">
         <f t="shared" si="90"/>
@@ -9496,12 +9504,12 @@
       </c>
       <c r="M44" s="58" t="str">
         <f t="shared" si="92"/>
-        <v>empate</v>
+        <v>Wydad Casablanca</v>
       </c>
       <c r="N44" s="59"/>
       <c r="O44" s="60">
         <f t="shared" si="110"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="P44" s="53" t="str">
         <f>Sorteios!I17</f>
@@ -9513,7 +9521,7 @@
       </c>
       <c r="R44" s="57">
         <f t="shared" si="112"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S44" s="43">
         <f>COUNTIF(J:J,P44)</f>
@@ -9525,19 +9533,19 @@
       </c>
       <c r="U44" s="43">
         <f>COUNTIF(M:M,P44)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V44" s="57">
         <f>SUMIF(E:E,P44,F:F)+SUMIF(I:I,P44,H:H)</f>
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="W44" s="57">
         <f>SUMIF(E:E,P44,H:H)+SUMIF(I:I,P44,F:F)</f>
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="X44" s="57">
         <f t="shared" si="113"/>
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="Y44" s="57">
         <f t="shared" si="114"/>
@@ -9564,7 +9572,7 @@
       </c>
       <c r="AF44" s="84" t="str">
         <f t="shared" si="118"/>
-        <v>Al Ain</v>
+        <v>Wydad Casablanca</v>
       </c>
       <c r="AG44" s="92">
         <f t="shared" si="119"/>
@@ -9572,7 +9580,7 @@
       </c>
       <c r="AH44" s="92">
         <f t="shared" si="120"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI44" s="92">
         <f t="shared" si="121"/>
@@ -9584,19 +9592,19 @@
       </c>
       <c r="AK44" s="92">
         <f t="shared" si="123"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL44" s="92">
         <f t="shared" si="124"/>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="AM44" s="92">
         <f t="shared" si="125"/>
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="AN44" s="93">
         <f t="shared" si="126"/>
-        <v>-11</v>
+        <v>-6</v>
       </c>
     </row>
     <row r="45" spans="1:40" x14ac:dyDescent="0.25">
@@ -10535,18 +10543,18 @@
     <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="109"/>
-      <c r="B4" s="180" t="s">
+      <c r="B4" s="179" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="181"/>
-      <c r="D4" s="181"/>
-      <c r="E4" s="181"/>
-      <c r="F4" s="181"/>
-      <c r="G4" s="181"/>
-      <c r="H4" s="181"/>
-      <c r="I4" s="181"/>
-      <c r="J4" s="181"/>
-      <c r="K4" s="182"/>
+      <c r="C4" s="180"/>
+      <c r="D4" s="180"/>
+      <c r="E4" s="180"/>
+      <c r="F4" s="180"/>
+      <c r="G4" s="180"/>
+      <c r="H4" s="180"/>
+      <c r="I4" s="180"/>
+      <c r="J4" s="180"/>
+      <c r="K4" s="181"/>
       <c r="L4" s="110"/>
       <c r="M4" s="111"/>
       <c r="N4" s="111"/>
@@ -10563,19 +10571,19 @@
       <c r="D5" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="183" t="s">
+      <c r="E5" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="183"/>
-      <c r="G5" s="183" t="s">
+      <c r="F5" s="182"/>
+      <c r="G5" s="182" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="183"/>
-      <c r="I5" s="183"/>
-      <c r="J5" s="183" t="s">
+      <c r="H5" s="182"/>
+      <c r="I5" s="182"/>
+      <c r="J5" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="184"/>
+      <c r="K5" s="183"/>
       <c r="L5" s="113"/>
       <c r="M5" s="113"/>
       <c r="N5" s="113"/>
@@ -10765,7 +10773,7 @@
       </c>
       <c r="E11" s="11" t="str">
         <f>IF('Fase de Grupos'!AH41=3,'Fase de Grupos'!AF41,"1º do Grupo G")</f>
-        <v>1º do Grupo G</v>
+        <v>Manchester City</v>
       </c>
       <c r="F11" s="121"/>
       <c r="G11" s="21"/>
@@ -10844,7 +10852,7 @@
       <c r="J13" s="141"/>
       <c r="K13" s="142" t="str">
         <f>IF('Fase de Grupos'!AH42=3,'Fase de Grupos'!AF42,"2º do Grupo G")</f>
-        <v>2º do Grupo G</v>
+        <v>Juventus</v>
       </c>
       <c r="L13" s="114" t="str">
         <f t="shared" si="0"/>
@@ -10863,18 +10871,18 @@
     </row>
     <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="109"/>
-      <c r="B16" s="180" t="s">
+      <c r="B16" s="179" t="s">
         <v>61</v>
       </c>
-      <c r="C16" s="181"/>
-      <c r="D16" s="181"/>
-      <c r="E16" s="181"/>
-      <c r="F16" s="181"/>
-      <c r="G16" s="181"/>
-      <c r="H16" s="181"/>
-      <c r="I16" s="181"/>
-      <c r="J16" s="181"/>
-      <c r="K16" s="182"/>
+      <c r="C16" s="180"/>
+      <c r="D16" s="180"/>
+      <c r="E16" s="180"/>
+      <c r="F16" s="180"/>
+      <c r="G16" s="180"/>
+      <c r="H16" s="180"/>
+      <c r="I16" s="180"/>
+      <c r="J16" s="180"/>
+      <c r="K16" s="181"/>
       <c r="L16" s="110"/>
       <c r="M16" s="111"/>
       <c r="N16" s="111"/>
@@ -10887,19 +10895,19 @@
       <c r="D17" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="183" t="s">
+      <c r="E17" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="F17" s="183"/>
-      <c r="G17" s="183" t="s">
+      <c r="F17" s="182"/>
+      <c r="G17" s="182" t="s">
         <v>13</v>
       </c>
-      <c r="H17" s="183"/>
-      <c r="I17" s="183"/>
-      <c r="J17" s="183" t="s">
+      <c r="H17" s="182"/>
+      <c r="I17" s="182"/>
+      <c r="J17" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="K17" s="184"/>
+      <c r="K17" s="183"/>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B18" s="129" t="s">
@@ -11045,18 +11053,18 @@
     </row>
     <row r="24" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A24" s="109"/>
-      <c r="B24" s="180" t="s">
+      <c r="B24" s="179" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="181"/>
-      <c r="D24" s="181"/>
-      <c r="E24" s="181"/>
-      <c r="F24" s="181"/>
-      <c r="G24" s="181"/>
-      <c r="H24" s="181"/>
-      <c r="I24" s="181"/>
-      <c r="J24" s="181"/>
-      <c r="K24" s="182"/>
+      <c r="C24" s="180"/>
+      <c r="D24" s="180"/>
+      <c r="E24" s="180"/>
+      <c r="F24" s="180"/>
+      <c r="G24" s="180"/>
+      <c r="H24" s="180"/>
+      <c r="I24" s="180"/>
+      <c r="J24" s="180"/>
+      <c r="K24" s="181"/>
       <c r="L24" s="110"/>
       <c r="M24" s="111"/>
       <c r="N24" s="111"/>
@@ -11072,19 +11080,19 @@
       <c r="D25" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="183" t="s">
+      <c r="E25" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="183"/>
-      <c r="G25" s="183" t="s">
+      <c r="F25" s="182"/>
+      <c r="G25" s="182" t="s">
         <v>13</v>
       </c>
-      <c r="H25" s="183"/>
-      <c r="I25" s="183"/>
-      <c r="J25" s="183" t="s">
+      <c r="H25" s="182"/>
+      <c r="I25" s="182"/>
+      <c r="J25" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="K25" s="184"/>
+      <c r="K25" s="183"/>
     </row>
     <row r="26" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B26" s="151" t="s">
@@ -11173,18 +11181,18 @@
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A31" s="109"/>
-      <c r="B31" s="180" t="s">
+      <c r="B31" s="179" t="s">
         <v>65</v>
       </c>
-      <c r="C31" s="181"/>
-      <c r="D31" s="181"/>
-      <c r="E31" s="181"/>
-      <c r="F31" s="181"/>
-      <c r="G31" s="181"/>
-      <c r="H31" s="181"/>
-      <c r="I31" s="181"/>
-      <c r="J31" s="181"/>
-      <c r="K31" s="182"/>
+      <c r="C31" s="180"/>
+      <c r="D31" s="180"/>
+      <c r="E31" s="180"/>
+      <c r="F31" s="180"/>
+      <c r="G31" s="180"/>
+      <c r="H31" s="180"/>
+      <c r="I31" s="180"/>
+      <c r="J31" s="180"/>
+      <c r="K31" s="181"/>
       <c r="L31" s="110"/>
       <c r="M31" s="111"/>
       <c r="N31" s="111"/>
@@ -11200,19 +11208,19 @@
       <c r="D32" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E32" s="183" t="s">
+      <c r="E32" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="F32" s="183"/>
-      <c r="G32" s="183" t="s">
+      <c r="F32" s="182"/>
+      <c r="G32" s="182" t="s">
         <v>13</v>
       </c>
-      <c r="H32" s="183"/>
-      <c r="I32" s="183"/>
-      <c r="J32" s="183" t="s">
+      <c r="H32" s="182"/>
+      <c r="I32" s="182"/>
+      <c r="J32" s="182" t="s">
         <v>12</v>
       </c>
-      <c r="K32" s="184"/>
+      <c r="K32" s="183"/>
     </row>
     <row r="33" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B33" s="161" t="s">
@@ -11260,11 +11268,11 @@
     </row>
     <row r="36" spans="1:17" s="137" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="135"/>
-      <c r="B36" s="179" t="s">
+      <c r="B36" s="184" t="s">
         <v>66</v>
       </c>
-      <c r="C36" s="179"/>
-      <c r="D36" s="179"/>
+      <c r="C36" s="184"/>
+      <c r="D36" s="184"/>
       <c r="E36" s="173" t="str">
         <f>IF(M33="1º Lugar","",M33)</f>
         <v/>
@@ -11284,11 +11292,11 @@
     </row>
     <row r="37" spans="1:17" s="137" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="135"/>
-      <c r="B37" s="179" t="s">
+      <c r="B37" s="184" t="s">
         <v>106</v>
       </c>
-      <c r="C37" s="179"/>
-      <c r="D37" s="179"/>
+      <c r="C37" s="184"/>
+      <c r="D37" s="184"/>
       <c r="E37" s="175" t="str">
         <f>IF(M34="2º Lugar","",M34)</f>
         <v/>
@@ -11416,11 +11424,12 @@
   </sheetData>
   <sheetProtection password="CC01" sheet="1" selectLockedCells="1"/>
   <mergeCells count="18">
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="B16:K16"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B31:K31"/>
+    <mergeCell ref="E32:F32"/>
+    <mergeCell ref="G32:I32"/>
+    <mergeCell ref="J32:K32"/>
+    <mergeCell ref="B36:D36"/>
     <mergeCell ref="B24:K24"/>
     <mergeCell ref="E25:F25"/>
     <mergeCell ref="G25:I25"/>
@@ -11428,12 +11437,11 @@
     <mergeCell ref="E17:F17"/>
     <mergeCell ref="G17:I17"/>
     <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B31:K31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B4:K4"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="G5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="B16:K16"/>
   </mergeCells>
   <conditionalFormatting sqref="F6">
     <cfRule type="expression" dxfId="31" priority="128">
@@ -11600,6 +11608,23 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DBF2846C41E31A469E3CED25F2422E48" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0c08e4af4d80db6585ac36ba965bb3a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2c8c20e6-817c-474f-b9c2-eb2b1ac24837" xmlns:ns4="dc8c2798-6aba-4af7-93a4-b89253b03650" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4e7db2db65f9cb533b4933096bc9b657" ns3:_="" ns4:_="">
     <xsd:import namespace="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
@@ -11832,24 +11857,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A45D7D45-1E18-48AE-827B-096C3C02C976}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83E7837-68AD-48B2-A1AB-AAB452317AF5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFBCCD5-5BDE-495C-BFE9-46A98A6BC529}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11866,29 +11899,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83E7837-68AD-48B2-A1AB-AAB452317AF5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A45D7D45-1E18-48AE-827B-096C3C02C976}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Att 1ª Fase Completa
</commit_message>
<xml_diff>
--- a/Mundial de Clubes FIFA 2025.xlsx
+++ b/Mundial de Clubes FIFA 2025.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjunior\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CF1DF614-1E29-4DC4-8FBC-057CA8F53B7E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A4C59CE-D37A-42D2-BF3C-3DC8FF3CA272}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24120" yWindow="1185" windowWidth="24240" windowHeight="13020" activeTab="2" xr2:uid="{076F3B28-812E-4458-A424-96085A053123}"/>
+    <workbookView xWindow="-24120" yWindow="1185" windowWidth="24240" windowHeight="13020" activeTab="3" xr2:uid="{076F3B28-812E-4458-A424-96085A053123}"/>
   </bookViews>
   <sheets>
     <sheet name="Classificados" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="566" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="118">
   <si>
     <t>Times</t>
   </si>
@@ -365,6 +365,24 @@
   <si>
     <t>2025 Mundial de Clubes FIFA</t>
   </si>
+  <si>
+    <t>Planilha feita por:</t>
+  </si>
+  <si>
+    <t>Maurilyn Júnior</t>
+  </si>
+  <si>
+    <t>github.com/maurilyn</t>
+  </si>
+  <si>
+    <t>linkedin/maurilyn</t>
+  </si>
+  <si>
+    <t>@maurilyn</t>
+  </si>
+  <si>
+    <t>maurilyn@gmail.com</t>
+  </si>
 </sst>
 </file>
 
@@ -375,7 +393,7 @@
     <numFmt numFmtId="165" formatCode="[$-416]d\-mmm;@"/>
     <numFmt numFmtId="166" formatCode="[$-416]dd\-mmm;@"/>
   </numFmts>
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="24" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -518,6 +536,21 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="11">
     <fill>
@@ -581,7 +614,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="41">
+  <borders count="44">
     <border>
       <left/>
       <right/>
@@ -1101,12 +1134,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="185">
+  <cellXfs count="189">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1598,6 +1676,9 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1613,8 +1694,19 @@
     <xf numFmtId="0" fontId="12" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="22" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="42" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="42" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="43" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4016,10 +4108,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45896CCF-F333-49AF-850B-159476231F1C}">
-  <dimension ref="A1:AN50"/>
+  <dimension ref="A1:AQ50"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="F49" sqref="F49"/>
+    <sheetView showRowColHeaders="0" workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4055,7 +4147,7 @@
     <col min="38" max="40" width="4.7109375" style="29" customWidth="1"/>
     <col min="41" max="41" width="9.140625" style="29"/>
     <col min="42" max="42" width="3.7109375" style="29" customWidth="1"/>
-    <col min="43" max="43" width="20.7109375" style="29" customWidth="1"/>
+    <col min="43" max="43" width="30.7109375" style="29" customWidth="1"/>
     <col min="44" max="16384" width="9.140625" style="29"/>
   </cols>
   <sheetData>
@@ -5915,7 +6007,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="17" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A17" s="50"/>
       <c r="B17" s="132" t="s">
         <v>45</v>
@@ -6060,7 +6152,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A18" s="50"/>
       <c r="B18" s="132" t="s">
         <v>45</v>
@@ -6205,7 +6297,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A19" s="50"/>
       <c r="B19" s="132" t="s">
         <v>45</v>
@@ -6350,7 +6442,7 @@
         <v>-1</v>
       </c>
     </row>
-    <row r="20" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:43" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="50"/>
       <c r="B20" s="133" t="s">
         <v>45</v>
@@ -6495,7 +6587,7 @@
         <v>-16</v>
       </c>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A21" s="50"/>
       <c r="B21" s="134" t="s">
         <v>40</v>
@@ -6570,8 +6662,11 @@
       <c r="AL21" s="88"/>
       <c r="AM21" s="88"/>
       <c r="AN21" s="89"/>
-    </row>
-    <row r="22" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ21" s="185" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="22" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A22" s="50"/>
       <c r="B22" s="132" t="s">
         <v>40</v>
@@ -6692,8 +6787,11 @@
       <c r="AN22" s="1" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="23" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ22" s="186" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="23" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A23" s="50"/>
       <c r="B23" s="132" t="s">
         <v>40</v>
@@ -6837,8 +6935,11 @@
         <f>VLOOKUP($AE23,$O$23:$X$26,10,FALSE)</f>
         <v>4</v>
       </c>
-    </row>
-    <row r="24" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ23" s="187" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A24" s="50"/>
       <c r="B24" s="132" t="s">
         <v>40</v>
@@ -6982,8 +7083,11 @@
         <f t="shared" ref="AN24:AN26" si="71">VLOOKUP($AE24,$O$23:$X$26,10,FALSE)</f>
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ24" s="187" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="25" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A25" s="50"/>
       <c r="B25" s="132" t="s">
         <v>40</v>
@@ -7127,8 +7231,11 @@
         <f t="shared" si="71"/>
         <v>-4</v>
       </c>
-    </row>
-    <row r="26" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="AQ25" s="187" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="26" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="50"/>
       <c r="B26" s="133" t="s">
         <v>40</v>
@@ -7272,8 +7379,11 @@
         <f t="shared" si="71"/>
         <v>-3</v>
       </c>
-    </row>
-    <row r="27" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="AQ26" s="188" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="27" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A27" s="50"/>
       <c r="B27" s="132" t="s">
         <v>39</v>
@@ -7349,7 +7459,7 @@
       <c r="AM27" s="88"/>
       <c r="AN27" s="89"/>
     </row>
-    <row r="28" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A28" s="50"/>
       <c r="B28" s="132" t="s">
         <v>39</v>
@@ -7471,7 +7581,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A29" s="50"/>
       <c r="B29" s="132" t="s">
         <v>39</v>
@@ -7616,7 +7726,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A30" s="50"/>
       <c r="B30" s="132" t="s">
         <v>39</v>
@@ -7761,7 +7871,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:43" x14ac:dyDescent="0.25">
       <c r="A31" s="50"/>
       <c r="B31" s="132" t="s">
         <v>39</v>
@@ -7906,7 +8016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:43" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="50"/>
       <c r="B32" s="133" t="s">
         <v>39</v>
@@ -9860,15 +9970,15 @@
       </c>
       <c r="Q47" s="43">
         <f>(S47*3)+(T47*1)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="R47" s="43">
         <f>SUM(S47:U47)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S47" s="43">
         <f>COUNTIF(J:J,P47)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="T47" s="43">
         <f>COUNTIF(K:K,P47)+COUNTIF(L:L,P47)</f>
@@ -9880,7 +9990,7 @@
       </c>
       <c r="V47" s="43">
         <f>SUMIF(E:E,P47,F:F)+SUMIF(I:I,P47,H:H)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="W47" s="43">
         <f>SUMIF(E:E,P47,H:H)+SUMIF(I:I,P47,F:F)</f>
@@ -9888,7 +9998,7 @@
       </c>
       <c r="X47" s="43">
         <f>V47-W47</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="Y47" s="43">
         <f>SUMPRODUCT(($Q$47:$Q$50=Q47)*($X$47:$X$50&gt;X47))</f>
@@ -9919,15 +10029,15 @@
       </c>
       <c r="AG47" s="90">
         <f>VLOOKUP($AE47,$O$47:$X$50,3,FALSE)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AH47" s="90">
         <f>VLOOKUP($AE47,$O$47:$X$50,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI47" s="90">
         <f>VLOOKUP($AE47,$O$47:$X$50,5,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AJ47" s="90">
         <f>VLOOKUP($AE47,$O$47:$X$50,6,FALSE)</f>
@@ -9939,7 +10049,7 @@
       </c>
       <c r="AL47" s="90">
         <f>VLOOKUP($AE47,$O$47:$X$50,8,FALSE)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="AM47" s="90">
         <f>VLOOKUP($AE47,$O$47:$X$50,9,FALSE)</f>
@@ -9947,7 +10057,7 @@
       </c>
       <c r="AN47" s="91">
         <f>VLOOKUP($AE47,$O$47:$X$50,10,FALSE)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="48" spans="1:40" x14ac:dyDescent="0.25">
@@ -9997,7 +10107,7 @@
       <c r="N48" s="50"/>
       <c r="O48" s="52">
         <f>RANK(Q48,$Q$47:$Q$50)+SUM(Y48:AB48)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P48" s="53" t="str">
         <f>Sorteios!L15</f>
@@ -10005,15 +10115,15 @@
       </c>
       <c r="Q48" s="43">
         <f t="shared" ref="Q48:Q50" si="127">(S48*3)+(T48*1)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="R48" s="43">
         <f t="shared" ref="R48:R50" si="128">SUM(S48:U48)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S48" s="43">
         <f>COUNTIF(J:J,P48)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="T48" s="43">
         <f>COUNTIF(K:K,P48)+COUNTIF(L:L,P48)</f>
@@ -10025,7 +10135,7 @@
       </c>
       <c r="V48" s="43">
         <f>SUMIF(E:E,P48,F:F)+SUMIF(I:I,P48,H:H)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="W48" s="43">
         <f>SUMIF(E:E,P48,H:H)+SUMIF(I:I,P48,F:F)</f>
@@ -10033,7 +10143,7 @@
       </c>
       <c r="X48" s="43">
         <f t="shared" ref="X48:X50" si="129">V48-W48</f>
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="Y48" s="43">
         <f t="shared" ref="Y48:Y50" si="130">SUMPRODUCT(($Q$47:$Q$50=Q48)*($X$47:$X$50&gt;X48))</f>
@@ -10060,15 +10170,15 @@
       </c>
       <c r="AF48" s="83" t="str">
         <f t="shared" ref="AF48:AF50" si="134">VLOOKUP($AE48,$O$47:$X$50,2,FALSE)</f>
-        <v>Red Bull Salzburg</v>
+        <v>Al-Hilal</v>
       </c>
       <c r="AG48" s="90">
         <f t="shared" ref="AG48:AG50" si="135">VLOOKUP($AE48,$O$47:$X$50,3,FALSE)</f>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="AH48" s="90">
         <f t="shared" ref="AH48:AH50" si="136">VLOOKUP($AE48,$O$47:$X$50,4,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI48" s="90">
         <f t="shared" ref="AI48:AI50" si="137">VLOOKUP($AE48,$O$47:$X$50,5,FALSE)</f>
@@ -10076,7 +10186,7 @@
       </c>
       <c r="AJ48" s="90">
         <f t="shared" ref="AJ48:AJ50" si="138">VLOOKUP($AE48,$O$47:$X$50,6,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AK48" s="90">
         <f t="shared" ref="AK48:AK50" si="139">VLOOKUP($AE48,$O$47:$X$50,7,FALSE)</f>
@@ -10084,7 +10194,7 @@
       </c>
       <c r="AL48" s="90">
         <f t="shared" ref="AL48:AL50" si="140">VLOOKUP($AE48,$O$47:$X$50,8,FALSE)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AM48" s="90">
         <f t="shared" ref="AM48:AM50" si="141">VLOOKUP($AE48,$O$47:$X$50,9,FALSE)</f>
@@ -10092,7 +10202,7 @@
       </c>
       <c r="AN48" s="91">
         <f t="shared" ref="AN48:AN50" si="142">VLOOKUP($AE48,$O$47:$X$50,10,FALSE)</f>
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="49" spans="1:40" x14ac:dyDescent="0.25">
@@ -10110,18 +10220,22 @@
         <f>P50</f>
         <v>Red Bull Salzburg</v>
       </c>
-      <c r="F49" s="21"/>
+      <c r="F49" s="21">
+        <v>0</v>
+      </c>
       <c r="G49" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="H49" s="21"/>
+      <c r="H49" s="21">
+        <v>3</v>
+      </c>
       <c r="I49" s="26" t="str">
         <f>P47</f>
         <v>Real Madrid</v>
       </c>
       <c r="J49" s="42" t="str">
         <f t="shared" si="89"/>
-        <v>empate</v>
+        <v>Real Madrid</v>
       </c>
       <c r="K49" s="43" t="str">
         <f t="shared" si="90"/>
@@ -10133,7 +10247,7 @@
       </c>
       <c r="M49" s="44" t="str">
         <f t="shared" si="92"/>
-        <v>empate</v>
+        <v>Red Bull Salzburg</v>
       </c>
       <c r="N49" s="50"/>
       <c r="O49" s="52">
@@ -10150,7 +10264,7 @@
       </c>
       <c r="R49" s="43">
         <f t="shared" si="128"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S49" s="43">
         <f>COUNTIF(J:J,P49)</f>
@@ -10162,7 +10276,7 @@
       </c>
       <c r="U49" s="43">
         <f>COUNTIF(M:M,P49)</f>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="V49" s="43">
         <f>SUMIF(E:E,P49,F:F)+SUMIF(I:I,P49,H:H)</f>
@@ -10170,11 +10284,11 @@
       </c>
       <c r="W49" s="43">
         <f>SUMIF(E:E,P49,H:H)+SUMIF(I:I,P49,F:F)</f>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="X49" s="43">
         <f t="shared" si="129"/>
-        <v>-3</v>
+        <v>-5</v>
       </c>
       <c r="Y49" s="43">
         <f t="shared" si="130"/>
@@ -10201,39 +10315,39 @@
       </c>
       <c r="AF49" s="83" t="str">
         <f t="shared" si="134"/>
-        <v>Al-Hilal</v>
+        <v>Red Bull Salzburg</v>
       </c>
       <c r="AG49" s="90">
         <f t="shared" si="135"/>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="AH49" s="90">
         <f t="shared" si="136"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI49" s="90">
         <f t="shared" si="137"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AJ49" s="90">
         <f t="shared" si="138"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="AK49" s="90">
         <f t="shared" si="139"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AL49" s="90">
         <f t="shared" si="140"/>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="AM49" s="90">
         <f t="shared" si="141"/>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="AN49" s="91">
         <f t="shared" si="142"/>
-        <v>0</v>
+        <v>-2</v>
       </c>
     </row>
     <row r="50" spans="1:40" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -10251,18 +10365,22 @@
         <f>P48</f>
         <v>Al-Hilal</v>
       </c>
-      <c r="F50" s="22"/>
+      <c r="F50" s="22">
+        <v>2</v>
+      </c>
       <c r="G50" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="H50" s="22"/>
+      <c r="H50" s="22">
+        <v>0</v>
+      </c>
       <c r="I50" s="27" t="str">
         <f>P49</f>
         <v>Pachuca</v>
       </c>
       <c r="J50" s="70" t="str">
         <f t="shared" si="89"/>
-        <v>empate</v>
+        <v>Al-Hilal</v>
       </c>
       <c r="K50" s="71" t="str">
         <f t="shared" si="90"/>
@@ -10274,12 +10392,12 @@
       </c>
       <c r="M50" s="72" t="str">
         <f t="shared" si="92"/>
-        <v>empate</v>
+        <v>Pachuca</v>
       </c>
       <c r="N50" s="50"/>
       <c r="O50" s="73">
         <f t="shared" si="143"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="P50" s="53" t="str">
         <f>Sorteios!L17</f>
@@ -10291,7 +10409,7 @@
       </c>
       <c r="R50" s="57">
         <f t="shared" si="128"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="S50" s="43">
         <f>COUNTIF(J:J,P50)</f>
@@ -10303,7 +10421,7 @@
       </c>
       <c r="U50" s="43">
         <f>COUNTIF(M:M,P50)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="V50" s="57">
         <f>SUMIF(E:E,P50,F:F)+SUMIF(I:I,P50,H:H)</f>
@@ -10311,15 +10429,15 @@
       </c>
       <c r="W50" s="57">
         <f>SUMIF(E:E,P50,H:H)+SUMIF(I:I,P50,F:F)</f>
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="X50" s="57">
         <f t="shared" si="129"/>
-        <v>1</v>
+        <v>-2</v>
       </c>
       <c r="Y50" s="57">
         <f t="shared" si="130"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Z50" s="57">
         <f t="shared" si="131"/>
@@ -10350,7 +10468,7 @@
       </c>
       <c r="AH50" s="92">
         <f t="shared" si="136"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AI50" s="92">
         <f t="shared" si="137"/>
@@ -10362,7 +10480,7 @@
       </c>
       <c r="AK50" s="92">
         <f t="shared" si="139"/>
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="AL50" s="92">
         <f t="shared" si="140"/>
@@ -10370,11 +10488,11 @@
       </c>
       <c r="AM50" s="92">
         <f t="shared" si="141"/>
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="AN50" s="93">
         <f t="shared" si="142"/>
-        <v>-3</v>
+        <v>-5</v>
       </c>
     </row>
   </sheetData>
@@ -10487,17 +10605,23 @@
       <formula1>0</formula1>
     </dataValidation>
   </dataValidations>
+  <hyperlinks>
+    <hyperlink ref="AQ24" r:id="rId1" xr:uid="{01B4A3FE-8413-4592-A66C-CE2A7AB4AB3D}"/>
+    <hyperlink ref="AQ25" r:id="rId2" xr:uid="{4E377EAC-6AE3-43BB-A2A1-B68D6C308526}"/>
+    <hyperlink ref="AQ26" r:id="rId3" display="'@maurilyn" xr:uid="{DC2F2CD8-9544-4CCC-B8C6-5257730E7639}"/>
+    <hyperlink ref="AQ23" r:id="rId4" xr:uid="{0848616C-667E-426F-A966-A5D1489F6686}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46B54D63-DE8A-4C85-9821-2A3779E27309}">
-  <dimension ref="A1:Q58"/>
+  <dimension ref="A1:Q54"/>
   <sheetViews>
-    <sheetView showRowColHeaders="0" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+    <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10515,7 +10639,9 @@
     <col min="11" max="11" width="22.7109375" style="118" customWidth="1"/>
     <col min="12" max="12" width="3.140625" style="114" hidden="1" customWidth="1"/>
     <col min="13" max="13" width="14.140625" style="115" hidden="1" customWidth="1"/>
-    <col min="14" max="17" width="9.140625" style="115"/>
+    <col min="14" max="15" width="9.140625" style="115"/>
+    <col min="16" max="16" width="30.7109375" style="115" customWidth="1"/>
+    <col min="17" max="17" width="9.140625" style="115"/>
     <col min="18" max="16384" width="9.140625" style="29"/>
   </cols>
   <sheetData>
@@ -10540,104 +10666,148 @@
       <c r="P1" s="108"/>
       <c r="Q1" s="108"/>
     </row>
-    <row r="3" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" s="109"/>
-      <c r="B4" s="179" t="s">
+    <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A3" s="109"/>
+      <c r="B3" s="180" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="180"/>
-      <c r="D4" s="180"/>
-      <c r="E4" s="180"/>
-      <c r="F4" s="180"/>
-      <c r="G4" s="180"/>
-      <c r="H4" s="180"/>
-      <c r="I4" s="180"/>
-      <c r="J4" s="180"/>
-      <c r="K4" s="181"/>
-      <c r="L4" s="110"/>
-      <c r="M4" s="111"/>
-      <c r="N4" s="111"/>
-      <c r="O4" s="111"/>
-      <c r="P4" s="111"/>
-      <c r="Q4" s="111"/>
-    </row>
-    <row r="5" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="112"/>
-      <c r="B5" s="148"/>
-      <c r="C5" s="149" t="s">
+      <c r="C3" s="181"/>
+      <c r="D3" s="181"/>
+      <c r="E3" s="181"/>
+      <c r="F3" s="181"/>
+      <c r="G3" s="181"/>
+      <c r="H3" s="181"/>
+      <c r="I3" s="181"/>
+      <c r="J3" s="181"/>
+      <c r="K3" s="182"/>
+      <c r="L3" s="110"/>
+      <c r="M3" s="111"/>
+      <c r="N3" s="111"/>
+      <c r="O3" s="111"/>
+      <c r="P3" s="185" t="s">
+        <v>112</v>
+      </c>
+      <c r="Q3" s="111"/>
+    </row>
+    <row r="4" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="112"/>
+      <c r="B4" s="148"/>
+      <c r="C4" s="149" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="150" t="s">
+      <c r="D4" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E5" s="182" t="s">
+      <c r="E4" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="F5" s="182"/>
-      <c r="G5" s="182" t="s">
+      <c r="F4" s="183"/>
+      <c r="G4" s="183" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="182"/>
-      <c r="I5" s="182"/>
-      <c r="J5" s="182" t="s">
+      <c r="H4" s="183"/>
+      <c r="I4" s="183"/>
+      <c r="J4" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="K5" s="183"/>
-      <c r="L5" s="113"/>
-      <c r="M5" s="113"/>
-      <c r="N5" s="113"/>
-      <c r="O5" s="113"/>
-      <c r="P5" s="113"/>
-      <c r="Q5" s="113"/>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B6" s="151" t="s">
+      <c r="K4" s="184"/>
+      <c r="L4" s="113"/>
+      <c r="M4" s="113"/>
+      <c r="N4" s="113"/>
+      <c r="O4" s="113"/>
+      <c r="P4" s="186" t="s">
+        <v>113</v>
+      </c>
+      <c r="Q4" s="113"/>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B5" s="151" t="s">
         <v>59</v>
       </c>
-      <c r="C6" s="152">
+      <c r="C5" s="152">
         <v>45836</v>
       </c>
-      <c r="D6" s="68" t="s">
+      <c r="D5" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="E6" s="20" t="str">
+      <c r="E5" s="20" t="str">
         <f>IF('Fase de Grupos'!AH5=3,'Fase de Grupos'!AF5,"1º do Grupo A")</f>
         <v>Palmeiras</v>
       </c>
-      <c r="F6" s="153"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="19" t="s">
+      <c r="F5" s="153"/>
+      <c r="G5" s="23"/>
+      <c r="H5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="23"/>
-      <c r="J6" s="154"/>
-      <c r="K6" s="155" t="str">
+      <c r="I5" s="23"/>
+      <c r="J5" s="154"/>
+      <c r="K5" s="155" t="str">
         <f>IF('Fase de Grupos'!AH12=3,'Fase de Grupos'!AF12,"2º do Grupo B")</f>
         <v>Botafogo</v>
       </c>
+      <c r="L5" s="114" t="str">
+        <f>IF(OR(G5="",I5=""),"",IF(G5=I5,"emp",""))</f>
+        <v/>
+      </c>
+      <c r="M5" s="115" t="str">
+        <f>IF(OR(G5="",I5=""),"Vencedor I",IF(G5&lt;&gt;I5,IF(G5&gt;I5,E5,K5),IF(SUM(F5:G5)=SUM(I5:J5),"Vencedor I",IF(SUM(F5:G5)&gt;SUM(I5:J5),E5,K5))))</f>
+        <v>Vencedor I</v>
+      </c>
+      <c r="P5" s="187" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B6" s="127" t="s">
+        <v>100</v>
+      </c>
+      <c r="C6" s="123">
+        <v>45836</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>42</v>
+      </c>
+      <c r="E6" s="11" t="str">
+        <f>IF('Fase de Grupos'!AH17=3,'Fase de Grupos'!AF17,"1º do Grupo C")</f>
+        <v>Benfica</v>
+      </c>
+      <c r="F6" s="121"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="21"/>
+      <c r="J6" s="122"/>
+      <c r="K6" s="138" t="str">
+        <f>IF('Fase de Grupos'!AH24=3,'Fase de Grupos'!AF24,"2º do Grupo D")</f>
+        <v>Chelsea</v>
+      </c>
       <c r="L6" s="114" t="str">
-        <f>IF(OR(G6="",I6=""),"",IF(G6=I6,"emp",""))</f>
+        <f t="shared" ref="L6:L12" si="0">IF(OR(G6="",I6=""),"",IF(G6=I6,"emp",""))</f>
         <v/>
       </c>
       <c r="M6" s="115" t="str">
-        <f>IF(OR(G6="",I6=""),"Vencedor I",IF(G6&lt;&gt;I6,IF(G6&gt;I6,E6,K6),IF(SUM(F6:G6)=SUM(I6:J6),"Vencedor I",IF(SUM(F6:G6)&gt;SUM(I6:J6),E6,K6))))</f>
-        <v>Vencedor I</v>
+        <f>IF(OR(G6="",I6=""),"Vencedor II",IF(G6&lt;&gt;I6,IF(G6&gt;I6,E6,K6),IF(SUM(F6:G6)=SUM(I6:J6),"Vencedor II",IF(SUM(F6:G6)&gt;SUM(I6:J6),E6,K6))))</f>
+        <v>Vencedor II</v>
+      </c>
+      <c r="P6" s="187" t="s">
+        <v>114</v>
       </c>
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B7" s="127" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="C7" s="123">
-        <v>45836</v>
+        <v>45837</v>
       </c>
       <c r="D7" s="40" t="s">
         <v>42</v>
       </c>
       <c r="E7" s="11" t="str">
-        <f>IF('Fase de Grupos'!AH17=3,'Fase de Grupos'!AF17,"1º do Grupo C")</f>
-        <v>Benfica</v>
+        <f>IF('Fase de Grupos'!AH11=3,'Fase de Grupos'!AF11,"1º do Grupo B")</f>
+        <v>Paris Saint-Germain</v>
       </c>
       <c r="F7" s="121"/>
       <c r="G7" s="21"/>
@@ -10647,31 +10817,34 @@
       <c r="I7" s="21"/>
       <c r="J7" s="122"/>
       <c r="K7" s="138" t="str">
-        <f>IF('Fase de Grupos'!AH24=3,'Fase de Grupos'!AF24,"2º do Grupo D")</f>
-        <v>Chelsea</v>
+        <f>IF('Fase de Grupos'!AH6=3,'Fase de Grupos'!AF6,"2º do Grupo A")</f>
+        <v>Inter Miami</v>
       </c>
       <c r="L7" s="114" t="str">
-        <f t="shared" ref="L7:L13" si="0">IF(OR(G7="",I7=""),"",IF(G7=I7,"emp",""))</f>
+        <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M7" s="115" t="str">
-        <f>IF(OR(G7="",I7=""),"Vencedor II",IF(G7&lt;&gt;I7,IF(G7&gt;I7,E7,K7),IF(SUM(F7:G7)=SUM(I7:J7),"Vencedor II",IF(SUM(F7:G7)&gt;SUM(I7:J7),E7,K7))))</f>
-        <v>Vencedor II</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+        <f>IF(OR(G7="",I7=""),"Vencedor III",IF(G7&lt;&gt;I7,IF(G7&gt;I7,E7,K7),IF(SUM(F7:G7)=SUM(I7:J7),"Vencedor III",IF(SUM(F7:G7)&gt;SUM(I7:J7),E7,K7))))</f>
+        <v>Vencedor III</v>
+      </c>
+      <c r="P7" s="187" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="127" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C8" s="123">
         <v>45837</v>
       </c>
       <c r="D8" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" s="11" t="str">
-        <f>IF('Fase de Grupos'!AH11=3,'Fase de Grupos'!AF11,"1º do Grupo B")</f>
-        <v>Paris Saint-Germain</v>
+        <f>IF('Fase de Grupos'!AH23=3,'Fase de Grupos'!AF23,"1º do Grupo D")</f>
+        <v>Flamengo</v>
       </c>
       <c r="F8" s="121"/>
       <c r="G8" s="21"/>
@@ -10681,31 +10854,34 @@
       <c r="I8" s="21"/>
       <c r="J8" s="122"/>
       <c r="K8" s="138" t="str">
-        <f>IF('Fase de Grupos'!AH6=3,'Fase de Grupos'!AF6,"2º do Grupo A")</f>
-        <v>Inter Miami</v>
+        <f>IF('Fase de Grupos'!AH18=3,'Fase de Grupos'!AF18,"2º do Grupo C")</f>
+        <v>Bayern de Munique</v>
       </c>
       <c r="L8" s="114" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M8" s="115" t="str">
-        <f>IF(OR(G8="",I8=""),"Vencedor III",IF(G8&lt;&gt;I8,IF(G8&gt;I8,E8,K8),IF(SUM(F8:G8)=SUM(I8:J8),"Vencedor III",IF(SUM(F8:G8)&gt;SUM(I8:J8),E8,K8))))</f>
-        <v>Vencedor III</v>
+        <f>IF(OR(G8="",I8=""),"Vencedor IV",IF(G8&lt;&gt;I8,IF(G8&gt;I8,E8,K8),IF(SUM(F8:G8)=SUM(I8:J8),"Vencedor IV",IF(SUM(F8:G8)&gt;SUM(I8:J8),E8,K8))))</f>
+        <v>Vencedor IV</v>
+      </c>
+      <c r="P8" s="188" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B9" s="127" t="s">
-        <v>102</v>
+        <v>38</v>
       </c>
       <c r="C9" s="123">
-        <v>45837</v>
+        <v>45838</v>
       </c>
       <c r="D9" s="40" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E9" s="11" t="str">
-        <f>IF('Fase de Grupos'!AH23=3,'Fase de Grupos'!AF23,"1º do Grupo D")</f>
-        <v>Flamengo</v>
+        <f>IF('Fase de Grupos'!AH29=3,'Fase de Grupos'!AF29,"1º do Grupo E")</f>
+        <v>Internazionale</v>
       </c>
       <c r="F9" s="121"/>
       <c r="G9" s="21"/>
@@ -10715,31 +10891,31 @@
       <c r="I9" s="21"/>
       <c r="J9" s="122"/>
       <c r="K9" s="138" t="str">
-        <f>IF('Fase de Grupos'!AH18=3,'Fase de Grupos'!AF18,"2º do Grupo C")</f>
-        <v>Bayern de Munique</v>
+        <f>IF('Fase de Grupos'!AH36=3,'Fase de Grupos'!AF36,"2º do Grupo F")</f>
+        <v>Fluminense</v>
       </c>
       <c r="L9" s="114" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M9" s="115" t="str">
-        <f>IF(OR(G9="",I9=""),"Vencedor IV",IF(G9&lt;&gt;I9,IF(G9&gt;I9,E9,K9),IF(SUM(F9:G9)=SUM(I9:J9),"Vencedor IV",IF(SUM(F9:G9)&gt;SUM(I9:J9),E9,K9))))</f>
-        <v>Vencedor IV</v>
+        <f>IF(OR(G9="",I9=""),"Vencedor V",IF(G9&lt;&gt;I9,IF(G9&gt;I9,E9,K9),IF(SUM(F9:G9)=SUM(I9:J9),"Vencedor V",IF(SUM(F9:G9)&gt;SUM(I9:J9),E9,K9))))</f>
+        <v>Vencedor V</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B10" s="127" t="s">
-        <v>38</v>
+        <v>103</v>
       </c>
       <c r="C10" s="123">
         <v>45838</v>
       </c>
       <c r="D10" s="40" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E10" s="11" t="str">
-        <f>IF('Fase de Grupos'!AH29=3,'Fase de Grupos'!AF29,"1º do Grupo E")</f>
-        <v>Internazionale</v>
+        <f>IF('Fase de Grupos'!AH41=3,'Fase de Grupos'!AF41,"1º do Grupo G")</f>
+        <v>Manchester City</v>
       </c>
       <c r="F10" s="121"/>
       <c r="G10" s="21"/>
@@ -10749,31 +10925,31 @@
       <c r="I10" s="21"/>
       <c r="J10" s="122"/>
       <c r="K10" s="138" t="str">
-        <f>IF('Fase de Grupos'!AH36=3,'Fase de Grupos'!AF36,"2º do Grupo F")</f>
-        <v>Fluminense</v>
+        <f>IF('Fase de Grupos'!AH48=3,'Fase de Grupos'!AF48,"2º do Grupo H")</f>
+        <v>Al-Hilal</v>
       </c>
       <c r="L10" s="114" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M10" s="115" t="str">
-        <f>IF(OR(G10="",I10=""),"Vencedor V",IF(G10&lt;&gt;I10,IF(G10&gt;I10,E10,K10),IF(SUM(F10:G10)=SUM(I10:J10),"Vencedor V",IF(SUM(F10:G10)&gt;SUM(I10:J10),E10,K10))))</f>
-        <v>Vencedor V</v>
+        <f>IF(OR(G10="",I10=""),"Vencedor VI",IF(G10&lt;&gt;I10,IF(G10&gt;I10,E10,K10),IF(SUM(F10:G10)=SUM(I10:J10),"Vencedor VI",IF(SUM(F10:G10)&gt;SUM(I10:J10),E10,K10))))</f>
+        <v>Vencedor VI</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B11" s="127" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C11" s="123">
-        <v>45838</v>
+        <v>45839</v>
       </c>
       <c r="D11" s="40" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E11" s="11" t="str">
-        <f>IF('Fase de Grupos'!AH41=3,'Fase de Grupos'!AF41,"1º do Grupo G")</f>
-        <v>Manchester City</v>
+        <f>IF('Fase de Grupos'!AH35=3,'Fase de Grupos'!AF35,"1º do Grupo F")</f>
+        <v>Borussia Dortmund</v>
       </c>
       <c r="F11" s="121"/>
       <c r="G11" s="21"/>
@@ -10783,536 +10959,505 @@
       <c r="I11" s="21"/>
       <c r="J11" s="122"/>
       <c r="K11" s="138" t="str">
-        <f>IF('Fase de Grupos'!AH48=3,'Fase de Grupos'!AF48,"2º do Grupo H")</f>
-        <v>2º do Grupo H</v>
+        <f>IF('Fase de Grupos'!AH30=3,'Fase de Grupos'!AF30,"2º do Grupo E")</f>
+        <v>Monterrey</v>
       </c>
       <c r="L11" s="114" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M11" s="115" t="str">
-        <f>IF(OR(G11="",I11=""),"Vencedor VI",IF(G11&lt;&gt;I11,IF(G11&gt;I11,E11,K11),IF(SUM(F11:G11)=SUM(I11:J11),"Vencedor VI",IF(SUM(F11:G11)&gt;SUM(I11:J11),E11,K11))))</f>
-        <v>Vencedor VI</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B12" s="127" t="s">
-        <v>104</v>
-      </c>
-      <c r="C12" s="123">
+        <f>IF(OR(G11="",I11=""),"Vencedor VII",IF(G11&lt;&gt;I11,IF(G11&gt;I11,E11,K11),IF(SUM(F11:G11)=SUM(I11:J11),"Vencedor VII",IF(SUM(F11:G11)&gt;SUM(I11:J11),E11,K11))))</f>
+        <v>Vencedor VII</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="128" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="139">
         <v>45839</v>
       </c>
-      <c r="D12" s="40" t="s">
-        <v>42</v>
-      </c>
-      <c r="E12" s="11" t="str">
-        <f>IF('Fase de Grupos'!AH35=3,'Fase de Grupos'!AF35,"1º do Grupo F")</f>
-        <v>Borussia Dortmund</v>
-      </c>
-      <c r="F12" s="121"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="12" t="s">
+      <c r="D12" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="E12" s="15" t="str">
+        <f>IF('Fase de Grupos'!AH47=3,'Fase de Grupos'!AF47,"1º do Grupo H")</f>
+        <v>Real Madrid</v>
+      </c>
+      <c r="F12" s="140"/>
+      <c r="G12" s="22"/>
+      <c r="H12" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="I12" s="21"/>
-      <c r="J12" s="122"/>
-      <c r="K12" s="138" t="str">
-        <f>IF('Fase de Grupos'!AH30=3,'Fase de Grupos'!AF30,"2º do Grupo E")</f>
-        <v>Monterrey</v>
+      <c r="I12" s="22"/>
+      <c r="J12" s="141"/>
+      <c r="K12" s="142" t="str">
+        <f>IF('Fase de Grupos'!AH42=3,'Fase de Grupos'!AF42,"2º do Grupo G")</f>
+        <v>Juventus</v>
       </c>
       <c r="L12" s="114" t="str">
         <f t="shared" si="0"/>
         <v/>
       </c>
       <c r="M12" s="115" t="str">
-        <f>IF(OR(G12="",I12=""),"Vencedor VII",IF(G12&lt;&gt;I12,IF(G12&gt;I12,E12,K12),IF(SUM(F12:G12)=SUM(I12:J12),"Vencedor VII",IF(SUM(F12:G12)&gt;SUM(I12:J12),E12,K12))))</f>
-        <v>Vencedor VII</v>
+        <f>IF(OR(G12="",I12=""),"Vencedor VIII",IF(G12&lt;&gt;I12,IF(G12&gt;I12,E12,K12),IF(SUM(F12:G12)=SUM(I12:J12),"Vencedor VIII",IF(SUM(F12:G12)&gt;SUM(I12:J12),E12,K12))))</f>
+        <v>Vencedor VIII</v>
       </c>
     </row>
     <row r="13" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13" s="128" t="s">
-        <v>105</v>
-      </c>
-      <c r="C13" s="139">
-        <v>45839</v>
-      </c>
-      <c r="D13" s="54" t="s">
+      <c r="C13" s="116"/>
+    </row>
+    <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="109"/>
+      <c r="B14" s="180" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="181"/>
+      <c r="D14" s="181"/>
+      <c r="E14" s="181"/>
+      <c r="F14" s="181"/>
+      <c r="G14" s="181"/>
+      <c r="H14" s="181"/>
+      <c r="I14" s="181"/>
+      <c r="J14" s="181"/>
+      <c r="K14" s="182"/>
+      <c r="L14" s="110"/>
+      <c r="M14" s="111"/>
+      <c r="N14" s="111"/>
+    </row>
+    <row r="15" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="148"/>
+      <c r="C15" s="149" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="150" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="183" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="183"/>
+      <c r="G15" s="183" t="s">
+        <v>13</v>
+      </c>
+      <c r="H15" s="183"/>
+      <c r="I15" s="183"/>
+      <c r="J15" s="183" t="s">
+        <v>12</v>
+      </c>
+      <c r="K15" s="184"/>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B16" s="129" t="s">
+        <v>15</v>
+      </c>
+      <c r="C16" s="156">
+        <v>45842</v>
+      </c>
+      <c r="D16" s="68" t="s">
+        <v>42</v>
+      </c>
+      <c r="E16" s="157" t="str">
+        <f>M5</f>
+        <v>Vencedor I</v>
+      </c>
+      <c r="F16" s="158"/>
+      <c r="G16" s="23"/>
+      <c r="H16" s="99" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="23"/>
+      <c r="J16" s="159"/>
+      <c r="K16" s="160" t="str">
+        <f>M6</f>
+        <v>Vencedor II</v>
+      </c>
+      <c r="L16" s="114" t="str">
+        <f>IF(OR(G16="",I16=""),"",IF(G16=I16,"emp",""))</f>
+        <v/>
+      </c>
+      <c r="M16" s="115" t="str">
+        <f>IF(OR(G16="",I16=""),"Vencedor A",IF(G16&lt;&gt;I16,IF(G16&gt;I16,E16,K16),IF(SUM(F16:G16)=SUM(I16:J16),"Vencedor A",IF(SUM(F16:G16)&gt;SUM(I16:J16),E16,K16))))</f>
+        <v>Vencedor A</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B17" s="130" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="124">
+        <v>45842</v>
+      </c>
+      <c r="D17" s="40" t="s">
         <v>41</v>
       </c>
-      <c r="E13" s="15" t="str">
-        <f>IF('Fase de Grupos'!AH47=3,'Fase de Grupos'!AF47,"1º do Grupo H")</f>
-        <v>1º do Grupo H</v>
-      </c>
-      <c r="F13" s="140"/>
-      <c r="G13" s="22"/>
-      <c r="H13" s="16" t="s">
+      <c r="E17" s="24" t="str">
+        <f>M9</f>
+        <v>Vencedor V</v>
+      </c>
+      <c r="F17" s="125"/>
+      <c r="G17" s="21"/>
+      <c r="H17" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="I13" s="22"/>
-      <c r="J13" s="141"/>
-      <c r="K13" s="142" t="str">
-        <f>IF('Fase de Grupos'!AH42=3,'Fase de Grupos'!AF42,"2º do Grupo G")</f>
-        <v>Juventus</v>
-      </c>
-      <c r="L13" s="114" t="str">
-        <f t="shared" si="0"/>
+      <c r="I17" s="21"/>
+      <c r="J17" s="126"/>
+      <c r="K17" s="143" t="str">
+        <f>M10</f>
+        <v>Vencedor VI</v>
+      </c>
+      <c r="L17" s="114" t="str">
+        <f t="shared" ref="L17:L19" si="1">IF(OR(G17="",I17=""),"",IF(G17=I17,"emp",""))</f>
         <v/>
       </c>
-      <c r="M13" s="115" t="str">
-        <f>IF(OR(G13="",I13=""),"Vencedor VIII",IF(G13&lt;&gt;I13,IF(G13&gt;I13,E13,K13),IF(SUM(F13:G13)=SUM(I13:J13),"Vencedor VIII",IF(SUM(F13:G13)&gt;SUM(I13:J13),E13,K13))))</f>
-        <v>Vencedor VIII</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C14" s="116"/>
-    </row>
-    <row r="15" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C15" s="116"/>
-    </row>
-    <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="109"/>
-      <c r="B16" s="179" t="s">
-        <v>61</v>
-      </c>
-      <c r="C16" s="180"/>
-      <c r="D16" s="180"/>
-      <c r="E16" s="180"/>
-      <c r="F16" s="180"/>
-      <c r="G16" s="180"/>
-      <c r="H16" s="180"/>
-      <c r="I16" s="180"/>
-      <c r="J16" s="180"/>
-      <c r="K16" s="181"/>
-      <c r="L16" s="110"/>
-      <c r="M16" s="111"/>
-      <c r="N16" s="111"/>
-    </row>
-    <row r="17" spans="1:17" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B17" s="148"/>
-      <c r="C17" s="149" t="s">
-        <v>10</v>
-      </c>
-      <c r="D17" s="150" t="s">
-        <v>11</v>
-      </c>
-      <c r="E17" s="182" t="s">
-        <v>12</v>
-      </c>
-      <c r="F17" s="182"/>
-      <c r="G17" s="182" t="s">
-        <v>13</v>
-      </c>
-      <c r="H17" s="182"/>
-      <c r="I17" s="182"/>
-      <c r="J17" s="182" t="s">
-        <v>12</v>
-      </c>
-      <c r="K17" s="183"/>
+      <c r="M17" s="115" t="str">
+        <f>IF(OR(G17="",I17=""),"Vencedor B",IF(G17&lt;&gt;I17,IF(G17&gt;I17,E17,K17),IF(SUM(F17:G17)=SUM(I17:J17),"Vencedor B",IF(SUM(F17:G17)&gt;SUM(I17:J17),E17,K17))))</f>
+        <v>Vencedor B</v>
+      </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B18" s="129" t="s">
-        <v>15</v>
-      </c>
-      <c r="C18" s="156">
-        <v>45842</v>
-      </c>
-      <c r="D18" s="68" t="s">
-        <v>42</v>
-      </c>
-      <c r="E18" s="157" t="str">
-        <f>M6</f>
-        <v>Vencedor I</v>
-      </c>
-      <c r="F18" s="158"/>
-      <c r="G18" s="23"/>
-      <c r="H18" s="99" t="s">
+      <c r="B18" s="130" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="124">
+        <v>45843</v>
+      </c>
+      <c r="D18" s="40" t="s">
+        <v>41</v>
+      </c>
+      <c r="E18" s="24" t="str">
+        <f>M7</f>
+        <v>Vencedor III</v>
+      </c>
+      <c r="F18" s="125"/>
+      <c r="G18" s="21"/>
+      <c r="H18" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="I18" s="23"/>
-      <c r="J18" s="159"/>
-      <c r="K18" s="160" t="str">
-        <f>M7</f>
-        <v>Vencedor II</v>
+      <c r="I18" s="21"/>
+      <c r="J18" s="126"/>
+      <c r="K18" s="143" t="str">
+        <f>M8</f>
+        <v>Vencedor IV</v>
       </c>
       <c r="L18" s="114" t="str">
-        <f>IF(OR(G18="",I18=""),"",IF(G18=I18,"emp",""))</f>
-        <v/>
-      </c>
-      <c r="M18" s="115" t="str">
-        <f>IF(OR(G18="",I18=""),"Vencedor A",IF(G18&lt;&gt;I18,IF(G18&gt;I18,E18,K18),IF(SUM(F18:G18)=SUM(I18:J18),"Vencedor A",IF(SUM(F18:G18)&gt;SUM(I18:J18),E18,K18))))</f>
-        <v>Vencedor A</v>
-      </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B19" s="130" t="s">
-        <v>43</v>
-      </c>
-      <c r="C19" s="124">
-        <v>45842</v>
-      </c>
-      <c r="D19" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="E19" s="24" t="str">
-        <f>M10</f>
-        <v>Vencedor V</v>
-      </c>
-      <c r="F19" s="125"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="90" t="s">
-        <v>17</v>
-      </c>
-      <c r="I19" s="21"/>
-      <c r="J19" s="126"/>
-      <c r="K19" s="143" t="str">
-        <f>M11</f>
-        <v>Vencedor VI</v>
-      </c>
-      <c r="L19" s="114" t="str">
-        <f t="shared" ref="L19:L21" si="1">IF(OR(G19="",I19=""),"",IF(G19=I19,"emp",""))</f>
-        <v/>
-      </c>
-      <c r="M19" s="115" t="str">
-        <f>IF(OR(G19="",I19=""),"Vencedor B",IF(G19&lt;&gt;I19,IF(G19&gt;I19,E19,K19),IF(SUM(F19:G19)=SUM(I19:J19),"Vencedor B",IF(SUM(F19:G19)&gt;SUM(I19:J19),E19,K19))))</f>
-        <v>Vencedor B</v>
-      </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B20" s="130" t="s">
-        <v>45</v>
-      </c>
-      <c r="C20" s="124">
-        <v>45843</v>
-      </c>
-      <c r="D20" s="40" t="s">
-        <v>41</v>
-      </c>
-      <c r="E20" s="24" t="str">
-        <f>M8</f>
-        <v>Vencedor III</v>
-      </c>
-      <c r="F20" s="125"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="90" t="s">
-        <v>17</v>
-      </c>
-      <c r="I20" s="21"/>
-      <c r="J20" s="126"/>
-      <c r="K20" s="143" t="str">
-        <f>M9</f>
-        <v>Vencedor IV</v>
-      </c>
-      <c r="L20" s="114" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="M20" s="115" t="str">
-        <f>IF(OR(G20="",I20=""),"Vencedor C",IF(G20&lt;&gt;I20,IF(G20&gt;I20,E20,K20),IF(SUM(F20:G20)=SUM(I20:J20),"Vencedor C",IF(SUM(F20:G20)&gt;SUM(I20:J20),E20,K20))))</f>
+      <c r="M18" s="115" t="str">
+        <f>IF(OR(G18="",I18=""),"Vencedor C",IF(G18&lt;&gt;I18,IF(G18&gt;I18,E18,K18),IF(SUM(F18:G18)=SUM(I18:J18),"Vencedor C",IF(SUM(F18:G18)&gt;SUM(I18:J18),E18,K18))))</f>
         <v>Vencedor C</v>
       </c>
     </row>
-    <row r="21" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="131" t="s">
+    <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="131" t="s">
         <v>40</v>
       </c>
-      <c r="C21" s="144">
+      <c r="C19" s="144">
         <v>45843</v>
       </c>
-      <c r="D21" s="54" t="s">
+      <c r="D19" s="54" t="s">
         <v>42</v>
       </c>
-      <c r="E21" s="25" t="str">
+      <c r="E19" s="25" t="str">
+        <f>M11</f>
+        <v>Vencedor VII</v>
+      </c>
+      <c r="F19" s="145"/>
+      <c r="G19" s="22"/>
+      <c r="H19" s="92" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="22"/>
+      <c r="J19" s="146"/>
+      <c r="K19" s="147" t="str">
         <f>M12</f>
-        <v>Vencedor VII</v>
-      </c>
-      <c r="F21" s="145"/>
-      <c r="G21" s="22"/>
-      <c r="H21" s="92" t="s">
-        <v>17</v>
-      </c>
-      <c r="I21" s="22"/>
-      <c r="J21" s="146"/>
-      <c r="K21" s="147" t="str">
-        <f>M13</f>
         <v>Vencedor VIII</v>
       </c>
-      <c r="L21" s="114" t="str">
+      <c r="L19" s="114" t="str">
         <f t="shared" si="1"/>
         <v/>
       </c>
-      <c r="M21" s="115" t="str">
-        <f>IF(OR(G21="",I21=""),"Vencedor D",IF(G21&lt;&gt;I21,IF(G21&gt;I21,E21,K21),IF(SUM(F21:G21)=SUM(I21:J21),"Vencedor D",IF(SUM(F21:G21)&gt;SUM(I21:J21),E21,K21))))</f>
+      <c r="M19" s="115" t="str">
+        <f>IF(OR(G19="",I19=""),"Vencedor D",IF(G19&lt;&gt;I19,IF(G19&gt;I19,E19,K19),IF(SUM(F19:G19)=SUM(I19:J19),"Vencedor D",IF(SUM(F19:G19)&gt;SUM(I19:J19),E19,K19))))</f>
         <v>Vencedor D</v>
       </c>
     </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C22" s="116"/>
-    </row>
-    <row r="23" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="116"/>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="109"/>
-      <c r="B24" s="179" t="s">
+    <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="116"/>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A21" s="109"/>
+      <c r="B21" s="180" t="s">
         <v>62</v>
       </c>
-      <c r="C24" s="180"/>
-      <c r="D24" s="180"/>
-      <c r="E24" s="180"/>
-      <c r="F24" s="180"/>
-      <c r="G24" s="180"/>
-      <c r="H24" s="180"/>
-      <c r="I24" s="180"/>
-      <c r="J24" s="180"/>
-      <c r="K24" s="181"/>
-      <c r="L24" s="110"/>
-      <c r="M24" s="111"/>
-      <c r="N24" s="111"/>
-      <c r="O24" s="111"/>
-      <c r="P24" s="111"/>
-      <c r="Q24" s="111"/>
-    </row>
-    <row r="25" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="148"/>
-      <c r="C25" s="149" t="s">
+      <c r="C21" s="181"/>
+      <c r="D21" s="181"/>
+      <c r="E21" s="181"/>
+      <c r="F21" s="181"/>
+      <c r="G21" s="181"/>
+      <c r="H21" s="181"/>
+      <c r="I21" s="181"/>
+      <c r="J21" s="181"/>
+      <c r="K21" s="182"/>
+      <c r="L21" s="110"/>
+      <c r="M21" s="111"/>
+      <c r="N21" s="111"/>
+      <c r="O21" s="111"/>
+      <c r="P21" s="111"/>
+      <c r="Q21" s="111"/>
+    </row>
+    <row r="22" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="148"/>
+      <c r="C22" s="149" t="s">
         <v>10</v>
       </c>
-      <c r="D25" s="150" t="s">
+      <c r="D22" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E25" s="182" t="s">
+      <c r="E22" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="F25" s="182"/>
-      <c r="G25" s="182" t="s">
+      <c r="F22" s="183"/>
+      <c r="G22" s="183" t="s">
         <v>13</v>
       </c>
-      <c r="H25" s="182"/>
-      <c r="I25" s="182"/>
-      <c r="J25" s="182" t="s">
+      <c r="H22" s="183"/>
+      <c r="I22" s="183"/>
+      <c r="J22" s="183" t="s">
         <v>12</v>
       </c>
-      <c r="K25" s="183"/>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="B26" s="151" t="s">
+      <c r="K22" s="184"/>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B23" s="151" t="s">
         <v>63</v>
       </c>
-      <c r="C26" s="152">
+      <c r="C23" s="152">
         <v>45846</v>
       </c>
-      <c r="D26" s="68" t="s">
+      <c r="D23" s="68" t="s">
         <v>41</v>
       </c>
-      <c r="E26" s="20" t="str">
+      <c r="E23" s="20" t="str">
+        <f>M16</f>
+        <v>Vencedor A</v>
+      </c>
+      <c r="F23" s="153"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="23"/>
+      <c r="J23" s="154"/>
+      <c r="K23" s="155" t="str">
+        <f>M17</f>
+        <v>Vencedor B</v>
+      </c>
+      <c r="L23" s="114" t="str">
+        <f>IF(OR(G23="",I23=""),"",IF(G23=I23,"emp",""))</f>
+        <v/>
+      </c>
+      <c r="M23" s="115" t="str">
+        <f>IF(OR(G23="",I23=""),"Vencedor S1",IF(G23&lt;&gt;I23,IF(G23&gt;I23,E23,K23),IF(SUM(F23:G23)=SUM(I23:J23),"Vencedor S1",IF(SUM(F23:G23)&gt;SUM(I23:J23),E23,K23))))</f>
+        <v>Vencedor S1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="128" t="s">
+        <v>64</v>
+      </c>
+      <c r="C24" s="139">
+        <v>45847</v>
+      </c>
+      <c r="D24" s="54" t="s">
+        <v>41</v>
+      </c>
+      <c r="E24" s="15" t="str">
         <f>M18</f>
-        <v>Vencedor A</v>
-      </c>
-      <c r="F26" s="153"/>
-      <c r="G26" s="23"/>
-      <c r="H26" s="19" t="s">
+        <v>Vencedor C</v>
+      </c>
+      <c r="F24" s="140"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="I26" s="23"/>
-      <c r="J26" s="154"/>
-      <c r="K26" s="155" t="str">
+      <c r="I24" s="22"/>
+      <c r="J24" s="141"/>
+      <c r="K24" s="142" t="str">
         <f>M19</f>
-        <v>Vencedor B</v>
-      </c>
-      <c r="L26" s="114" t="str">
-        <f>IF(OR(G26="",I26=""),"",IF(G26=I26,"emp",""))</f>
+        <v>Vencedor D</v>
+      </c>
+      <c r="L24" s="114" t="str">
+        <f t="shared" ref="L24" si="2">IF(OR(G24="",I24=""),"",IF(G24=I24,"emp",""))</f>
         <v/>
       </c>
+      <c r="M24" s="115" t="str">
+        <f>IF(OR(G24="",I24=""),"Vencedor S2",IF(G24&lt;&gt;I24,IF(G24&gt;I24,E24,K24),IF(SUM(F24:G24)=SUM(I24:J24),"Vencedor S2",IF(SUM(F24:G24)&gt;SUM(I24:J24),E24,K24))))</f>
+        <v>Vencedor S2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C25" s="116"/>
+      <c r="M25" s="115" t="str">
+        <f>IF(OR(G23="",I23=""),"Perdedor S1",IF(G23&lt;&gt;I23,IF(G23&lt;I23,E23,K23),IF(SUM(F23:G23)=SUM(I23:J23),"Perdedor S1",IF(SUM(F23:G23)&lt;SUM(I23:J23),E23,K23))))</f>
+        <v>Perdedor S1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="116"/>
       <c r="M26" s="115" t="str">
-        <f>IF(OR(G26="",I26=""),"Vencedor S1",IF(G26&lt;&gt;I26,IF(G26&gt;I26,E26,K26),IF(SUM(F26:G26)=SUM(I26:J26),"Vencedor S1",IF(SUM(F26:G26)&gt;SUM(I26:J26),E26,K26))))</f>
+        <f>IF(OR(G24="",I24=""),"Perdedor S2",IF(G24&lt;&gt;I24,IF(G24&lt;I24,E24,K24),IF(SUM(F24:G24)=SUM(I24:J24),"Perdedor S2",IF(SUM(F24:G24)&lt;SUM(I24:J24),E24,K24))))</f>
+        <v>Perdedor S2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A27" s="109"/>
+      <c r="B27" s="180" t="s">
+        <v>65</v>
+      </c>
+      <c r="C27" s="181"/>
+      <c r="D27" s="181"/>
+      <c r="E27" s="181"/>
+      <c r="F27" s="181"/>
+      <c r="G27" s="181"/>
+      <c r="H27" s="181"/>
+      <c r="I27" s="181"/>
+      <c r="J27" s="181"/>
+      <c r="K27" s="182"/>
+      <c r="L27" s="110"/>
+      <c r="M27" s="111"/>
+      <c r="N27" s="111"/>
+      <c r="O27" s="111"/>
+      <c r="P27" s="111"/>
+      <c r="Q27" s="111"/>
+    </row>
+    <row r="28" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="148"/>
+      <c r="C28" s="149" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="150" t="s">
+        <v>11</v>
+      </c>
+      <c r="E28" s="183" t="s">
+        <v>12</v>
+      </c>
+      <c r="F28" s="183"/>
+      <c r="G28" s="183" t="s">
+        <v>13</v>
+      </c>
+      <c r="H28" s="183"/>
+      <c r="I28" s="183"/>
+      <c r="J28" s="183" t="s">
+        <v>12</v>
+      </c>
+      <c r="K28" s="184"/>
+    </row>
+    <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="161" t="s">
+        <v>53</v>
+      </c>
+      <c r="C29" s="162">
+        <v>45851</v>
+      </c>
+      <c r="D29" s="163" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="164" t="str">
+        <f>M23</f>
         <v>Vencedor S1</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="128" t="s">
-        <v>64</v>
-      </c>
-      <c r="C27" s="139">
-        <v>45847</v>
-      </c>
-      <c r="D27" s="54" t="s">
-        <v>41</v>
-      </c>
-      <c r="E27" s="15" t="str">
-        <f>M20</f>
-        <v>Vencedor C</v>
-      </c>
-      <c r="F27" s="140"/>
-      <c r="G27" s="22"/>
-      <c r="H27" s="16" t="s">
+      <c r="F29" s="165"/>
+      <c r="G29" s="166"/>
+      <c r="H29" s="167" t="s">
         <v>17</v>
       </c>
-      <c r="I27" s="22"/>
-      <c r="J27" s="141"/>
-      <c r="K27" s="142" t="str">
-        <f>M21</f>
-        <v>Vencedor D</v>
-      </c>
-      <c r="L27" s="114" t="str">
-        <f t="shared" ref="L27" si="2">IF(OR(G27="",I27=""),"",IF(G27=I27,"emp",""))</f>
+      <c r="I29" s="166"/>
+      <c r="J29" s="168"/>
+      <c r="K29" s="169" t="str">
+        <f>M24</f>
+        <v>Vencedor S2</v>
+      </c>
+      <c r="L29" s="114" t="str">
+        <f>IF(OR(G29="",I29=""),"",IF(G29=I29,"emp",""))</f>
         <v/>
       </c>
-      <c r="M27" s="115" t="str">
-        <f>IF(OR(G27="",I27=""),"Vencedor S2",IF(G27&lt;&gt;I27,IF(G27&gt;I27,E27,K27),IF(SUM(F27:G27)=SUM(I27:J27),"Vencedor S2",IF(SUM(F27:G27)&gt;SUM(I27:J27),E27,K27))))</f>
-        <v>Vencedor S2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C28" s="116"/>
-      <c r="M28" s="115" t="str">
-        <f>IF(OR(G26="",I26=""),"Perdedor S1",IF(G26&lt;&gt;I26,IF(G26&lt;I26,E26,K26),IF(SUM(F26:G26)=SUM(I26:J26),"Perdedor S1",IF(SUM(F26:G26)&lt;SUM(I26:J26),E26,K26))))</f>
-        <v>Perdedor S1</v>
-      </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C29" s="116"/>
       <c r="M29" s="115" t="str">
-        <f>IF(OR(G27="",I27=""),"Perdedor S2",IF(G27&lt;&gt;I27,IF(G27&lt;I27,E27,K27),IF(SUM(F27:G27)=SUM(I27:J27),"Perdedor S2",IF(SUM(F27:G27)&lt;SUM(I27:J27),E27,K27))))</f>
-        <v>Perdedor S2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <f>IF(OR(G29="",I29=""),"1º Lugar",IF(G29&lt;&gt;I29,IF(G29&gt;I29,E29,K29),IF(SUM(F29:G29)=SUM(I29:J29),"1º Lugar",IF(SUM(F29:G29)&gt;SUM(I29:J29),E29,K29))))</f>
+        <v>1º Lugar</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C30" s="116"/>
+      <c r="M30" s="115" t="str">
+        <f>IF(OR(G29="",I29=""),"2º Lugar",IF(G29&lt;&gt;I29,IF(G29&lt;I29,E29,K29),IF(SUM(F29:G29)=SUM(I29:J29),"2º Lugar",IF(SUM(F29:G29)&lt;SUM(I29:J29),E29,K29))))</f>
+        <v>2º Lugar</v>
+      </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A31" s="109"/>
-      <c r="B31" s="179" t="s">
-        <v>65</v>
-      </c>
-      <c r="C31" s="180"/>
-      <c r="D31" s="180"/>
-      <c r="E31" s="180"/>
-      <c r="F31" s="180"/>
-      <c r="G31" s="180"/>
-      <c r="H31" s="180"/>
-      <c r="I31" s="180"/>
-      <c r="J31" s="180"/>
-      <c r="K31" s="181"/>
-      <c r="L31" s="110"/>
-      <c r="M31" s="111"/>
-      <c r="N31" s="111"/>
-      <c r="O31" s="111"/>
-      <c r="P31" s="111"/>
-      <c r="Q31" s="111"/>
-    </row>
-    <row r="32" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B32" s="148"/>
-      <c r="C32" s="149" t="s">
-        <v>10</v>
-      </c>
-      <c r="D32" s="150" t="s">
-        <v>11</v>
-      </c>
-      <c r="E32" s="182" t="s">
-        <v>12</v>
-      </c>
-      <c r="F32" s="182"/>
-      <c r="G32" s="182" t="s">
-        <v>13</v>
-      </c>
-      <c r="H32" s="182"/>
-      <c r="I32" s="182"/>
-      <c r="J32" s="182" t="s">
-        <v>12</v>
-      </c>
-      <c r="K32" s="183"/>
-    </row>
-    <row r="33" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B33" s="161" t="s">
-        <v>53</v>
-      </c>
-      <c r="C33" s="162">
-        <v>45851</v>
-      </c>
-      <c r="D33" s="163" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="164" t="str">
-        <f>M26</f>
-        <v>Vencedor S1</v>
-      </c>
-      <c r="F33" s="165"/>
-      <c r="G33" s="166"/>
-      <c r="H33" s="167" t="s">
-        <v>17</v>
-      </c>
-      <c r="I33" s="166"/>
-      <c r="J33" s="168"/>
-      <c r="K33" s="169" t="str">
-        <f>M27</f>
-        <v>Vencedor S2</v>
-      </c>
-      <c r="L33" s="114" t="str">
-        <f>IF(OR(G33="",I33=""),"",IF(G33=I33,"emp",""))</f>
+      <c r="C31" s="116"/>
+    </row>
+    <row r="32" spans="1:17" s="137" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="135"/>
+      <c r="B32" s="179" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="179"/>
+      <c r="D32" s="179"/>
+      <c r="E32" s="173" t="str">
+        <f>IF(M29="1º Lugar","",M29)</f>
         <v/>
       </c>
-      <c r="M33" s="115" t="str">
-        <f>IF(OR(G33="",I33=""),"1º Lugar",IF(G33&lt;&gt;I33,IF(G33&gt;I33,E33,K33),IF(SUM(F33:G33)=SUM(I33:J33),"1º Lugar",IF(SUM(F33:G33)&gt;SUM(I33:J33),E33,K33))))</f>
-        <v>1º Lugar</v>
-      </c>
+      <c r="F32" s="173"/>
+      <c r="G32" s="173"/>
+      <c r="H32" s="174"/>
+      <c r="I32" s="174"/>
+      <c r="J32" s="135"/>
+      <c r="K32" s="135"/>
+      <c r="L32" s="136"/>
+      <c r="M32" s="136"/>
+      <c r="N32" s="136"/>
+      <c r="O32" s="136"/>
+      <c r="P32" s="136"/>
+      <c r="Q32" s="136"/>
+    </row>
+    <row r="33" spans="1:17" s="137" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="135"/>
+      <c r="B33" s="179" t="s">
+        <v>106</v>
+      </c>
+      <c r="C33" s="179"/>
+      <c r="D33" s="179"/>
+      <c r="E33" s="175" t="str">
+        <f>IF(M30="2º Lugar","",M30)</f>
+        <v/>
+      </c>
+      <c r="F33" s="175"/>
+      <c r="G33" s="175"/>
+      <c r="H33" s="174"/>
+      <c r="I33" s="174"/>
+      <c r="J33" s="135"/>
+      <c r="K33" s="135"/>
+      <c r="L33" s="136"/>
+      <c r="M33" s="136"/>
+      <c r="N33" s="136"/>
+      <c r="O33" s="136"/>
+      <c r="P33" s="136"/>
+      <c r="Q33" s="136"/>
     </row>
     <row r="34" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C34" s="116"/>
-      <c r="M34" s="115" t="str">
-        <f>IF(OR(G33="",I33=""),"2º Lugar",IF(G33&lt;&gt;I33,IF(G33&lt;I33,E33,K33),IF(SUM(F33:G33)=SUM(I33:J33),"2º Lugar",IF(SUM(F33:G33)&lt;SUM(I33:J33),E33,K33))))</f>
-        <v>2º Lugar</v>
-      </c>
     </row>
     <row r="35" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C35" s="116"/>
     </row>
-    <row r="36" spans="1:17" s="137" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="135"/>
-      <c r="B36" s="184" t="s">
-        <v>66</v>
-      </c>
-      <c r="C36" s="184"/>
-      <c r="D36" s="184"/>
-      <c r="E36" s="173" t="str">
-        <f>IF(M33="1º Lugar","",M33)</f>
-        <v/>
-      </c>
-      <c r="F36" s="173"/>
-      <c r="G36" s="173"/>
-      <c r="H36" s="174"/>
-      <c r="I36" s="174"/>
-      <c r="J36" s="135"/>
-      <c r="K36" s="135"/>
-      <c r="L36" s="136"/>
-      <c r="M36" s="136"/>
-      <c r="N36" s="136"/>
-      <c r="O36" s="136"/>
-      <c r="P36" s="136"/>
-      <c r="Q36" s="136"/>
-    </row>
-    <row r="37" spans="1:17" s="137" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="135"/>
-      <c r="B37" s="184" t="s">
-        <v>106</v>
-      </c>
-      <c r="C37" s="184"/>
-      <c r="D37" s="184"/>
-      <c r="E37" s="175" t="str">
-        <f>IF(M34="2º Lugar","",M34)</f>
-        <v/>
-      </c>
-      <c r="F37" s="175"/>
-      <c r="G37" s="175"/>
-      <c r="H37" s="174"/>
-      <c r="I37" s="174"/>
-      <c r="J37" s="135"/>
-      <c r="K37" s="135"/>
-      <c r="L37" s="136"/>
-      <c r="M37" s="136"/>
-      <c r="N37" s="136"/>
-      <c r="O37" s="136"/>
-      <c r="P37" s="136"/>
-      <c r="Q37" s="136"/>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C36" s="116"/>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="C37" s="116"/>
     </row>
     <row r="38" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C38" s="116"/>
@@ -11333,16 +11478,32 @@
       <c r="C43" s="116"/>
     </row>
     <row r="44" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C44" s="116"/>
+      <c r="C44" s="50"/>
+      <c r="D44" s="50"/>
+      <c r="E44" s="50"/>
+      <c r="H44" s="50"/>
+      <c r="K44" s="50"/>
     </row>
     <row r="45" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C45" s="116"/>
+      <c r="C45" s="50"/>
+      <c r="D45" s="50"/>
+      <c r="E45" s="50"/>
+      <c r="H45" s="50"/>
+      <c r="K45" s="50"/>
     </row>
     <row r="46" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C46" s="116"/>
+      <c r="C46" s="50"/>
+      <c r="D46" s="50"/>
+      <c r="E46" s="50"/>
+      <c r="H46" s="50"/>
+      <c r="K46" s="50"/>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="C47" s="116"/>
+      <c r="C47" s="50"/>
+      <c r="D47" s="50"/>
+      <c r="E47" s="50"/>
+      <c r="H47" s="50"/>
+      <c r="K47" s="50"/>
     </row>
     <row r="48" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C48" s="50"/>
@@ -11393,238 +11554,199 @@
       <c r="H54" s="50"/>
       <c r="K54" s="50"/>
     </row>
-    <row r="55" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C55" s="50"/>
-      <c r="D55" s="50"/>
-      <c r="E55" s="50"/>
-      <c r="H55" s="50"/>
-      <c r="K55" s="50"/>
-    </row>
-    <row r="56" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C56" s="50"/>
-      <c r="D56" s="50"/>
-      <c r="E56" s="50"/>
-      <c r="H56" s="50"/>
-      <c r="K56" s="50"/>
-    </row>
-    <row r="57" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C57" s="50"/>
-      <c r="D57" s="50"/>
-      <c r="E57" s="50"/>
-      <c r="H57" s="50"/>
-      <c r="K57" s="50"/>
-    </row>
-    <row r="58" spans="3:11" x14ac:dyDescent="0.25">
-      <c r="C58" s="50"/>
-      <c r="D58" s="50"/>
-      <c r="E58" s="50"/>
-      <c r="H58" s="50"/>
-      <c r="K58" s="50"/>
-    </row>
   </sheetData>
   <sheetProtection password="CC01" sheet="1" selectLockedCells="1"/>
   <mergeCells count="18">
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B31:K31"/>
-    <mergeCell ref="E32:F32"/>
-    <mergeCell ref="G32:I32"/>
-    <mergeCell ref="J32:K32"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B24:K24"/>
-    <mergeCell ref="E25:F25"/>
-    <mergeCell ref="G25:I25"/>
-    <mergeCell ref="J25:K25"/>
-    <mergeCell ref="E17:F17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="J17:K17"/>
-    <mergeCell ref="B4:K4"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="G5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="B16:K16"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="B14:K14"/>
+    <mergeCell ref="B21:K21"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="G22:I22"/>
+    <mergeCell ref="J22:K22"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="G15:I15"/>
+    <mergeCell ref="J15:K15"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B27:K27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="B32:D32"/>
   </mergeCells>
-  <conditionalFormatting sqref="F6">
+  <conditionalFormatting sqref="F5">
     <cfRule type="expression" dxfId="31" priority="128">
+      <formula>L5="emp"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J5">
+    <cfRule type="expression" dxfId="30" priority="127">
+      <formula>L5="emp"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5:K12">
+    <cfRule type="expression" dxfId="29" priority="12">
+      <formula>$K5=$M5</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="28" priority="126">
+      <formula>Q5="emp"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K5:K12">
+    <cfRule type="expression" dxfId="27" priority="125">
+      <formula>Q5="emp"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B32:D33">
+    <cfRule type="expression" dxfId="26" priority="118">
+      <formula>E32&lt;&gt;""</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F16:F19">
+    <cfRule type="expression" dxfId="25" priority="47">
+      <formula>L16="emp"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="J16:J19">
+    <cfRule type="expression" dxfId="24" priority="46">
+      <formula>L16="emp"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K16:K19">
+    <cfRule type="expression" dxfId="23" priority="45">
+      <formula>Q16="emp"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F6:F12">
+    <cfRule type="expression" dxfId="22" priority="42">
       <formula>L6="emp"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J6">
-    <cfRule type="expression" dxfId="30" priority="127">
+  <conditionalFormatting sqref="J6:J12">
+    <cfRule type="expression" dxfId="21" priority="41">
       <formula>L6="emp"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6:K13">
-    <cfRule type="expression" dxfId="29" priority="12">
-      <formula>$K6=$M6</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="28" priority="126">
+  <conditionalFormatting sqref="K6:K12">
+    <cfRule type="expression" dxfId="20" priority="40">
       <formula>Q6="emp"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K6:K13">
-    <cfRule type="expression" dxfId="27" priority="125">
+  <conditionalFormatting sqref="K6:K12">
+    <cfRule type="expression" dxfId="19" priority="39">
       <formula>Q6="emp"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B36:D37">
-    <cfRule type="expression" dxfId="26" priority="118">
-      <formula>E36&lt;&gt;""</formula>
+  <conditionalFormatting sqref="F23">
+    <cfRule type="expression" dxfId="18" priority="30">
+      <formula>L23="emp"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F18:F21">
-    <cfRule type="expression" dxfId="25" priority="47">
-      <formula>L18="emp"</formula>
+  <conditionalFormatting sqref="J23">
+    <cfRule type="expression" dxfId="17" priority="29">
+      <formula>L23="emp"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J18:J21">
-    <cfRule type="expression" dxfId="24" priority="46">
-      <formula>L18="emp"</formula>
+  <conditionalFormatting sqref="F24">
+    <cfRule type="expression" dxfId="16" priority="24">
+      <formula>L24="emp"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K18:K21">
-    <cfRule type="expression" dxfId="23" priority="45">
-      <formula>Q18="emp"</formula>
+  <conditionalFormatting sqref="J24">
+    <cfRule type="expression" dxfId="15" priority="23">
+      <formula>L24="emp"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F7:F13">
-    <cfRule type="expression" dxfId="22" priority="42">
-      <formula>L7="emp"</formula>
+  <conditionalFormatting sqref="F29">
+    <cfRule type="expression" dxfId="14" priority="18">
+      <formula>L29="emp"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="J7:J13">
-    <cfRule type="expression" dxfId="21" priority="41">
-      <formula>L7="emp"</formula>
+  <conditionalFormatting sqref="J29">
+    <cfRule type="expression" dxfId="13" priority="17">
+      <formula>L29="emp"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K7:K13">
-    <cfRule type="expression" dxfId="20" priority="40">
-      <formula>Q7="emp"</formula>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="expression" dxfId="12" priority="14">
+      <formula>$E5=$M5</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K7:K13">
-    <cfRule type="expression" dxfId="19" priority="39">
-      <formula>Q7="emp"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F26">
-    <cfRule type="expression" dxfId="18" priority="30">
-      <formula>L26="emp"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J26">
-    <cfRule type="expression" dxfId="17" priority="29">
-      <formula>L26="emp"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F27">
-    <cfRule type="expression" dxfId="16" priority="24">
-      <formula>L27="emp"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J27">
-    <cfRule type="expression" dxfId="15" priority="23">
-      <formula>L27="emp"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F33">
-    <cfRule type="expression" dxfId="14" priority="18">
-      <formula>L33="emp"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="J33">
-    <cfRule type="expression" dxfId="13" priority="17">
-      <formula>L33="emp"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E6">
-    <cfRule type="expression" dxfId="12" priority="14">
+  <conditionalFormatting sqref="E6:E12">
+    <cfRule type="expression" dxfId="11" priority="13">
       <formula>$E6=$M6</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E7:E13">
-    <cfRule type="expression" dxfId="11" priority="13">
-      <formula>$E7=$M7</formula>
+  <conditionalFormatting sqref="E16">
+    <cfRule type="expression" dxfId="10" priority="11">
+      <formula>$E16=$M16</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E18">
-    <cfRule type="expression" dxfId="10" priority="11">
-      <formula>$E18=$M18</formula>
+  <conditionalFormatting sqref="E17:E19">
+    <cfRule type="expression" dxfId="9" priority="10">
+      <formula>$E17=$M17</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E19:E21">
-    <cfRule type="expression" dxfId="9" priority="10">
-      <formula>$E19=$M19</formula>
+  <conditionalFormatting sqref="K16">
+    <cfRule type="expression" dxfId="8" priority="9">
+      <formula>$K16=$M16</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K18">
-    <cfRule type="expression" dxfId="8" priority="9">
-      <formula>$K18=$M18</formula>
+  <conditionalFormatting sqref="K17:K19">
+    <cfRule type="expression" dxfId="7" priority="8">
+      <formula>$K17=$M17</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K19:K21">
-    <cfRule type="expression" dxfId="7" priority="8">
-      <formula>$K19=$M19</formula>
+  <conditionalFormatting sqref="E23:E24">
+    <cfRule type="expression" dxfId="6" priority="7">
+      <formula>$E23=$M23</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E26:E27">
-    <cfRule type="expression" dxfId="6" priority="7">
-      <formula>$E26=$M26</formula>
+  <conditionalFormatting sqref="K23:K24">
+    <cfRule type="expression" dxfId="5" priority="4">
+      <formula>$K23=$M23</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="6">
+      <formula>Q23="emp"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K26:K27">
-    <cfRule type="expression" dxfId="5" priority="4">
-      <formula>$K26=$M26</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="6">
-      <formula>Q26="emp"</formula>
+  <conditionalFormatting sqref="K23:K24">
+    <cfRule type="expression" dxfId="3" priority="5">
+      <formula>Q23="emp"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K26:K27">
-    <cfRule type="expression" dxfId="3" priority="5">
-      <formula>Q26="emp"</formula>
+  <conditionalFormatting sqref="E29">
+    <cfRule type="expression" dxfId="2" priority="3">
+      <formula>$E29=$M29</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E33">
-    <cfRule type="expression" dxfId="2" priority="3">
-      <formula>$E33=$M33</formula>
+  <conditionalFormatting sqref="K29">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>Q29="emp"</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K33">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>Q33="emp"</formula>
+  <conditionalFormatting sqref="K29">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>$K29=$M29</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="K33">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>$K33=$M33</formula>
-    </cfRule>
-  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="P6" r:id="rId1" xr:uid="{FA28365E-AA3E-4C12-B848-1BAC5B0903E7}"/>
+    <hyperlink ref="P7" r:id="rId2" xr:uid="{CEC0526F-081A-4963-93B8-24BD35DC852D}"/>
+    <hyperlink ref="P8" r:id="rId3" display="'@maurilyn" xr:uid="{C41EA837-8F64-4B0D-BC0A-EF38BACCDE0A}"/>
+    <hyperlink ref="P5" r:id="rId4" xr:uid="{6393D514-18C3-41B8-90C7-8500F7D8DDEE}"/>
+  </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId5"/>
   <ignoredErrors>
-    <ignoredError sqref="E19:E20 K19:K20" formula="1"/>
+    <ignoredError sqref="E17:E18 K17:K18" formula="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100DBF2846C41E31A469E3CED25F2422E48" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d0c08e4af4d80db6585ac36ba965bb3a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2c8c20e6-817c-474f-b9c2-eb2b1ac24837" xmlns:ns4="dc8c2798-6aba-4af7-93a4-b89253b03650" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4e7db2db65f9cb533b4933096bc9b657" ns3:_="" ns4:_="">
     <xsd:import namespace="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
@@ -11857,32 +11979,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A45D7D45-1E18-48AE-827B-096C3C02C976}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83E7837-68AD-48B2-A1AB-AAB452317AF5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BDFBCCD5-5BDE-495C-BFE9-46A98A6BC529}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -11899,4 +12013,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83E7837-68AD-48B2-A1AB-AAB452317AF5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
+    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A45D7D45-1E18-48AE-827B-096C3C02C976}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Att Jogo 54 (oitavas)
</commit_message>
<xml_diff>
--- a/Mundial de Clubes FIFA 2025.xlsx
+++ b/Mundial de Clubes FIFA 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjunior\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8A4C59CE-D37A-42D2-BF3C-3DC8FF3CA272}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{F04B7A1A-BCEF-4412-A37E-76170F7F9972}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="1185" windowWidth="24240" windowHeight="13020" activeTab="3" xr2:uid="{076F3B28-812E-4458-A424-96085A053123}"/>
   </bookViews>
@@ -1673,27 +1673,6 @@
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="3" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1707,6 +1686,27 @@
     <xf numFmtId="0" fontId="23" fillId="5" borderId="43" xfId="1" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -4209,11 +4209,11 @@
       <c r="E2" s="76" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="178" t="s">
+      <c r="F2" s="182" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="178"/>
-      <c r="H2" s="178"/>
+      <c r="G2" s="182"/>
+      <c r="H2" s="182"/>
       <c r="I2" s="77" t="s">
         <v>68</v>
       </c>
@@ -6662,7 +6662,7 @@
       <c r="AL21" s="88"/>
       <c r="AM21" s="88"/>
       <c r="AN21" s="89"/>
-      <c r="AQ21" s="185" t="s">
+      <c r="AQ21" s="178" t="s">
         <v>112</v>
       </c>
     </row>
@@ -6787,7 +6787,7 @@
       <c r="AN22" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AQ22" s="186" t="s">
+      <c r="AQ22" s="179" t="s">
         <v>113</v>
       </c>
     </row>
@@ -6935,7 +6935,7 @@
         <f>VLOOKUP($AE23,$O$23:$X$26,10,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="AQ23" s="187" t="s">
+      <c r="AQ23" s="180" t="s">
         <v>117</v>
       </c>
     </row>
@@ -7083,7 +7083,7 @@
         <f t="shared" ref="AN24:AN26" si="71">VLOOKUP($AE24,$O$23:$X$26,10,FALSE)</f>
         <v>3</v>
       </c>
-      <c r="AQ24" s="187" t="s">
+      <c r="AQ24" s="180" t="s">
         <v>114</v>
       </c>
     </row>
@@ -7231,7 +7231,7 @@
         <f t="shared" si="71"/>
         <v>-4</v>
       </c>
-      <c r="AQ25" s="187" t="s">
+      <c r="AQ25" s="180" t="s">
         <v>115</v>
       </c>
     </row>
@@ -7379,7 +7379,7 @@
         <f t="shared" si="71"/>
         <v>-3</v>
       </c>
-      <c r="AQ26" s="188" t="s">
+      <c r="AQ26" s="181" t="s">
         <v>116</v>
       </c>
     </row>
@@ -10621,7 +10621,7 @@
   <dimension ref="A1:Q54"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10669,23 +10669,23 @@
     <row r="2" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" s="109"/>
-      <c r="B3" s="180" t="s">
+      <c r="B3" s="183" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="181"/>
-      <c r="D3" s="181"/>
-      <c r="E3" s="181"/>
-      <c r="F3" s="181"/>
-      <c r="G3" s="181"/>
-      <c r="H3" s="181"/>
-      <c r="I3" s="181"/>
-      <c r="J3" s="181"/>
-      <c r="K3" s="182"/>
+      <c r="C3" s="184"/>
+      <c r="D3" s="184"/>
+      <c r="E3" s="184"/>
+      <c r="F3" s="184"/>
+      <c r="G3" s="184"/>
+      <c r="H3" s="184"/>
+      <c r="I3" s="184"/>
+      <c r="J3" s="184"/>
+      <c r="K3" s="185"/>
       <c r="L3" s="110"/>
       <c r="M3" s="111"/>
       <c r="N3" s="111"/>
       <c r="O3" s="111"/>
-      <c r="P3" s="185" t="s">
+      <c r="P3" s="178" t="s">
         <v>112</v>
       </c>
       <c r="Q3" s="111"/>
@@ -10699,24 +10699,24 @@
       <c r="D4" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E4" s="183" t="s">
+      <c r="E4" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="183"/>
-      <c r="G4" s="183" t="s">
+      <c r="F4" s="186"/>
+      <c r="G4" s="186" t="s">
         <v>13</v>
       </c>
-      <c r="H4" s="183"/>
-      <c r="I4" s="183"/>
-      <c r="J4" s="183" t="s">
+      <c r="H4" s="186"/>
+      <c r="I4" s="186"/>
+      <c r="J4" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="K4" s="184"/>
+      <c r="K4" s="187"/>
       <c r="L4" s="113"/>
       <c r="M4" s="113"/>
       <c r="N4" s="113"/>
       <c r="O4" s="113"/>
-      <c r="P4" s="186" t="s">
+      <c r="P4" s="179" t="s">
         <v>113</v>
       </c>
       <c r="Q4" s="113"/>
@@ -10736,11 +10736,15 @@
         <v>Palmeiras</v>
       </c>
       <c r="F5" s="153"/>
-      <c r="G5" s="23"/>
+      <c r="G5" s="23">
+        <v>1</v>
+      </c>
       <c r="H5" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="23"/>
+      <c r="I5" s="23">
+        <v>0</v>
+      </c>
       <c r="J5" s="154"/>
       <c r="K5" s="155" t="str">
         <f>IF('Fase de Grupos'!AH12=3,'Fase de Grupos'!AF12,"2º do Grupo B")</f>
@@ -10752,9 +10756,9 @@
       </c>
       <c r="M5" s="115" t="str">
         <f>IF(OR(G5="",I5=""),"Vencedor I",IF(G5&lt;&gt;I5,IF(G5&gt;I5,E5,K5),IF(SUM(F5:G5)=SUM(I5:J5),"Vencedor I",IF(SUM(F5:G5)&gt;SUM(I5:J5),E5,K5))))</f>
-        <v>Vencedor I</v>
-      </c>
-      <c r="P5" s="187" t="s">
+        <v>Palmeiras</v>
+      </c>
+      <c r="P5" s="180" t="s">
         <v>117</v>
       </c>
     </row>
@@ -10773,11 +10777,15 @@
         <v>Benfica</v>
       </c>
       <c r="F6" s="121"/>
-      <c r="G6" s="21"/>
+      <c r="G6" s="21">
+        <v>1</v>
+      </c>
       <c r="H6" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="21"/>
+      <c r="I6" s="21">
+        <v>4</v>
+      </c>
       <c r="J6" s="122"/>
       <c r="K6" s="138" t="str">
         <f>IF('Fase de Grupos'!AH24=3,'Fase de Grupos'!AF24,"2º do Grupo D")</f>
@@ -10789,9 +10797,9 @@
       </c>
       <c r="M6" s="115" t="str">
         <f>IF(OR(G6="",I6=""),"Vencedor II",IF(G6&lt;&gt;I6,IF(G6&gt;I6,E6,K6),IF(SUM(F6:G6)=SUM(I6:J6),"Vencedor II",IF(SUM(F6:G6)&gt;SUM(I6:J6),E6,K6))))</f>
-        <v>Vencedor II</v>
-      </c>
-      <c r="P6" s="187" t="s">
+        <v>Chelsea</v>
+      </c>
+      <c r="P6" s="180" t="s">
         <v>114</v>
       </c>
     </row>
@@ -10810,11 +10818,15 @@
         <v>Paris Saint-Germain</v>
       </c>
       <c r="F7" s="121"/>
-      <c r="G7" s="21"/>
+      <c r="G7" s="21">
+        <v>4</v>
+      </c>
       <c r="H7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="I7" s="21"/>
+      <c r="I7" s="21">
+        <v>0</v>
+      </c>
       <c r="J7" s="122"/>
       <c r="K7" s="138" t="str">
         <f>IF('Fase de Grupos'!AH6=3,'Fase de Grupos'!AF6,"2º do Grupo A")</f>
@@ -10826,9 +10838,9 @@
       </c>
       <c r="M7" s="115" t="str">
         <f>IF(OR(G7="",I7=""),"Vencedor III",IF(G7&lt;&gt;I7,IF(G7&gt;I7,E7,K7),IF(SUM(F7:G7)=SUM(I7:J7),"Vencedor III",IF(SUM(F7:G7)&gt;SUM(I7:J7),E7,K7))))</f>
-        <v>Vencedor III</v>
-      </c>
-      <c r="P7" s="187" t="s">
+        <v>Paris Saint-Germain</v>
+      </c>
+      <c r="P7" s="180" t="s">
         <v>115</v>
       </c>
     </row>
@@ -10847,11 +10859,15 @@
         <v>Flamengo</v>
       </c>
       <c r="F8" s="121"/>
-      <c r="G8" s="21"/>
+      <c r="G8" s="21">
+        <v>2</v>
+      </c>
       <c r="H8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="21"/>
+      <c r="I8" s="21">
+        <v>4</v>
+      </c>
       <c r="J8" s="122"/>
       <c r="K8" s="138" t="str">
         <f>IF('Fase de Grupos'!AH18=3,'Fase de Grupos'!AF18,"2º do Grupo C")</f>
@@ -10863,9 +10879,9 @@
       </c>
       <c r="M8" s="115" t="str">
         <f>IF(OR(G8="",I8=""),"Vencedor IV",IF(G8&lt;&gt;I8,IF(G8&gt;I8,E8,K8),IF(SUM(F8:G8)=SUM(I8:J8),"Vencedor IV",IF(SUM(F8:G8)&gt;SUM(I8:J8),E8,K8))))</f>
-        <v>Vencedor IV</v>
-      </c>
-      <c r="P8" s="188" t="s">
+        <v>Bayern de Munique</v>
+      </c>
+      <c r="P8" s="181" t="s">
         <v>116</v>
       </c>
     </row>
@@ -10884,11 +10900,15 @@
         <v>Internazionale</v>
       </c>
       <c r="F9" s="121"/>
-      <c r="G9" s="21"/>
+      <c r="G9" s="21">
+        <v>0</v>
+      </c>
       <c r="H9" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="I9" s="21"/>
+      <c r="I9" s="21">
+        <v>2</v>
+      </c>
       <c r="J9" s="122"/>
       <c r="K9" s="138" t="str">
         <f>IF('Fase de Grupos'!AH36=3,'Fase de Grupos'!AF36,"2º do Grupo F")</f>
@@ -10900,7 +10920,7 @@
       </c>
       <c r="M9" s="115" t="str">
         <f>IF(OR(G9="",I9=""),"Vencedor V",IF(G9&lt;&gt;I9,IF(G9&gt;I9,E9,K9),IF(SUM(F9:G9)=SUM(I9:J9),"Vencedor V",IF(SUM(F9:G9)&gt;SUM(I9:J9),E9,K9))))</f>
-        <v>Vencedor V</v>
+        <v>Fluminense</v>
       </c>
     </row>
     <row r="10" spans="1:17" x14ac:dyDescent="0.25">
@@ -10918,11 +10938,15 @@
         <v>Manchester City</v>
       </c>
       <c r="F10" s="121"/>
-      <c r="G10" s="21"/>
+      <c r="G10" s="21">
+        <v>3</v>
+      </c>
       <c r="H10" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="I10" s="21"/>
+      <c r="I10" s="21">
+        <v>4</v>
+      </c>
       <c r="J10" s="122"/>
       <c r="K10" s="138" t="str">
         <f>IF('Fase de Grupos'!AH48=3,'Fase de Grupos'!AF48,"2º do Grupo H")</f>
@@ -10934,7 +10958,7 @@
       </c>
       <c r="M10" s="115" t="str">
         <f>IF(OR(G10="",I10=""),"Vencedor VI",IF(G10&lt;&gt;I10,IF(G10&gt;I10,E10,K10),IF(SUM(F10:G10)=SUM(I10:J10),"Vencedor VI",IF(SUM(F10:G10)&gt;SUM(I10:J10),E10,K10))))</f>
-        <v>Vencedor VI</v>
+        <v>Al-Hilal</v>
       </c>
     </row>
     <row r="11" spans="1:17" x14ac:dyDescent="0.25">
@@ -11010,18 +11034,18 @@
     </row>
     <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="109"/>
-      <c r="B14" s="180" t="s">
+      <c r="B14" s="183" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="181"/>
-      <c r="D14" s="181"/>
-      <c r="E14" s="181"/>
-      <c r="F14" s="181"/>
-      <c r="G14" s="181"/>
-      <c r="H14" s="181"/>
-      <c r="I14" s="181"/>
-      <c r="J14" s="181"/>
-      <c r="K14" s="182"/>
+      <c r="C14" s="184"/>
+      <c r="D14" s="184"/>
+      <c r="E14" s="184"/>
+      <c r="F14" s="184"/>
+      <c r="G14" s="184"/>
+      <c r="H14" s="184"/>
+      <c r="I14" s="184"/>
+      <c r="J14" s="184"/>
+      <c r="K14" s="185"/>
       <c r="L14" s="110"/>
       <c r="M14" s="111"/>
       <c r="N14" s="111"/>
@@ -11034,19 +11058,19 @@
       <c r="D15" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E15" s="183" t="s">
+      <c r="E15" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="F15" s="183"/>
-      <c r="G15" s="183" t="s">
+      <c r="F15" s="186"/>
+      <c r="G15" s="186" t="s">
         <v>13</v>
       </c>
-      <c r="H15" s="183"/>
-      <c r="I15" s="183"/>
-      <c r="J15" s="183" t="s">
+      <c r="H15" s="186"/>
+      <c r="I15" s="186"/>
+      <c r="J15" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="K15" s="184"/>
+      <c r="K15" s="187"/>
     </row>
     <row r="16" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B16" s="129" t="s">
@@ -11060,7 +11084,7 @@
       </c>
       <c r="E16" s="157" t="str">
         <f>M5</f>
-        <v>Vencedor I</v>
+        <v>Palmeiras</v>
       </c>
       <c r="F16" s="158"/>
       <c r="G16" s="23"/>
@@ -11071,7 +11095,7 @@
       <c r="J16" s="159"/>
       <c r="K16" s="160" t="str">
         <f>M6</f>
-        <v>Vencedor II</v>
+        <v>Chelsea</v>
       </c>
       <c r="L16" s="114" t="str">
         <f>IF(OR(G16="",I16=""),"",IF(G16=I16,"emp",""))</f>
@@ -11094,7 +11118,7 @@
       </c>
       <c r="E17" s="24" t="str">
         <f>M9</f>
-        <v>Vencedor V</v>
+        <v>Fluminense</v>
       </c>
       <c r="F17" s="125"/>
       <c r="G17" s="21"/>
@@ -11105,7 +11129,7 @@
       <c r="J17" s="126"/>
       <c r="K17" s="143" t="str">
         <f>M10</f>
-        <v>Vencedor VI</v>
+        <v>Al-Hilal</v>
       </c>
       <c r="L17" s="114" t="str">
         <f t="shared" ref="L17:L19" si="1">IF(OR(G17="",I17=""),"",IF(G17=I17,"emp",""))</f>
@@ -11128,7 +11152,7 @@
       </c>
       <c r="E18" s="24" t="str">
         <f>M7</f>
-        <v>Vencedor III</v>
+        <v>Paris Saint-Germain</v>
       </c>
       <c r="F18" s="125"/>
       <c r="G18" s="21"/>
@@ -11139,7 +11163,7 @@
       <c r="J18" s="126"/>
       <c r="K18" s="143" t="str">
         <f>M8</f>
-        <v>Vencedor IV</v>
+        <v>Bayern de Munique</v>
       </c>
       <c r="L18" s="114" t="str">
         <f t="shared" si="1"/>
@@ -11189,18 +11213,18 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="109"/>
-      <c r="B21" s="180" t="s">
+      <c r="B21" s="183" t="s">
         <v>62</v>
       </c>
-      <c r="C21" s="181"/>
-      <c r="D21" s="181"/>
-      <c r="E21" s="181"/>
-      <c r="F21" s="181"/>
-      <c r="G21" s="181"/>
-      <c r="H21" s="181"/>
-      <c r="I21" s="181"/>
-      <c r="J21" s="181"/>
-      <c r="K21" s="182"/>
+      <c r="C21" s="184"/>
+      <c r="D21" s="184"/>
+      <c r="E21" s="184"/>
+      <c r="F21" s="184"/>
+      <c r="G21" s="184"/>
+      <c r="H21" s="184"/>
+      <c r="I21" s="184"/>
+      <c r="J21" s="184"/>
+      <c r="K21" s="185"/>
       <c r="L21" s="110"/>
       <c r="M21" s="111"/>
       <c r="N21" s="111"/>
@@ -11216,19 +11240,19 @@
       <c r="D22" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="183" t="s">
+      <c r="E22" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="F22" s="183"/>
-      <c r="G22" s="183" t="s">
+      <c r="F22" s="186"/>
+      <c r="G22" s="186" t="s">
         <v>13</v>
       </c>
-      <c r="H22" s="183"/>
-      <c r="I22" s="183"/>
-      <c r="J22" s="183" t="s">
+      <c r="H22" s="186"/>
+      <c r="I22" s="186"/>
+      <c r="J22" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="K22" s="184"/>
+      <c r="K22" s="187"/>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B23" s="151" t="s">
@@ -11314,18 +11338,18 @@
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A27" s="109"/>
-      <c r="B27" s="180" t="s">
+      <c r="B27" s="183" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="181"/>
-      <c r="D27" s="181"/>
-      <c r="E27" s="181"/>
-      <c r="F27" s="181"/>
-      <c r="G27" s="181"/>
-      <c r="H27" s="181"/>
-      <c r="I27" s="181"/>
-      <c r="J27" s="181"/>
-      <c r="K27" s="182"/>
+      <c r="C27" s="184"/>
+      <c r="D27" s="184"/>
+      <c r="E27" s="184"/>
+      <c r="F27" s="184"/>
+      <c r="G27" s="184"/>
+      <c r="H27" s="184"/>
+      <c r="I27" s="184"/>
+      <c r="J27" s="184"/>
+      <c r="K27" s="185"/>
       <c r="L27" s="110"/>
       <c r="M27" s="111"/>
       <c r="N27" s="111"/>
@@ -11341,19 +11365,19 @@
       <c r="D28" s="150" t="s">
         <v>11</v>
       </c>
-      <c r="E28" s="183" t="s">
+      <c r="E28" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="F28" s="183"/>
-      <c r="G28" s="183" t="s">
+      <c r="F28" s="186"/>
+      <c r="G28" s="186" t="s">
         <v>13</v>
       </c>
-      <c r="H28" s="183"/>
-      <c r="I28" s="183"/>
-      <c r="J28" s="183" t="s">
+      <c r="H28" s="186"/>
+      <c r="I28" s="186"/>
+      <c r="J28" s="186" t="s">
         <v>12</v>
       </c>
-      <c r="K28" s="184"/>
+      <c r="K28" s="187"/>
     </row>
     <row r="29" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B29" s="161" t="s">
@@ -11401,11 +11425,11 @@
     </row>
     <row r="32" spans="1:17" s="137" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="135"/>
-      <c r="B32" s="179" t="s">
+      <c r="B32" s="188" t="s">
         <v>66</v>
       </c>
-      <c r="C32" s="179"/>
-      <c r="D32" s="179"/>
+      <c r="C32" s="188"/>
+      <c r="D32" s="188"/>
       <c r="E32" s="173" t="str">
         <f>IF(M29="1º Lugar","",M29)</f>
         <v/>
@@ -11425,11 +11449,11 @@
     </row>
     <row r="33" spans="1:17" s="137" customFormat="1" ht="25.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="135"/>
-      <c r="B33" s="179" t="s">
+      <c r="B33" s="188" t="s">
         <v>106</v>
       </c>
-      <c r="C33" s="179"/>
-      <c r="D33" s="179"/>
+      <c r="C33" s="188"/>
+      <c r="D33" s="188"/>
       <c r="E33" s="175" t="str">
         <f>IF(M30="2º Lugar","",M30)</f>
         <v/>
@@ -11557,11 +11581,12 @@
   </sheetData>
   <sheetProtection password="CC01" sheet="1" selectLockedCells="1"/>
   <mergeCells count="18">
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="E4:F4"/>
-    <mergeCell ref="G4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="B14:K14"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B27:K27"/>
+    <mergeCell ref="E28:F28"/>
+    <mergeCell ref="G28:I28"/>
+    <mergeCell ref="J28:K28"/>
+    <mergeCell ref="B32:D32"/>
     <mergeCell ref="B21:K21"/>
     <mergeCell ref="E22:F22"/>
     <mergeCell ref="G22:I22"/>
@@ -11569,12 +11594,11 @@
     <mergeCell ref="E15:F15"/>
     <mergeCell ref="G15:I15"/>
     <mergeCell ref="J15:K15"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B27:K27"/>
-    <mergeCell ref="E28:F28"/>
-    <mergeCell ref="G28:I28"/>
-    <mergeCell ref="J28:K28"/>
-    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="E4:F4"/>
+    <mergeCell ref="G4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="B14:K14"/>
   </mergeCells>
   <conditionalFormatting sqref="F5">
     <cfRule type="expression" dxfId="31" priority="128">
@@ -11980,20 +12004,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="dc8c2798-6aba-4af7-93a4-b89253b03650" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -12016,26 +12040,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83E7837-68AD-48B2-A1AB-AAB452317AF5}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A45D7D45-1E18-48AE-827B-096C3C02C976}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
-    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A45D7D45-1E18-48AE-827B-096C3C02C976}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83E7837-68AD-48B2-A1AB-AAB452317AF5}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Com todos os resultados
</commit_message>
<xml_diff>
--- a/Mundial de Clubes FIFA 2025.xlsx
+++ b/Mundial de Clubes FIFA 2025.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mjunior\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3280A3D5-8391-42FE-8C4F-6C1420ED7D29}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0AAC8A65-4C90-408C-B210-27AAACF65CEE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-24120" yWindow="1185" windowWidth="24240" windowHeight="13020" activeTab="3" xr2:uid="{076F3B28-812E-4458-A424-96085A053123}"/>
   </bookViews>
@@ -10621,7 +10621,7 @@
   <dimension ref="A1:Q54"/>
   <sheetViews>
     <sheetView showRowColHeaders="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11095,11 +11095,15 @@
         <v>Palmeiras</v>
       </c>
       <c r="F16" s="158"/>
-      <c r="G16" s="23"/>
+      <c r="G16" s="23">
+        <v>1</v>
+      </c>
       <c r="H16" s="99" t="s">
         <v>17</v>
       </c>
-      <c r="I16" s="23"/>
+      <c r="I16" s="23">
+        <v>2</v>
+      </c>
       <c r="J16" s="159"/>
       <c r="K16" s="160" t="str">
         <f>M6</f>
@@ -11111,7 +11115,7 @@
       </c>
       <c r="M16" s="115" t="str">
         <f>IF(OR(G16="",I16=""),"Vencedor A",IF(G16&lt;&gt;I16,IF(G16&gt;I16,E16,K16),IF(SUM(F16:G16)=SUM(I16:J16),"Vencedor A",IF(SUM(F16:G16)&gt;SUM(I16:J16),E16,K16))))</f>
-        <v>Vencedor A</v>
+        <v>Chelsea</v>
       </c>
     </row>
     <row r="17" spans="1:17" x14ac:dyDescent="0.25">
@@ -11129,11 +11133,15 @@
         <v>Fluminense</v>
       </c>
       <c r="F17" s="125"/>
-      <c r="G17" s="21"/>
+      <c r="G17" s="21">
+        <v>2</v>
+      </c>
       <c r="H17" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="I17" s="21"/>
+      <c r="I17" s="21">
+        <v>1</v>
+      </c>
       <c r="J17" s="126"/>
       <c r="K17" s="143" t="str">
         <f>M10</f>
@@ -11145,7 +11153,7 @@
       </c>
       <c r="M17" s="115" t="str">
         <f>IF(OR(G17="",I17=""),"Vencedor B",IF(G17&lt;&gt;I17,IF(G17&gt;I17,E17,K17),IF(SUM(F17:G17)=SUM(I17:J17),"Vencedor B",IF(SUM(F17:G17)&gt;SUM(I17:J17),E17,K17))))</f>
-        <v>Vencedor B</v>
+        <v>Fluminense</v>
       </c>
     </row>
     <row r="18" spans="1:17" x14ac:dyDescent="0.25">
@@ -11163,11 +11171,15 @@
         <v>Paris Saint-Germain</v>
       </c>
       <c r="F18" s="125"/>
-      <c r="G18" s="21"/>
+      <c r="G18" s="21">
+        <v>2</v>
+      </c>
       <c r="H18" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="I18" s="21"/>
+      <c r="I18" s="21">
+        <v>0</v>
+      </c>
       <c r="J18" s="126"/>
       <c r="K18" s="143" t="str">
         <f>M8</f>
@@ -11179,7 +11191,7 @@
       </c>
       <c r="M18" s="115" t="str">
         <f>IF(OR(G18="",I18=""),"Vencedor C",IF(G18&lt;&gt;I18,IF(G18&gt;I18,E18,K18),IF(SUM(F18:G18)=SUM(I18:J18),"Vencedor C",IF(SUM(F18:G18)&gt;SUM(I18:J18),E18,K18))))</f>
-        <v>Vencedor C</v>
+        <v>Paris Saint-Germain</v>
       </c>
     </row>
     <row r="19" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11197,11 +11209,15 @@
         <v>Borussia Dortmund</v>
       </c>
       <c r="F19" s="145"/>
-      <c r="G19" s="22"/>
+      <c r="G19" s="22">
+        <v>2</v>
+      </c>
       <c r="H19" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="I19" s="22"/>
+      <c r="I19" s="22">
+        <v>3</v>
+      </c>
       <c r="J19" s="146"/>
       <c r="K19" s="147" t="str">
         <f>M12</f>
@@ -11213,7 +11229,7 @@
       </c>
       <c r="M19" s="115" t="str">
         <f>IF(OR(G19="",I19=""),"Vencedor D",IF(G19&lt;&gt;I19,IF(G19&gt;I19,E19,K19),IF(SUM(F19:G19)=SUM(I19:J19),"Vencedor D",IF(SUM(F19:G19)&gt;SUM(I19:J19),E19,K19))))</f>
-        <v>Vencedor D</v>
+        <v>Real Madrid</v>
       </c>
     </row>
     <row r="20" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11274,18 +11290,22 @@
       </c>
       <c r="E23" s="20" t="str">
         <f>M16</f>
-        <v>Vencedor A</v>
+        <v>Chelsea</v>
       </c>
       <c r="F23" s="153"/>
-      <c r="G23" s="23"/>
+      <c r="G23" s="23">
+        <v>2</v>
+      </c>
       <c r="H23" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="I23" s="23"/>
+      <c r="I23" s="23">
+        <v>0</v>
+      </c>
       <c r="J23" s="154"/>
       <c r="K23" s="155" t="str">
         <f>M17</f>
-        <v>Vencedor B</v>
+        <v>Fluminense</v>
       </c>
       <c r="L23" s="114" t="str">
         <f>IF(OR(G23="",I23=""),"",IF(G23=I23,"emp",""))</f>
@@ -11293,7 +11313,7 @@
       </c>
       <c r="M23" s="115" t="str">
         <f>IF(OR(G23="",I23=""),"Vencedor S1",IF(G23&lt;&gt;I23,IF(G23&gt;I23,E23,K23),IF(SUM(F23:G23)=SUM(I23:J23),"Vencedor S1",IF(SUM(F23:G23)&gt;SUM(I23:J23),E23,K23))))</f>
-        <v>Vencedor S1</v>
+        <v>Chelsea</v>
       </c>
     </row>
     <row r="24" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -11308,18 +11328,22 @@
       </c>
       <c r="E24" s="15" t="str">
         <f>M18</f>
-        <v>Vencedor C</v>
+        <v>Paris Saint-Germain</v>
       </c>
       <c r="F24" s="140"/>
-      <c r="G24" s="22"/>
+      <c r="G24" s="22">
+        <v>4</v>
+      </c>
       <c r="H24" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="I24" s="22"/>
+      <c r="I24" s="22">
+        <v>0</v>
+      </c>
       <c r="J24" s="141"/>
       <c r="K24" s="142" t="str">
         <f>M19</f>
-        <v>Vencedor D</v>
+        <v>Real Madrid</v>
       </c>
       <c r="L24" s="114" t="str">
         <f t="shared" ref="L24" si="2">IF(OR(G24="",I24=""),"",IF(G24=I24,"emp",""))</f>
@@ -11327,21 +11351,21 @@
       </c>
       <c r="M24" s="115" t="str">
         <f>IF(OR(G24="",I24=""),"Vencedor S2",IF(G24&lt;&gt;I24,IF(G24&gt;I24,E24,K24),IF(SUM(F24:G24)=SUM(I24:J24),"Vencedor S2",IF(SUM(F24:G24)&gt;SUM(I24:J24),E24,K24))))</f>
-        <v>Vencedor S2</v>
+        <v>Paris Saint-Germain</v>
       </c>
     </row>
     <row r="25" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C25" s="116"/>
       <c r="M25" s="115" t="str">
         <f>IF(OR(G23="",I23=""),"Perdedor S1",IF(G23&lt;&gt;I23,IF(G23&lt;I23,E23,K23),IF(SUM(F23:G23)=SUM(I23:J23),"Perdedor S1",IF(SUM(F23:G23)&lt;SUM(I23:J23),E23,K23))))</f>
-        <v>Perdedor S1</v>
+        <v>Fluminense</v>
       </c>
     </row>
     <row r="26" spans="1:17" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="116"/>
       <c r="M26" s="115" t="str">
         <f>IF(OR(G24="",I24=""),"Perdedor S2",IF(G24&lt;&gt;I24,IF(G24&lt;I24,E24,K24),IF(SUM(F24:G24)=SUM(I24:J24),"Perdedor S2",IF(SUM(F24:G24)&lt;SUM(I24:J24),E24,K24))))</f>
-        <v>Perdedor S2</v>
+        <v>Real Madrid</v>
       </c>
     </row>
     <row r="27" spans="1:17" x14ac:dyDescent="0.25">
@@ -11399,18 +11423,22 @@
       </c>
       <c r="E29" s="164" t="str">
         <f>M23</f>
-        <v>Vencedor S1</v>
+        <v>Chelsea</v>
       </c>
       <c r="F29" s="165"/>
-      <c r="G29" s="166"/>
+      <c r="G29" s="166">
+        <v>3</v>
+      </c>
       <c r="H29" s="167" t="s">
         <v>17</v>
       </c>
-      <c r="I29" s="166"/>
+      <c r="I29" s="166">
+        <v>0</v>
+      </c>
       <c r="J29" s="168"/>
       <c r="K29" s="169" t="str">
         <f>M24</f>
-        <v>Vencedor S2</v>
+        <v>Paris Saint-Germain</v>
       </c>
       <c r="L29" s="114" t="str">
         <f>IF(OR(G29="",I29=""),"",IF(G29=I29,"emp",""))</f>
@@ -11418,14 +11446,14 @@
       </c>
       <c r="M29" s="115" t="str">
         <f>IF(OR(G29="",I29=""),"1º Lugar",IF(G29&lt;&gt;I29,IF(G29&gt;I29,E29,K29),IF(SUM(F29:G29)=SUM(I29:J29),"1º Lugar",IF(SUM(F29:G29)&gt;SUM(I29:J29),E29,K29))))</f>
-        <v>1º Lugar</v>
+        <v>Chelsea</v>
       </c>
     </row>
     <row r="30" spans="1:17" x14ac:dyDescent="0.25">
       <c r="C30" s="116"/>
       <c r="M30" s="115" t="str">
         <f>IF(OR(G29="",I29=""),"2º Lugar",IF(G29&lt;&gt;I29,IF(G29&lt;I29,E29,K29),IF(SUM(F29:G29)=SUM(I29:J29),"2º Lugar",IF(SUM(F29:G29)&lt;SUM(I29:J29),E29,K29))))</f>
-        <v>2º Lugar</v>
+        <v>Paris Saint-Germain</v>
       </c>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
@@ -11440,7 +11468,7 @@
       <c r="D32" s="183"/>
       <c r="E32" s="173" t="str">
         <f>IF(M29="1º Lugar","",M29)</f>
-        <v/>
+        <v>Chelsea</v>
       </c>
       <c r="F32" s="173"/>
       <c r="G32" s="173"/>
@@ -11464,7 +11492,7 @@
       <c r="D33" s="183"/>
       <c r="E33" s="175" t="str">
         <f>IF(M30="2º Lugar","",M30)</f>
-        <v/>
+        <v>Paris Saint-Germain</v>
       </c>
       <c r="F33" s="175"/>
       <c r="G33" s="175"/>
@@ -12032,15 +12060,15 @@
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C83E7837-68AD-48B2-A1AB-AAB452317AF5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
     <ds:schemaRef ds:uri="dc8c2798-6aba-4af7-93a4-b89253b03650"/>
     <ds:schemaRef ds:uri="2c8c20e6-817c-474f-b9c2-eb2b1ac24837"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>